<commit_message>
Updated BB notes and also added full param estimates for rstan
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2140" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="OSPREE" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="211">
   <si>
     <t>param</t>
   </si>
@@ -227,12 +227,486 @@
   <si>
     <t>centered and scaled (z-score) brms</t>
   </si>
+  <si>
+    <t>sigma_a_sp</t>
+  </si>
+  <si>
+    <t>sigma_b_force_sp</t>
+  </si>
+  <si>
+    <t>sigma_b_photo_sp</t>
+  </si>
+  <si>
+    <t>sigma_b_chill_sp</t>
+  </si>
+  <si>
+    <t>sigma_y</t>
+  </si>
+  <si>
+    <t>a_sp[1]</t>
+  </si>
+  <si>
+    <t>a_sp[2]</t>
+  </si>
+  <si>
+    <t>a_sp[3]</t>
+  </si>
+  <si>
+    <t>a_sp[4]</t>
+  </si>
+  <si>
+    <t>a_sp[5]</t>
+  </si>
+  <si>
+    <t>a_sp[6]</t>
+  </si>
+  <si>
+    <t>a_sp[7]</t>
+  </si>
+  <si>
+    <t>a_sp[8]</t>
+  </si>
+  <si>
+    <t>a_sp[9]</t>
+  </si>
+  <si>
+    <t>a_sp[10]</t>
+  </si>
+  <si>
+    <t>a_sp[11]</t>
+  </si>
+  <si>
+    <t>a_sp[12]</t>
+  </si>
+  <si>
+    <t>a_sp[13]</t>
+  </si>
+  <si>
+    <t>a_sp[14]</t>
+  </si>
+  <si>
+    <t>a_sp[15]</t>
+  </si>
+  <si>
+    <t>a_sp[16]</t>
+  </si>
+  <si>
+    <t>a_sp[17]</t>
+  </si>
+  <si>
+    <t>a_sp[18]</t>
+  </si>
+  <si>
+    <t>a_sp[19]</t>
+  </si>
+  <si>
+    <t>a_sp[20]</t>
+  </si>
+  <si>
+    <t>a_sp[21]</t>
+  </si>
+  <si>
+    <t>a_sp[22]</t>
+  </si>
+  <si>
+    <t>a_sp[23]</t>
+  </si>
+  <si>
+    <t>a_sp[24]</t>
+  </si>
+  <si>
+    <t>a_sp[25]</t>
+  </si>
+  <si>
+    <t>a_sp[26]</t>
+  </si>
+  <si>
+    <t>a_sp[27]</t>
+  </si>
+  <si>
+    <t>a_sp[28]</t>
+  </si>
+  <si>
+    <t>a_sp[29]</t>
+  </si>
+  <si>
+    <t>a_sp[30]</t>
+  </si>
+  <si>
+    <t>a_sp[31]</t>
+  </si>
+  <si>
+    <t>a_sp[32]</t>
+  </si>
+  <si>
+    <t>a_sp[33]</t>
+  </si>
+  <si>
+    <t>a_sp[34]</t>
+  </si>
+  <si>
+    <t>a_sp[35]</t>
+  </si>
+  <si>
+    <t>a_sp[36]</t>
+  </si>
+  <si>
+    <t>a_sp[37]</t>
+  </si>
+  <si>
+    <t>a_sp[38]</t>
+  </si>
+  <si>
+    <t>b_force[1]</t>
+  </si>
+  <si>
+    <t>b_force[2]</t>
+  </si>
+  <si>
+    <t>b_force[3]</t>
+  </si>
+  <si>
+    <t>b_force[4]</t>
+  </si>
+  <si>
+    <t>b_force[5]</t>
+  </si>
+  <si>
+    <t>b_force[6]</t>
+  </si>
+  <si>
+    <t>b_force[7]</t>
+  </si>
+  <si>
+    <t>b_force[8]</t>
+  </si>
+  <si>
+    <t>b_force[9]</t>
+  </si>
+  <si>
+    <t>b_force[10]</t>
+  </si>
+  <si>
+    <t>b_force[11]</t>
+  </si>
+  <si>
+    <t>b_force[12]</t>
+  </si>
+  <si>
+    <t>b_force[13]</t>
+  </si>
+  <si>
+    <t>b_force[14]</t>
+  </si>
+  <si>
+    <t>b_force[15]</t>
+  </si>
+  <si>
+    <t>b_force[16]</t>
+  </si>
+  <si>
+    <t>b_force[17]</t>
+  </si>
+  <si>
+    <t>b_force[18]</t>
+  </si>
+  <si>
+    <t>b_force[19]</t>
+  </si>
+  <si>
+    <t>b_force[20]</t>
+  </si>
+  <si>
+    <t>b_force[21]</t>
+  </si>
+  <si>
+    <t>b_force[22]</t>
+  </si>
+  <si>
+    <t>b_force[23]</t>
+  </si>
+  <si>
+    <t>b_force[24]</t>
+  </si>
+  <si>
+    <t>b_force[25]</t>
+  </si>
+  <si>
+    <t>b_force[26]</t>
+  </si>
+  <si>
+    <t>b_force[27]</t>
+  </si>
+  <si>
+    <t>b_force[28]</t>
+  </si>
+  <si>
+    <t>b_force[29]</t>
+  </si>
+  <si>
+    <t>b_force[30]</t>
+  </si>
+  <si>
+    <t>b_force[31]</t>
+  </si>
+  <si>
+    <t>b_force[32]</t>
+  </si>
+  <si>
+    <t>b_force[33]</t>
+  </si>
+  <si>
+    <t>b_force[34]</t>
+  </si>
+  <si>
+    <t>b_force[35]</t>
+  </si>
+  <si>
+    <t>b_force[36]</t>
+  </si>
+  <si>
+    <t>b_force[37]</t>
+  </si>
+  <si>
+    <t>b_force[38]</t>
+  </si>
+  <si>
+    <t>b_photo[1]</t>
+  </si>
+  <si>
+    <t>b_photo[2]</t>
+  </si>
+  <si>
+    <t>b_photo[3]</t>
+  </si>
+  <si>
+    <t>b_photo[4]</t>
+  </si>
+  <si>
+    <t>b_photo[5]</t>
+  </si>
+  <si>
+    <t>b_photo[6]</t>
+  </si>
+  <si>
+    <t>b_photo[7]</t>
+  </si>
+  <si>
+    <t>b_photo[8]</t>
+  </si>
+  <si>
+    <t>b_photo[9]</t>
+  </si>
+  <si>
+    <t>b_photo[10]</t>
+  </si>
+  <si>
+    <t>b_photo[11]</t>
+  </si>
+  <si>
+    <t>b_photo[12]</t>
+  </si>
+  <si>
+    <t>b_photo[13]</t>
+  </si>
+  <si>
+    <t>b_photo[14]</t>
+  </si>
+  <si>
+    <t>b_photo[15]</t>
+  </si>
+  <si>
+    <t>b_photo[16]</t>
+  </si>
+  <si>
+    <t>b_photo[17]</t>
+  </si>
+  <si>
+    <t>b_photo[18]</t>
+  </si>
+  <si>
+    <t>b_photo[19]</t>
+  </si>
+  <si>
+    <t>b_photo[20]</t>
+  </si>
+  <si>
+    <t>b_photo[21]</t>
+  </si>
+  <si>
+    <t>b_photo[22]</t>
+  </si>
+  <si>
+    <t>b_photo[23]</t>
+  </si>
+  <si>
+    <t>b_photo[24]</t>
+  </si>
+  <si>
+    <t>b_photo[25]</t>
+  </si>
+  <si>
+    <t>b_photo[26]</t>
+  </si>
+  <si>
+    <t>b_photo[27]</t>
+  </si>
+  <si>
+    <t>b_photo[28]</t>
+  </si>
+  <si>
+    <t>b_photo[29]</t>
+  </si>
+  <si>
+    <t>b_photo[30]</t>
+  </si>
+  <si>
+    <t>b_photo[31]</t>
+  </si>
+  <si>
+    <t>b_photo[32]</t>
+  </si>
+  <si>
+    <t>b_photo[33]</t>
+  </si>
+  <si>
+    <t>b_photo[34]</t>
+  </si>
+  <si>
+    <t>b_photo[35]</t>
+  </si>
+  <si>
+    <t>b_photo[36]</t>
+  </si>
+  <si>
+    <t>b_photo[37]</t>
+  </si>
+  <si>
+    <t>b_photo[38]</t>
+  </si>
+  <si>
+    <t>b_chill[1]</t>
+  </si>
+  <si>
+    <t>b_chill[2]</t>
+  </si>
+  <si>
+    <t>b_chill[3]</t>
+  </si>
+  <si>
+    <t>b_chill[4]</t>
+  </si>
+  <si>
+    <t>b_chill[5]</t>
+  </si>
+  <si>
+    <t>b_chill[6]</t>
+  </si>
+  <si>
+    <t>b_chill[7]</t>
+  </si>
+  <si>
+    <t>b_chill[8]</t>
+  </si>
+  <si>
+    <t>b_chill[9]</t>
+  </si>
+  <si>
+    <t>b_chill[10]</t>
+  </si>
+  <si>
+    <t>b_chill[11]</t>
+  </si>
+  <si>
+    <t>b_chill[12]</t>
+  </si>
+  <si>
+    <t>b_chill[13]</t>
+  </si>
+  <si>
+    <t>b_chill[14]</t>
+  </si>
+  <si>
+    <t>b_chill[15]</t>
+  </si>
+  <si>
+    <t>b_chill[16]</t>
+  </si>
+  <si>
+    <t>b_chill[17]</t>
+  </si>
+  <si>
+    <t>b_chill[18]</t>
+  </si>
+  <si>
+    <t>b_chill[19]</t>
+  </si>
+  <si>
+    <t>b_chill[20]</t>
+  </si>
+  <si>
+    <t>b_chill[21]</t>
+  </si>
+  <si>
+    <t>b_chill[22]</t>
+  </si>
+  <si>
+    <t>b_chill[23]</t>
+  </si>
+  <si>
+    <t>b_chill[24]</t>
+  </si>
+  <si>
+    <t>b_chill[25]</t>
+  </si>
+  <si>
+    <t>b_chill[26]</t>
+  </si>
+  <si>
+    <t>b_chill[27]</t>
+  </si>
+  <si>
+    <t>b_chill[28]</t>
+  </si>
+  <si>
+    <t>b_chill[29]</t>
+  </si>
+  <si>
+    <t>b_chill[30]</t>
+  </si>
+  <si>
+    <t>b_chill[31]</t>
+  </si>
+  <si>
+    <t>b_chill[32]</t>
+  </si>
+  <si>
+    <t>b_chill[33]</t>
+  </si>
+  <si>
+    <t>b_chill[34]</t>
+  </si>
+  <si>
+    <t>b_chill[35]</t>
+  </si>
+  <si>
+    <t>b_chill[36]</t>
+  </si>
+  <si>
+    <t>b_chill[37]</t>
+  </si>
+  <si>
+    <t>b_chill[38]</t>
+  </si>
+  <si>
+    <t>sumer.wi (see models_stan_plotting.R)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,6 +741,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -369,7 +850,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="55">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -425,8 +906,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -450,8 +939,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="55">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -479,6 +969,10 @@
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -506,6 +1000,10 @@
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -835,10 +1333,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R10"/>
+  <dimension ref="A1:R177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+      <selection activeCell="F14" sqref="F14:F177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1219,6 +1717,1815 @@
       </c>
       <c r="N10">
         <v>0.26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="C13" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="17">
+        <v>94.814463700000005</v>
+      </c>
+      <c r="F14">
+        <v>28.872777539617999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="17">
+        <v>-1.860117198</v>
+      </c>
+      <c r="F15">
+        <v>-4.9562006055646002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="17">
+        <v>-1.3263480139999999</v>
+      </c>
+      <c r="F16">
+        <v>-4.2589914505628004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="17">
+        <v>-6.8969933729999999</v>
+      </c>
+      <c r="F17">
+        <v>-10.240670101168901</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="17">
+        <v>25.112935619999998</v>
+      </c>
+      <c r="F18">
+        <v>9.8248067343748602</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="17">
+        <v>1.029588543</v>
+      </c>
+      <c r="F19">
+        <v>5.9249822487714203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="17">
+        <v>0.85328422800000003</v>
+      </c>
+      <c r="F20">
+        <v>5.5081353669091202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="17">
+        <v>1.9058692450000001</v>
+      </c>
+      <c r="F21">
+        <v>6.8662963935424903</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="17">
+        <v>14.64285143</v>
+      </c>
+      <c r="F22">
+        <v>14.576457996142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="17">
+        <v>110.5143128</v>
+      </c>
+      <c r="F23">
+        <v>36.0742584453942</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="17">
+        <v>79.248405340000005</v>
+      </c>
+      <c r="F24">
+        <v>29.777249149686501</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" s="17">
+        <v>117.639062</v>
+      </c>
+      <c r="F25">
+        <v>37.084387520987001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="17">
+        <v>93.611210380000003</v>
+      </c>
+      <c r="F26">
+        <v>31.6588994701502</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="17">
+        <v>77.547297169999993</v>
+      </c>
+      <c r="F27">
+        <v>31.9968569977116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="17">
+        <v>106.098086</v>
+      </c>
+      <c r="F28">
+        <v>32.2374466525226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="17">
+        <v>100.1006405</v>
+      </c>
+      <c r="F29">
+        <v>31.6828410408663</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="17">
+        <v>99.937920500000004</v>
+      </c>
+      <c r="F30">
+        <v>28.511381598813699</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="17">
+        <v>54.929282360000002</v>
+      </c>
+      <c r="F31">
+        <v>18.9990208169569</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="17">
+        <v>52.213019520000003</v>
+      </c>
+      <c r="F32">
+        <v>18.5438871879768</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="17">
+        <v>96.846787230000004</v>
+      </c>
+      <c r="F33">
+        <v>29.4793194429358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="17">
+        <v>95.262957450000002</v>
+      </c>
+      <c r="F34">
+        <v>27.025363791550301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="17">
+        <v>87.891082220000001</v>
+      </c>
+      <c r="F35">
+        <v>22.741965056386402</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="17">
+        <v>85.843369199999998</v>
+      </c>
+      <c r="F36">
+        <v>19.607586871152499</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="17">
+        <v>152.1433112</v>
+      </c>
+      <c r="F37">
+        <v>46.869632122144502</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="17">
+        <v>143.9225194</v>
+      </c>
+      <c r="F38">
+        <v>53.760615123866799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C39" s="17">
+        <v>95.667895459999997</v>
+      </c>
+      <c r="F39">
+        <v>35.259097752470602</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="17">
+        <v>73.744354599999994</v>
+      </c>
+      <c r="F40">
+        <v>20.147456494830301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="17">
+        <v>106.9252761</v>
+      </c>
+      <c r="F41">
+        <v>31.851274133252101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" s="17">
+        <v>105.9088204</v>
+      </c>
+      <c r="F42">
+        <v>43.790248393613098</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" s="17">
+        <v>90.158385490000001</v>
+      </c>
+      <c r="F43">
+        <v>22.369492630013699</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C44" s="17">
+        <v>96.865078490000002</v>
+      </c>
+      <c r="F44">
+        <v>32.090613090099701</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C45" s="17">
+        <v>75.11756733</v>
+      </c>
+      <c r="F45">
+        <v>23.825673139029799</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" s="17">
+        <v>79.427001750000002</v>
+      </c>
+      <c r="F46">
+        <v>24.472450110836299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" s="17">
+        <v>94.170321270000002</v>
+      </c>
+      <c r="F47">
+        <v>22.622747976625899</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="17">
+        <v>147.87725549999999</v>
+      </c>
+      <c r="F48">
+        <v>37.767461164483002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="17">
+        <v>142.45959959999999</v>
+      </c>
+      <c r="F49">
+        <v>42.987997380496097</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" s="17">
+        <v>102.8968931</v>
+      </c>
+      <c r="F50">
+        <v>37.623748144585598</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C51" s="17">
+        <v>94.960570599999997</v>
+      </c>
+      <c r="F51">
+        <v>29.771227537573701</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C52" s="17">
+        <v>58.289234149999999</v>
+      </c>
+      <c r="F52">
+        <v>22.198221481673201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" s="17">
+        <v>84.971670439999997</v>
+      </c>
+      <c r="F53">
+        <v>27.575649772829902</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C54" s="17">
+        <v>76.931306950000007</v>
+      </c>
+      <c r="F54">
+        <v>19.0758077887103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C55" s="17">
+        <v>79.814054229999996</v>
+      </c>
+      <c r="F55">
+        <v>15.9349819449343</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" s="17">
+        <v>88.67181961</v>
+      </c>
+      <c r="F56">
+        <v>24.005080989770502</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C57" s="17">
+        <v>75.010805500000004</v>
+      </c>
+      <c r="F57">
+        <v>20.755401162536501</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C58" s="17">
+        <v>96.224918869999996</v>
+      </c>
+      <c r="F58">
+        <v>20.368347391399901</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="17">
+        <v>104.2732484</v>
+      </c>
+      <c r="F59">
+        <v>19.766051348883099</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C60" s="17">
+        <v>101.4558696</v>
+      </c>
+      <c r="F60">
+        <v>27.9274234955287</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C61" s="17">
+        <v>-2.211713848</v>
+      </c>
+      <c r="F61">
+        <v>-7.6044208361044703</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="17">
+        <v>-1.11959371</v>
+      </c>
+      <c r="F62">
+        <v>-0.79935892096311001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C63" s="17">
+        <v>-2.2994903029999998</v>
+      </c>
+      <c r="F63">
+        <v>-7.4304054034129097</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="17">
+        <v>-1.6205861939999999</v>
+      </c>
+      <c r="F64">
+        <v>-2.0627900491187399</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" s="17">
+        <v>-0.82331376899999997</v>
+      </c>
+      <c r="F65">
+        <v>0.88222690937126702</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C66" s="17">
+        <v>-2.4049952889999999</v>
+      </c>
+      <c r="F66">
+        <v>-9.4037386928712099</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" s="17">
+        <v>-2.4274128730000002</v>
+      </c>
+      <c r="F67">
+        <v>-8.7973570037979503</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68" s="17">
+        <v>-2.0218172870000002</v>
+      </c>
+      <c r="F68">
+        <v>-6.3460202592396699</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C69" s="17">
+        <v>-0.98675659400000004</v>
+      </c>
+      <c r="F69">
+        <v>-0.255387708596715</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C70" s="17">
+        <v>-1.0824256539999999</v>
+      </c>
+      <c r="F70">
+        <v>-0.59797458502107603</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="17">
+        <v>-1.538400907</v>
+      </c>
+      <c r="F71">
+        <v>-3.4219332781429701</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C72" s="17">
+        <v>-2.1347896369999999</v>
+      </c>
+      <c r="F72">
+        <v>-6.8620097334040802</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C73" s="17">
+        <v>-2.0072762819999999</v>
+      </c>
+      <c r="F73">
+        <v>-5.2631478529636802</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C74" s="17">
+        <v>-2.2132342569999999</v>
+      </c>
+      <c r="F74">
+        <v>-6.4685831937033296</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75" s="17">
+        <v>-1.0861069409999999</v>
+      </c>
+      <c r="F75">
+        <v>-1.64852628233444</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C76" s="17">
+        <v>-3.6722116219999998</v>
+      </c>
+      <c r="F76">
+        <v>-15.6888579113165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C77" s="17">
+        <v>-1.503086105</v>
+      </c>
+      <c r="F77">
+        <v>-3.3517179050517698</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C78" s="17">
+        <v>-1.330016563</v>
+      </c>
+      <c r="F78">
+        <v>-1.699141433359</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C79" s="17">
+        <v>-1.7371725730000001</v>
+      </c>
+      <c r="F79">
+        <v>-5.4429735076255596</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" s="17">
+        <v>-3.5863414050000002</v>
+      </c>
+      <c r="F80">
+        <v>-14.0978090444989</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C81" s="17">
+        <v>-1.4353871460000001</v>
+      </c>
+      <c r="F81">
+        <v>-2.1874988960713999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C82" s="17">
+        <v>-2.0120124509999999</v>
+      </c>
+      <c r="F82">
+        <v>-6.1232093943700603</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C83" s="17">
+        <v>-1.0002978360000001</v>
+      </c>
+      <c r="F83">
+        <v>0.64368775634179298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C84" s="17">
+        <v>-1.399484602</v>
+      </c>
+      <c r="F84">
+        <v>-0.35726724661598003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C85" s="17">
+        <v>-2.2618060400000002</v>
+      </c>
+      <c r="F85">
+        <v>-7.2826415060251097</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C86" s="17">
+        <v>-3.525203876</v>
+      </c>
+      <c r="F86">
+        <v>-15.2741953597024</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C87" s="17">
+        <v>-3.2320859099999999</v>
+      </c>
+      <c r="F87">
+        <v>-12.5357089588242</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C88" s="17">
+        <v>-2.1571557619999999</v>
+      </c>
+      <c r="F88">
+        <v>-6.4894932240029402</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C89" s="17">
+        <v>-1.822812305</v>
+      </c>
+      <c r="F89">
+        <v>-4.33369475559034</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C90" s="17">
+        <v>0.547821259</v>
+      </c>
+      <c r="F90">
+        <v>7.5382172491077997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C91" s="17">
+        <v>-1.5082813180000001</v>
+      </c>
+      <c r="F91">
+        <v>-1.81606289253831</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C92" s="17">
+        <v>-1.6162300940000001</v>
+      </c>
+      <c r="F92">
+        <v>-2.87593378127346</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C93" s="17">
+        <v>-2.106364605</v>
+      </c>
+      <c r="F93">
+        <v>-4.4559349265356802</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C94" s="17">
+        <v>-1.6255794729999999</v>
+      </c>
+      <c r="F94">
+        <v>-3.47352961711064</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C95" s="17">
+        <v>-1.469568502</v>
+      </c>
+      <c r="F95">
+        <v>-2.4734316101729998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C96" s="17">
+        <v>-2.1437939309999998</v>
+      </c>
+      <c r="F96">
+        <v>-6.5560231842482999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C97" s="17">
+        <v>-2.5343310290000001</v>
+      </c>
+      <c r="F97">
+        <v>-8.7558381888342698</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C98" s="17">
+        <v>-1.6384720500000001</v>
+      </c>
+      <c r="F98">
+        <v>-5.1458331569432003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C99" s="17">
+        <v>-1.292939751</v>
+      </c>
+      <c r="F99">
+        <v>-5.7545240231605304</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C100" s="17">
+        <v>-1.0607837339999999</v>
+      </c>
+      <c r="F100">
+        <v>-2.2116331485436</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C101" s="17">
+        <v>-1.6967920000000001</v>
+      </c>
+      <c r="F101">
+        <v>-8.0863605263077396</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C102" s="17">
+        <v>-1.3187428299999999</v>
+      </c>
+      <c r="F102">
+        <v>-4.3160484095908096</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C103" s="17">
+        <v>-1.2755335160000001</v>
+      </c>
+      <c r="F103">
+        <v>-3.4546581835470498</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C104" s="17">
+        <v>-0.98444991000000004</v>
+      </c>
+      <c r="F104">
+        <v>-2.1818301142508698</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C105" s="17">
+        <v>-1.0058950250000001</v>
+      </c>
+      <c r="F105">
+        <v>-2.0520507170885698</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C106" s="17">
+        <v>-2.1869500450000001</v>
+      </c>
+      <c r="F106">
+        <v>-9.3491398805293198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C107" s="17">
+        <v>-1.000557524</v>
+      </c>
+      <c r="F107">
+        <v>-1.7989081023675799</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C108" s="17">
+        <v>-0.85144982499999999</v>
+      </c>
+      <c r="F108">
+        <v>-0.88203705218684703</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C109" s="17">
+        <v>-1.2034885479999999</v>
+      </c>
+      <c r="F109">
+        <v>-3.5229240185414601</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C110" s="17">
+        <v>-1.3264061700000001</v>
+      </c>
+      <c r="F110">
+        <v>-3.8979243771010901</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C111" s="17">
+        <v>-1.2605519510000001</v>
+      </c>
+      <c r="F111">
+        <v>-2.8514176399676598</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C112" s="17">
+        <v>-1.0713101410000001</v>
+      </c>
+      <c r="F112">
+        <v>-2.13344840547648</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C113" s="17">
+        <v>-3.4554528709999999</v>
+      </c>
+      <c r="F113">
+        <v>-17.723878642431099</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C114" s="17">
+        <v>-0.73228888199999997</v>
+      </c>
+      <c r="F114">
+        <v>-2.8115836833671199</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C115" s="17">
+        <v>-1.2694831440000001</v>
+      </c>
+      <c r="F115">
+        <v>-4.8778867493016902</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6">
+      <c r="A116" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C116" s="17">
+        <v>-1.277481262</v>
+      </c>
+      <c r="F116">
+        <v>-2.2300566411645102</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6">
+      <c r="A117" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C117" s="17">
+        <v>-1.8540429970000001</v>
+      </c>
+      <c r="F117">
+        <v>-7.9201708601130996</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6">
+      <c r="A118" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C118" s="17">
+        <v>0.47940949799999999</v>
+      </c>
+      <c r="F118">
+        <v>7.1145900034110499</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6">
+      <c r="A119" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C119" s="17">
+        <v>-1.1936774699999999</v>
+      </c>
+      <c r="F119">
+        <v>-2.92396248645142</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6">
+      <c r="A120" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C120" s="17">
+        <v>-0.92901788399999996</v>
+      </c>
+      <c r="F120">
+        <v>-1.5818151757586201</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6">
+      <c r="A121" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C121" s="17">
+        <v>-1.3161578249999999</v>
+      </c>
+      <c r="F121">
+        <v>-2.3392034180091801</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6">
+      <c r="A122" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C122" s="17">
+        <v>-1.134418047</v>
+      </c>
+      <c r="F122">
+        <v>-1.9141370813698899</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6">
+      <c r="A123" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C123" s="17">
+        <v>-0.99250506999999999</v>
+      </c>
+      <c r="F123">
+        <v>-2.0471495556789301</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6">
+      <c r="A124" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C124" s="17">
+        <v>-1.0473612050000001</v>
+      </c>
+      <c r="F124">
+        <v>-7.0492602941017299</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6">
+      <c r="A125" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C125" s="17">
+        <v>-1.1508566309999999</v>
+      </c>
+      <c r="F125">
+        <v>-4.8474910488270799</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6">
+      <c r="A126" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C126" s="17">
+        <v>-1.1209454940000001</v>
+      </c>
+      <c r="F126">
+        <v>-3.9040360299961598</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6">
+      <c r="A127" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C127" s="17">
+        <v>-1.664803402</v>
+      </c>
+      <c r="F127">
+        <v>-6.4809363851313604</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6">
+      <c r="A128" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C128" s="17">
+        <v>-2.335638957</v>
+      </c>
+      <c r="F128">
+        <v>-10.324207438637099</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6">
+      <c r="A129" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C129" s="17">
+        <v>-1.094796404</v>
+      </c>
+      <c r="F129">
+        <v>-2.2602169770151002</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C130" s="17">
+        <v>-1.7747992429999999</v>
+      </c>
+      <c r="F130">
+        <v>-5.5378084506324203</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C131" s="17">
+        <v>-0.97719068200000003</v>
+      </c>
+      <c r="F131">
+        <v>-0.78779205675369102</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C132" s="17">
+        <v>-1.308950882</v>
+      </c>
+      <c r="F132">
+        <v>-3.26822786862023</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C133" s="17">
+        <v>-1.2509183610000001</v>
+      </c>
+      <c r="F133">
+        <v>-2.2152855838393402</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C134" s="17">
+        <v>-2.300630575</v>
+      </c>
+      <c r="F134">
+        <v>-10.108073257002401</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C135" s="17">
+        <v>-1.341631349</v>
+      </c>
+      <c r="F135">
+        <v>-4.2767398602837803</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C136" s="17">
+        <v>-1.8308629780000001</v>
+      </c>
+      <c r="F136">
+        <v>-8.6070487815047496</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C137" s="17">
+        <v>-6.897118539</v>
+      </c>
+      <c r="F137">
+        <v>-11.536988066518299</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C138" s="17">
+        <v>-6.7552686480000004</v>
+      </c>
+      <c r="F138">
+        <v>-10.2488752061957</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C139" s="17">
+        <v>-6.8046791879999997</v>
+      </c>
+      <c r="F139">
+        <v>-11.1573953090369</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C140" s="17">
+        <v>-6.1646410429999996</v>
+      </c>
+      <c r="F140">
+        <v>-8.2061103698879894</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C141" s="17">
+        <v>-6.2656440150000003</v>
+      </c>
+      <c r="F141">
+        <v>-6.7929176799041997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C142" s="17">
+        <v>-7.2948766149999997</v>
+      </c>
+      <c r="F142">
+        <v>-12.447441878663099</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6">
+      <c r="A143" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C143" s="17">
+        <v>-6.0828205300000002</v>
+      </c>
+      <c r="F143">
+        <v>-7.4790176849791603</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6">
+      <c r="A144" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C144" s="17">
+        <v>-4.8291021670000003</v>
+      </c>
+      <c r="F144">
+        <v>-3.70463860250939</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6">
+      <c r="A145" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C145" s="17">
+        <v>-4.958667653</v>
+      </c>
+      <c r="F145">
+        <v>-3.9136786401124302</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6">
+      <c r="A146" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C146" s="17">
+        <v>-4.577585193</v>
+      </c>
+      <c r="F146">
+        <v>-2.8563714470575898</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6">
+      <c r="A147" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C147" s="17">
+        <v>-8.4265167569999999</v>
+      </c>
+      <c r="F147">
+        <v>-16.0898029702625</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6">
+      <c r="A148" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C148" s="17">
+        <v>-6.3206566400000002</v>
+      </c>
+      <c r="F148">
+        <v>-8.4383380086097795</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6">
+      <c r="A149" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C149" s="17">
+        <v>-6.5234073840000004</v>
+      </c>
+      <c r="F149">
+        <v>-8.80634264258115</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6">
+      <c r="A150" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="C150" s="17">
+        <v>-6.5338266909999998</v>
+      </c>
+      <c r="F150">
+        <v>-9.2068654020608598</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6">
+      <c r="A151" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C151" s="17">
+        <v>-10.665304020000001</v>
+      </c>
+      <c r="F151">
+        <v>-23.790441957207801</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6">
+      <c r="A152" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C152" s="17">
+        <v>-6.887223724</v>
+      </c>
+      <c r="F152">
+        <v>-10.5906045462725</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6">
+      <c r="A153" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C153" s="17">
+        <v>-6.7165885860000003</v>
+      </c>
+      <c r="F153">
+        <v>-9.6175177507994896</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6">
+      <c r="A154" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C154" s="17">
+        <v>-6.6846708530000001</v>
+      </c>
+      <c r="F154">
+        <v>-8.6090538816656696</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6">
+      <c r="A155" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C155" s="17">
+        <v>-7.7230365299999999</v>
+      </c>
+      <c r="F155">
+        <v>-13.877554918440801</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6">
+      <c r="A156" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C156" s="17">
+        <v>-5.3369577369999996</v>
+      </c>
+      <c r="F156">
+        <v>-5.3041465413262099</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6">
+      <c r="A157" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="C157" s="17">
+        <v>-9.098733824</v>
+      </c>
+      <c r="F157">
+        <v>-17.126830884541999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6">
+      <c r="A158" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C158" s="17">
+        <v>-7.1151102570000004</v>
+      </c>
+      <c r="F158">
+        <v>-11.2340640120901</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6">
+      <c r="A159" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C159" s="17">
+        <v>-7.2546955930000001</v>
+      </c>
+      <c r="F159">
+        <v>-9.8983598549914102</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6">
+      <c r="A160" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="C160" s="17">
+        <v>-6.8537062649999996</v>
+      </c>
+      <c r="F160">
+        <v>-8.4847366465141594</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6">
+      <c r="A161" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C161" s="17">
+        <v>-7.6229570889999998</v>
+      </c>
+      <c r="F161">
+        <v>-13.4419296536323</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6">
+      <c r="A162" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="C162" s="17">
+        <v>-10.40300238</v>
+      </c>
+      <c r="F162">
+        <v>-24.536435340682299</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6">
+      <c r="A163" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C163" s="17">
+        <v>-8.8452509450000001</v>
+      </c>
+      <c r="F163">
+        <v>-18.941298822543299</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6">
+      <c r="A164" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C164" s="17">
+        <v>-5.8638908220000001</v>
+      </c>
+      <c r="F164">
+        <v>-6.5501243787505201</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6">
+      <c r="A165" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C165" s="17">
+        <v>-5.5828554160000001</v>
+      </c>
+      <c r="F165">
+        <v>-5.7087471246316897</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6">
+      <c r="A166" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C166" s="17">
+        <v>-6.1100515660000001</v>
+      </c>
+      <c r="F166">
+        <v>-8.0214845535710602</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6">
+      <c r="A167" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C167" s="17">
+        <v>-6.7188374749999999</v>
+      </c>
+      <c r="F167">
+        <v>-8.79301280547846</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6">
+      <c r="A168" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="C168" s="17">
+        <v>-4.9407132650000003</v>
+      </c>
+      <c r="F168">
+        <v>-2.9714934190400801</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6">
+      <c r="A169" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C169" s="17">
+        <v>-7.599781267</v>
+      </c>
+      <c r="F169">
+        <v>-7.5180384367053001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6">
+      <c r="A170" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C170" s="17">
+        <v>-7.4875352900000003</v>
+      </c>
+      <c r="F170">
+        <v>-12.3244639894406</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6">
+      <c r="A171" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C171" s="17">
+        <v>-6.2956824239999998</v>
+      </c>
+      <c r="F171">
+        <v>-7.4308129320985401</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6">
+      <c r="A172" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C172" s="17">
+        <v>-5.1578048179999998</v>
+      </c>
+      <c r="F172">
+        <v>-4.2959740161039104</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6">
+      <c r="A173" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C173" s="17">
+        <v>-8.0718366469999996</v>
+      </c>
+      <c r="F173">
+        <v>-14.704543884051899</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6">
+      <c r="A174" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="C174" s="17">
+        <v>-8.4299853099999993</v>
+      </c>
+      <c r="F174">
+        <v>-14.357072917312401</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6">
+      <c r="A175" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C175" s="17">
+        <v>0.125935295</v>
+      </c>
+      <c r="F175">
+        <v>2.2046594901758398</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6">
+      <c r="A176" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C176" s="17">
+        <v>0.104218877</v>
+      </c>
+      <c r="F176">
+        <v>2.1628863085605099</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6">
+      <c r="A177" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C177" s="17">
+        <v>7.256635E-3</v>
+      </c>
+      <c r="F177">
+        <v>0.42242222246427802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Messy code after running models ...
... cleaning up now!
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="20" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="6940" yWindow="3120" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="OSPREE" sheetId="1" r:id="rId1"/>
-    <sheet name="Flynn_exp" sheetId="2" r:id="rId2"/>
-    <sheet name="meta" sheetId="3" r:id="rId3"/>
+    <sheet name="OSPREE_more" sheetId="4" r:id="rId2"/>
+    <sheet name="Flynn_exp" sheetId="2" r:id="rId3"/>
+    <sheet name="meta" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="243">
   <si>
     <t>param</t>
   </si>
@@ -701,11 +702,110 @@
   <si>
     <t>sumer.wi (see models_stan_plotting.R)</t>
   </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>sp_n</t>
+  </si>
+  <si>
+    <t>model</t>
+  </si>
+  <si>
+    <t>study_n</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>preds centered</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>data info</t>
+  </si>
+  <si>
+    <t>nointer_2level_studyint_ncp</t>
+  </si>
+  <si>
+    <t>exp &amp; ramped for: photo and force</t>
+  </si>
+  <si>
+    <t>exp for: photo and exp force</t>
+  </si>
+  <si>
+    <t>spcomplex</t>
+  </si>
+  <si>
+    <t>no, did not use</t>
+  </si>
+  <si>
+    <t>no, but used only species with 2 or more datasetIDs</t>
+  </si>
+  <si>
+    <t>model notes</t>
+  </si>
+  <si>
+    <t>741 divergent transition, banana plot on sigma_photo; 800+ when NCP on photo only; down to 2 only with NCP on force and photo (but does not look like the chains coverged for intercepts; but they do for the SLOPES)</t>
+  </si>
+  <si>
+    <t>0 div transitions, chains for intercepts look okay, but not great -- still some n_eff issues (no Rhat issues)</t>
+  </si>
+  <si>
+    <t>nointer_2level_interceptonly</t>
+  </si>
+  <si>
+    <t>insanely fast and looks good</t>
+  </si>
+  <si>
+    <t>nointer_2level.stan</t>
+  </si>
+  <si>
+    <t>nointer_2level_interceptonly.stan</t>
+  </si>
+  <si>
+    <t>27 divergent transitions; no easy to diagnose issue</t>
+  </si>
+  <si>
+    <t>winternosp_2level.stan</t>
+  </si>
+  <si>
+    <t>no problems; seems fine!</t>
+  </si>
+  <si>
+    <t>1891 div trans; intercepts again awful; slopes (ones I looked at) okay</t>
+  </si>
+  <si>
+    <t>nointer_2level_negbin_ncp.stan</t>
+  </si>
+  <si>
+    <t>Not sure</t>
+  </si>
+  <si>
+    <t>prob 30</t>
+  </si>
+  <si>
+    <t>I think: exp for: photo and exp force</t>
+  </si>
+  <si>
+    <t>not sure (did not keep good notes)</t>
+  </si>
+  <si>
+    <t>looks good</t>
+  </si>
+  <si>
+    <t>yes, used</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -850,7 +950,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="63">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -914,8 +1014,88 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -940,8 +1120,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="63">
+  <cellStyles count="143">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -973,6 +1172,46 @@
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1004,6 +1243,46 @@
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1335,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:F177"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3541,6 +3820,1521 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L189"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="13.5" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="22" customFormat="1" ht="45">
+      <c r="A1" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="K1" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="C2" s="19"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" t="s">
+        <v>220</v>
+      </c>
+      <c r="G3" t="s">
+        <v>220</v>
+      </c>
+      <c r="H3" t="s">
+        <v>220</v>
+      </c>
+      <c r="I3" t="s">
+        <v>220</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="K3" t="s">
+        <v>220</v>
+      </c>
+      <c r="L3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" t="s">
+        <v>223</v>
+      </c>
+      <c r="D4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E4" t="s">
+        <v>224</v>
+      </c>
+      <c r="F4" t="s">
+        <v>224</v>
+      </c>
+      <c r="G4" t="s">
+        <v>223</v>
+      </c>
+      <c r="H4" t="s">
+        <v>223</v>
+      </c>
+      <c r="I4" t="s">
+        <v>223</v>
+      </c>
+      <c r="J4" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="K4" t="s">
+        <v>223</v>
+      </c>
+      <c r="L4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D5" t="s">
+        <v>227</v>
+      </c>
+      <c r="E5" t="s">
+        <v>229</v>
+      </c>
+      <c r="F5" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5" t="s">
+        <v>232</v>
+      </c>
+      <c r="I5" t="s">
+        <v>234</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="L5" s="24" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B7">
+        <v>2651</v>
+      </c>
+      <c r="C7">
+        <v>2148</v>
+      </c>
+      <c r="D7">
+        <v>1565</v>
+      </c>
+      <c r="E7">
+        <v>1565</v>
+      </c>
+      <c r="F7">
+        <v>1565</v>
+      </c>
+      <c r="G7">
+        <v>2651</v>
+      </c>
+      <c r="H7">
+        <v>2651</v>
+      </c>
+      <c r="I7">
+        <v>2651</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="K7" s="24">
+        <v>2651</v>
+      </c>
+      <c r="L7" s="24">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B8">
+        <v>200</v>
+      </c>
+      <c r="C8">
+        <v>181</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <v>32</v>
+      </c>
+      <c r="G8">
+        <v>200</v>
+      </c>
+      <c r="H8">
+        <v>200</v>
+      </c>
+      <c r="I8">
+        <v>200</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="K8" s="24">
+        <v>200</v>
+      </c>
+      <c r="L8" s="24">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>214</v>
+      </c>
+      <c r="B9">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10" t="s">
+        <v>217</v>
+      </c>
+      <c r="G10" t="s">
+        <v>217</v>
+      </c>
+      <c r="H10" t="s">
+        <v>217</v>
+      </c>
+      <c r="I10" t="s">
+        <v>217</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="L10" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>211</v>
+      </c>
+      <c r="B14">
+        <v>11.2</v>
+      </c>
+      <c r="C14">
+        <v>5.6</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>-3.2</v>
+      </c>
+      <c r="C15">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="D15">
+        <v>10.7</v>
+      </c>
+      <c r="E15">
+        <v>29.3</v>
+      </c>
+      <c r="F15">
+        <v>29.4</v>
+      </c>
+      <c r="G15">
+        <v>34.5</v>
+      </c>
+      <c r="H15">
+        <v>30.2</v>
+      </c>
+      <c r="I15">
+        <v>30.5</v>
+      </c>
+      <c r="J15" s="24">
+        <f>EXP(3.27)</f>
+        <v>26.311339343265892</v>
+      </c>
+      <c r="K15" s="24">
+        <f>EXP(3.3)</f>
+        <v>27.112638920657883</v>
+      </c>
+      <c r="L15" s="24">
+        <f>EXP(3.3)</f>
+        <v>27.112638920657883</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>19.5</v>
+      </c>
+      <c r="C16">
+        <v>4.2</v>
+      </c>
+      <c r="D16">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>-4.4000000000000004</v>
+      </c>
+      <c r="C17">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="D17">
+        <v>-5.6</v>
+      </c>
+      <c r="E17">
+        <v>-6.2</v>
+      </c>
+      <c r="F17">
+        <v>-6.3</v>
+      </c>
+      <c r="G17">
+        <v>-6.2</v>
+      </c>
+      <c r="H17">
+        <v>-5.7</v>
+      </c>
+      <c r="I17">
+        <v>-6.11</v>
+      </c>
+      <c r="J17" s="24">
+        <f>-(EXP(3.27)-EXP(3.27-0.25))</f>
+        <v>-5.8200476590729515</v>
+      </c>
+      <c r="K17" s="24">
+        <f>-(EXP(3.3)-EXP(3.3-0.16))</f>
+        <v>-4.0087720619357086</v>
+      </c>
+      <c r="L17" s="24">
+        <f>-(EXP(3.3)-EXP(3.3-0.2))</f>
+        <v>-4.9146876392162575</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>-0.5</v>
+      </c>
+      <c r="C18">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+      <c r="E18">
+        <v>-0.92</v>
+      </c>
+      <c r="F18">
+        <v>-1.2</v>
+      </c>
+      <c r="G18">
+        <v>-0.92</v>
+      </c>
+      <c r="H18">
+        <v>-0.89</v>
+      </c>
+      <c r="I18">
+        <v>-1.2</v>
+      </c>
+      <c r="J18" s="24">
+        <f>-(EXP(3.27)-EXP(3.27-0.05))</f>
+        <v>-1.2832191619280771</v>
+      </c>
+      <c r="K18" s="24">
+        <f>-(EXP(3.3)-EXP(3.3-0.05))</f>
+        <v>-1.3222990034648205</v>
+      </c>
+      <c r="L18" s="24">
+        <f>-(EXP(3.3)-EXP(3.3-0.1))</f>
+        <v>-2.5801087235485411</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>-9.5</v>
+      </c>
+      <c r="C19">
+        <v>-9.4</v>
+      </c>
+      <c r="D19">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="E19">
+        <v>-7.5</v>
+      </c>
+      <c r="F19">
+        <v>-9.9</v>
+      </c>
+      <c r="G19">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="H19">
+        <v>-9.4</v>
+      </c>
+      <c r="I19">
+        <v>-9.1</v>
+      </c>
+      <c r="J19" s="24">
+        <f>-(EXP(3.27)-EXP(3.27-0.31))</f>
+        <v>-7.0133675877631347</v>
+      </c>
+      <c r="K19" s="24">
+        <f>-(EXP(3.3)-EXP(3.3-0.3))</f>
+        <v>-7.0271019974702149</v>
+      </c>
+      <c r="L19" s="24">
+        <f>-(EXP(3.3)-EXP(3.3-0.35))</f>
+        <v>-8.0066851924262394</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22">
+        <v>-2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="17"/>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="17"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="17"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="17"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="17"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="17"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="17"/>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="17"/>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" s="17"/>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" s="17"/>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="17"/>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="17"/>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="17"/>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="17"/>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="17"/>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="17"/>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="17"/>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="17"/>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="17"/>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="17"/>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="17"/>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="17"/>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="17"/>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B49" s="17"/>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B50" s="17"/>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="17"/>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="17"/>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="17"/>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B54" s="17"/>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B55" s="17"/>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="17"/>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B57" s="17"/>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B58" s="17"/>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B59" s="17"/>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B60" s="17"/>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B61" s="17"/>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="17"/>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B63" s="17"/>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B64" s="17"/>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B65" s="17"/>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" s="17"/>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B67" s="17"/>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="17"/>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B69" s="17"/>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B70" s="17"/>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="B71" s="17"/>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" s="17"/>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="17"/>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B74" s="17"/>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" s="17"/>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76" s="17"/>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B77" s="17"/>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B78" s="17"/>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B79" s="17"/>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B80" s="17"/>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B81" s="17"/>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="B82" s="17"/>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B83" s="17"/>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="B84" s="17"/>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B85" s="17"/>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86" s="17"/>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="B87" s="17"/>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="B88" s="17"/>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B89" s="17"/>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B90" s="17"/>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B91" s="17"/>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B92" s="17"/>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B93" s="17"/>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B94" s="17"/>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="B95" s="17"/>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96" s="17"/>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B97" s="17"/>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B98" s="17"/>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B99" s="17"/>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B100" s="17"/>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B101" s="17"/>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B102" s="17"/>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B103" s="17"/>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B104" s="17"/>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="B105" s="17"/>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B106" s="17"/>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="B107" s="17"/>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="B108" s="17"/>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B109" s="17"/>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="B110" s="17"/>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B111" s="17"/>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="B112" s="17"/>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="B113" s="17"/>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="B114" s="17"/>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B115" s="17"/>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B116" s="17"/>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B117" s="17"/>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="B118" s="17"/>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="B119" s="17"/>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="B120" s="17"/>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="B121" s="17"/>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="B122" s="17"/>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B123" s="17"/>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="B124" s="17"/>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B125" s="17"/>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B126" s="17"/>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B127" s="17"/>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B128" s="17"/>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B129" s="17"/>
+    </row>
+    <row r="130" spans="1:2">
+      <c r="A130" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="B130" s="17"/>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B131" s="17"/>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="B132" s="17"/>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="B133" s="17"/>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B134" s="17"/>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="B135" s="17"/>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="B136" s="17"/>
+    </row>
+    <row r="137" spans="1:2">
+      <c r="A137" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="B137" s="17"/>
+    </row>
+    <row r="138" spans="1:2">
+      <c r="A138" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B138" s="17"/>
+    </row>
+    <row r="139" spans="1:2">
+      <c r="A139" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="B139" s="17"/>
+    </row>
+    <row r="140" spans="1:2">
+      <c r="A140" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="B140" s="17"/>
+    </row>
+    <row r="141" spans="1:2">
+      <c r="A141" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="B141" s="17"/>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="B142" s="17"/>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="B143" s="17"/>
+    </row>
+    <row r="144" spans="1:2">
+      <c r="A144" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="B144" s="17"/>
+    </row>
+    <row r="145" spans="1:2">
+      <c r="A145" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B145" s="17"/>
+    </row>
+    <row r="146" spans="1:2">
+      <c r="A146" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="B146" s="17"/>
+    </row>
+    <row r="147" spans="1:2">
+      <c r="A147" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B147" s="17"/>
+    </row>
+    <row r="148" spans="1:2">
+      <c r="A148" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="B148" s="17"/>
+    </row>
+    <row r="149" spans="1:2">
+      <c r="A149" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="B149" s="17"/>
+    </row>
+    <row r="150" spans="1:2">
+      <c r="A150" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="B150" s="17"/>
+    </row>
+    <row r="151" spans="1:2">
+      <c r="A151" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="B151" s="17"/>
+    </row>
+    <row r="152" spans="1:2">
+      <c r="A152" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B152" s="17"/>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B153" s="17"/>
+    </row>
+    <row r="154" spans="1:2">
+      <c r="A154" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="B154" s="17"/>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B155" s="17"/>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="B156" s="17"/>
+    </row>
+    <row r="157" spans="1:2">
+      <c r="A157" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="B157" s="17"/>
+    </row>
+    <row r="158" spans="1:2">
+      <c r="A158" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="B158" s="17"/>
+    </row>
+    <row r="159" spans="1:2">
+      <c r="A159" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B159" s="17"/>
+    </row>
+    <row r="160" spans="1:2">
+      <c r="A160" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="B160" s="17"/>
+    </row>
+    <row r="161" spans="1:2">
+      <c r="A161" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B161" s="17"/>
+    </row>
+    <row r="162" spans="1:2">
+      <c r="A162" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="B162" s="17"/>
+    </row>
+    <row r="163" spans="1:2">
+      <c r="A163" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B163" s="17"/>
+    </row>
+    <row r="164" spans="1:2">
+      <c r="A164" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B164" s="17"/>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B165" s="17"/>
+    </row>
+    <row r="166" spans="1:2">
+      <c r="A166" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B166" s="17"/>
+    </row>
+    <row r="167" spans="1:2">
+      <c r="A167" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="B167" s="17"/>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="B168" s="17"/>
+    </row>
+    <row r="169" spans="1:2">
+      <c r="A169" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="B169" s="17"/>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="B170" s="17"/>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="B171" s="17"/>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="B172" s="17"/>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B173" s="17"/>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B174" s="17"/>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B175" s="17"/>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="B176" s="17"/>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B177" s="17"/>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="B178" s="17"/>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="B179" s="17"/>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="B180" s="17"/>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B181" s="17"/>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B182" s="17"/>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="B183" s="17"/>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="B184" s="17"/>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="B185" s="17"/>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B186" s="17"/>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B187" s="17"/>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B188" s="17"/>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B189" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3731,7 +5525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A21"/>
   <sheetViews>

</xml_diff>

<commit_message>
updating model summaries with dans additions
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ailene.ettinger/Documents/GitHub/ospree/analyses/bb_analysis/modelnotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FE6BCC-755A-BA43-A295-D165DB7EC5F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11372E49-EAE3-B54F-954D-A69718A58B1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="1940" windowWidth="34100" windowHeight="21560" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22320" yWindow="3740" windowWidth="34100" windowHeight="21560" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6897" uniqueCount="1030">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6930" uniqueCount="1031">
   <si>
     <t>param</t>
   </si>
@@ -3200,6 +3200,9 @@
   </si>
   <si>
     <t>b_force[203]</t>
+  </si>
+  <si>
+    <t>fine, 1 interation exceed max tree depth of 10</t>
   </si>
 </sst>
 </file>
@@ -27514,7 +27517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6D529A-6CA5-AC41-BF7D-A21CE31120D9}">
   <dimension ref="A1:P1119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
@@ -54824,15 +54827,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F14AA82-A8DC-F342-8CD0-03A4F78929EF}">
-  <dimension ref="A1:F1091"/>
+  <dimension ref="A1:G1091"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>212</v>
       </c>
@@ -54851,8 +54854,11 @@
       <c r="F1" t="s">
         <v>988</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>217</v>
       </c>
@@ -54872,7 +54878,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>221</v>
       </c>
@@ -54892,7 +54898,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>280</v>
       </c>
@@ -54911,13 +54917,16 @@
       <c r="F5" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>214</v>
       </c>
@@ -54936,8 +54945,11 @@
       <c r="F8">
         <v>1731</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>1731</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>211</v>
       </c>
@@ -54956,16 +54968,22 @@
       <c r="F9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>213</v>
       </c>
       <c r="D10">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>215</v>
       </c>
@@ -54984,8 +55002,11 @@
       <c r="F11" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -54999,21 +55020,27 @@
         <v>5.6251972019999998</v>
       </c>
       <c r="E13">
-        <v>29.798171780000001</v>
+        <v>29.832518289999999</v>
       </c>
       <c r="F13">
-        <v>30.00658709</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30.046419220000001</v>
+      </c>
+      <c r="G13">
+        <v>13.007923160000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="D14">
         <v>17.194815030000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14">
+        <v>12.23426562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -55027,13 +55054,16 @@
         <v>-5.5921031000000001</v>
       </c>
       <c r="E15">
-        <v>-6.133612931</v>
+        <v>-6.17595296</v>
       </c>
       <c r="F15">
-        <v>-6.4222531089999997</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.4524519949999997</v>
+      </c>
+      <c r="G15">
+        <v>-5.9506461350000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -55047,13 +55077,16 @@
         <v>-0.43277759799999999</v>
       </c>
       <c r="E16">
-        <v>-1.3508065359999999</v>
+        <v>-1.3717414750000001</v>
       </c>
       <c r="F16">
-        <v>-1.598533534</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.588308968</v>
+      </c>
+      <c r="G16">
+        <v>-0.403418049</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -55067,13 +55100,16 @@
         <v>-10.38923035</v>
       </c>
       <c r="E17">
-        <v>-9.5045080469999998</v>
+        <v>-9.5913333079999994</v>
       </c>
       <c r="F17">
-        <v>-9.3369558319999992</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-9.405938398</v>
+      </c>
+      <c r="G17">
+        <v>-10.150360360000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>52</v>
       </c>
@@ -55087,21 +55123,27 @@
         <v>9.5763016909999994</v>
       </c>
       <c r="E18">
-        <v>10.81355432</v>
+        <v>10.820538819999999</v>
       </c>
       <c r="F18">
-        <v>10.65372604</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10.687392210000001</v>
+      </c>
+      <c r="G18">
+        <v>9.8225740199999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>242</v>
       </c>
       <c r="D19">
         <v>20.33111057</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19">
+        <v>19.817351349999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -55115,13 +55157,16 @@
         <v>0.57049782800000004</v>
       </c>
       <c r="E20">
-        <v>6.6349959690000002</v>
+        <v>6.623611779</v>
       </c>
       <c r="F20">
-        <v>6.4879466929999996</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6.4785875920000002</v>
+      </c>
+      <c r="G20">
+        <v>0.58843635400000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>54</v>
       </c>
@@ -55135,13 +55180,16 @@
         <v>0.34669504899999998</v>
       </c>
       <c r="E21">
-        <v>5.6957790719999997</v>
+        <v>5.7065869830000002</v>
       </c>
       <c r="F21">
-        <v>5.5284367760000004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>5.5068926510000002</v>
+      </c>
+      <c r="G21">
+        <v>0.35615491300000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>55</v>
       </c>
@@ -55155,13 +55203,16 @@
         <v>6.0725641660000003</v>
       </c>
       <c r="E22">
-        <v>6.9750019239999999</v>
+        <v>6.9381158699999999</v>
       </c>
       <c r="F22">
-        <v>6.9165530649999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>6.8981475510000001</v>
+      </c>
+      <c r="G22">
+        <v>6.184385926</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -55175,21 +55226,27 @@
         <v>12.53663283</v>
       </c>
       <c r="E23">
-        <v>14.841873469999999</v>
+        <v>14.84063763</v>
       </c>
       <c r="F23">
-        <v>14.74048359</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>14.7374145</v>
+      </c>
+      <c r="G23">
+        <v>12.609407170000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>210</v>
       </c>
       <c r="D24">
         <v>8.4334477690000007</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24">
+        <v>6.4744415679999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -55197,7 +55254,7 @@
         <v>0.89575970000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -55205,7 +55262,7 @@
         <v>1.5957716</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -55213,12 +55270,12 @@
         <v>-1.7851355</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -55232,13 +55289,16 @@
         <v>15.504457909999999</v>
       </c>
       <c r="E30">
-        <v>38.559672730000003</v>
+        <v>38.509962369999997</v>
       </c>
       <c r="F30">
-        <v>38.529092980000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38.550075120000002</v>
+      </c>
+      <c r="G30">
+        <v>22.710859589999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>58</v>
       </c>
@@ -55252,13 +55312,16 @@
         <v>-0.220706291</v>
       </c>
       <c r="E31">
-        <v>28.920119679999999</v>
+        <v>28.91158192</v>
       </c>
       <c r="F31">
-        <v>28.83468607</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28.785735299999999</v>
+      </c>
+      <c r="G31">
+        <v>6.8079183939999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>59</v>
       </c>
@@ -55272,13 +55335,16 @@
         <v>15.6862698</v>
       </c>
       <c r="E32">
-        <v>40.148806069999999</v>
+        <v>40.13226581</v>
       </c>
       <c r="F32">
-        <v>40.256030529999997</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>40.232854080000003</v>
+      </c>
+      <c r="G32">
+        <v>22.854457400000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>60</v>
       </c>
@@ -55292,13 +55358,16 @@
         <v>11.20726063</v>
       </c>
       <c r="E33">
-        <v>32.254712750000003</v>
+        <v>32.393734369999997</v>
       </c>
       <c r="F33">
-        <v>32.989098570000003</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32.938282100000002</v>
+      </c>
+      <c r="G33">
+        <v>18.55053938</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>61</v>
       </c>
@@ -55312,13 +55381,16 @@
         <v>7.0501576090000002</v>
       </c>
       <c r="E34">
-        <v>29.957267250000001</v>
+        <v>32.825127520000002</v>
       </c>
       <c r="F34">
-        <v>30.065988690000001</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>32.89458509</v>
+      </c>
+      <c r="G34">
+        <v>13.951987880000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>62</v>
       </c>
@@ -55332,13 +55404,16 @@
         <v>6.9486877969999998</v>
       </c>
       <c r="E35">
-        <v>32.806999849999997</v>
+        <v>31.406831929999999</v>
       </c>
       <c r="F35">
-        <v>32.951350890000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31.143860960000001</v>
+      </c>
+      <c r="G35">
+        <v>14.47231683</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -55352,13 +55427,16 @@
         <v>7.4614601289999998</v>
       </c>
       <c r="E36">
-        <v>31.26020784</v>
+        <v>31.768858340000001</v>
       </c>
       <c r="F36">
-        <v>31.10848678</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31.62891007</v>
+      </c>
+      <c r="G36">
+        <v>10.16128391</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -55372,13 +55450,16 @@
         <v>3.3844346199999999</v>
       </c>
       <c r="E37">
-        <v>31.675886510000002</v>
+        <v>18.50670014</v>
       </c>
       <c r="F37">
-        <v>31.613308079999999</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>18.51632682</v>
+      </c>
+      <c r="G37">
+        <v>6.8285590190000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>65</v>
       </c>
@@ -55392,13 +55473,16 @@
         <v>5.8553734249999998</v>
       </c>
       <c r="E38">
-        <v>18.478218460000001</v>
+        <v>17.393300029999999</v>
       </c>
       <c r="F38">
-        <v>18.51161072</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>17.633040359999999</v>
+      </c>
+      <c r="G38">
+        <v>7.4456438189999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>66</v>
       </c>
@@ -55412,13 +55496,16 @@
         <v>-6.43653E-2</v>
       </c>
       <c r="E39">
-        <v>17.388650120000001</v>
+        <v>30.148165070000001</v>
       </c>
       <c r="F39">
-        <v>17.629579329999999</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+        <v>30.117095259999999</v>
+      </c>
+      <c r="G39">
+        <v>10.551215880000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>67</v>
       </c>
@@ -55432,13 +55519,16 @@
         <v>0.52508654099999996</v>
       </c>
       <c r="E40">
-        <v>30.115272950000001</v>
+        <v>27.769968689999999</v>
       </c>
       <c r="F40">
-        <v>30.04439781</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+        <v>27.740208280000001</v>
+      </c>
+      <c r="G40">
+        <v>8.1107611219999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>68</v>
       </c>
@@ -55452,13 +55542,16 @@
         <v>3.7340329300000001</v>
       </c>
       <c r="E41">
-        <v>27.77838513</v>
+        <v>23.541662729999999</v>
       </c>
       <c r="F41">
-        <v>27.66282593</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+        <v>23.524565240000001</v>
+      </c>
+      <c r="G41">
+        <v>6.0919235980000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -55472,13 +55565,16 @@
         <v>1.1264898270000001</v>
       </c>
       <c r="E42">
-        <v>23.503158710000001</v>
+        <v>19.970330310000001</v>
       </c>
       <c r="F42">
-        <v>23.526806959999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20.322998940000002</v>
+      </c>
+      <c r="G42">
+        <v>0.62315778200000005</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>70</v>
       </c>
@@ -55492,13 +55588,16 @@
         <v>-0.86594967499999997</v>
       </c>
       <c r="E43">
-        <v>19.960954749999999</v>
+        <v>49.905000020000003</v>
       </c>
       <c r="F43">
-        <v>20.36127711</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+        <v>49.835310280000002</v>
+      </c>
+      <c r="G43">
+        <v>25.407185210000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>71</v>
       </c>
@@ -55512,13 +55611,16 @@
         <v>-6.2896396550000002</v>
       </c>
       <c r="E44">
-        <v>49.92630157</v>
+        <v>54.671434169999998</v>
       </c>
       <c r="F44">
-        <v>49.819147129999998</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+        <v>54.860355900000002</v>
+      </c>
+      <c r="G44">
+        <v>32.403157839999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>72</v>
       </c>
@@ -55532,13 +55634,16 @@
         <v>18.294173279999999</v>
       </c>
       <c r="E45">
-        <v>54.788989989999997</v>
+        <v>37.491009499999997</v>
       </c>
       <c r="F45">
-        <v>54.835044920000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37.29149219</v>
+      </c>
+      <c r="G45">
+        <v>21.755574410000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>73</v>
       </c>
@@ -55552,13 +55657,16 @@
         <v>24.728576390000001</v>
       </c>
       <c r="E46">
-        <v>37.403286790000003</v>
+        <v>20.940014529999999</v>
       </c>
       <c r="F46">
-        <v>37.345573299999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21.23818434</v>
+      </c>
+      <c r="G46">
+        <v>3.9539645289999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -55572,13 +55680,16 @@
         <v>14.660700909999999</v>
       </c>
       <c r="E47">
-        <v>20.975732059999999</v>
+        <v>43.356237950000001</v>
       </c>
       <c r="F47">
-        <v>21.237238040000001</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+        <v>43.685910300000003</v>
+      </c>
+      <c r="G47">
+        <v>26.227895220000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>75</v>
       </c>
@@ -55592,13 +55703,16 @@
         <v>-3.004220992</v>
       </c>
       <c r="E48">
-        <v>29.73808902</v>
+        <v>31.89564193</v>
       </c>
       <c r="F48">
-        <v>29.959633830000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31.079716619999999</v>
+      </c>
+      <c r="G48">
+        <v>13.25787238</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>76</v>
       </c>
@@ -55612,13 +55726,16 @@
         <v>5.2351330880000004</v>
       </c>
       <c r="E49">
-        <v>43.39851453</v>
+        <v>24.170008760000002</v>
       </c>
       <c r="F49">
-        <v>43.675695089999998</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24.36572812</v>
+      </c>
+      <c r="G49">
+        <v>7.3500042920000004</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -55632,13 +55749,16 @@
         <v>19.215894540000001</v>
       </c>
       <c r="E50">
-        <v>31.815520190000001</v>
+        <v>24.668828059999999</v>
       </c>
       <c r="F50">
-        <v>31.064743230000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24.715500339999998</v>
+      </c>
+      <c r="G50">
+        <v>2.2190053359999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>78</v>
       </c>
@@ -55652,13 +55772,16 @@
         <v>-7.4466105230000004</v>
       </c>
       <c r="E51">
-        <v>24.167075310000001</v>
+        <v>22.198231360000001</v>
       </c>
       <c r="F51">
-        <v>24.29878823</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21.9155798</v>
+      </c>
+      <c r="G51">
+        <v>1.91956507</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -55672,13 +55795,16 @@
         <v>6.4025096640000001</v>
       </c>
       <c r="E52">
-        <v>24.66816047</v>
+        <v>37.917486629999999</v>
       </c>
       <c r="F52">
-        <v>24.755685790000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37.693282359999998</v>
+      </c>
+      <c r="G52">
+        <v>27.977932450000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>80</v>
       </c>
@@ -55692,13 +55818,16 @@
         <v>0.34144351099999998</v>
       </c>
       <c r="E53">
-        <v>22.244219380000001</v>
+        <v>47.98131076</v>
       </c>
       <c r="F53">
-        <v>21.91591828</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48.002807519999998</v>
+      </c>
+      <c r="G53">
+        <v>25.434247490000001</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>81</v>
       </c>
@@ -55712,13 +55841,16 @@
         <v>-4.5439834149999996</v>
       </c>
       <c r="E54">
-        <v>37.931997760000002</v>
+        <v>38.627854919999997</v>
       </c>
       <c r="F54">
-        <v>37.695969419999997</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38.728504549999997</v>
+      </c>
+      <c r="G54">
+        <v>21.41662676</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>82</v>
       </c>
@@ -55732,13 +55864,16 @@
         <v>-4.9917420129999996</v>
       </c>
       <c r="E55">
-        <v>47.991592220000001</v>
+        <v>38.875813020000002</v>
       </c>
       <c r="F55">
-        <v>47.997084319999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38.993483159999997</v>
+      </c>
+      <c r="G55">
+        <v>17.178114799999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>83</v>
       </c>
@@ -55752,13 +55887,16 @@
         <v>20.88968156</v>
       </c>
       <c r="E56">
-        <v>38.613781539999998</v>
+        <v>30.402213750000001</v>
       </c>
       <c r="F56">
-        <v>38.575686599999997</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31.189585940000001</v>
+      </c>
+      <c r="G56">
+        <v>17.786727070000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>84</v>
       </c>
@@ -55772,13 +55910,16 @@
         <v>18.410460629999999</v>
       </c>
       <c r="E57">
-        <v>38.809683149999998</v>
+        <v>18.198711459999998</v>
       </c>
       <c r="F57">
-        <v>38.894824540000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20.479849909999999</v>
+      </c>
+      <c r="G57">
+        <v>7.4350952079999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>85</v>
       </c>
@@ -55792,13 +55933,16 @@
         <v>14.26045899</v>
       </c>
       <c r="E58">
-        <v>30.42996218</v>
+        <v>28.523269209999999</v>
       </c>
       <c r="F58">
-        <v>31.038184260000001</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28.629359109999999</v>
+      </c>
+      <c r="G58">
+        <v>10.923093590000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -55812,13 +55956,16 @@
         <v>10.23795619</v>
       </c>
       <c r="E59">
-        <v>18.197736290000002</v>
+        <v>19.05421291</v>
       </c>
       <c r="F59">
-        <v>20.482861700000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+        <v>19.542805260000002</v>
+      </c>
+      <c r="G59">
+        <v>5.493413339</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>87</v>
       </c>
@@ -55832,13 +55979,16 @@
         <v>10.4417294</v>
       </c>
       <c r="E60">
-        <v>28.4126318</v>
+        <v>15.494253219999999</v>
       </c>
       <c r="F60">
-        <v>28.434127069999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+        <v>16.594945110000001</v>
+      </c>
+      <c r="G60">
+        <v>-2.5521074810000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>88</v>
       </c>
@@ -55852,13 +56002,16 @@
         <v>0.65002020100000002</v>
       </c>
       <c r="E61">
-        <v>19.117962540000001</v>
+        <v>24.391215249999998</v>
       </c>
       <c r="F61">
-        <v>19.4953225</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24.55817437</v>
+      </c>
+      <c r="G61">
+        <v>6.9376494019999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>89</v>
       </c>
@@ -55872,13 +56025,16 @@
         <v>3.9681436329999999</v>
       </c>
       <c r="E62">
-        <v>15.513041660000001</v>
+        <v>21.827299100000001</v>
       </c>
       <c r="F62">
-        <v>16.908230289999999</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+        <v>22.083255609999998</v>
+      </c>
+      <c r="G62">
+        <v>4.5896431939999998</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>90</v>
       </c>
@@ -55892,13 +56048,16 @@
         <v>-1.3255991380000001</v>
       </c>
       <c r="E63">
-        <v>24.292059330000001</v>
+        <v>22.177581759999999</v>
       </c>
       <c r="F63">
-        <v>24.523094749999998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+        <v>22.785978459999999</v>
+      </c>
+      <c r="G63">
+        <v>15.803091780000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>91</v>
       </c>
@@ -55912,13 +56071,16 @@
         <v>-9.6654234849999998</v>
       </c>
       <c r="E64">
-        <v>21.853009950000001</v>
+        <v>20.271293499999999</v>
       </c>
       <c r="F64">
-        <v>22.036313450000002</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+        <v>20.202635069999999</v>
+      </c>
+      <c r="G64">
+        <v>13.80605645</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>92</v>
       </c>
@@ -55931,14 +56093,8 @@
       <c r="D65">
         <v>3.9612223000000002E-2</v>
       </c>
-      <c r="E65">
-        <v>22.179185109999999</v>
-      </c>
-      <c r="F65">
-        <v>22.849186209999999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>93</v>
       </c>
@@ -55951,14 +56107,8 @@
       <c r="D66">
         <v>-2.304787352</v>
       </c>
-      <c r="E66">
-        <v>20.267898550000002</v>
-      </c>
-      <c r="F66">
-        <v>20.199494940000001</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>94</v>
       </c>
@@ -55972,7 +56122,7 @@
         <v>8.7170058449999992</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>286</v>
       </c>
@@ -55986,7 +56136,7 @@
         <v>7.099003873</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>287</v>
       </c>
@@ -56000,7 +56150,7 @@
         <v>4.6333450599999999</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>288</v>
       </c>
@@ -56014,7 +56164,7 @@
         <v>5.065418384</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>171</v>
       </c>
@@ -56028,13 +56178,16 @@
         <v>-11.50144839</v>
       </c>
       <c r="E71">
-        <v>-10.50408569</v>
+        <v>-10.678776429999999</v>
       </c>
       <c r="F71">
-        <v>-10.688280969999999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-10.678080680000001</v>
+      </c>
+      <c r="G71">
+        <v>-11.42236802</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>172</v>
       </c>
@@ -56048,13 +56201,16 @@
         <v>-8.6758721780000005</v>
       </c>
       <c r="E72">
-        <v>-8.6224331129999996</v>
+        <v>-8.7806096419999999</v>
       </c>
       <c r="F72">
-        <v>-8.0072484839999998</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-7.8900304329999997</v>
+      </c>
+      <c r="G72">
+        <v>-9.1091713470000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>173</v>
       </c>
@@ -56068,13 +56224,16 @@
         <v>-13.369654329999999</v>
       </c>
       <c r="E73">
-        <v>-11.478918289999999</v>
+        <v>-11.37255706</v>
       </c>
       <c r="F73">
-        <v>-10.9734225</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-10.96669831</v>
+      </c>
+      <c r="G73">
+        <v>-13.29912062</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>174</v>
       </c>
@@ -56088,13 +56247,16 @@
         <v>-9.5166939750000008</v>
       </c>
       <c r="E74">
-        <v>-4.8905538479999997</v>
+        <v>-4.9182511519999998</v>
       </c>
       <c r="F74">
-        <v>-6.4007158779999997</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.406286368</v>
+      </c>
+      <c r="G74">
+        <v>-9.6135725880000003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>175</v>
       </c>
@@ -56108,13 +56270,16 @@
         <v>-16.65868253</v>
       </c>
       <c r="E75">
-        <v>-9.4955086160000004</v>
+        <v>-7.041931881</v>
       </c>
       <c r="F75">
-        <v>-9.2963848109999994</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.6047718929999997</v>
+      </c>
+      <c r="G75">
+        <v>-9.4312087679999994</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>176</v>
       </c>
@@ -56128,13 +56293,16 @@
         <v>-9.4889325249999992</v>
       </c>
       <c r="E76">
-        <v>-7.044971608</v>
+        <v>-12.288384349999999</v>
       </c>
       <c r="F76">
-        <v>-6.5966250400000002</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-12.556326609999999</v>
+      </c>
+      <c r="G76">
+        <v>-13.17918441</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>177</v>
       </c>
@@ -56148,13 +56316,16 @@
         <v>-13.19484031</v>
       </c>
       <c r="E77">
-        <v>-12.218507089999999</v>
+        <v>-7.6991542610000003</v>
       </c>
       <c r="F77">
-        <v>-12.539181409999999</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-7.3969692519999999</v>
+      </c>
+      <c r="G77">
+        <v>-8.0936128509999996</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>178</v>
       </c>
@@ -56168,13 +56339,16 @@
         <v>-8.2138069970000007</v>
       </c>
       <c r="E78">
-        <v>-7.6034633789999999</v>
+        <v>-5.2042955949999996</v>
       </c>
       <c r="F78">
-        <v>-7.3767807510000001</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-4.3917189570000001</v>
+      </c>
+      <c r="G78">
+        <v>-3.9907945429999998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>179</v>
       </c>
@@ -56188,13 +56362,16 @@
         <v>-9.852415916</v>
       </c>
       <c r="E79">
-        <v>-5.18813908</v>
+        <v>-3.5856514079999999</v>
       </c>
       <c r="F79">
-        <v>-4.3745797130000001</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-3.4955679370000001</v>
+      </c>
+      <c r="G79">
+        <v>-4.7333389730000004</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>180</v>
       </c>
@@ -56208,13 +56385,16 @@
         <v>-4.0159340139999999</v>
       </c>
       <c r="E80">
-        <v>-3.5899678750000001</v>
+        <v>-15.19890704</v>
       </c>
       <c r="F80">
-        <v>-3.4857209629999999</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-15.166378999999999</v>
+      </c>
+      <c r="G80">
+        <v>-12.083018109999999</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>181</v>
       </c>
@@ -56228,13 +56408,16 @@
         <v>-4.7301313929999997</v>
       </c>
       <c r="E81">
-        <v>-15.170934920000001</v>
+        <v>-8.4896641220000006</v>
       </c>
       <c r="F81">
-        <v>-15.109564779999999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-7.9980939009999998</v>
+      </c>
+      <c r="G81">
+        <v>-8.6936809119999996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -56248,13 +56431,16 @@
         <v>-12.268933799999999</v>
       </c>
       <c r="E82">
-        <v>-8.3390443249999997</v>
+        <v>-8.6558747870000001</v>
       </c>
       <c r="F82">
-        <v>-7.9076009789999997</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-8.0964628120000004</v>
+      </c>
+      <c r="G82">
+        <v>-8.9962407049999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>183</v>
       </c>
@@ -56268,13 +56454,16 @@
         <v>-8.6801441449999999</v>
       </c>
       <c r="E83">
-        <v>-8.5948772959999999</v>
+        <v>-9.4228216109999998</v>
       </c>
       <c r="F83">
-        <v>-8.0698334969999994</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-8.7938070419999992</v>
+      </c>
+      <c r="G83">
+        <v>-11.82029206</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>184</v>
       </c>
@@ -56288,13 +56477,16 @@
         <v>-9.1239621690000003</v>
       </c>
       <c r="E84">
-        <v>-9.4298622099999996</v>
+        <v>-23.235721519999998</v>
       </c>
       <c r="F84">
-        <v>-8.8341852440000004</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-23.06353476</v>
+      </c>
+      <c r="G84">
+        <v>-11.454144830000001</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>185</v>
       </c>
@@ -56308,13 +56500,16 @@
         <v>-11.889131239999999</v>
       </c>
       <c r="E85">
-        <v>-23.255868490000001</v>
+        <v>-10.888205859999999</v>
       </c>
       <c r="F85">
-        <v>-23.0889761</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-10.40137928</v>
+      </c>
+      <c r="G85">
+        <v>-12.094129799999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>186</v>
       </c>
@@ -56328,13 +56523,16 @@
         <v>-11.3820146</v>
       </c>
       <c r="E86">
-        <v>-10.9380215</v>
+        <v>-8.8216880910000004</v>
       </c>
       <c r="F86">
-        <v>-10.37604625</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-8.679340667</v>
+      </c>
+      <c r="G86">
+        <v>-9.3288408530000009</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>187</v>
       </c>
@@ -56348,13 +56546,16 @@
         <v>-9.6373865989999992</v>
       </c>
       <c r="E87">
-        <v>-8.7554393869999991</v>
+        <v>-8.3856699799999994</v>
       </c>
       <c r="F87">
-        <v>-8.5613584100000004</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-7.9678407519999999</v>
+      </c>
+      <c r="G87">
+        <v>-8.8774093670000003</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>188</v>
       </c>
@@ -56368,13 +56569,16 @@
         <v>-9.4344042819999991</v>
       </c>
       <c r="E88">
-        <v>-8.3440179099999998</v>
+        <v>-4.4004358679999998</v>
       </c>
       <c r="F88">
-        <v>-7.9061718880000003</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-3.6246874390000001</v>
+      </c>
+      <c r="G88">
+        <v>-7.0369628759999996</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>189</v>
       </c>
@@ -56388,13 +56592,16 @@
         <v>-9.1078877699999996</v>
       </c>
       <c r="E89">
-        <v>-9.5050545759999991</v>
+        <v>-10.67261339</v>
       </c>
       <c r="F89">
-        <v>-9.3074714590000003</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-10.10328863</v>
+      </c>
+      <c r="G89">
+        <v>-11.08924126</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>190</v>
       </c>
@@ -56408,13 +56615,16 @@
         <v>-5.3453657059999999</v>
       </c>
       <c r="E90">
-        <v>-4.366365075</v>
+        <v>-9.8575719629999998</v>
       </c>
       <c r="F90">
-        <v>-3.6001341990000002</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-9.4257025970000008</v>
+      </c>
+      <c r="G90">
+        <v>-10.55498792</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>191</v>
       </c>
@@ -56428,13 +56638,16 @@
         <v>-7.02513626</v>
       </c>
       <c r="E91">
-        <v>-10.47999566</v>
+        <v>-8.5521062319999999</v>
       </c>
       <c r="F91">
-        <v>-9.9619102480000006</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-8.2162707079999997</v>
+      </c>
+      <c r="G91">
+        <v>-7.9978496080000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>192</v>
       </c>
@@ -56448,13 +56661,16 @@
         <v>-17.339880480000001</v>
       </c>
       <c r="E92">
-        <v>-9.7739971440000009</v>
+        <v>-12.506647210000001</v>
       </c>
       <c r="F92">
-        <v>-9.3082621670000005</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-13.069772990000001</v>
+      </c>
+      <c r="G92">
+        <v>-11.7955969</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>193</v>
       </c>
@@ -56468,13 +56684,16 @@
         <v>-11.18178344</v>
       </c>
       <c r="E93">
-        <v>-8.5468457539999996</v>
+        <v>-24.081027800000001</v>
       </c>
       <c r="F93">
-        <v>-8.0775471640000003</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-24.173186789999999</v>
+      </c>
+      <c r="G93">
+        <v>-25.767405069999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>194</v>
       </c>
@@ -56488,13 +56707,16 @@
         <v>-10.621267530000001</v>
       </c>
       <c r="E94">
-        <v>-12.434173449999999</v>
+        <v>-17.101994529999999</v>
       </c>
       <c r="F94">
-        <v>-13.052120520000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-16.459531460000001</v>
+      </c>
+      <c r="G94">
+        <v>-16.739639050000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>195</v>
       </c>
@@ -56508,13 +56730,16 @@
         <v>-8.2729745640000001</v>
       </c>
       <c r="E95">
-        <v>-24.15641085</v>
+        <v>-13.88600506</v>
       </c>
       <c r="F95">
-        <v>-24.183218589999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-13.08094088</v>
+      </c>
+      <c r="G95">
+        <v>-16.379213310000001</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>196</v>
       </c>
@@ -56528,13 +56753,16 @@
         <v>-11.95461927</v>
       </c>
       <c r="E96">
-        <v>-17.14231771</v>
+        <v>-6.5497902010000004</v>
       </c>
       <c r="F96">
-        <v>-16.48159193</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.0740018490000001</v>
+      </c>
+      <c r="G96">
+        <v>-7.5863942389999997</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>197</v>
       </c>
@@ -56548,13 +56776,16 @@
         <v>-25.69223981</v>
       </c>
       <c r="E97">
-        <v>-13.87572636</v>
+        <v>-4.0403056079999997</v>
       </c>
       <c r="F97">
-        <v>-12.969248800000001</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-4.9282816619999998</v>
+      </c>
+      <c r="G97">
+        <v>-9.925146582</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>198</v>
       </c>
@@ -56568,13 +56799,16 @@
         <v>-16.653008400000001</v>
       </c>
       <c r="E98">
-        <v>-6.5529814049999997</v>
+        <v>-5.2053940240000003</v>
       </c>
       <c r="F98">
-        <v>-6.0037276730000002</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.833885242</v>
+      </c>
+      <c r="G98">
+        <v>-2.490109178</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>199</v>
       </c>
@@ -56588,13 +56822,16 @@
         <v>-16.37266018</v>
       </c>
       <c r="E99">
-        <v>-3.867404353</v>
+        <v>-8.3802788929999998</v>
       </c>
       <c r="F99">
-        <v>-4.9071277750000002</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-7.9606202420000001</v>
+      </c>
+      <c r="G99">
+        <v>-8.7683741229999992</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>200</v>
       </c>
@@ -56608,13 +56845,16 @@
         <v>-7.679242736</v>
       </c>
       <c r="E100">
-        <v>-5.1915475000000004</v>
+        <v>-3.1131249080000001</v>
       </c>
       <c r="F100">
-        <v>-6.8459487499999998</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.7530638870000002</v>
+      </c>
+      <c r="G100">
+        <v>-6.7613839420000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>201</v>
       </c>
@@ -56628,13 +56868,16 @@
         <v>-9.7983471840000007</v>
       </c>
       <c r="E101">
-        <v>-8.3443694159999993</v>
+        <v>-6.0208324510000004</v>
       </c>
       <c r="F101">
-        <v>-7.7841672229999999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.6588619229999999</v>
+      </c>
+      <c r="G101">
+        <v>-5.8290840140000002</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>202</v>
       </c>
@@ -56648,13 +56891,16 @@
         <v>-2.4770235230000002</v>
       </c>
       <c r="E102">
-        <v>-3.0396893770000002</v>
+        <v>-11.92613777</v>
       </c>
       <c r="F102">
-        <v>-2.7203704379999998</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-11.38020137</v>
+      </c>
+      <c r="G102">
+        <v>-12.45162685</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>203</v>
       </c>
@@ -56668,13 +56914,16 @@
         <v>-8.8367433030000004</v>
       </c>
       <c r="E103">
-        <v>-5.9673701929999998</v>
+        <v>-7.2595535440000001</v>
       </c>
       <c r="F103">
-        <v>-6.3040792059999999</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.8085243870000003</v>
+      </c>
+      <c r="G103">
+        <v>-7.7178984120000003</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>204</v>
       </c>
@@ -56688,13 +56937,16 @@
         <v>-6.8285820629999998</v>
       </c>
       <c r="E104">
-        <v>-11.818815430000001</v>
+        <v>-2.7516219259999999</v>
       </c>
       <c r="F104">
-        <v>-11.347312759999999</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.6901596539999999</v>
+      </c>
+      <c r="G104">
+        <v>-3.1592606249999999</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>205</v>
       </c>
@@ -56708,13 +56960,16 @@
         <v>-6.0393109230000004</v>
       </c>
       <c r="E105">
-        <v>-7.2754686949999998</v>
+        <v>-14.010940980000001</v>
       </c>
       <c r="F105">
-        <v>-6.8216772700000003</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-14.00650282</v>
+      </c>
+      <c r="G105">
+        <v>-17.19716523</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>206</v>
       </c>
@@ -56727,14 +56982,8 @@
       <c r="D106">
         <v>-12.644671689999999</v>
       </c>
-      <c r="E106">
-        <v>-2.6179350669999999</v>
-      </c>
-      <c r="F106">
-        <v>-2.6445745660000002</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>207</v>
       </c>
@@ -56747,14 +56996,8 @@
       <c r="D107">
         <v>-7.9151009669999999</v>
       </c>
-      <c r="E107">
-        <v>-14.001959490000001</v>
-      </c>
-      <c r="F107">
-        <v>-14.01086199</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>208</v>
       </c>
@@ -56768,7 +57011,7 @@
         <v>-3.208250558</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>448</v>
       </c>
@@ -56782,7 +57025,7 @@
         <v>-17.181795839999999</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>449</v>
       </c>
@@ -56796,7 +57039,7 @@
         <v>-11.507613989999999</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>450</v>
       </c>
@@ -56810,7 +57053,7 @@
         <v>-11.063626599999999</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>133</v>
       </c>
@@ -56824,13 +57067,16 @@
         <v>-0.70366551799999999</v>
       </c>
       <c r="E112">
-        <v>-1.54249627</v>
+        <v>-1.627697003</v>
       </c>
       <c r="F112">
-        <v>-1.6345281819999999</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.5669306949999999</v>
+      </c>
+      <c r="G112">
+        <v>-0.68810243500000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>134</v>
       </c>
@@ -56844,13 +57090,16 @@
         <v>-0.78350229599999999</v>
       </c>
       <c r="E113">
-        <v>-1.101949801</v>
+        <v>-1.1439493430000001</v>
       </c>
       <c r="F113">
-        <v>-1.6202482199999999</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.720036906</v>
+      </c>
+      <c r="G113">
+        <v>-0.70202260699999997</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>135</v>
       </c>
@@ -56864,13 +57113,16 @@
         <v>0.58628923399999999</v>
       </c>
       <c r="E114">
-        <v>1.2470463890000001</v>
+        <v>1.1977126979999999</v>
       </c>
       <c r="F114">
-        <v>1.1412949590000001</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1.129267314</v>
+      </c>
+      <c r="G114">
+        <v>0.56769618700000002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>136</v>
       </c>
@@ -56884,13 +57136,16 @@
         <v>-0.28423729199999997</v>
       </c>
       <c r="E115">
-        <v>-1.2985261720000001</v>
+        <v>-1.248114599</v>
       </c>
       <c r="F115">
-        <v>-1.426161416</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.3706021829999999</v>
+      </c>
+      <c r="G115">
+        <v>-0.188485139</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>137</v>
       </c>
@@ -56904,13 +57159,16 @@
         <v>4.4918854000000001E-2</v>
       </c>
       <c r="E116">
-        <v>-1.2462005839999999</v>
+        <v>-1.7980429060000001</v>
       </c>
       <c r="F116">
-        <v>-1.582312736</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.877093849</v>
+      </c>
+      <c r="G116">
+        <v>-0.93009996800000005</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>138</v>
       </c>
@@ -56924,13 +57182,16 @@
         <v>-0.97550925700000002</v>
       </c>
       <c r="E117">
-        <v>-1.7980865290000001</v>
+        <v>-0.78020702600000003</v>
       </c>
       <c r="F117">
-        <v>-1.866155706</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.4929988619999999</v>
+      </c>
+      <c r="G117">
+        <v>0.50805517499999997</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>139</v>
       </c>
@@ -56944,13 +57205,16 @@
         <v>0.48723192500000001</v>
       </c>
       <c r="E118">
-        <v>-0.740413337</v>
+        <v>-0.67199349500000005</v>
       </c>
       <c r="F118">
-        <v>-2.5016483260000002</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.5809587650000001</v>
+      </c>
+      <c r="G118">
+        <v>-8.6604519000000005E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>140</v>
       </c>
@@ -56964,13 +57228,16 @@
         <v>-0.109138734</v>
       </c>
       <c r="E119">
-        <v>-0.674116838</v>
+        <v>-0.611395409</v>
       </c>
       <c r="F119">
-        <v>-2.607267604</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.535860617</v>
+      </c>
+      <c r="G119">
+        <v>-1.9009855550000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>141</v>
       </c>
@@ -56984,13 +57251,16 @@
         <v>-0.68149007399999995</v>
       </c>
       <c r="E120">
-        <v>-0.61021801200000003</v>
+        <v>-0.79282485199999997</v>
       </c>
       <c r="F120">
-        <v>-1.5092126800000001</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.2397723620000001</v>
+      </c>
+      <c r="G120">
+        <v>-1.8375550389999999</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>142</v>
       </c>
@@ -57004,13 +57274,16 @@
         <v>-1.916757979</v>
       </c>
       <c r="E121">
-        <v>-0.80797556699999995</v>
+        <v>-1.073391845</v>
       </c>
       <c r="F121">
-        <v>-1.2337688920000001</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.4726749729999999</v>
+      </c>
+      <c r="G121">
+        <v>-0.238443082</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>143</v>
       </c>
@@ -57024,13 +57297,16 @@
         <v>-1.8472521369999999</v>
       </c>
       <c r="E122">
-        <v>-1.0947939870000001</v>
+        <v>-2.0249707809999999</v>
       </c>
       <c r="F122">
-        <v>-1.5042115519999999</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.2576517389999999</v>
+      </c>
+      <c r="G122">
+        <v>-0.99043092600000004</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>144</v>
       </c>
@@ -57044,13 +57320,16 @@
         <v>-0.131545408</v>
       </c>
       <c r="E123">
-        <v>-1.9555954600000001</v>
+        <v>-0.52458647700000005</v>
       </c>
       <c r="F123">
-        <v>-2.2881058630000002</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.86252148200000001</v>
+      </c>
+      <c r="G123">
+        <v>-0.19751938199999999</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>145</v>
       </c>
@@ -57064,13 +57343,16 @@
         <v>-0.99192897899999999</v>
       </c>
       <c r="E124">
-        <v>-0.59233664500000005</v>
+        <v>-0.41631469599999998</v>
       </c>
       <c r="F124">
-        <v>-0.83864300199999997</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.238500987</v>
+      </c>
+      <c r="G124">
+        <v>3.0696534000000001E-2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>146</v>
       </c>
@@ -57084,13 +57366,16 @@
         <v>-0.24778525700000001</v>
       </c>
       <c r="E125">
-        <v>-0.44359893900000003</v>
+        <v>-15.39141613</v>
       </c>
       <c r="F125">
-        <v>-0.21267143199999999</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-15.38615184</v>
+      </c>
+      <c r="G125">
+        <v>-6.478633297</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>147</v>
       </c>
@@ -57104,13 +57389,16 @@
         <v>6.2881300000000003E-3</v>
       </c>
       <c r="E126">
-        <v>-15.378446930000001</v>
+        <v>-1.362053994</v>
       </c>
       <c r="F126">
-        <v>-15.41161353</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.3820553760000001</v>
+      </c>
+      <c r="G126">
+        <v>-0.71719174500000005</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>148</v>
       </c>
@@ -57124,13 +57412,16 @@
         <v>-6.4266707839999997</v>
       </c>
       <c r="E127">
-        <v>-1.35642284</v>
+        <v>-2.1853631500000001</v>
       </c>
       <c r="F127">
-        <v>-1.4186499669999999</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.7994263770000001</v>
+      </c>
+      <c r="G127">
+        <v>-1.19235281</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>149</v>
       </c>
@@ -57144,13 +57435,16 @@
         <v>-0.66645996100000005</v>
       </c>
       <c r="E128">
-        <v>-2.2781341799999999</v>
+        <v>-0.24926853400000001</v>
       </c>
       <c r="F128">
-        <v>-1.8848876299999999</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.58513356699999997</v>
+      </c>
+      <c r="G128">
+        <v>1.1170869999999999E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>150</v>
       </c>
@@ -57164,13 +57458,16 @@
         <v>-1.2015288340000001</v>
       </c>
       <c r="E129">
-        <v>-0.23749030900000001</v>
+        <v>14.593279900000001</v>
       </c>
       <c r="F129">
-        <v>-0.68920368799999998</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13.48351416</v>
+      </c>
+      <c r="G129">
+        <v>9.2254736610000005</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>151</v>
       </c>
@@ -57184,13 +57481,16 @@
         <v>-4.4690924E-2</v>
       </c>
       <c r="E130">
-        <v>-1.2436185369999999</v>
+        <v>-0.46960242800000002</v>
       </c>
       <c r="F130">
-        <v>-1.5953122900000001</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.5893889050000001</v>
+      </c>
+      <c r="G130">
+        <v>-0.26801866800000002</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>152</v>
       </c>
@@ -57204,13 +57504,16 @@
         <v>-0.66559978099999995</v>
       </c>
       <c r="E131">
-        <v>14.56826278</v>
+        <v>-0.54653925800000003</v>
       </c>
       <c r="F131">
-        <v>13.52534417</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.672523066</v>
+      </c>
+      <c r="G131">
+        <v>-0.12774176700000001</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>153</v>
       </c>
@@ -57224,13 +57527,16 @@
         <v>9.0209837010000005</v>
       </c>
       <c r="E132">
-        <v>-0.48969938899999998</v>
+        <v>-0.42749201199999998</v>
       </c>
       <c r="F132">
-        <v>-1.6023410760000001</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.78703204100000002</v>
+      </c>
+      <c r="G132">
+        <v>-8.4623113E-2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>154</v>
       </c>
@@ -57244,13 +57550,16 @@
         <v>0.319612226</v>
       </c>
       <c r="E133">
-        <v>-0.52273712000000006</v>
+        <v>-1.28566059</v>
       </c>
       <c r="F133">
-        <v>-0.73968992200000006</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.9364971310000001</v>
+      </c>
+      <c r="G133">
+        <v>0.58109891400000002</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>155</v>
       </c>
@@ -57264,13 +57573,16 @@
         <v>-0.30998133700000002</v>
       </c>
       <c r="E134">
-        <v>-0.38875378700000002</v>
+        <v>-5.2913808019999999</v>
       </c>
       <c r="F134">
-        <v>-0.73815480200000005</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-4.6638952370000002</v>
+      </c>
+      <c r="G134">
+        <v>-1.2345695379999999</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>156</v>
       </c>
@@ -57284,13 +57596,16 @@
         <v>-0.211857516</v>
       </c>
       <c r="E135">
-        <v>-1.301150536</v>
+        <v>-3.1875003190000002</v>
       </c>
       <c r="F135">
-        <v>-1.829894278</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-3.0691407289999999</v>
+      </c>
+      <c r="G135">
+        <v>-1.8790009910000001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>157</v>
       </c>
@@ -57304,13 +57619,16 @@
         <v>-6.761029E-3</v>
       </c>
       <c r="E136">
-        <v>-5.3639086589999998</v>
+        <v>4.5401126930000002</v>
       </c>
       <c r="F136">
-        <v>-4.7306284810000001</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+        <v>3.5239846780000001</v>
+      </c>
+      <c r="G136">
+        <v>2.6602626749999998</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>158</v>
       </c>
@@ -57324,13 +57642,16 @@
         <v>0.49174409600000002</v>
       </c>
       <c r="E137">
-        <v>-3.0583274029999998</v>
+        <v>-1.601610505</v>
       </c>
       <c r="F137">
-        <v>-3.0553179240000001</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.605105811</v>
+      </c>
+      <c r="G137">
+        <v>-0.81834406699999995</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>159</v>
       </c>
@@ -57344,13 +57665,16 @@
         <v>-1.2066836320000001</v>
       </c>
       <c r="E138">
-        <v>4.4903337920000004</v>
+        <v>-4.5473793110000003</v>
       </c>
       <c r="F138">
-        <v>3.578691209</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-3.784510756</v>
+      </c>
+      <c r="G138">
+        <v>-1.2131572820000001</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>160</v>
       </c>
@@ -57364,13 +57688,16 @@
         <v>-1.8883339690000001</v>
       </c>
       <c r="E139">
-        <v>-1.5472034050000001</v>
+        <v>-6.3449149970000001</v>
       </c>
       <c r="F139">
-        <v>-1.6037146819999999</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.8114805450000002</v>
+      </c>
+      <c r="G139">
+        <v>0.69423808200000003</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>161</v>
       </c>
@@ -57384,13 +57711,16 @@
         <v>2.4921936819999999</v>
       </c>
       <c r="E140">
-        <v>-4.3797040579999997</v>
+        <v>0.29928017000000001</v>
       </c>
       <c r="F140">
-        <v>-3.910855094</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.26778464000000002</v>
+      </c>
+      <c r="G140">
+        <v>0.30234963100000001</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>162</v>
       </c>
@@ -57404,13 +57734,16 @@
         <v>-0.81771637699999999</v>
       </c>
       <c r="E141">
-        <v>-6.3326432869999998</v>
+        <v>-3.933400566</v>
       </c>
       <c r="F141">
-        <v>-6.8158070459999998</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-4.3293286650000002</v>
+      </c>
+      <c r="G141">
+        <v>-1.702074128</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>163</v>
       </c>
@@ -57424,13 +57757,16 @@
         <v>-1.2836173179999999</v>
       </c>
       <c r="E142">
-        <v>0.22923033700000001</v>
+        <v>-0.91085142900000005</v>
       </c>
       <c r="F142">
-        <v>0.124953088</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.86942153099999997</v>
+      </c>
+      <c r="G142">
+        <v>-0.65517245599999996</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>164</v>
       </c>
@@ -57444,13 +57780,16 @@
         <v>0.64485883700000002</v>
       </c>
       <c r="E143">
-        <v>-3.8920127400000002</v>
+        <v>-1.028281435</v>
       </c>
       <c r="F143">
-        <v>-4.3459286730000004</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.1304949689999999</v>
+      </c>
+      <c r="G143">
+        <v>-0.48558965500000001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>165</v>
       </c>
@@ -57464,13 +57803,16 @@
         <v>0.34454116800000001</v>
       </c>
       <c r="E144">
-        <v>-0.96077446600000005</v>
+        <v>0.231567575</v>
       </c>
       <c r="F144">
-        <v>0.91240526899999996</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.15452690999999999</v>
+      </c>
+      <c r="G144">
+        <v>0.42606930799999998</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>166</v>
       </c>
@@ -57484,13 +57826,16 @@
         <v>-1.6776416919999999</v>
       </c>
       <c r="E145">
-        <v>-1.1335538060000001</v>
+        <v>-2.8511609689999999</v>
       </c>
       <c r="F145">
-        <v>-1.181551899</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-3.1817345939999999</v>
+      </c>
+      <c r="G145">
+        <v>-1.520415606</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>167</v>
       </c>
@@ -57504,13 +57849,16 @@
         <v>-0.70272491299999995</v>
       </c>
       <c r="E146">
-        <v>0.21106697199999999</v>
+        <v>-4.6104506709999997</v>
       </c>
       <c r="F146">
-        <v>-0.183238175</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.7008177849999999</v>
+      </c>
+      <c r="G146">
+        <v>-2.965290516</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>168</v>
       </c>
@@ -57523,14 +57871,8 @@
       <c r="D147">
         <v>-0.53106676200000003</v>
       </c>
-      <c r="E147">
-        <v>-2.7046627189999999</v>
-      </c>
-      <c r="F147">
-        <v>-3.1040212199999999</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>169</v>
       </c>
@@ -57543,14 +57885,8 @@
       <c r="D148">
         <v>0.31447302399999999</v>
       </c>
-      <c r="E148">
-        <v>-4.5927750879999998</v>
-      </c>
-      <c r="F148">
-        <v>-2.7309416020000001</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>170</v>
       </c>
@@ -57564,7 +57900,7 @@
         <v>-1.5158220250000001</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>610</v>
       </c>
@@ -57578,7 +57914,7 @@
         <v>-2.952463442</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>611</v>
       </c>
@@ -57592,7 +57928,7 @@
         <v>-0.58928871599999999</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>612</v>
       </c>
@@ -57606,7 +57942,7 @@
         <v>-0.67189302699999998</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>95</v>
       </c>
@@ -57620,13 +57956,16 @@
         <v>-10.325107360000001</v>
       </c>
       <c r="E153">
-        <v>-9.4475470270000006</v>
+        <v>-9.4254060039999992</v>
       </c>
       <c r="F153">
-        <v>-9.6720522070000001</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-9.6440500589999996</v>
+      </c>
+      <c r="G153">
+        <v>-10.465240830000001</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>96</v>
       </c>
@@ -57640,13 +57979,16 @@
         <v>0.772517483</v>
       </c>
       <c r="E154">
-        <v>-2.0258249990000001</v>
+        <v>-2.0960113599999999</v>
       </c>
       <c r="F154">
-        <v>-3.1725941959999999</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-3.1724150080000002</v>
+      </c>
+      <c r="G154">
+        <v>1.107612692</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>97</v>
       </c>
@@ -57660,13 +58002,16 @@
         <v>-9.3678431720000006</v>
       </c>
       <c r="E155">
-        <v>-9.2662234740000002</v>
+        <v>-9.2497904759999994</v>
       </c>
       <c r="F155">
-        <v>-9.8284709009999993</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-9.8184370659999995</v>
+      </c>
+      <c r="G155">
+        <v>-9.4275873370000003</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>98</v>
       </c>
@@ -57680,13 +58025,16 @@
         <v>-1.401189537</v>
       </c>
       <c r="E156">
-        <v>-2.6877014680000002</v>
+        <v>-2.7976920679999999</v>
       </c>
       <c r="F156">
-        <v>-2.8206150239999999</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.7696627060000001</v>
+      </c>
+      <c r="G156">
+        <v>-1.5416374500000001</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>99</v>
       </c>
@@ -57700,13 +58048,16 @@
         <v>-4.2927207369999998</v>
       </c>
       <c r="E157">
-        <v>-6.2927315080000001</v>
+        <v>0.27784435899999999</v>
       </c>
       <c r="F157">
-        <v>-6.4642511699999998</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.62622204599999998</v>
+      </c>
+      <c r="G157">
+        <v>-2.8722385E-2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>100</v>
       </c>
@@ -57720,13 +58071,16 @@
         <v>-2.9192300000000001E-3</v>
       </c>
       <c r="E158">
-        <v>0.218790917</v>
+        <v>-9.3019916859999991</v>
       </c>
       <c r="F158">
-        <v>-0.57611203600000005</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-10.006040949999999</v>
+      </c>
+      <c r="G158">
+        <v>-8.6127776740000002</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>101</v>
       </c>
@@ -57740,13 +58094,16 @@
         <v>-8.4342274069999998</v>
       </c>
       <c r="E159">
-        <v>-9.3131248689999993</v>
+        <v>-8.1917536089999992</v>
       </c>
       <c r="F159">
-        <v>-9.9758104470000006</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-8.3832558899999992</v>
+      </c>
+      <c r="G159">
+        <v>-8.6629370990000005</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>102</v>
       </c>
@@ -57760,13 +58117,16 @@
         <v>-8.5795524850000007</v>
       </c>
       <c r="E160">
-        <v>-8.2581235569999993</v>
+        <v>3.6811285999999999E-2</v>
       </c>
       <c r="F160">
-        <v>-8.3583898669999996</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.333081918</v>
+      </c>
+      <c r="G160">
+        <v>-4.2296466170000002</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>103</v>
       </c>
@@ -57780,13 +58140,16 @@
         <v>-4.7575144549999999</v>
       </c>
       <c r="E161">
-        <v>1.5604081000000001E-2</v>
+        <v>-2.658767654</v>
       </c>
       <c r="F161">
-        <v>-1.3189689330000001</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.632384388</v>
+      </c>
+      <c r="G161">
+        <v>-3.6191177080000001</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>104</v>
       </c>
@@ -57800,13 +58163,16 @@
         <v>-4.1073590360000001</v>
       </c>
       <c r="E162">
-        <v>-2.6744561359999999</v>
+        <v>-3.8037737570000001</v>
       </c>
       <c r="F162">
-        <v>-1.6321695409999999</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-4.6301363919999998</v>
+      </c>
+      <c r="G162">
+        <v>-0.69036659199999995</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>105</v>
       </c>
@@ -57820,13 +58186,16 @@
         <v>-3.5970907780000001</v>
       </c>
       <c r="E163">
-        <v>-3.7146953969999998</v>
+        <v>-8.1768965470000001</v>
       </c>
       <c r="F163">
-        <v>-4.5735952869999998</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-8.6599303419999991</v>
+      </c>
+      <c r="G163">
+        <v>-6.354570786</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>106</v>
       </c>
@@ -57840,13 +58209,16 @@
         <v>-0.73818325200000001</v>
       </c>
       <c r="E164">
-        <v>-7.9568667470000003</v>
+        <v>-5.9381187339999997</v>
       </c>
       <c r="F164">
-        <v>-8.5821623480000007</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.217659727</v>
+      </c>
+      <c r="G164">
+        <v>-5.9562999230000004</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>107</v>
       </c>
@@ -57860,13 +58232,16 @@
         <v>-6.0659458700000002</v>
       </c>
       <c r="E165">
-        <v>-5.8849090679999998</v>
+        <v>-7.5903539330000003</v>
       </c>
       <c r="F165">
-        <v>-6.1127452829999998</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-8.1470876210000007</v>
+      </c>
+      <c r="G165">
+        <v>-9.5150841370000006</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>108</v>
       </c>
@@ -57880,13 +58255,16 @@
         <v>-5.726194703</v>
       </c>
       <c r="E166">
-        <v>-7.5720429180000002</v>
+        <v>-4.2183413490000001</v>
       </c>
       <c r="F166">
-        <v>-8.1310843130000006</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-4.6001465110000002</v>
+      </c>
+      <c r="G166">
+        <v>-6.126638421</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>109</v>
       </c>
@@ -57900,13 +58278,16 @@
         <v>-9.3325819699999997</v>
       </c>
       <c r="E167">
-        <v>-4.1822474300000003</v>
+        <v>-18.08533212</v>
       </c>
       <c r="F167">
-        <v>-4.5958275630000003</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-18.994653509999999</v>
+      </c>
+      <c r="G167">
+        <v>-14.165226690000001</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>110</v>
       </c>
@@ -57920,13 +58301,16 @@
         <v>-6.1142553069999996</v>
       </c>
       <c r="E168">
-        <v>-18.141427220000001</v>
+        <v>-4.4008804020000003</v>
       </c>
       <c r="F168">
-        <v>-19.00848585</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-5.0461569470000001</v>
+      </c>
+      <c r="G168">
+        <v>-5.3126856309999999</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>111</v>
       </c>
@@ -57940,13 +58324,16 @@
         <v>-13.45726973</v>
       </c>
       <c r="E169">
-        <v>-4.4363062109999998</v>
+        <v>-2.3224364799999999</v>
       </c>
       <c r="F169">
-        <v>-5.0845560450000002</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.9482535080000001</v>
+      </c>
+      <c r="G169">
+        <v>-3.4841809669999999</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>112</v>
       </c>
@@ -57960,13 +58347,16 @@
         <v>-5.1681343589999997</v>
       </c>
       <c r="E170">
-        <v>-2.3447881430000002</v>
+        <v>-12.22297286</v>
       </c>
       <c r="F170">
-        <v>-2.9162535030000001</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-11.889395970000001</v>
+      </c>
+      <c r="G170">
+        <v>-10.27097595</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>113</v>
       </c>
@@ -57980,13 +58370,16 @@
         <v>-3.3356343129999999</v>
       </c>
       <c r="E171">
-        <v>-6.1959574990000004</v>
+        <v>-5.8404387030000002</v>
       </c>
       <c r="F171">
-        <v>-6.3406916310000003</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.191859494</v>
+      </c>
+      <c r="G171">
+        <v>-5.196615006</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>114</v>
       </c>
@@ -58000,13 +58393,16 @@
         <v>-6.0004753849999997</v>
       </c>
       <c r="E172">
-        <v>-12.18460651</v>
+        <v>-0.105760435</v>
       </c>
       <c r="F172">
-        <v>-11.8906296</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-0.85170961199999995</v>
+      </c>
+      <c r="G172">
+        <v>-0.91064858900000001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>115</v>
       </c>
@@ -58020,13 +58416,16 @@
         <v>-10.14875754</v>
       </c>
       <c r="E173">
-        <v>-5.8242502649999999</v>
+        <v>-0.82930074200000004</v>
       </c>
       <c r="F173">
-        <v>-6.2341178370000003</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-1.7484895300000001</v>
+      </c>
+      <c r="G173">
+        <v>1.8625183249999999</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>116</v>
       </c>
@@ -58040,13 +58439,16 @@
         <v>-1.7969195529999999</v>
       </c>
       <c r="E174">
-        <v>-5.7432816999999997E-2</v>
+        <v>-7.5671431450000002</v>
       </c>
       <c r="F174">
-        <v>-0.84909501600000004</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.5321662720000004</v>
+      </c>
+      <c r="G174">
+        <v>-7.1500640119999996</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>117</v>
       </c>
@@ -58060,13 +58462,16 @@
         <v>-5.1787540740000004</v>
       </c>
       <c r="E175">
-        <v>-0.87745889499999996</v>
+        <v>-16.319625859999999</v>
       </c>
       <c r="F175">
-        <v>-1.6491723979999999</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-15.850551980000001</v>
+      </c>
+      <c r="G175">
+        <v>-17.538611400000001</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>118</v>
       </c>
@@ -58080,13 +58485,16 @@
         <v>-0.79803011199999996</v>
       </c>
       <c r="E176">
-        <v>-7.4970360859999996</v>
+        <v>-16.690050800000002</v>
       </c>
       <c r="F176">
-        <v>-6.4682074199999997</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-17.247816570000001</v>
+      </c>
+      <c r="G176">
+        <v>-13.72255125</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>119</v>
       </c>
@@ -58100,13 +58508,16 @@
         <v>1.7506116279999999</v>
       </c>
       <c r="E177">
-        <v>-16.32399655</v>
+        <v>-15.073896960000001</v>
       </c>
       <c r="F177">
-        <v>-15.834863090000001</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-15.404222559999999</v>
+      </c>
+      <c r="G177">
+        <v>-15.11742199</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>120</v>
       </c>
@@ -58120,13 +58531,16 @@
         <v>-7.0846340689999998</v>
       </c>
       <c r="E178">
-        <v>-16.661374089999999</v>
+        <v>-7.095139144</v>
       </c>
       <c r="F178">
-        <v>-17.222049890000001</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-7.7095811349999996</v>
+      </c>
+      <c r="G178">
+        <v>-4.1239047519999996</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>121</v>
       </c>
@@ -58140,13 +58554,16 @@
         <v>-17.426601519999998</v>
       </c>
       <c r="E179">
-        <v>-15.06397278</v>
+        <v>-5.4346685939999997</v>
       </c>
       <c r="F179">
-        <v>-15.46910031</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-5.7371203660000001</v>
+      </c>
+      <c r="G179">
+        <v>-2.605830772</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>122</v>
       </c>
@@ -58160,13 +58577,16 @@
         <v>-13.589441430000001</v>
       </c>
       <c r="E180">
-        <v>-7.0714329420000004</v>
+        <v>8.8555827909999998</v>
       </c>
       <c r="F180">
-        <v>-7.6104572490000004</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+        <v>8.0535980180000006</v>
+      </c>
+      <c r="G180">
+        <v>1.2595785559999999</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>123</v>
       </c>
@@ -58180,13 +58600,16 @@
         <v>-15.02977164</v>
       </c>
       <c r="E181">
-        <v>-5.4828486139999999</v>
+        <v>-2.1114853309999999</v>
       </c>
       <c r="F181">
-        <v>-5.6297092009999998</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.5680807630000002</v>
+      </c>
+      <c r="G181">
+        <v>-2.0944478470000001</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>124</v>
       </c>
@@ -58200,13 +58623,16 @@
         <v>-4.0748576129999998</v>
       </c>
       <c r="E182">
-        <v>8.8743059639999995</v>
+        <v>-4.957230246</v>
       </c>
       <c r="F182">
-        <v>8.0579280939999993</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-4.0369469420000001</v>
+      </c>
+      <c r="G182">
+        <v>-2.7723193450000001</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>125</v>
       </c>
@@ -58220,13 +58646,16 @@
         <v>-2.5804035000000001</v>
       </c>
       <c r="E183">
-        <v>-2.0460515149999998</v>
+        <v>-5.2860753760000003</v>
       </c>
       <c r="F183">
-        <v>-2.498519548</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-6.0655738870000002</v>
+      </c>
+      <c r="G183">
+        <v>-7.1225834199999998</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>126</v>
       </c>
@@ -58240,13 +58669,16 @@
         <v>1.2708237710000001</v>
       </c>
       <c r="E184">
-        <v>-4.9157239949999996</v>
+        <v>-3.6172372450000001</v>
       </c>
       <c r="F184">
-        <v>-4.0777562920000001</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-4.0540408230000002</v>
+      </c>
+      <c r="G184">
+        <v>-3.6804819489999998</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>127</v>
       </c>
@@ -58260,13 +58692,16 @@
         <v>-1.9570819399999999</v>
       </c>
       <c r="E185">
-        <v>-5.2747450059999998</v>
+        <v>-2.962682397</v>
       </c>
       <c r="F185">
-        <v>-5.9412941740000003</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-3.43618581</v>
+      </c>
+      <c r="G185">
+        <v>-3.852048006</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>128</v>
       </c>
@@ -58280,13 +58715,16 @@
         <v>-2.7629196789999999</v>
       </c>
       <c r="E186">
-        <v>-3.4604023850000001</v>
+        <v>-9.469511013</v>
       </c>
       <c r="F186">
-        <v>-4.049599111</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-8.6653146460000006</v>
+      </c>
+      <c r="G186">
+        <v>-7.7490571819999996</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>129</v>
       </c>
@@ -58300,13 +58738,16 @@
         <v>-6.9823272919999999</v>
       </c>
       <c r="E187">
-        <v>-2.907540129</v>
+        <v>-10.631306260000001</v>
       </c>
       <c r="F187">
-        <v>-3.3659699010000002</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-9.6703604680000002</v>
+      </c>
+      <c r="G187">
+        <v>-9.193843244</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>130</v>
       </c>
@@ -58319,14 +58760,8 @@
       <c r="D188">
         <v>-3.5833610519999999</v>
       </c>
-      <c r="E188">
-        <v>-9.4388054070000003</v>
-      </c>
-      <c r="F188">
-        <v>-8.5810792500000002</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>131</v>
       </c>
@@ -58339,14 +58774,8 @@
       <c r="D189">
         <v>-3.7050488580000001</v>
       </c>
-      <c r="E189">
-        <v>-10.63643628</v>
-      </c>
-      <c r="F189">
-        <v>-9.6701682170000005</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>132</v>
       </c>
@@ -58360,7 +58789,7 @@
         <v>-7.6691199210000001</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>772</v>
       </c>
@@ -58374,7 +58803,7 @@
         <v>-9.1324956739999994</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>773</v>
       </c>
@@ -58388,7 +58817,7 @@
         <v>-5.8447880449999996</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>774</v>
       </c>
@@ -58402,247 +58831,337 @@
         <v>-2.8066329759999999</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>243</v>
       </c>
       <c r="D207">
         <v>12.97241816</v>
       </c>
-    </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G207" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>244</v>
       </c>
       <c r="D208">
         <v>17.748413859999999</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G208" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>245</v>
       </c>
       <c r="D209">
         <v>-4.462540883</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G209" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>246</v>
       </c>
       <c r="D210">
         <v>0.35670532100000002</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G210" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>247</v>
       </c>
       <c r="D211">
         <v>7.8455568189999996</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G211" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>248</v>
       </c>
       <c r="D212">
         <v>-2.116066166</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G212" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>249</v>
       </c>
       <c r="D213">
         <v>5.7116827800000003</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G213" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>250</v>
       </c>
       <c r="D214">
         <v>12.74922449</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G214" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>251</v>
       </c>
       <c r="D215">
         <v>33.22703903</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G215" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>252</v>
       </c>
       <c r="D216">
         <v>63.90633021</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G216" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>253</v>
       </c>
       <c r="D217">
         <v>82.514940780000003</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G217" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>254</v>
       </c>
       <c r="D218">
         <v>39.553648199999998</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G218" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>255</v>
       </c>
       <c r="D219">
         <v>-0.33015101000000002</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G219" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>256</v>
       </c>
       <c r="D220">
         <v>-2.374881502</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G220" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>257</v>
       </c>
       <c r="D221">
         <v>0.35025503200000002</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G221" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>258</v>
       </c>
       <c r="D222">
         <v>18.367232130000001</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G222" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>259</v>
       </c>
       <c r="D223">
         <v>9.5921649589999998</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G223" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>260</v>
       </c>
       <c r="D224">
         <v>16.042256550000001</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G224" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>261</v>
       </c>
       <c r="D225">
         <v>16.881996180000002</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G225" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>262</v>
       </c>
       <c r="D226">
         <v>27.355248830000001</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G226" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>263</v>
       </c>
       <c r="D227">
         <v>9.0922228960000009</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G227" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>264</v>
       </c>
       <c r="D228">
         <v>-9.9991328040000003</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G228" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>265</v>
       </c>
       <c r="D229">
         <v>11.51212806</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G229" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>266</v>
       </c>
       <c r="D230">
         <v>30.45542846</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G230" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>267</v>
       </c>
       <c r="D231">
         <v>-6.7317602230000002</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G231" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>268</v>
       </c>
       <c r="D232">
         <v>25.1415869</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G232" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>269</v>
       </c>
       <c r="D233">
         <v>27.155081450000001</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G233" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>270</v>
       </c>
       <c r="D234">
         <v>24.998354729999999</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G234" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>271</v>
       </c>
       <c r="D235">
         <v>60.888056560000003</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G235" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>272</v>
       </c>
       <c r="D236">
         <v>-2.1394526709999999</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G236" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>273</v>
       </c>
@@ -58650,7 +59169,7 @@
         <v>-1.562072312</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>274</v>
       </c>
@@ -58658,7 +59177,7 @@
         <v>2.59599767</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>275</v>
       </c>
@@ -58666,7 +59185,7 @@
         <v>28.267741740000002</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>276</v>
       </c>

</xml_diff>

<commit_message>
Work on weinberger mainly
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4580" yWindow="1580" windowWidth="25160" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="920" yWindow="2360" windowWidth="14780" windowHeight="16020" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
-    <sheet name="OSPREE_7Dec2018" sheetId="6" r:id="rId2"/>
-    <sheet name="OSPREE_compare_ALL (4 Dec 2018)" sheetId="12" r:id="rId3"/>
-    <sheet name="OSPREE_compare" sheetId="4" r:id="rId4"/>
-    <sheet name="Flynn_exp" sheetId="2" r:id="rId5"/>
-    <sheet name="2018NovEarly_Lizzie" sheetId="5" r:id="rId6"/>
-    <sheet name="2018Jun-Aug_LizzieAilene" sheetId="1" r:id="rId7"/>
+    <sheet name="weinberger" sheetId="13" r:id="rId2"/>
+    <sheet name="OSPREE_7Dec2018" sheetId="6" r:id="rId3"/>
+    <sheet name="OSPREE_compare_ALL (4 Dec 2018)" sheetId="12" r:id="rId4"/>
+    <sheet name="OSPREE_compare" sheetId="4" r:id="rId5"/>
+    <sheet name="Flynn_exp" sheetId="2" r:id="rId6"/>
+    <sheet name="2018NovEarly_Lizzie" sheetId="5" r:id="rId7"/>
+    <sheet name="2018Jun-Aug_LizzieAilene" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3941" uniqueCount="1046">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3973" uniqueCount="1057">
   <si>
     <t>param</t>
   </si>
@@ -3239,6 +3240,39 @@
   </si>
   <si>
     <t>After all this we decided a few things (see comparing models on OSPREE wiki) and moved on with just the model with no interactions and no study, see OSPREE_7Dec2018 tab for that.</t>
+  </si>
+  <si>
+    <t>weinberger_fewint</t>
+  </si>
+  <si>
+    <t>b_weinberger</t>
+  </si>
+  <si>
+    <t>b_cw</t>
+  </si>
+  <si>
+    <t>b_pw</t>
+  </si>
+  <si>
+    <t>b_fw</t>
+  </si>
+  <si>
+    <t>incl fldest; matching spp</t>
+  </si>
+  <si>
+    <t>wein_intpoolonly</t>
+  </si>
+  <si>
+    <t>no fldest; matching spp</t>
+  </si>
+  <si>
+    <t>incl fldest (all spp)</t>
+  </si>
+  <si>
+    <t>no fldest from nonwein (all spp)</t>
+  </si>
+  <si>
+    <t>I also added the weinberger tab today, see weinberger.R for the model code.</t>
   </si>
 </sst>
 </file>
@@ -3411,8 +3445,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="277">
+  <cellStyleXfs count="313">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3754,7 +3824,7 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="277">
+  <cellStyles count="313">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3893,6 +3963,24 @@
     <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4031,6 +4119,24 @@
     <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4368,10 +4474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="H54" sqref="H54"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4689,6 +4795,11 @@
     <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>1045</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>1056</v>
       </c>
     </row>
   </sheetData>
@@ -4704,10 +4815,394 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1052</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="G3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1053</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8">
+        <v>1556</v>
+      </c>
+      <c r="C8">
+        <v>1356</v>
+      </c>
+      <c r="D8">
+        <v>1230</v>
+      </c>
+      <c r="E8">
+        <v>1034</v>
+      </c>
+      <c r="F8">
+        <v>1556</v>
+      </c>
+      <c r="G8">
+        <v>1356</v>
+      </c>
+      <c r="H8">
+        <v>1230</v>
+      </c>
+      <c r="I8">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>37</v>
+      </c>
+      <c r="D9">
+        <v>28</v>
+      </c>
+      <c r="E9">
+        <v>28</v>
+      </c>
+      <c r="F9">
+        <v>37</v>
+      </c>
+      <c r="G9">
+        <v>37</v>
+      </c>
+      <c r="H9">
+        <v>28</v>
+      </c>
+      <c r="I9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>29</v>
+      </c>
+      <c r="C13">
+        <v>27</v>
+      </c>
+      <c r="D13">
+        <v>29.6</v>
+      </c>
+      <c r="E13">
+        <v>27.9</v>
+      </c>
+      <c r="F13">
+        <v>31.2</v>
+      </c>
+      <c r="G13">
+        <v>30.5</v>
+      </c>
+      <c r="H13">
+        <v>32</v>
+      </c>
+      <c r="I13">
+        <v>31.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>-3.6</v>
+      </c>
+      <c r="C14">
+        <v>-0.9</v>
+      </c>
+      <c r="D14">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="E14">
+        <v>0.7</v>
+      </c>
+      <c r="F14">
+        <v>-4.3</v>
+      </c>
+      <c r="G14">
+        <v>-1.9</v>
+      </c>
+      <c r="H14">
+        <v>-3.7</v>
+      </c>
+      <c r="I14">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>-3.1</v>
+      </c>
+      <c r="C15">
+        <v>-3.4</v>
+      </c>
+      <c r="D15">
+        <v>-3.2</v>
+      </c>
+      <c r="E15">
+        <v>-3.9</v>
+      </c>
+      <c r="F15">
+        <v>-2.1</v>
+      </c>
+      <c r="G15">
+        <v>-1.5</v>
+      </c>
+      <c r="H15">
+        <v>-2.1</v>
+      </c>
+      <c r="I15">
+        <v>-1.4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>-13</v>
+      </c>
+      <c r="C16">
+        <v>-13.4</v>
+      </c>
+      <c r="D16">
+        <v>-13.5</v>
+      </c>
+      <c r="E16">
+        <v>-13.9</v>
+      </c>
+      <c r="F16">
+        <v>-8.1</v>
+      </c>
+      <c r="G16">
+        <v>-7.2</v>
+      </c>
+      <c r="H16">
+        <v>-8.1999999999999993</v>
+      </c>
+      <c r="I16">
+        <v>-7.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="21" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B17">
+        <v>2.4</v>
+      </c>
+      <c r="C17">
+        <v>4.5</v>
+      </c>
+      <c r="D17">
+        <v>2.5</v>
+      </c>
+      <c r="E17">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F17">
+        <v>-0.7</v>
+      </c>
+      <c r="G17">
+        <v>-1.3</v>
+      </c>
+      <c r="H17">
+        <v>-0.2</v>
+      </c>
+      <c r="I17">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B18">
+        <v>4.8</v>
+      </c>
+      <c r="C18">
+        <v>5.3</v>
+      </c>
+      <c r="D18">
+        <v>5.2</v>
+      </c>
+      <c r="E18">
+        <v>5.6</v>
+      </c>
+      <c r="F18">
+        <v>-1.8</v>
+      </c>
+      <c r="G18">
+        <v>-3.1</v>
+      </c>
+      <c r="H18">
+        <v>-0.6</v>
+      </c>
+      <c r="I18">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B19">
+        <v>-0.05</v>
+      </c>
+      <c r="C19">
+        <v>0.7</v>
+      </c>
+      <c r="D19">
+        <v>-0.6</v>
+      </c>
+      <c r="E19">
+        <v>0.6</v>
+      </c>
+      <c r="F19">
+        <v>-0.4</v>
+      </c>
+      <c r="G19">
+        <v>-0.9</v>
+      </c>
+      <c r="H19">
+        <v>-1.4</v>
+      </c>
+      <c r="I19">
+        <v>-1.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B20">
+        <v>0.08</v>
+      </c>
+      <c r="C20">
+        <v>-2.2999999999999998</v>
+      </c>
+      <c r="D20">
+        <v>0.7</v>
+      </c>
+      <c r="E20">
+        <v>-1.9</v>
+      </c>
+      <c r="F20">
+        <v>-1</v>
+      </c>
+      <c r="G20">
+        <v>-4</v>
+      </c>
+      <c r="H20">
+        <v>1.2</v>
+      </c>
+      <c r="I20">
+        <v>-1.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P1161"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A27" sqref="A1:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11037,7 +11532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA1207"/>
   <sheetViews>
@@ -62372,7 +62867,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1187"/>
   <sheetViews>
@@ -77329,7 +77824,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -77521,7 +78016,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N39"/>
   <sheetViews>
@@ -78435,7 +78930,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R177"/>
   <sheetViews>

</xml_diff>

<commit_message>
a little more model work
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11540" yWindow="180" windowWidth="18640" windowHeight="15420" tabRatio="500"/>
+    <workbookView xWindow="2640" yWindow="860" windowWidth="18640" windowHeight="15420" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3977" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3981" uniqueCount="1058">
   <si>
     <t>param</t>
   </si>
@@ -3448,8 +3448,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="317">
+  <cellStyleXfs count="325">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3831,7 +3839,7 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="317">
+  <cellStyles count="325">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3990,6 +3998,10 @@
     <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4148,6 +4160,10 @@
     <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4487,7 +4503,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
@@ -5210,29 +5226,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1161"/>
+  <dimension ref="A1:R1161"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="6" width="18.5" style="21" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="13.5" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.1640625" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" customWidth="1"/>
-    <col min="13" max="13" width="15.5" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
-    <col min="15" max="15" width="14.33203125" customWidth="1"/>
-    <col min="16" max="17" width="10.83203125" style="19"/>
+    <col min="2" max="7" width="18.5" style="21" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" customWidth="1"/>
+    <col min="14" max="14" width="15.5" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" customWidth="1"/>
+    <col min="17" max="18" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="18" customFormat="1">
+    <row r="1" spans="1:11" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
         <v>212</v>
       </c>
@@ -5242,10 +5258,10 @@
       <c r="C1" t="s">
         <v>1057</v>
       </c>
-      <c r="D1" s="17" t="s">
-        <v>992</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="D1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="17" t="s">
         <v>992</v>
       </c>
       <c r="F1" t="s">
@@ -5254,18 +5270,21 @@
       <c r="G1" t="s">
         <v>992</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" t="s">
+        <v>992</v>
+      </c>
+      <c r="I1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="D2" s="22"/>
-      <c r="G2" s="21"/>
-    </row>
-    <row r="3" spans="1:10">
+    <row r="2" spans="1:11">
+      <c r="E2" s="22"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>217</v>
       </c>
@@ -5275,17 +5294,17 @@
       <c r="C3" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>1034</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="F3" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="G3" s="22" t="s">
         <v>1034</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>1032</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>1032</v>
@@ -5293,9 +5312,12 @@
       <c r="I3" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="J3" s="21"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="J3" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="K3" s="21"/>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>221</v>
       </c>
@@ -5305,27 +5327,30 @@
       <c r="C4" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="E4" s="21" t="s">
-        <v>1035</v>
+      <c r="E4" s="22" t="s">
+        <v>1031</v>
       </c>
       <c r="F4" s="21" t="s">
         <v>1035</v>
       </c>
       <c r="G4" s="21" t="s">
+        <v>1035</v>
+      </c>
+      <c r="H4" s="21" t="s">
         <v>1033</v>
-      </c>
-      <c r="H4" s="22" t="s">
-        <v>1037</v>
       </c>
       <c r="I4" s="22" t="s">
         <v>1037</v>
       </c>
-      <c r="J4" s="21"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="J4" s="22" t="s">
+        <v>1037</v>
+      </c>
+      <c r="K4" s="21"/>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>280</v>
       </c>
@@ -5353,16 +5378,19 @@
       <c r="I5" s="21" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="J5" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>224</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>1038</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>214</v>
       </c>
@@ -5373,25 +5401,28 @@
         <v>1556</v>
       </c>
       <c r="D8" s="23">
+        <v>1556</v>
+      </c>
+      <c r="E8" s="23">
         <v>1097</v>
       </c>
-      <c r="E8" s="23">
+      <c r="F8" s="23">
         <v>2651</v>
       </c>
-      <c r="F8" s="23">
+      <c r="G8" s="23">
         <v>2112</v>
       </c>
-      <c r="G8" s="23">
+      <c r="H8" s="23">
         <v>1953</v>
-      </c>
-      <c r="H8">
-        <v>1556</v>
       </c>
       <c r="I8">
         <v>1556</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="J8">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>211</v>
       </c>
@@ -5402,40 +5433,43 @@
         <v>37</v>
       </c>
       <c r="D9" s="23">
+        <v>37</v>
+      </c>
+      <c r="E9" s="23">
         <v>25</v>
       </c>
-      <c r="E9" s="23">
+      <c r="F9" s="23">
         <v>200</v>
       </c>
-      <c r="F9" s="23">
+      <c r="G9" s="23">
         <v>179</v>
       </c>
-      <c r="G9" s="23">
+      <c r="H9" s="23">
         <v>41</v>
-      </c>
-      <c r="H9">
-        <v>37</v>
       </c>
       <c r="I9">
         <v>37</v>
       </c>
-      <c r="J9" s="23"/>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="J9">
+        <v>37</v>
+      </c>
+      <c r="K9" s="23"/>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>213</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
-      <c r="I10">
+      <c r="G10" s="23"/>
+      <c r="J10">
         <v>30</v>
       </c>
-      <c r="J10" s="23"/>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="K10" s="23"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>215</v>
       </c>
@@ -5443,11 +5477,11 @@
         <v>1036</v>
       </c>
       <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
-    </row>
-    <row r="13" spans="1:10" s="21" customFormat="1">
+      <c r="G11" s="23"/>
+    </row>
+    <row r="13" spans="1:11" s="21" customFormat="1">
       <c r="A13" s="21" t="s">
         <v>5</v>
       </c>
@@ -5458,33 +5492,36 @@
         <v>30.66</v>
       </c>
       <c r="D13" s="21">
+        <v>31.211466999999999</v>
+      </c>
+      <c r="E13" s="21">
         <v>31.880268000000001</v>
       </c>
-      <c r="E13" s="21">
+      <c r="F13" s="21">
         <v>30.716964999999998</v>
       </c>
-      <c r="F13" s="21">
+      <c r="G13" s="21">
         <v>29.746556000000002</v>
       </c>
-      <c r="G13" s="21">
+      <c r="H13" s="21">
         <v>29.076453999999998</v>
       </c>
-      <c r="H13" s="21">
+      <c r="I13" s="21">
         <v>29.443950000000001</v>
       </c>
-      <c r="I13" s="21">
+      <c r="J13" s="21">
         <v>11.154477999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="21" customFormat="1">
+    <row r="14" spans="1:11" s="21" customFormat="1">
       <c r="A14" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I14" s="21">
+      <c r="J14" s="21">
         <v>17.8</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="21" customFormat="1" ht="14" customHeight="1">
+    <row r="15" spans="1:11" s="21" customFormat="1" ht="14" customHeight="1">
       <c r="A15" s="21" t="s">
         <v>7</v>
       </c>
@@ -5495,25 +5532,28 @@
         <v>-4.7</v>
       </c>
       <c r="D15" s="21">
+        <v>-3.9753639999999999</v>
+      </c>
+      <c r="E15" s="21">
         <v>-6.589467</v>
       </c>
-      <c r="E15" s="21">
+      <c r="F15" s="21">
         <v>-4.670153</v>
       </c>
-      <c r="F15" s="21">
+      <c r="G15" s="21">
         <v>-6.3059329999999996</v>
       </c>
-      <c r="G15" s="21">
+      <c r="H15" s="21">
         <v>-4.2054489999999998</v>
       </c>
-      <c r="H15" s="21">
+      <c r="I15" s="21">
         <v>-4.4239769999999998</v>
       </c>
-      <c r="I15" s="21">
+      <c r="J15" s="21">
         <v>-11.179836</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="21" customFormat="1">
+    <row r="16" spans="1:11" s="21" customFormat="1">
       <c r="A16" s="21" t="s">
         <v>8</v>
       </c>
@@ -5524,25 +5564,28 @@
         <v>-2.2999999999999998</v>
       </c>
       <c r="D16" s="21">
+        <v>-3.5504150000000001</v>
+      </c>
+      <c r="E16" s="21">
         <v>-2.3749199999999999</v>
       </c>
-      <c r="E16" s="21">
+      <c r="F16" s="21">
         <v>-1.740626</v>
       </c>
-      <c r="F16" s="21">
+      <c r="G16" s="21">
         <v>-1.149972</v>
       </c>
-      <c r="G16" s="21">
+      <c r="H16" s="21">
         <v>-3.8012999999999999</v>
       </c>
-      <c r="H16" s="21">
+      <c r="I16" s="21">
         <v>-4.6329729999999998</v>
       </c>
-      <c r="I16" s="21">
+      <c r="J16" s="21">
         <v>-1.4</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="21" customFormat="1">
+    <row r="17" spans="1:10" s="21" customFormat="1">
       <c r="A17" s="21" t="s">
         <v>9</v>
       </c>
@@ -5553,951 +5596,964 @@
         <v>-8.5</v>
       </c>
       <c r="D17" s="21">
+        <v>-10.401221</v>
+      </c>
+      <c r="E17" s="21">
         <v>-9.9066620000000007</v>
       </c>
-      <c r="E17" s="21">
+      <c r="F17" s="21">
         <v>-8.6652190000000004</v>
       </c>
-      <c r="F17" s="21">
+      <c r="G17" s="21">
         <v>-9.8209820000000008</v>
       </c>
-      <c r="G17" s="21">
+      <c r="H17" s="21">
         <v>-10.442672999999999</v>
       </c>
-      <c r="H17" s="21">
+      <c r="I17" s="21">
         <v>-10.520892</v>
       </c>
-      <c r="I17" s="21">
+      <c r="J17" s="21">
         <v>-9.7576470000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="D25" s="21">
+        <v>1.47323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:9">
+      <c r="D26" s="21">
+        <v>1.0277529999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:9">
+      <c r="D27" s="21">
+        <v>-1.052503</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29" s="15" t="s">
         <v>972</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>57</v>
       </c>
-      <c r="G30" s="17"/>
-    </row>
-    <row r="31" spans="1:9">
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31" t="s">
         <v>58</v>
       </c>
-      <c r="G31" s="17"/>
-    </row>
-    <row r="32" spans="1:9">
+      <c r="H31" s="17"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>59</v>
       </c>
-      <c r="G32" s="17"/>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="17"/>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>60</v>
       </c>
-      <c r="G33" s="17"/>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>61</v>
       </c>
-      <c r="G34" s="17"/>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="17"/>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>62</v>
       </c>
-      <c r="G35" s="17"/>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="17"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>63</v>
       </c>
-      <c r="G36" s="17"/>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="17"/>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>64</v>
       </c>
-      <c r="G37" s="17"/>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="17"/>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>65</v>
       </c>
-      <c r="G38" s="17"/>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="17"/>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>66</v>
       </c>
-      <c r="G39" s="17"/>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="H39" s="17"/>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="17"/>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="H40" s="17"/>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>68</v>
       </c>
-      <c r="G41" s="17"/>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="H41" s="17"/>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>69</v>
       </c>
-      <c r="G42" s="17"/>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="H42" s="17"/>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>70</v>
       </c>
-      <c r="G43" s="17"/>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="H43" s="17"/>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>71</v>
       </c>
-      <c r="G44" s="17"/>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="H44" s="17"/>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>72</v>
       </c>
-      <c r="G45" s="17"/>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="H45" s="17"/>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>73</v>
       </c>
-      <c r="G46" s="17"/>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="H46" s="17"/>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>74</v>
       </c>
-      <c r="G47" s="17"/>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="H47" s="17"/>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>75</v>
       </c>
-      <c r="G48" s="17"/>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="H48" s="17"/>
+    </row>
+    <row r="49" spans="1:8">
       <c r="A49" t="s">
         <v>76</v>
       </c>
-      <c r="G49" s="17"/>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="H49" s="17"/>
+    </row>
+    <row r="50" spans="1:8">
       <c r="A50" t="s">
         <v>77</v>
       </c>
-      <c r="G50" s="17"/>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="1:8">
       <c r="A51" t="s">
         <v>78</v>
       </c>
-      <c r="G51" s="17"/>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="H51" s="17"/>
+    </row>
+    <row r="52" spans="1:8">
       <c r="A52" t="s">
         <v>79</v>
       </c>
-      <c r="G52" s="17"/>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="H52" s="17"/>
+    </row>
+    <row r="53" spans="1:8">
       <c r="A53" t="s">
         <v>80</v>
       </c>
-      <c r="G53" s="17"/>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="H53" s="17"/>
+    </row>
+    <row r="54" spans="1:8">
       <c r="A54" t="s">
         <v>81</v>
       </c>
-      <c r="G54" s="17"/>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="H54" s="17"/>
+    </row>
+    <row r="55" spans="1:8">
       <c r="A55" t="s">
         <v>82</v>
       </c>
-      <c r="G55" s="17"/>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="H55" s="17"/>
+    </row>
+    <row r="56" spans="1:8">
       <c r="A56" t="s">
         <v>83</v>
       </c>
-      <c r="G56" s="17"/>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="H56" s="17"/>
+    </row>
+    <row r="57" spans="1:8">
       <c r="A57" t="s">
         <v>84</v>
       </c>
-      <c r="G57" s="17"/>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="H57" s="17"/>
+    </row>
+    <row r="58" spans="1:8">
       <c r="A58" t="s">
         <v>85</v>
       </c>
-      <c r="G58" s="17"/>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="H58" s="17"/>
+    </row>
+    <row r="59" spans="1:8">
       <c r="A59" t="s">
         <v>86</v>
       </c>
-      <c r="G59" s="17"/>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="H59" s="17"/>
+    </row>
+    <row r="60" spans="1:8">
       <c r="A60" t="s">
         <v>87</v>
       </c>
-      <c r="G60" s="17"/>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="H60" s="17"/>
+    </row>
+    <row r="61" spans="1:8">
       <c r="A61" t="s">
         <v>88</v>
       </c>
-      <c r="G61" s="17"/>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="H61" s="17"/>
+    </row>
+    <row r="62" spans="1:8">
       <c r="A62" t="s">
         <v>89</v>
       </c>
-      <c r="G62" s="17"/>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="H62" s="17"/>
+    </row>
+    <row r="63" spans="1:8">
       <c r="A63" t="s">
         <v>90</v>
       </c>
-      <c r="G63" s="17"/>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="H63" s="17"/>
+    </row>
+    <row r="64" spans="1:8">
       <c r="A64" t="s">
         <v>91</v>
       </c>
-      <c r="G64" s="17"/>
-    </row>
-    <row r="65" spans="1:8">
+      <c r="H64" s="17"/>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65" t="s">
         <v>92</v>
       </c>
-      <c r="G65" s="17"/>
-    </row>
-    <row r="66" spans="1:8">
+      <c r="H65" s="17"/>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66" t="s">
         <v>93</v>
       </c>
-      <c r="G66" s="17"/>
-    </row>
-    <row r="67" spans="1:8">
+      <c r="H66" s="17"/>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67" t="s">
         <v>94</v>
       </c>
-      <c r="G67" s="17"/>
-    </row>
-    <row r="68" spans="1:8">
+      <c r="H67" s="17"/>
+    </row>
+    <row r="68" spans="1:9">
       <c r="B68" s="22"/>
       <c r="C68" s="22"/>
       <c r="D68" s="22"/>
       <c r="E68" s="22"/>
       <c r="F68" s="22"/>
-      <c r="G68" s="17"/>
+      <c r="G68" s="22"/>
       <c r="H68" s="17"/>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="G69" s="17"/>
-    </row>
-    <row r="70" spans="1:8">
-      <c r="G70" s="17"/>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="G71" s="17"/>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="G72" s="17"/>
-    </row>
-    <row r="73" spans="1:8">
+      <c r="I68" s="17"/>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="H69" s="17"/>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="H70" s="17"/>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="H71" s="17"/>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="H72" s="17"/>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73" s="17"/>
-      <c r="G73" s="17"/>
-    </row>
-    <row r="74" spans="1:8">
+      <c r="H73" s="17"/>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74" t="s">
         <v>171</v>
       </c>
-      <c r="G74" s="17"/>
-    </row>
-    <row r="75" spans="1:8">
+      <c r="H74" s="17"/>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75" t="s">
         <v>172</v>
       </c>
-      <c r="G75" s="17"/>
-    </row>
-    <row r="76" spans="1:8">
+      <c r="H75" s="17"/>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76" t="s">
         <v>173</v>
       </c>
-      <c r="G76" s="17"/>
-    </row>
-    <row r="77" spans="1:8">
+      <c r="H76" s="17"/>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77" t="s">
         <v>174</v>
       </c>
-      <c r="G77" s="17"/>
-    </row>
-    <row r="78" spans="1:8">
+      <c r="H77" s="17"/>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78" t="s">
         <v>175</v>
       </c>
-      <c r="G78" s="17"/>
-    </row>
-    <row r="79" spans="1:8">
+      <c r="H78" s="17"/>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79" t="s">
         <v>176</v>
       </c>
-      <c r="G79" s="17"/>
-    </row>
-    <row r="80" spans="1:8">
+      <c r="H79" s="17"/>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80" t="s">
         <v>177</v>
       </c>
-      <c r="G80" s="17"/>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="H80" s="17"/>
+    </row>
+    <row r="81" spans="1:8">
       <c r="A81" t="s">
         <v>178</v>
       </c>
-      <c r="G81" s="17"/>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="H81" s="17"/>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" t="s">
         <v>179</v>
       </c>
-      <c r="G82" s="17"/>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="H82" s="17"/>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" t="s">
         <v>180</v>
       </c>
-      <c r="G83" s="17"/>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="H83" s="17"/>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" t="s">
         <v>181</v>
       </c>
-      <c r="G84" s="17"/>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="H84" s="17"/>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" t="s">
         <v>182</v>
       </c>
-      <c r="G85" s="17"/>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="H85" s="17"/>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" t="s">
         <v>183</v>
       </c>
-      <c r="G86" s="17"/>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="H86" s="17"/>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" t="s">
         <v>184</v>
       </c>
-      <c r="G87" s="17"/>
-    </row>
-    <row r="88" spans="1:7">
+      <c r="H87" s="17"/>
+    </row>
+    <row r="88" spans="1:8">
       <c r="A88" t="s">
         <v>185</v>
       </c>
-      <c r="G88" s="17"/>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="H88" s="17"/>
+    </row>
+    <row r="89" spans="1:8">
       <c r="A89" t="s">
         <v>186</v>
       </c>
-      <c r="G89" s="17"/>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="H89" s="17"/>
+    </row>
+    <row r="90" spans="1:8">
       <c r="A90" t="s">
         <v>187</v>
       </c>
-      <c r="G90" s="17"/>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="H90" s="17"/>
+    </row>
+    <row r="91" spans="1:8">
       <c r="A91" t="s">
         <v>188</v>
       </c>
-      <c r="G91" s="17"/>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="H91" s="17"/>
+    </row>
+    <row r="92" spans="1:8">
       <c r="A92" t="s">
         <v>189</v>
       </c>
-      <c r="G92" s="17"/>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="H92" s="17"/>
+    </row>
+    <row r="93" spans="1:8">
       <c r="A93" t="s">
         <v>190</v>
       </c>
-      <c r="G93" s="17"/>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="H93" s="17"/>
+    </row>
+    <row r="94" spans="1:8">
       <c r="A94" t="s">
         <v>191</v>
       </c>
-      <c r="G94" s="17"/>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="H94" s="17"/>
+    </row>
+    <row r="95" spans="1:8">
       <c r="A95" t="s">
         <v>192</v>
       </c>
-      <c r="G95" s="17"/>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="H95" s="17"/>
+    </row>
+    <row r="96" spans="1:8">
       <c r="A96" t="s">
         <v>193</v>
       </c>
-      <c r="G96" s="17"/>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="H96" s="17"/>
+    </row>
+    <row r="97" spans="1:8">
       <c r="A97" t="s">
         <v>194</v>
       </c>
-      <c r="G97" s="17"/>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="H97" s="17"/>
+    </row>
+    <row r="98" spans="1:8">
       <c r="A98" t="s">
         <v>195</v>
       </c>
-      <c r="G98" s="17"/>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="H98" s="17"/>
+    </row>
+    <row r="99" spans="1:8">
       <c r="A99" t="s">
         <v>196</v>
       </c>
-      <c r="G99" s="17"/>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="H99" s="17"/>
+    </row>
+    <row r="100" spans="1:8">
       <c r="A100" t="s">
         <v>197</v>
       </c>
-      <c r="G100" s="17"/>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="H100" s="17"/>
+    </row>
+    <row r="101" spans="1:8">
       <c r="A101" t="s">
         <v>198</v>
       </c>
-      <c r="G101" s="17"/>
-    </row>
-    <row r="102" spans="1:7">
+      <c r="H101" s="17"/>
+    </row>
+    <row r="102" spans="1:8">
       <c r="A102" t="s">
         <v>199</v>
       </c>
-      <c r="G102" s="17"/>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="H102" s="17"/>
+    </row>
+    <row r="103" spans="1:8">
       <c r="A103" t="s">
         <v>200</v>
       </c>
-      <c r="G103" s="17"/>
-    </row>
-    <row r="104" spans="1:7">
+      <c r="H103" s="17"/>
+    </row>
+    <row r="104" spans="1:8">
       <c r="A104" t="s">
         <v>201</v>
       </c>
-      <c r="G104" s="17"/>
-    </row>
-    <row r="105" spans="1:7">
+      <c r="H104" s="17"/>
+    </row>
+    <row r="105" spans="1:8">
       <c r="A105" t="s">
         <v>202</v>
       </c>
-      <c r="G105" s="17"/>
-    </row>
-    <row r="106" spans="1:7">
+      <c r="H105" s="17"/>
+    </row>
+    <row r="106" spans="1:8">
       <c r="A106" t="s">
         <v>203</v>
       </c>
-      <c r="G106" s="17"/>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="H106" s="17"/>
+    </row>
+    <row r="107" spans="1:8">
       <c r="A107" t="s">
         <v>204</v>
       </c>
-      <c r="G107" s="17"/>
-    </row>
-    <row r="108" spans="1:7">
+      <c r="H107" s="17"/>
+    </row>
+    <row r="108" spans="1:8">
       <c r="A108" t="s">
         <v>205</v>
       </c>
-      <c r="G108" s="17"/>
-    </row>
-    <row r="109" spans="1:7">
+      <c r="H108" s="17"/>
+    </row>
+    <row r="109" spans="1:8">
       <c r="A109" t="s">
         <v>206</v>
       </c>
-      <c r="G109" s="17"/>
-    </row>
-    <row r="110" spans="1:7">
+      <c r="H109" s="17"/>
+    </row>
+    <row r="110" spans="1:8">
       <c r="A110" t="s">
         <v>207</v>
       </c>
-      <c r="G110" s="17"/>
-    </row>
-    <row r="111" spans="1:7">
+      <c r="H110" s="17"/>
+    </row>
+    <row r="111" spans="1:8">
       <c r="A111" t="s">
         <v>208</v>
       </c>
-      <c r="G111" s="17"/>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="G112" s="17"/>
-    </row>
-    <row r="113" spans="1:7">
-      <c r="G113" s="17"/>
-    </row>
-    <row r="114" spans="1:7">
-      <c r="G114" s="17"/>
-    </row>
-    <row r="115" spans="1:7">
-      <c r="G115" s="17"/>
-    </row>
-    <row r="116" spans="1:7">
-      <c r="G116" s="17"/>
-    </row>
-    <row r="117" spans="1:7">
-      <c r="G117" s="17"/>
-    </row>
-    <row r="118" spans="1:7">
+      <c r="H111" s="17"/>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="H112" s="17"/>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="H113" s="17"/>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="H114" s="17"/>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="H115" s="17"/>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="H116" s="17"/>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="H117" s="17"/>
+    </row>
+    <row r="118" spans="1:8">
       <c r="A118" t="s">
         <v>133</v>
       </c>
-      <c r="G118" s="17"/>
-    </row>
-    <row r="119" spans="1:7">
+      <c r="H118" s="17"/>
+    </row>
+    <row r="119" spans="1:8">
       <c r="A119" t="s">
         <v>134</v>
       </c>
-      <c r="G119" s="17"/>
-    </row>
-    <row r="120" spans="1:7">
+      <c r="H119" s="17"/>
+    </row>
+    <row r="120" spans="1:8">
       <c r="A120" t="s">
         <v>135</v>
       </c>
-      <c r="G120" s="17"/>
-    </row>
-    <row r="121" spans="1:7">
+      <c r="H120" s="17"/>
+    </row>
+    <row r="121" spans="1:8">
       <c r="A121" t="s">
         <v>136</v>
       </c>
-      <c r="G121" s="17"/>
-    </row>
-    <row r="122" spans="1:7">
+      <c r="H121" s="17"/>
+    </row>
+    <row r="122" spans="1:8">
       <c r="A122" t="s">
         <v>137</v>
       </c>
-      <c r="G122" s="17"/>
-    </row>
-    <row r="123" spans="1:7">
+      <c r="H122" s="17"/>
+    </row>
+    <row r="123" spans="1:8">
       <c r="A123" t="s">
         <v>138</v>
       </c>
-      <c r="G123" s="17"/>
-    </row>
-    <row r="124" spans="1:7">
+      <c r="H123" s="17"/>
+    </row>
+    <row r="124" spans="1:8">
       <c r="A124" t="s">
         <v>139</v>
       </c>
-      <c r="G124" s="17"/>
-    </row>
-    <row r="125" spans="1:7">
+      <c r="H124" s="17"/>
+    </row>
+    <row r="125" spans="1:8">
       <c r="A125" t="s">
         <v>140</v>
       </c>
-      <c r="G125" s="17"/>
-    </row>
-    <row r="126" spans="1:7">
+      <c r="H125" s="17"/>
+    </row>
+    <row r="126" spans="1:8">
       <c r="A126" t="s">
         <v>141</v>
       </c>
-      <c r="G126" s="17"/>
-    </row>
-    <row r="127" spans="1:7">
+      <c r="H126" s="17"/>
+    </row>
+    <row r="127" spans="1:8">
       <c r="A127" t="s">
         <v>142</v>
       </c>
-      <c r="G127" s="17"/>
-    </row>
-    <row r="128" spans="1:7">
+      <c r="H127" s="17"/>
+    </row>
+    <row r="128" spans="1:8">
       <c r="A128" t="s">
         <v>143</v>
       </c>
-      <c r="G128" s="17"/>
-    </row>
-    <row r="129" spans="1:7">
+      <c r="H128" s="17"/>
+    </row>
+    <row r="129" spans="1:8">
       <c r="A129" t="s">
         <v>144</v>
       </c>
-      <c r="G129" s="17"/>
-    </row>
-    <row r="130" spans="1:7">
+      <c r="H129" s="17"/>
+    </row>
+    <row r="130" spans="1:8">
       <c r="A130" t="s">
         <v>145</v>
       </c>
-      <c r="G130" s="17"/>
-    </row>
-    <row r="131" spans="1:7">
+      <c r="H130" s="17"/>
+    </row>
+    <row r="131" spans="1:8">
       <c r="A131" t="s">
         <v>146</v>
       </c>
-      <c r="G131" s="17"/>
-    </row>
-    <row r="132" spans="1:7">
+      <c r="H131" s="17"/>
+    </row>
+    <row r="132" spans="1:8">
       <c r="A132" t="s">
         <v>147</v>
       </c>
-      <c r="G132" s="17"/>
-    </row>
-    <row r="133" spans="1:7">
+      <c r="H132" s="17"/>
+    </row>
+    <row r="133" spans="1:8">
       <c r="A133" t="s">
         <v>148</v>
       </c>
-      <c r="G133" s="17"/>
-    </row>
-    <row r="134" spans="1:7">
+      <c r="H133" s="17"/>
+    </row>
+    <row r="134" spans="1:8">
       <c r="A134" t="s">
         <v>149</v>
       </c>
-      <c r="G134" s="17"/>
-    </row>
-    <row r="135" spans="1:7">
+      <c r="H134" s="17"/>
+    </row>
+    <row r="135" spans="1:8">
       <c r="A135" t="s">
         <v>150</v>
       </c>
-      <c r="G135" s="17"/>
-    </row>
-    <row r="136" spans="1:7">
+      <c r="H135" s="17"/>
+    </row>
+    <row r="136" spans="1:8">
       <c r="A136" t="s">
         <v>151</v>
       </c>
-      <c r="G136" s="17"/>
-    </row>
-    <row r="137" spans="1:7">
+      <c r="H136" s="17"/>
+    </row>
+    <row r="137" spans="1:8">
       <c r="A137" t="s">
         <v>152</v>
       </c>
-      <c r="G137" s="17"/>
-    </row>
-    <row r="138" spans="1:7">
+      <c r="H137" s="17"/>
+    </row>
+    <row r="138" spans="1:8">
       <c r="A138" t="s">
         <v>153</v>
       </c>
-      <c r="G138" s="17"/>
-    </row>
-    <row r="139" spans="1:7">
+      <c r="H138" s="17"/>
+    </row>
+    <row r="139" spans="1:8">
       <c r="A139" t="s">
         <v>154</v>
       </c>
-      <c r="G139" s="17"/>
-    </row>
-    <row r="140" spans="1:7">
+      <c r="H139" s="17"/>
+    </row>
+    <row r="140" spans="1:8">
       <c r="A140" t="s">
         <v>155</v>
       </c>
-      <c r="G140" s="17"/>
-    </row>
-    <row r="141" spans="1:7">
+      <c r="H140" s="17"/>
+    </row>
+    <row r="141" spans="1:8">
       <c r="A141" t="s">
         <v>156</v>
       </c>
-      <c r="G141" s="17"/>
-    </row>
-    <row r="142" spans="1:7">
+      <c r="H141" s="17"/>
+    </row>
+    <row r="142" spans="1:8">
       <c r="A142" t="s">
         <v>157</v>
       </c>
-      <c r="G142" s="17"/>
-    </row>
-    <row r="143" spans="1:7">
+      <c r="H142" s="17"/>
+    </row>
+    <row r="143" spans="1:8">
       <c r="A143" t="s">
         <v>158</v>
       </c>
-      <c r="G143" s="17"/>
-    </row>
-    <row r="144" spans="1:7">
+      <c r="H143" s="17"/>
+    </row>
+    <row r="144" spans="1:8">
       <c r="A144" t="s">
         <v>159</v>
       </c>
-      <c r="G144" s="17"/>
-    </row>
-    <row r="145" spans="1:7">
+      <c r="H144" s="17"/>
+    </row>
+    <row r="145" spans="1:8">
       <c r="A145" t="s">
         <v>160</v>
       </c>
-      <c r="G145" s="17"/>
-    </row>
-    <row r="146" spans="1:7">
+      <c r="H145" s="17"/>
+    </row>
+    <row r="146" spans="1:8">
       <c r="A146" t="s">
         <v>161</v>
       </c>
-      <c r="G146" s="17"/>
-    </row>
-    <row r="147" spans="1:7">
+      <c r="H146" s="17"/>
+    </row>
+    <row r="147" spans="1:8">
       <c r="A147" t="s">
         <v>162</v>
       </c>
-      <c r="G147" s="17"/>
-    </row>
-    <row r="148" spans="1:7">
+      <c r="H147" s="17"/>
+    </row>
+    <row r="148" spans="1:8">
       <c r="A148" t="s">
         <v>163</v>
       </c>
-      <c r="G148" s="17"/>
-    </row>
-    <row r="149" spans="1:7">
+      <c r="H148" s="17"/>
+    </row>
+    <row r="149" spans="1:8">
       <c r="A149" t="s">
         <v>164</v>
       </c>
-      <c r="G149" s="17"/>
-    </row>
-    <row r="150" spans="1:7">
+      <c r="H149" s="17"/>
+    </row>
+    <row r="150" spans="1:8">
       <c r="A150" t="s">
         <v>165</v>
       </c>
-      <c r="G150" s="17"/>
-    </row>
-    <row r="151" spans="1:7">
+      <c r="H150" s="17"/>
+    </row>
+    <row r="151" spans="1:8">
       <c r="A151" t="s">
         <v>166</v>
       </c>
-      <c r="G151" s="17"/>
-    </row>
-    <row r="152" spans="1:7">
+      <c r="H151" s="17"/>
+    </row>
+    <row r="152" spans="1:8">
       <c r="A152" t="s">
         <v>167</v>
       </c>
-      <c r="G152" s="17"/>
-    </row>
-    <row r="153" spans="1:7">
+      <c r="H152" s="17"/>
+    </row>
+    <row r="153" spans="1:8">
       <c r="A153" t="s">
         <v>168</v>
       </c>
-      <c r="G153" s="17"/>
-    </row>
-    <row r="154" spans="1:7">
+      <c r="H153" s="17"/>
+    </row>
+    <row r="154" spans="1:8">
       <c r="A154" t="s">
         <v>169</v>
       </c>
-      <c r="G154" s="17"/>
-    </row>
-    <row r="155" spans="1:7">
+      <c r="H154" s="17"/>
+    </row>
+    <row r="155" spans="1:8">
       <c r="A155" t="s">
         <v>170</v>
       </c>
-      <c r="G155" s="17"/>
-    </row>
-    <row r="156" spans="1:7">
-      <c r="G156" s="17"/>
-    </row>
-    <row r="157" spans="1:7">
-      <c r="G157" s="17"/>
-    </row>
-    <row r="158" spans="1:7">
-      <c r="G158" s="17"/>
-    </row>
-    <row r="159" spans="1:7">
-      <c r="G159" s="17"/>
-    </row>
-    <row r="160" spans="1:7">
-      <c r="G160" s="17"/>
-    </row>
-    <row r="161" spans="1:7">
-      <c r="G161" s="17"/>
-    </row>
-    <row r="162" spans="1:7">
+      <c r="H155" s="17"/>
+    </row>
+    <row r="156" spans="1:8">
+      <c r="H156" s="17"/>
+    </row>
+    <row r="157" spans="1:8">
+      <c r="H157" s="17"/>
+    </row>
+    <row r="158" spans="1:8">
+      <c r="H158" s="17"/>
+    </row>
+    <row r="159" spans="1:8">
+      <c r="H159" s="17"/>
+    </row>
+    <row r="160" spans="1:8">
+      <c r="H160" s="17"/>
+    </row>
+    <row r="161" spans="1:8">
+      <c r="H161" s="17"/>
+    </row>
+    <row r="162" spans="1:8">
       <c r="A162" t="s">
         <v>95</v>
       </c>
-      <c r="G162" s="17"/>
-    </row>
-    <row r="163" spans="1:7">
+      <c r="H162" s="17"/>
+    </row>
+    <row r="163" spans="1:8">
       <c r="A163" t="s">
         <v>96</v>
       </c>
-      <c r="G163" s="17"/>
-    </row>
-    <row r="164" spans="1:7">
+      <c r="H163" s="17"/>
+    </row>
+    <row r="164" spans="1:8">
       <c r="A164" t="s">
         <v>97</v>
       </c>
-      <c r="G164" s="17"/>
-    </row>
-    <row r="165" spans="1:7">
+      <c r="H164" s="17"/>
+    </row>
+    <row r="165" spans="1:8">
       <c r="A165" t="s">
         <v>98</v>
       </c>
-      <c r="G165" s="17"/>
-    </row>
-    <row r="166" spans="1:7">
+      <c r="H165" s="17"/>
+    </row>
+    <row r="166" spans="1:8">
       <c r="A166" t="s">
         <v>99</v>
       </c>
-      <c r="G166" s="17"/>
-    </row>
-    <row r="167" spans="1:7">
+      <c r="H166" s="17"/>
+    </row>
+    <row r="167" spans="1:8">
       <c r="A167" t="s">
         <v>100</v>
       </c>
-      <c r="G167" s="17"/>
-    </row>
-    <row r="168" spans="1:7">
+      <c r="H167" s="17"/>
+    </row>
+    <row r="168" spans="1:8">
       <c r="A168" t="s">
         <v>101</v>
       </c>
-      <c r="G168" s="17"/>
-    </row>
-    <row r="169" spans="1:7">
+      <c r="H168" s="17"/>
+    </row>
+    <row r="169" spans="1:8">
       <c r="A169" t="s">
         <v>102</v>
       </c>
-      <c r="G169" s="17"/>
-    </row>
-    <row r="170" spans="1:7">
+      <c r="H169" s="17"/>
+    </row>
+    <row r="170" spans="1:8">
       <c r="A170" t="s">
         <v>103</v>
       </c>
-      <c r="G170" s="17"/>
-    </row>
-    <row r="171" spans="1:7">
+      <c r="H170" s="17"/>
+    </row>
+    <row r="171" spans="1:8">
       <c r="A171" t="s">
         <v>104</v>
       </c>
-      <c r="G171" s="17"/>
-    </row>
-    <row r="172" spans="1:7">
+      <c r="H171" s="17"/>
+    </row>
+    <row r="172" spans="1:8">
       <c r="A172" t="s">
         <v>105</v>
       </c>
-      <c r="G172" s="17"/>
-    </row>
-    <row r="173" spans="1:7">
+      <c r="H172" s="17"/>
+    </row>
+    <row r="173" spans="1:8">
       <c r="A173" t="s">
         <v>106</v>
       </c>
-      <c r="G173" s="17"/>
-    </row>
-    <row r="174" spans="1:7">
+      <c r="H173" s="17"/>
+    </row>
+    <row r="174" spans="1:8">
       <c r="A174" t="s">
         <v>107</v>
       </c>
-      <c r="G174" s="17"/>
-    </row>
-    <row r="175" spans="1:7">
+      <c r="H174" s="17"/>
+    </row>
+    <row r="175" spans="1:8">
       <c r="A175" t="s">
         <v>108</v>
       </c>
-      <c r="G175" s="17"/>
-    </row>
-    <row r="176" spans="1:7">
+      <c r="H175" s="17"/>
+    </row>
+    <row r="176" spans="1:8">
       <c r="A176" t="s">
         <v>109</v>
       </c>
-      <c r="G176" s="17"/>
-    </row>
-    <row r="177" spans="1:7">
+      <c r="H176" s="17"/>
+    </row>
+    <row r="177" spans="1:8">
       <c r="A177" t="s">
         <v>110</v>
       </c>
-      <c r="G177" s="17"/>
-    </row>
-    <row r="178" spans="1:7">
+      <c r="H177" s="17"/>
+    </row>
+    <row r="178" spans="1:8">
       <c r="A178" t="s">
         <v>111</v>
       </c>
-      <c r="G178" s="17"/>
-    </row>
-    <row r="179" spans="1:7">
+      <c r="H178" s="17"/>
+    </row>
+    <row r="179" spans="1:8">
       <c r="A179" t="s">
         <v>112</v>
       </c>
-      <c r="G179" s="17"/>
-    </row>
-    <row r="180" spans="1:7">
+      <c r="H179" s="17"/>
+    </row>
+    <row r="180" spans="1:8">
       <c r="A180" t="s">
         <v>113</v>
       </c>
-      <c r="G180" s="17"/>
-    </row>
-    <row r="181" spans="1:7">
+      <c r="H180" s="17"/>
+    </row>
+    <row r="181" spans="1:8">
       <c r="A181" t="s">
         <v>114</v>
       </c>
-      <c r="G181" s="17"/>
-    </row>
-    <row r="182" spans="1:7">
+      <c r="H181" s="17"/>
+    </row>
+    <row r="182" spans="1:8">
       <c r="A182" t="s">
         <v>115</v>
       </c>
-      <c r="G182" s="17"/>
-    </row>
-    <row r="183" spans="1:7">
+      <c r="H182" s="17"/>
+    </row>
+    <row r="183" spans="1:8">
       <c r="A183" t="s">
         <v>116</v>
       </c>
@@ -6506,9 +6562,10 @@
       <c r="D183" s="22"/>
       <c r="E183" s="22"/>
       <c r="F183" s="22"/>
-      <c r="G183" s="17"/>
-    </row>
-    <row r="184" spans="1:7">
+      <c r="G183" s="22"/>
+      <c r="H183" s="17"/>
+    </row>
+    <row r="184" spans="1:8">
       <c r="A184" t="s">
         <v>117</v>
       </c>
@@ -6517,9 +6574,10 @@
       <c r="D184" s="22"/>
       <c r="E184" s="22"/>
       <c r="F184" s="22"/>
-      <c r="G184" s="17"/>
-    </row>
-    <row r="185" spans="1:7">
+      <c r="G184" s="22"/>
+      <c r="H184" s="17"/>
+    </row>
+    <row r="185" spans="1:8">
       <c r="A185" t="s">
         <v>118</v>
       </c>
@@ -6528,39 +6586,40 @@
       <c r="D185" s="22"/>
       <c r="E185" s="22"/>
       <c r="F185" s="22"/>
-      <c r="G185" s="17"/>
-    </row>
-    <row r="186" spans="1:7">
+      <c r="G185" s="22"/>
+      <c r="H185" s="17"/>
+    </row>
+    <row r="186" spans="1:8">
       <c r="A186" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:8">
       <c r="A187" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:8">
       <c r="A188" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:8">
       <c r="A189" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:8">
       <c r="A190" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:8">
       <c r="A191" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:8">
       <c r="A192" t="s">
         <v>125</v>
       </c>
@@ -10668,244 +10727,244 @@
         <v>907</v>
       </c>
     </row>
-    <row r="1025" spans="1:7">
+    <row r="1025" spans="1:8">
       <c r="A1025" t="s">
         <v>908</v>
       </c>
-      <c r="G1025" s="17"/>
-    </row>
-    <row r="1026" spans="1:7">
+      <c r="H1025" s="17"/>
+    </row>
+    <row r="1026" spans="1:8">
       <c r="A1026" t="s">
         <v>909</v>
       </c>
-      <c r="G1026" s="17"/>
-    </row>
-    <row r="1027" spans="1:7">
+      <c r="H1026" s="17"/>
+    </row>
+    <row r="1027" spans="1:8">
       <c r="A1027" t="s">
         <v>910</v>
       </c>
-      <c r="G1027" s="17"/>
-    </row>
-    <row r="1028" spans="1:7">
+      <c r="H1027" s="17"/>
+    </row>
+    <row r="1028" spans="1:8">
       <c r="A1028" t="s">
         <v>911</v>
       </c>
-      <c r="G1028" s="17"/>
-    </row>
-    <row r="1029" spans="1:7">
+      <c r="H1028" s="17"/>
+    </row>
+    <row r="1029" spans="1:8">
       <c r="A1029" t="s">
         <v>912</v>
       </c>
-      <c r="G1029" s="17"/>
-    </row>
-    <row r="1030" spans="1:7">
+      <c r="H1029" s="17"/>
+    </row>
+    <row r="1030" spans="1:8">
       <c r="A1030" t="s">
         <v>913</v>
       </c>
-      <c r="G1030" s="17"/>
-    </row>
-    <row r="1031" spans="1:7">
+      <c r="H1030" s="17"/>
+    </row>
+    <row r="1031" spans="1:8">
       <c r="A1031" t="s">
         <v>914</v>
       </c>
-      <c r="G1031" s="17"/>
-    </row>
-    <row r="1032" spans="1:7">
+      <c r="H1031" s="17"/>
+    </row>
+    <row r="1032" spans="1:8">
       <c r="A1032" t="s">
         <v>915</v>
       </c>
-      <c r="G1032" s="17"/>
-    </row>
-    <row r="1033" spans="1:7">
+      <c r="H1032" s="17"/>
+    </row>
+    <row r="1033" spans="1:8">
       <c r="A1033" t="s">
         <v>916</v>
       </c>
-      <c r="G1033" s="17"/>
-    </row>
-    <row r="1034" spans="1:7">
+      <c r="H1033" s="17"/>
+    </row>
+    <row r="1034" spans="1:8">
       <c r="A1034" t="s">
         <v>917</v>
       </c>
-      <c r="G1034" s="17"/>
-    </row>
-    <row r="1035" spans="1:7">
+      <c r="H1034" s="17"/>
+    </row>
+    <row r="1035" spans="1:8">
       <c r="A1035" t="s">
         <v>918</v>
       </c>
-      <c r="G1035" s="17"/>
-    </row>
-    <row r="1036" spans="1:7">
+      <c r="H1035" s="17"/>
+    </row>
+    <row r="1036" spans="1:8">
       <c r="A1036" t="s">
         <v>919</v>
       </c>
-      <c r="G1036" s="17"/>
-    </row>
-    <row r="1037" spans="1:7">
+      <c r="H1036" s="17"/>
+    </row>
+    <row r="1037" spans="1:8">
       <c r="A1037" t="s">
         <v>920</v>
       </c>
-      <c r="G1037" s="17"/>
-    </row>
-    <row r="1038" spans="1:7">
+      <c r="H1037" s="17"/>
+    </row>
+    <row r="1038" spans="1:8">
       <c r="A1038" t="s">
         <v>921</v>
       </c>
-      <c r="G1038" s="17"/>
-    </row>
-    <row r="1039" spans="1:7">
+      <c r="H1038" s="17"/>
+    </row>
+    <row r="1039" spans="1:8">
       <c r="A1039" t="s">
         <v>922</v>
       </c>
-      <c r="G1039" s="17"/>
-    </row>
-    <row r="1040" spans="1:7">
+      <c r="H1039" s="17"/>
+    </row>
+    <row r="1040" spans="1:8">
       <c r="A1040" t="s">
         <v>923</v>
       </c>
-      <c r="G1040" s="17"/>
-    </row>
-    <row r="1041" spans="1:7">
+      <c r="H1040" s="17"/>
+    </row>
+    <row r="1041" spans="1:8">
       <c r="A1041" t="s">
         <v>924</v>
       </c>
-      <c r="G1041" s="17"/>
-    </row>
-    <row r="1042" spans="1:7">
+      <c r="H1041" s="17"/>
+    </row>
+    <row r="1042" spans="1:8">
       <c r="A1042" t="s">
         <v>925</v>
       </c>
-      <c r="G1042" s="17"/>
-    </row>
-    <row r="1043" spans="1:7">
+      <c r="H1042" s="17"/>
+    </row>
+    <row r="1043" spans="1:8">
       <c r="A1043" t="s">
         <v>926</v>
       </c>
-      <c r="G1043" s="17"/>
-    </row>
-    <row r="1044" spans="1:7">
+      <c r="H1043" s="17"/>
+    </row>
+    <row r="1044" spans="1:8">
       <c r="A1044" t="s">
         <v>927</v>
       </c>
-      <c r="G1044" s="17"/>
-    </row>
-    <row r="1045" spans="1:7">
+      <c r="H1044" s="17"/>
+    </row>
+    <row r="1045" spans="1:8">
       <c r="A1045" t="s">
         <v>928</v>
       </c>
-      <c r="G1045" s="17"/>
-    </row>
-    <row r="1046" spans="1:7">
+      <c r="H1045" s="17"/>
+    </row>
+    <row r="1046" spans="1:8">
       <c r="A1046" t="s">
         <v>929</v>
       </c>
-      <c r="G1046" s="17"/>
-    </row>
-    <row r="1047" spans="1:7">
+      <c r="H1046" s="17"/>
+    </row>
+    <row r="1047" spans="1:8">
       <c r="A1047" t="s">
         <v>930</v>
       </c>
-      <c r="G1047" s="17"/>
-    </row>
-    <row r="1048" spans="1:7">
+      <c r="H1047" s="17"/>
+    </row>
+    <row r="1048" spans="1:8">
       <c r="A1048" t="s">
         <v>931</v>
       </c>
-      <c r="G1048" s="17"/>
-    </row>
-    <row r="1049" spans="1:7">
+      <c r="H1048" s="17"/>
+    </row>
+    <row r="1049" spans="1:8">
       <c r="A1049" t="s">
         <v>932</v>
       </c>
-      <c r="G1049" s="17"/>
-    </row>
-    <row r="1050" spans="1:7">
+      <c r="H1049" s="17"/>
+    </row>
+    <row r="1050" spans="1:8">
       <c r="A1050" t="s">
         <v>933</v>
       </c>
-      <c r="G1050" s="17"/>
-    </row>
-    <row r="1051" spans="1:7">
-      <c r="G1051" s="17"/>
-    </row>
-    <row r="1052" spans="1:7">
+      <c r="H1050" s="17"/>
+    </row>
+    <row r="1051" spans="1:8">
+      <c r="H1051" s="17"/>
+    </row>
+    <row r="1052" spans="1:8">
       <c r="A1052" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="G1052" s="17"/>
-    </row>
-    <row r="1053" spans="1:7">
+      <c r="H1052" s="17"/>
+    </row>
+    <row r="1053" spans="1:8">
       <c r="A1053" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="G1053" s="17"/>
-    </row>
-    <row r="1054" spans="1:7">
+      <c r="H1053" s="17"/>
+    </row>
+    <row r="1054" spans="1:8">
       <c r="A1054" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="G1054" s="17"/>
-    </row>
-    <row r="1055" spans="1:7">
+      <c r="H1054" s="17"/>
+    </row>
+    <row r="1055" spans="1:8">
       <c r="A1055" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="G1055" s="17"/>
-    </row>
-    <row r="1056" spans="1:7">
+      <c r="H1055" s="17"/>
+    </row>
+    <row r="1056" spans="1:8">
       <c r="A1056" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="G1056" s="17"/>
-    </row>
-    <row r="1057" spans="1:7">
+      <c r="H1056" s="17"/>
+    </row>
+    <row r="1057" spans="1:8">
       <c r="A1057" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="G1057" s="17"/>
-    </row>
-    <row r="1058" spans="1:7">
+      <c r="H1057" s="17"/>
+    </row>
+    <row r="1058" spans="1:8">
       <c r="A1058" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="G1058" s="17"/>
-    </row>
-    <row r="1059" spans="1:7">
+      <c r="H1058" s="17"/>
+    </row>
+    <row r="1059" spans="1:8">
       <c r="A1059" s="17" t="s">
         <v>250</v>
       </c>
-      <c r="G1059" s="17"/>
-    </row>
-    <row r="1060" spans="1:7">
+      <c r="H1059" s="17"/>
+    </row>
+    <row r="1060" spans="1:8">
       <c r="A1060" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="G1060" s="17"/>
-    </row>
-    <row r="1061" spans="1:7">
+      <c r="H1060" s="17"/>
+    </row>
+    <row r="1061" spans="1:8">
       <c r="A1061" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="G1061" s="17"/>
-    </row>
-    <row r="1062" spans="1:7">
+      <c r="H1061" s="17"/>
+    </row>
+    <row r="1062" spans="1:8">
       <c r="A1062" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="G1062" s="17"/>
-    </row>
-    <row r="1063" spans="1:7">
+      <c r="H1062" s="17"/>
+    </row>
+    <row r="1063" spans="1:8">
       <c r="A1063" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="G1063" s="17"/>
-    </row>
-    <row r="1064" spans="1:7">
+      <c r="H1063" s="17"/>
+    </row>
+    <row r="1064" spans="1:8">
       <c r="A1064" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="G1064" s="17"/>
-    </row>
-    <row r="1065" spans="1:7">
+      <c r="H1064" s="17"/>
+    </row>
+    <row r="1065" spans="1:8">
       <c r="A1065" s="17" t="s">
         <v>256</v>
       </c>
@@ -10914,8 +10973,9 @@
       <c r="D1065"/>
       <c r="E1065"/>
       <c r="F1065"/>
-    </row>
-    <row r="1066" spans="1:7">
+      <c r="G1065"/>
+    </row>
+    <row r="1066" spans="1:8">
       <c r="A1066" s="17" t="s">
         <v>257</v>
       </c>
@@ -10924,8 +10984,9 @@
       <c r="D1066"/>
       <c r="E1066"/>
       <c r="F1066"/>
-    </row>
-    <row r="1067" spans="1:7">
+      <c r="G1066"/>
+    </row>
+    <row r="1067" spans="1:8">
       <c r="A1067" s="17" t="s">
         <v>258</v>
       </c>
@@ -10934,8 +10995,9 @@
       <c r="D1067"/>
       <c r="E1067"/>
       <c r="F1067"/>
-    </row>
-    <row r="1068" spans="1:7">
+      <c r="G1067"/>
+    </row>
+    <row r="1068" spans="1:8">
       <c r="A1068" s="17" t="s">
         <v>259</v>
       </c>
@@ -10944,8 +11006,9 @@
       <c r="D1068"/>
       <c r="E1068"/>
       <c r="F1068"/>
-    </row>
-    <row r="1069" spans="1:7">
+      <c r="G1068"/>
+    </row>
+    <row r="1069" spans="1:8">
       <c r="A1069" s="17" t="s">
         <v>260</v>
       </c>
@@ -10954,8 +11017,9 @@
       <c r="D1069"/>
       <c r="E1069"/>
       <c r="F1069"/>
-    </row>
-    <row r="1070" spans="1:7">
+      <c r="G1069"/>
+    </row>
+    <row r="1070" spans="1:8">
       <c r="A1070" s="17" t="s">
         <v>261</v>
       </c>
@@ -10964,8 +11028,9 @@
       <c r="D1070"/>
       <c r="E1070"/>
       <c r="F1070"/>
-    </row>
-    <row r="1071" spans="1:7">
+      <c r="G1070"/>
+    </row>
+    <row r="1071" spans="1:8">
       <c r="A1071" s="17" t="s">
         <v>262</v>
       </c>
@@ -10974,8 +11039,9 @@
       <c r="D1071"/>
       <c r="E1071"/>
       <c r="F1071"/>
-    </row>
-    <row r="1072" spans="1:7">
+      <c r="G1071"/>
+    </row>
+    <row r="1072" spans="1:8">
       <c r="A1072" s="17" t="s">
         <v>263</v>
       </c>
@@ -10984,8 +11050,9 @@
       <c r="D1072"/>
       <c r="E1072"/>
       <c r="F1072"/>
-    </row>
-    <row r="1073" spans="1:6">
+      <c r="G1072"/>
+    </row>
+    <row r="1073" spans="1:7">
       <c r="A1073" s="17" t="s">
         <v>264</v>
       </c>
@@ -10994,8 +11061,9 @@
       <c r="D1073"/>
       <c r="E1073"/>
       <c r="F1073"/>
-    </row>
-    <row r="1074" spans="1:6">
+      <c r="G1073"/>
+    </row>
+    <row r="1074" spans="1:7">
       <c r="A1074" s="17" t="s">
         <v>265</v>
       </c>
@@ -11004,8 +11072,9 @@
       <c r="D1074"/>
       <c r="E1074"/>
       <c r="F1074"/>
-    </row>
-    <row r="1075" spans="1:6">
+      <c r="G1074"/>
+    </row>
+    <row r="1075" spans="1:7">
       <c r="A1075" s="17" t="s">
         <v>266</v>
       </c>
@@ -11014,8 +11083,9 @@
       <c r="D1075"/>
       <c r="E1075"/>
       <c r="F1075"/>
-    </row>
-    <row r="1076" spans="1:6">
+      <c r="G1075"/>
+    </row>
+    <row r="1076" spans="1:7">
       <c r="A1076" s="17" t="s">
         <v>267</v>
       </c>
@@ -11024,8 +11094,9 @@
       <c r="D1076"/>
       <c r="E1076"/>
       <c r="F1076"/>
-    </row>
-    <row r="1077" spans="1:6">
+      <c r="G1076"/>
+    </row>
+    <row r="1077" spans="1:7">
       <c r="A1077" s="17" t="s">
         <v>268</v>
       </c>
@@ -11034,8 +11105,9 @@
       <c r="D1077"/>
       <c r="E1077"/>
       <c r="F1077"/>
-    </row>
-    <row r="1078" spans="1:6">
+      <c r="G1077"/>
+    </row>
+    <row r="1078" spans="1:7">
       <c r="A1078" s="17" t="s">
         <v>269</v>
       </c>
@@ -11044,8 +11116,9 @@
       <c r="D1078"/>
       <c r="E1078"/>
       <c r="F1078"/>
-    </row>
-    <row r="1079" spans="1:6">
+      <c r="G1078"/>
+    </row>
+    <row r="1079" spans="1:7">
       <c r="A1079" s="17" t="s">
         <v>270</v>
       </c>
@@ -11054,8 +11127,9 @@
       <c r="D1079"/>
       <c r="E1079"/>
       <c r="F1079"/>
-    </row>
-    <row r="1080" spans="1:6">
+      <c r="G1079"/>
+    </row>
+    <row r="1080" spans="1:7">
       <c r="A1080" s="17" t="s">
         <v>271</v>
       </c>
@@ -11064,8 +11138,9 @@
       <c r="D1080"/>
       <c r="E1080"/>
       <c r="F1080"/>
-    </row>
-    <row r="1081" spans="1:6">
+      <c r="G1080"/>
+    </row>
+    <row r="1081" spans="1:7">
       <c r="A1081" s="17" t="s">
         <v>272</v>
       </c>
@@ -11074,8 +11149,9 @@
       <c r="D1081"/>
       <c r="E1081"/>
       <c r="F1081"/>
-    </row>
-    <row r="1082" spans="1:6">
+      <c r="G1081"/>
+    </row>
+    <row r="1082" spans="1:7">
       <c r="A1082" s="17" t="s">
         <v>273</v>
       </c>
@@ -11084,8 +11160,9 @@
       <c r="D1082"/>
       <c r="E1082"/>
       <c r="F1082"/>
-    </row>
-    <row r="1083" spans="1:6">
+      <c r="G1082"/>
+    </row>
+    <row r="1083" spans="1:7">
       <c r="A1083" s="17" t="s">
         <v>274</v>
       </c>
@@ -11094,8 +11171,9 @@
       <c r="D1083"/>
       <c r="E1083"/>
       <c r="F1083"/>
-    </row>
-    <row r="1084" spans="1:6">
+      <c r="G1083"/>
+    </row>
+    <row r="1084" spans="1:7">
       <c r="A1084" s="17" t="s">
         <v>275</v>
       </c>
@@ -11104,8 +11182,9 @@
       <c r="D1084"/>
       <c r="E1084"/>
       <c r="F1084"/>
-    </row>
-    <row r="1085" spans="1:6">
+      <c r="G1084"/>
+    </row>
+    <row r="1085" spans="1:7">
       <c r="A1085" s="17" t="s">
         <v>276</v>
       </c>
@@ -11114,8 +11193,9 @@
       <c r="D1085"/>
       <c r="E1085"/>
       <c r="F1085"/>
-    </row>
-    <row r="1086" spans="1:6">
+      <c r="G1085"/>
+    </row>
+    <row r="1086" spans="1:7">
       <c r="A1086" s="17" t="s">
         <v>277</v>
       </c>
@@ -11124,8 +11204,9 @@
       <c r="D1086"/>
       <c r="E1086"/>
       <c r="F1086"/>
-    </row>
-    <row r="1087" spans="1:6">
+      <c r="G1086"/>
+    </row>
+    <row r="1087" spans="1:7">
       <c r="A1087" s="17" t="s">
         <v>934</v>
       </c>
@@ -11134,8 +11215,9 @@
       <c r="D1087"/>
       <c r="E1087"/>
       <c r="F1087"/>
-    </row>
-    <row r="1088" spans="1:6">
+      <c r="G1087"/>
+    </row>
+    <row r="1088" spans="1:7">
       <c r="A1088" s="17" t="s">
         <v>935</v>
       </c>
@@ -11144,8 +11226,9 @@
       <c r="D1088"/>
       <c r="E1088"/>
       <c r="F1088"/>
-    </row>
-    <row r="1089" spans="1:6">
+      <c r="G1088"/>
+    </row>
+    <row r="1089" spans="1:7">
       <c r="A1089" s="17" t="s">
         <v>936</v>
       </c>
@@ -11154,8 +11237,9 @@
       <c r="D1089"/>
       <c r="E1089"/>
       <c r="F1089"/>
-    </row>
-    <row r="1090" spans="1:6">
+      <c r="G1089"/>
+    </row>
+    <row r="1090" spans="1:7">
       <c r="A1090" s="17" t="s">
         <v>937</v>
       </c>
@@ -11164,8 +11248,9 @@
       <c r="D1090"/>
       <c r="E1090"/>
       <c r="F1090"/>
-    </row>
-    <row r="1091" spans="1:6">
+      <c r="G1090"/>
+    </row>
+    <row r="1091" spans="1:7">
       <c r="A1091" s="17" t="s">
         <v>938</v>
       </c>
@@ -11174,496 +11259,567 @@
       <c r="D1091"/>
       <c r="E1091"/>
       <c r="F1091"/>
-    </row>
-    <row r="1092" spans="1:6">
+      <c r="G1091"/>
+    </row>
+    <row r="1092" spans="1:7">
       <c r="B1092"/>
       <c r="C1092"/>
       <c r="D1092"/>
       <c r="E1092"/>
       <c r="F1092"/>
-    </row>
-    <row r="1093" spans="1:6">
+      <c r="G1092"/>
+    </row>
+    <row r="1093" spans="1:7">
       <c r="B1093"/>
       <c r="C1093"/>
       <c r="D1093"/>
       <c r="E1093"/>
       <c r="F1093"/>
-    </row>
-    <row r="1094" spans="1:6">
+      <c r="G1093"/>
+    </row>
+    <row r="1094" spans="1:7">
       <c r="B1094"/>
       <c r="C1094"/>
       <c r="D1094"/>
       <c r="E1094"/>
       <c r="F1094"/>
-    </row>
-    <row r="1095" spans="1:6">
+      <c r="G1094"/>
+    </row>
+    <row r="1095" spans="1:7">
       <c r="B1095"/>
       <c r="C1095"/>
       <c r="D1095"/>
       <c r="E1095"/>
       <c r="F1095"/>
-    </row>
-    <row r="1096" spans="1:6">
+      <c r="G1095"/>
+    </row>
+    <row r="1096" spans="1:7">
       <c r="B1096"/>
       <c r="C1096"/>
       <c r="D1096"/>
       <c r="E1096"/>
       <c r="F1096"/>
-    </row>
-    <row r="1097" spans="1:6">
+      <c r="G1096"/>
+    </row>
+    <row r="1097" spans="1:7">
       <c r="B1097"/>
       <c r="C1097"/>
       <c r="D1097"/>
       <c r="E1097"/>
       <c r="F1097"/>
-    </row>
-    <row r="1098" spans="1:6">
+      <c r="G1097"/>
+    </row>
+    <row r="1098" spans="1:7">
       <c r="B1098"/>
       <c r="C1098"/>
       <c r="D1098"/>
       <c r="E1098"/>
       <c r="F1098"/>
-    </row>
-    <row r="1099" spans="1:6">
+      <c r="G1098"/>
+    </row>
+    <row r="1099" spans="1:7">
       <c r="B1099"/>
       <c r="C1099"/>
       <c r="D1099"/>
       <c r="E1099"/>
       <c r="F1099"/>
-    </row>
-    <row r="1100" spans="1:6">
+      <c r="G1099"/>
+    </row>
+    <row r="1100" spans="1:7">
       <c r="B1100"/>
       <c r="C1100"/>
       <c r="D1100"/>
       <c r="E1100"/>
       <c r="F1100"/>
-    </row>
-    <row r="1101" spans="1:6">
+      <c r="G1100"/>
+    </row>
+    <row r="1101" spans="1:7">
       <c r="B1101"/>
       <c r="C1101"/>
       <c r="D1101"/>
       <c r="E1101"/>
       <c r="F1101"/>
-    </row>
-    <row r="1102" spans="1:6">
+      <c r="G1101"/>
+    </row>
+    <row r="1102" spans="1:7">
       <c r="B1102"/>
       <c r="C1102"/>
       <c r="D1102"/>
       <c r="E1102"/>
       <c r="F1102"/>
-    </row>
-    <row r="1103" spans="1:6">
+      <c r="G1102"/>
+    </row>
+    <row r="1103" spans="1:7">
       <c r="B1103"/>
       <c r="C1103"/>
       <c r="D1103"/>
       <c r="E1103"/>
       <c r="F1103"/>
-    </row>
-    <row r="1104" spans="1:6">
+      <c r="G1103"/>
+    </row>
+    <row r="1104" spans="1:7">
       <c r="B1104"/>
       <c r="C1104"/>
       <c r="D1104"/>
       <c r="E1104"/>
       <c r="F1104"/>
-    </row>
-    <row r="1105" spans="2:6">
+      <c r="G1104"/>
+    </row>
+    <row r="1105" spans="2:7">
       <c r="B1105"/>
       <c r="C1105"/>
       <c r="D1105"/>
       <c r="E1105"/>
       <c r="F1105"/>
-    </row>
-    <row r="1106" spans="2:6">
+      <c r="G1105"/>
+    </row>
+    <row r="1106" spans="2:7">
       <c r="B1106"/>
       <c r="C1106"/>
       <c r="D1106"/>
       <c r="E1106"/>
       <c r="F1106"/>
-    </row>
-    <row r="1107" spans="2:6">
+      <c r="G1106"/>
+    </row>
+    <row r="1107" spans="2:7">
       <c r="B1107"/>
       <c r="C1107"/>
       <c r="D1107"/>
       <c r="E1107"/>
       <c r="F1107"/>
-    </row>
-    <row r="1108" spans="2:6">
+      <c r="G1107"/>
+    </row>
+    <row r="1108" spans="2:7">
       <c r="B1108"/>
       <c r="C1108"/>
       <c r="D1108"/>
       <c r="E1108"/>
       <c r="F1108"/>
-    </row>
-    <row r="1109" spans="2:6">
+      <c r="G1108"/>
+    </row>
+    <row r="1109" spans="2:7">
       <c r="B1109"/>
       <c r="C1109"/>
       <c r="D1109"/>
       <c r="E1109"/>
       <c r="F1109"/>
-    </row>
-    <row r="1110" spans="2:6">
+      <c r="G1109"/>
+    </row>
+    <row r="1110" spans="2:7">
       <c r="B1110"/>
       <c r="C1110"/>
       <c r="D1110"/>
       <c r="E1110"/>
       <c r="F1110"/>
-    </row>
-    <row r="1111" spans="2:6">
+      <c r="G1110"/>
+    </row>
+    <row r="1111" spans="2:7">
       <c r="B1111"/>
       <c r="C1111"/>
       <c r="D1111"/>
       <c r="E1111"/>
       <c r="F1111"/>
-    </row>
-    <row r="1112" spans="2:6">
+      <c r="G1111"/>
+    </row>
+    <row r="1112" spans="2:7">
       <c r="B1112"/>
       <c r="C1112"/>
       <c r="D1112"/>
       <c r="E1112"/>
       <c r="F1112"/>
-    </row>
-    <row r="1113" spans="2:6">
+      <c r="G1112"/>
+    </row>
+    <row r="1113" spans="2:7">
       <c r="B1113"/>
       <c r="C1113"/>
       <c r="D1113"/>
       <c r="E1113"/>
       <c r="F1113"/>
-    </row>
-    <row r="1114" spans="2:6">
+      <c r="G1113"/>
+    </row>
+    <row r="1114" spans="2:7">
       <c r="B1114"/>
       <c r="C1114"/>
       <c r="D1114"/>
       <c r="E1114"/>
       <c r="F1114"/>
-    </row>
-    <row r="1115" spans="2:6">
+      <c r="G1114"/>
+    </row>
+    <row r="1115" spans="2:7">
       <c r="B1115"/>
       <c r="C1115"/>
       <c r="D1115"/>
       <c r="E1115"/>
       <c r="F1115"/>
-    </row>
-    <row r="1116" spans="2:6">
+      <c r="G1115"/>
+    </row>
+    <row r="1116" spans="2:7">
       <c r="B1116"/>
       <c r="C1116"/>
       <c r="D1116"/>
       <c r="E1116"/>
       <c r="F1116"/>
-    </row>
-    <row r="1117" spans="2:6">
+      <c r="G1116"/>
+    </row>
+    <row r="1117" spans="2:7">
       <c r="B1117"/>
       <c r="C1117"/>
       <c r="D1117"/>
       <c r="E1117"/>
       <c r="F1117"/>
-    </row>
-    <row r="1118" spans="2:6">
+      <c r="G1117"/>
+    </row>
+    <row r="1118" spans="2:7">
       <c r="B1118"/>
       <c r="C1118"/>
       <c r="D1118"/>
       <c r="E1118"/>
       <c r="F1118"/>
-    </row>
-    <row r="1119" spans="2:6">
+      <c r="G1118"/>
+    </row>
+    <row r="1119" spans="2:7">
       <c r="B1119"/>
       <c r="C1119"/>
       <c r="D1119"/>
       <c r="E1119"/>
       <c r="F1119"/>
-    </row>
-    <row r="1120" spans="2:6">
+      <c r="G1119"/>
+    </row>
+    <row r="1120" spans="2:7">
       <c r="B1120"/>
       <c r="C1120"/>
       <c r="D1120"/>
       <c r="E1120"/>
       <c r="F1120"/>
-    </row>
-    <row r="1121" spans="2:6">
+      <c r="G1120"/>
+    </row>
+    <row r="1121" spans="2:7">
       <c r="B1121"/>
       <c r="C1121"/>
       <c r="D1121"/>
       <c r="E1121"/>
       <c r="F1121"/>
-    </row>
-    <row r="1122" spans="2:6">
+      <c r="G1121"/>
+    </row>
+    <row r="1122" spans="2:7">
       <c r="B1122"/>
       <c r="C1122"/>
       <c r="D1122"/>
       <c r="E1122"/>
       <c r="F1122"/>
-    </row>
-    <row r="1123" spans="2:6">
+      <c r="G1122"/>
+    </row>
+    <row r="1123" spans="2:7">
       <c r="B1123"/>
       <c r="C1123"/>
       <c r="D1123"/>
       <c r="E1123"/>
       <c r="F1123"/>
-    </row>
-    <row r="1124" spans="2:6">
+      <c r="G1123"/>
+    </row>
+    <row r="1124" spans="2:7">
       <c r="B1124"/>
       <c r="C1124"/>
       <c r="D1124"/>
       <c r="E1124"/>
       <c r="F1124"/>
-    </row>
-    <row r="1125" spans="2:6">
+      <c r="G1124"/>
+    </row>
+    <row r="1125" spans="2:7">
       <c r="B1125"/>
       <c r="C1125"/>
       <c r="D1125"/>
       <c r="E1125"/>
       <c r="F1125"/>
-    </row>
-    <row r="1126" spans="2:6">
+      <c r="G1125"/>
+    </row>
+    <row r="1126" spans="2:7">
       <c r="B1126"/>
       <c r="C1126"/>
       <c r="D1126"/>
       <c r="E1126"/>
       <c r="F1126"/>
-    </row>
-    <row r="1127" spans="2:6">
+      <c r="G1126"/>
+    </row>
+    <row r="1127" spans="2:7">
       <c r="B1127"/>
       <c r="C1127"/>
       <c r="D1127"/>
       <c r="E1127"/>
       <c r="F1127"/>
-    </row>
-    <row r="1128" spans="2:6">
+      <c r="G1127"/>
+    </row>
+    <row r="1128" spans="2:7">
       <c r="B1128"/>
       <c r="C1128"/>
       <c r="D1128"/>
       <c r="E1128"/>
       <c r="F1128"/>
-    </row>
-    <row r="1129" spans="2:6">
+      <c r="G1128"/>
+    </row>
+    <row r="1129" spans="2:7">
       <c r="B1129"/>
       <c r="C1129"/>
       <c r="D1129"/>
       <c r="E1129"/>
       <c r="F1129"/>
-    </row>
-    <row r="1130" spans="2:6">
+      <c r="G1129"/>
+    </row>
+    <row r="1130" spans="2:7">
       <c r="B1130"/>
       <c r="C1130"/>
       <c r="D1130"/>
       <c r="E1130"/>
       <c r="F1130"/>
-    </row>
-    <row r="1131" spans="2:6">
+      <c r="G1130"/>
+    </row>
+    <row r="1131" spans="2:7">
       <c r="B1131"/>
       <c r="C1131"/>
       <c r="D1131"/>
       <c r="E1131"/>
       <c r="F1131"/>
-    </row>
-    <row r="1132" spans="2:6">
+      <c r="G1131"/>
+    </row>
+    <row r="1132" spans="2:7">
       <c r="B1132"/>
       <c r="C1132"/>
       <c r="D1132"/>
       <c r="E1132"/>
       <c r="F1132"/>
-    </row>
-    <row r="1133" spans="2:6">
+      <c r="G1132"/>
+    </row>
+    <row r="1133" spans="2:7">
       <c r="B1133"/>
       <c r="C1133"/>
       <c r="D1133"/>
       <c r="E1133"/>
       <c r="F1133"/>
-    </row>
-    <row r="1134" spans="2:6">
+      <c r="G1133"/>
+    </row>
+    <row r="1134" spans="2:7">
       <c r="B1134"/>
       <c r="C1134"/>
       <c r="D1134"/>
       <c r="E1134"/>
       <c r="F1134"/>
-    </row>
-    <row r="1135" spans="2:6">
+      <c r="G1134"/>
+    </row>
+    <row r="1135" spans="2:7">
       <c r="B1135"/>
       <c r="C1135"/>
       <c r="D1135"/>
       <c r="E1135"/>
       <c r="F1135"/>
-    </row>
-    <row r="1136" spans="2:6">
+      <c r="G1135"/>
+    </row>
+    <row r="1136" spans="2:7">
       <c r="B1136"/>
       <c r="C1136"/>
       <c r="D1136"/>
       <c r="E1136"/>
       <c r="F1136"/>
-    </row>
-    <row r="1137" spans="2:6">
+      <c r="G1136"/>
+    </row>
+    <row r="1137" spans="2:7">
       <c r="B1137"/>
       <c r="C1137"/>
       <c r="D1137"/>
       <c r="E1137"/>
       <c r="F1137"/>
-    </row>
-    <row r="1138" spans="2:6">
+      <c r="G1137"/>
+    </row>
+    <row r="1138" spans="2:7">
       <c r="B1138"/>
       <c r="C1138"/>
       <c r="D1138"/>
       <c r="E1138"/>
       <c r="F1138"/>
-    </row>
-    <row r="1139" spans="2:6">
+      <c r="G1138"/>
+    </row>
+    <row r="1139" spans="2:7">
       <c r="B1139"/>
       <c r="C1139"/>
       <c r="D1139"/>
       <c r="E1139"/>
       <c r="F1139"/>
-    </row>
-    <row r="1140" spans="2:6">
+      <c r="G1139"/>
+    </row>
+    <row r="1140" spans="2:7">
       <c r="B1140"/>
       <c r="C1140"/>
       <c r="D1140"/>
       <c r="E1140"/>
       <c r="F1140"/>
-    </row>
-    <row r="1141" spans="2:6">
+      <c r="G1140"/>
+    </row>
+    <row r="1141" spans="2:7">
       <c r="B1141"/>
       <c r="C1141"/>
       <c r="D1141"/>
       <c r="E1141"/>
       <c r="F1141"/>
-    </row>
-    <row r="1142" spans="2:6">
+      <c r="G1141"/>
+    </row>
+    <row r="1142" spans="2:7">
       <c r="B1142"/>
       <c r="C1142"/>
       <c r="D1142"/>
       <c r="E1142"/>
       <c r="F1142"/>
-    </row>
-    <row r="1143" spans="2:6">
+      <c r="G1142"/>
+    </row>
+    <row r="1143" spans="2:7">
       <c r="B1143"/>
       <c r="C1143"/>
       <c r="D1143"/>
       <c r="E1143"/>
       <c r="F1143"/>
-    </row>
-    <row r="1144" spans="2:6">
+      <c r="G1143"/>
+    </row>
+    <row r="1144" spans="2:7">
       <c r="B1144"/>
       <c r="C1144"/>
       <c r="D1144"/>
       <c r="E1144"/>
       <c r="F1144"/>
-    </row>
-    <row r="1145" spans="2:6">
+      <c r="G1144"/>
+    </row>
+    <row r="1145" spans="2:7">
       <c r="B1145"/>
       <c r="C1145"/>
       <c r="D1145"/>
       <c r="E1145"/>
       <c r="F1145"/>
-    </row>
-    <row r="1146" spans="2:6">
+      <c r="G1145"/>
+    </row>
+    <row r="1146" spans="2:7">
       <c r="B1146"/>
       <c r="C1146"/>
       <c r="D1146"/>
       <c r="E1146"/>
       <c r="F1146"/>
-    </row>
-    <row r="1147" spans="2:6">
+      <c r="G1146"/>
+    </row>
+    <row r="1147" spans="2:7">
       <c r="B1147"/>
       <c r="C1147"/>
       <c r="D1147"/>
       <c r="E1147"/>
       <c r="F1147"/>
-    </row>
-    <row r="1148" spans="2:6">
+      <c r="G1147"/>
+    </row>
+    <row r="1148" spans="2:7">
       <c r="B1148"/>
       <c r="C1148"/>
       <c r="D1148"/>
       <c r="E1148"/>
       <c r="F1148"/>
-    </row>
-    <row r="1149" spans="2:6">
+      <c r="G1148"/>
+    </row>
+    <row r="1149" spans="2:7">
       <c r="B1149"/>
       <c r="C1149"/>
       <c r="D1149"/>
       <c r="E1149"/>
       <c r="F1149"/>
-    </row>
-    <row r="1150" spans="2:6">
+      <c r="G1149"/>
+    </row>
+    <row r="1150" spans="2:7">
       <c r="B1150"/>
       <c r="C1150"/>
       <c r="D1150"/>
       <c r="E1150"/>
       <c r="F1150"/>
-    </row>
-    <row r="1151" spans="2:6">
+      <c r="G1150"/>
+    </row>
+    <row r="1151" spans="2:7">
       <c r="B1151"/>
       <c r="C1151"/>
       <c r="D1151"/>
       <c r="E1151"/>
       <c r="F1151"/>
-    </row>
-    <row r="1152" spans="2:6">
+      <c r="G1151"/>
+    </row>
+    <row r="1152" spans="2:7">
       <c r="B1152"/>
       <c r="C1152"/>
       <c r="D1152"/>
       <c r="E1152"/>
       <c r="F1152"/>
-    </row>
-    <row r="1153" spans="2:6">
+      <c r="G1152"/>
+    </row>
+    <row r="1153" spans="2:7">
       <c r="B1153"/>
       <c r="C1153"/>
       <c r="D1153"/>
       <c r="E1153"/>
       <c r="F1153"/>
-    </row>
-    <row r="1154" spans="2:6">
+      <c r="G1153"/>
+    </row>
+    <row r="1154" spans="2:7">
       <c r="B1154"/>
       <c r="C1154"/>
       <c r="D1154"/>
       <c r="E1154"/>
       <c r="F1154"/>
-    </row>
-    <row r="1155" spans="2:6">
+      <c r="G1154"/>
+    </row>
+    <row r="1155" spans="2:7">
       <c r="B1155"/>
       <c r="C1155"/>
       <c r="D1155"/>
       <c r="E1155"/>
       <c r="F1155"/>
-    </row>
-    <row r="1156" spans="2:6">
+      <c r="G1155"/>
+    </row>
+    <row r="1156" spans="2:7">
       <c r="B1156"/>
       <c r="C1156"/>
       <c r="D1156"/>
       <c r="E1156"/>
       <c r="F1156"/>
-    </row>
-    <row r="1157" spans="2:6">
+      <c r="G1156"/>
+    </row>
+    <row r="1157" spans="2:7">
       <c r="B1157"/>
       <c r="C1157"/>
       <c r="D1157"/>
       <c r="E1157"/>
       <c r="F1157"/>
-    </row>
-    <row r="1158" spans="2:6">
+      <c r="G1157"/>
+    </row>
+    <row r="1158" spans="2:7">
       <c r="B1158"/>
       <c r="C1158"/>
       <c r="D1158"/>
       <c r="E1158"/>
       <c r="F1158"/>
-    </row>
-    <row r="1159" spans="2:6">
+      <c r="G1158"/>
+    </row>
+    <row r="1159" spans="2:7">
       <c r="B1159"/>
       <c r="C1159"/>
       <c r="D1159"/>
       <c r="E1159"/>
       <c r="F1159"/>
-    </row>
-    <row r="1160" spans="2:6">
+      <c r="G1159"/>
+    </row>
+    <row r="1160" spans="2:7">
       <c r="B1160"/>
       <c r="C1160"/>
       <c r="D1160"/>
       <c r="E1160"/>
       <c r="F1160"/>
-    </row>
-    <row r="1161" spans="2:6">
+      <c r="G1160"/>
+    </row>
+    <row r="1161" spans="2:7">
       <c r="B1161"/>
       <c r="C1161"/>
       <c r="D1161"/>
       <c r="E1161"/>
       <c r="F1161"/>
+      <c r="G1161"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11680,8 +11836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA1207"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="Y13" sqref="Y13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Adding plyr to bbleadin and updating tab names in one file
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="860" windowWidth="18640" windowHeight="15420" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="2520" yWindow="0" windowWidth="17700" windowHeight="19600" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
     <sheet name="weinberger" sheetId="13" r:id="rId2"/>
-    <sheet name="OSPREE_7Dec2018" sheetId="6" r:id="rId3"/>
+    <sheet name="OSPREE_after6Dec2018" sheetId="6" r:id="rId3"/>
     <sheet name="OSPREE_compare_ALL (4 Dec 2018)" sheetId="12" r:id="rId4"/>
     <sheet name="OSPREE_compare" sheetId="4" r:id="rId5"/>
     <sheet name="Flynn_exp" sheetId="2" r:id="rId6"/>
@@ -3239,9 +3239,6 @@
     <t>But actually we think this is an issue with Nacho's compilation, the few that Lizzie tried run fine.</t>
   </si>
   <si>
-    <t>After all this we decided a few things (see comparing models on OSPREE wiki) and moved on with just the model with no interactions and no study, see OSPREE_7Dec2018 tab for that.</t>
-  </si>
-  <si>
     <t>weinberger_fewint</t>
   </si>
   <si>
@@ -3276,6 +3273,9 @@
   </si>
   <si>
     <t>m2l.nib</t>
+  </si>
+  <si>
+    <t>After all this we decided a few things (see comparing models on OSPREE wiki) and moved on with just the model with no interactions and no study, see OSPREE_after6Dec2018 tab for that.</t>
   </si>
 </sst>
 </file>
@@ -3339,7 +3339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3355,6 +3355,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3775,7 +3781,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3838,6 +3844,7 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="325">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -4504,7 +4511,7 @@
   <dimension ref="A1:H72"/>
   <sheetViews>
     <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+      <selection activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4821,12 +4828,12 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>1045</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
     </row>
   </sheetData>
@@ -4844,8 +4851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F13:F16"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4855,73 +4862,97 @@
         <v>212</v>
       </c>
       <c r="B1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="C1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D1" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="E1" t="s">
-        <v>1046</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1052</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1052</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1052</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1052</v>
-      </c>
+        <v>1045</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>1051</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>1051</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>217</v>
       </c>
       <c r="B3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C3" t="s">
         <v>1054</v>
       </c>
-      <c r="C3" t="s">
-        <v>1055</v>
-      </c>
       <c r="D3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="E3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F3" s="38" t="s">
         <v>1053</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" s="38" t="s">
         <v>1054</v>
       </c>
-      <c r="G3" t="s">
-        <v>1055</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1051</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1053</v>
+      <c r="H3" s="38" t="s">
+        <v>1050</v>
+      </c>
+      <c r="I3" s="38" t="s">
+        <v>1052</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>221</v>
       </c>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>280</v>
       </c>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>224</v>
       </c>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
@@ -4939,16 +4970,16 @@
       <c r="E8">
         <v>1034</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="38">
         <v>1556</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="38">
         <v>1356</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="38">
         <v>1230</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="38">
         <v>1034</v>
       </c>
     </row>
@@ -4968,18 +4999,36 @@
       <c r="E9">
         <v>28</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="38">
         <v>37</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="38">
         <v>37</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="38">
         <v>28</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="38">
         <v>28</v>
       </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="21" t="s">
@@ -4997,16 +5046,16 @@
       <c r="E13">
         <v>27.9</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="38">
         <v>31.2</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="38">
         <v>30.5</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="38">
         <v>32</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="38">
         <v>31.9</v>
       </c>
     </row>
@@ -5026,16 +5075,16 @@
       <c r="E14">
         <v>0.7</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="38">
         <v>-4.3</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="38">
         <v>-1.9</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="38">
         <v>-3.7</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="38">
         <v>-1.7</v>
       </c>
     </row>
@@ -5055,16 +5104,16 @@
       <c r="E15">
         <v>-3.9</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="38">
         <v>-2.1</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="38">
         <v>-1.5</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="38">
         <v>-2.1</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="38">
         <v>-1.4</v>
       </c>
     </row>
@@ -5084,22 +5133,22 @@
       <c r="E16">
         <v>-13.9</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="38">
         <v>-8.1</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="38">
         <v>-7.2</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="38">
         <v>-8.1999999999999993</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="38">
         <v>-7.3</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="21" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B17">
         <v>2.4</v>
@@ -5113,22 +5162,22 @@
       <c r="E17">
         <v>4.4000000000000004</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="38">
         <v>-0.7</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="38">
         <v>-1.3</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="38">
         <v>-0.2</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="38">
         <v>-1.2</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B18">
         <v>4.8</v>
@@ -5142,22 +5191,22 @@
       <c r="E18">
         <v>5.6</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="38">
         <v>-1.8</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="38">
         <v>-3.1</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="38">
         <v>-0.6</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="38">
         <v>-2</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B19">
         <v>-0.05</v>
@@ -5171,22 +5220,22 @@
       <c r="E19">
         <v>0.6</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="38">
         <v>-0.4</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="38">
         <v>-0.9</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="38">
         <v>-1.4</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="38">
         <v>-1.7</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="B20">
         <v>0.08</v>
@@ -5200,16 +5249,16 @@
       <c r="E20">
         <v>-1.9</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="38">
         <v>-1</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="38">
         <v>-4</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="38">
         <v>1.2</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="38">
         <v>-1.7</v>
       </c>
     </row>
@@ -5229,7 +5278,7 @@
   <dimension ref="A1:R1161"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5256,7 +5305,7 @@
         <v>992</v>
       </c>
       <c r="C1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>1</v>

</xml_diff>

<commit_message>
adding chillport models too bb_compre
no crops and crops, both with sp complex and expramp.fp
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="0" windowWidth="17700" windowHeight="19600" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="902" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
     <sheet name="weinberger" sheetId="13" r:id="rId2"/>
-    <sheet name="OSPREE_after6Dec2018" sheetId="6" r:id="rId3"/>
-    <sheet name="OSPREE_compare_ALL (4 Dec 2018)" sheetId="12" r:id="rId4"/>
-    <sheet name="OSPREE_compare" sheetId="4" r:id="rId5"/>
-    <sheet name="Flynn_exp" sheetId="2" r:id="rId6"/>
-    <sheet name="2018NovEarly_Lizzie" sheetId="5" r:id="rId7"/>
-    <sheet name="2018Jun-Aug_LizzieAilene" sheetId="1" r:id="rId8"/>
+    <sheet name="chillportmods" sheetId="14" r:id="rId3"/>
+    <sheet name="OSPREE_after6Dec2018" sheetId="6" r:id="rId4"/>
+    <sheet name="OSPREE_compare_ALL (4 Dec 2018)" sheetId="12" r:id="rId5"/>
+    <sheet name="OSPREE_compare" sheetId="4" r:id="rId6"/>
+    <sheet name="Flynn_exp" sheetId="2" r:id="rId7"/>
+    <sheet name="2018NovEarly_Lizzie" sheetId="5" r:id="rId8"/>
+    <sheet name="2018Jun-Aug_LizzieAilene" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3981" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4007" uniqueCount="1060">
   <si>
     <t>param</t>
   </si>
@@ -3276,6 +3277,12 @@
   </si>
   <si>
     <t>After all this we decided a few things (see comparing models on OSPREE wiki) and moved on with just the model with no interactions and no study, see OSPREE_after6Dec2018 tab for that.</t>
+  </si>
+  <si>
+    <t>chillports</t>
+  </si>
+  <si>
+    <t>spcomplex, allcrops</t>
   </si>
 </sst>
 </file>
@@ -5275,9 +5282,214 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" t="s">
+        <v>992</v>
+      </c>
+      <c r="C1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="21" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>1058</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1059</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>214</v>
+      </c>
+      <c r="B8">
+        <v>1556</v>
+      </c>
+      <c r="C8">
+        <v>1807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9">
+        <v>37</v>
+      </c>
+      <c r="C9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>31.66</v>
+      </c>
+      <c r="C13">
+        <v>29.81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>-4.47</v>
+      </c>
+      <c r="C14">
+        <v>-3.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>-3.18</v>
+      </c>
+      <c r="C15">
+        <v>-3.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>-9.11</v>
+      </c>
+      <c r="C16">
+        <v>-9.0299999999999994</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="21"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18">
+        <v>10.66</v>
+      </c>
+      <c r="C18">
+        <v>10.56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19">
+        <v>6.02</v>
+      </c>
+      <c r="C19">
+        <v>6.49</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20">
+        <v>4.16</v>
+      </c>
+      <c r="C20">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21">
+        <v>7.5</v>
+      </c>
+      <c r="C21">
+        <v>7.57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22">
+        <v>15.85</v>
+      </c>
+      <c r="C22">
+        <v>15.43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -11881,7 +12093,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BA1207"/>
   <sheetViews>
@@ -63216,7 +63428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M1187"/>
   <sheetViews>
@@ -78173,7 +78385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -78365,7 +78577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:N39"/>
   <sheetViews>
@@ -79279,7 +79491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R177"/>
   <sheetViews>

</xml_diff>

<commit_message>
added some weinberger R2s to model compare
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="902" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30580" windowHeight="16060" tabRatio="902" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4007" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4009" uniqueCount="1062">
   <si>
     <t>param</t>
   </si>
@@ -3283,6 +3283,12 @@
   </si>
   <si>
     <t>spcomplex, allcrops</t>
+  </si>
+  <si>
+    <t>R^2</t>
+  </si>
+  <si>
+    <t>all run with chill portions</t>
   </si>
 </sst>
 </file>
@@ -4858,11 +4864,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
+    <col min="9" max="9" width="33.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="18" t="s">
@@ -4950,6 +4965,9 @@
       <c r="A6" t="s">
         <v>224</v>
       </c>
+      <c r="B6" t="s">
+        <v>1061</v>
+      </c>
       <c r="F6" s="38"/>
       <c r="G6" s="38"/>
       <c r="H6" s="38"/>
@@ -5020,8 +5038,21 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
+      <c r="A10" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B10">
+        <v>0.59560000000000002</v>
+      </c>
+      <c r="C10">
+        <v>0.57750000000000001</v>
+      </c>
+      <c r="F10" s="38">
+        <v>0.442</v>
+      </c>
+      <c r="G10" s="38">
+        <v>0.42870000000000003</v>
+      </c>
       <c r="H10" s="38"/>
       <c r="I10" s="38"/>
     </row>
@@ -5284,7 +5315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Easing back into work ....
Small updates to models, slowly marching toward my plot tasks.
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19440" yWindow="0" windowWidth="29820" windowHeight="24340" tabRatio="902" activeTab="3"/>
+    <workbookView xWindow="7480" yWindow="2320" windowWidth="25600" windowHeight="16000" tabRatio="902" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4084" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4095" uniqueCount="1070">
   <si>
     <t>param</t>
   </si>
@@ -3310,6 +3310,9 @@
   </si>
   <si>
     <t>5 divergent transitions; intercept chains wandering</t>
+  </si>
+  <si>
+    <t>many (&gt;5K) divegernt transitions; intercept chains wandering</t>
   </si>
 </sst>
 </file>
@@ -3494,8 +3497,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="377">
+  <cellStyleXfs count="387">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3944,7 +3957,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="377">
+  <cellStyles count="387">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4133,6 +4146,11 @@
     <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4321,6 +4339,11 @@
     <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5682,29 +5705,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA1164"/>
+  <dimension ref="A1:AC1164"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="17.1640625" customWidth="1"/>
-    <col min="11" max="16" width="18.5" style="21" customWidth="1"/>
-    <col min="17" max="17" width="17.1640625" customWidth="1"/>
-    <col min="18" max="18" width="15" customWidth="1"/>
-    <col min="19" max="19" width="13.5" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" customWidth="1"/>
-    <col min="21" max="21" width="13.1640625" customWidth="1"/>
-    <col min="22" max="22" width="11.83203125" customWidth="1"/>
-    <col min="23" max="23" width="15.5" customWidth="1"/>
-    <col min="24" max="24" width="12.6640625" customWidth="1"/>
-    <col min="25" max="25" width="14.33203125" customWidth="1"/>
-    <col min="26" max="27" width="10.83203125" style="19"/>
+    <col min="1" max="12" width="17.1640625" customWidth="1"/>
+    <col min="13" max="18" width="18.5" style="21" customWidth="1"/>
+    <col min="19" max="19" width="17.1640625" customWidth="1"/>
+    <col min="20" max="20" width="15" customWidth="1"/>
+    <col min="21" max="21" width="13.5" customWidth="1"/>
+    <col min="22" max="22" width="13.6640625" customWidth="1"/>
+    <col min="23" max="23" width="13.1640625" customWidth="1"/>
+    <col min="24" max="24" width="11.83203125" customWidth="1"/>
+    <col min="25" max="25" width="15.5" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" customWidth="1"/>
+    <col min="27" max="27" width="14.33203125" customWidth="1"/>
+    <col min="28" max="29" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="18" customFormat="1">
+    <row r="1" spans="1:22" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
         <v>212</v>
       </c>
@@ -5727,41 +5750,47 @@
         <v>1</v>
       </c>
       <c r="H1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="18" t="s">
         <v>976</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>976</v>
       </c>
-      <c r="J1"/>
-      <c r="K1" t="s">
+      <c r="L1"/>
+      <c r="M1" t="s">
         <v>992</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>1054</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="O1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="17" t="s">
-        <v>992</v>
-      </c>
-      <c r="O1" t="s">
-        <v>992</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="P1" s="17" t="s">
         <v>992</v>
       </c>
       <c r="Q1" t="s">
         <v>992</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" t="s">
+        <v>992</v>
+      </c>
+      <c r="S1" t="s">
+        <v>992</v>
+      </c>
+      <c r="T1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="18" t="s">
+      <c r="U1" s="18" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="18" customFormat="1">
+    <row r="2" spans="1:22" s="18" customFormat="1">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -5773,12 +5802,14 @@
       <c r="J2"/>
       <c r="K2"/>
       <c r="L2"/>
-      <c r="N2" s="17"/>
-      <c r="O2"/>
-      <c r="P2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="P2" s="17"/>
       <c r="Q2"/>
-    </row>
-    <row r="3" spans="1:20" s="40" customFormat="1">
+      <c r="R2"/>
+      <c r="S2"/>
+    </row>
+    <row r="3" spans="1:22" s="40" customFormat="1">
       <c r="A3" s="40" t="s">
         <v>1066</v>
       </c>
@@ -5795,12 +5826,14 @@
       <c r="J3" s="41"/>
       <c r="K3" s="41"/>
       <c r="L3" s="41"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="P3" s="42"/>
       <c r="Q3" s="41"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="R3" s="41"/>
+      <c r="S3" s="41"/>
+    </row>
+    <row r="4" spans="1:22">
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -5810,10 +5843,12 @@
       <c r="H4" s="21"/>
       <c r="I4" s="21"/>
       <c r="J4" s="21"/>
-      <c r="N4" s="22"/>
-      <c r="Q4" s="21"/>
-    </row>
-    <row r="5" spans="1:20">
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="P4" s="22"/>
+      <c r="S4" s="21"/>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -5841,18 +5876,18 @@
       <c r="I5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="J5" s="21"/>
+      <c r="J5" s="21" t="s">
+        <v>1032</v>
+      </c>
       <c r="K5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="L5" s="21" t="s">
-        <v>1032</v>
-      </c>
+      <c r="L5" s="21"/>
       <c r="M5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="N5" s="22" t="s">
-        <v>1034</v>
+      <c r="N5" s="21" t="s">
+        <v>1032</v>
       </c>
       <c r="O5" s="21" t="s">
         <v>1032</v>
@@ -5863,15 +5898,21 @@
       <c r="Q5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="R5" s="21" t="s">
-        <v>1032</v>
+      <c r="R5" s="22" t="s">
+        <v>1034</v>
       </c>
       <c r="S5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="T5" s="21"/>
-    </row>
-    <row r="6" spans="1:20">
+      <c r="T5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="U5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="V5" s="21"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>221</v>
       </c>
@@ -5899,37 +5940,43 @@
       <c r="I6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="J6" s="21"/>
+      <c r="J6" s="21" t="s">
+        <v>1031</v>
+      </c>
       <c r="K6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="L6" s="21" t="s">
-        <v>1031</v>
-      </c>
+      <c r="L6" s="21"/>
       <c r="M6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="N6" s="22" t="s">
+      <c r="N6" s="21" t="s">
         <v>1031</v>
       </c>
       <c r="O6" s="21" t="s">
+        <v>1031</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>1031</v>
+      </c>
+      <c r="Q6" s="21" t="s">
         <v>1035</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="R6" s="21" t="s">
         <v>1035</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="S6" s="21" t="s">
         <v>1033</v>
       </c>
-      <c r="R6" s="22" t="s">
+      <c r="T6" s="22" t="s">
         <v>1036</v>
       </c>
-      <c r="S6" s="22" t="s">
+      <c r="U6" s="22" t="s">
         <v>1036</v>
       </c>
-      <c r="T6" s="21"/>
-    </row>
-    <row r="7" spans="1:20">
+      <c r="V6" s="21"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>280</v>
       </c>
@@ -5944,16 +5991,14 @@
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
-      <c r="I7" s="21" t="s">
+      <c r="I7" s="21"/>
+      <c r="J7" t="s">
+        <v>1069</v>
+      </c>
+      <c r="K7" s="21" t="s">
         <v>1068</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>281</v>
-      </c>
+      <c r="L7" s="21"/>
       <c r="M7" s="21" t="s">
         <v>281</v>
       </c>
@@ -5975,17 +6020,17 @@
       <c r="S7" s="21" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="8" spans="1:20">
+      <c r="T7" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="U7" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>224</v>
       </c>
-      <c r="K8" s="21" t="s">
-        <v>1064</v>
-      </c>
-      <c r="L8" s="21" t="s">
-        <v>1064</v>
-      </c>
       <c r="M8" s="21" t="s">
         <v>1064</v>
       </c>
@@ -6004,11 +6049,17 @@
       <c r="R8" s="21" t="s">
         <v>1064</v>
       </c>
-      <c r="S8" t="s">
+      <c r="S8" s="21" t="s">
+        <v>1064</v>
+      </c>
+      <c r="T8" s="21" t="s">
+        <v>1064</v>
+      </c>
+      <c r="U8" t="s">
         <v>1065</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>1063</v>
       </c>
@@ -6034,15 +6085,15 @@
         <v>1056</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>1062</v>
-      </c>
-      <c r="J9" s="21"/>
+        <v>1056</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>1056</v>
+      </c>
       <c r="K9" s="21" t="s">
         <v>1062</v>
       </c>
-      <c r="L9" s="21" t="s">
-        <v>1062</v>
-      </c>
+      <c r="L9" s="21"/>
       <c r="M9" s="21" t="s">
         <v>1062</v>
       </c>
@@ -6064,8 +6115,14 @@
       <c r="S9" s="21" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="11" spans="1:20">
+      <c r="T9" s="21" t="s">
+        <v>1062</v>
+      </c>
+      <c r="U9" s="21" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>214</v>
       </c>
@@ -6091,37 +6148,43 @@
         <v>1524</v>
       </c>
       <c r="I11">
+        <v>2497</v>
+      </c>
+      <c r="J11">
+        <v>2497</v>
+      </c>
+      <c r="K11">
         <v>1524</v>
-      </c>
-      <c r="K11" s="23">
-        <v>1556</v>
-      </c>
-      <c r="L11" s="23">
-        <v>1556</v>
       </c>
       <c r="M11" s="23">
         <v>1556</v>
       </c>
       <c r="N11" s="23">
+        <v>1556</v>
+      </c>
+      <c r="O11" s="23">
+        <v>1556</v>
+      </c>
+      <c r="P11" s="23">
         <v>1097</v>
       </c>
-      <c r="O11" s="23">
+      <c r="Q11" s="23">
         <v>2651</v>
       </c>
-      <c r="P11" s="23">
+      <c r="R11" s="23">
         <v>2112</v>
       </c>
-      <c r="Q11" s="23">
+      <c r="S11" s="23">
         <v>1953</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>1556</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>1556</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>211</v>
       </c>
@@ -6147,52 +6210,58 @@
         <v>37</v>
       </c>
       <c r="I12">
-        <v>37</v>
-      </c>
-      <c r="K12" s="23">
-        <v>37</v>
-      </c>
-      <c r="L12" s="23">
+        <v>199</v>
+      </c>
+      <c r="J12">
+        <v>199</v>
+      </c>
+      <c r="K12">
         <v>37</v>
       </c>
       <c r="M12" s="23">
         <v>37</v>
       </c>
       <c r="N12" s="23">
+        <v>37</v>
+      </c>
+      <c r="O12" s="23">
+        <v>37</v>
+      </c>
+      <c r="P12" s="23">
         <v>25</v>
       </c>
-      <c r="O12" s="23">
+      <c r="Q12" s="23">
         <v>200</v>
       </c>
-      <c r="P12" s="23">
+      <c r="R12" s="23">
         <v>179</v>
       </c>
-      <c r="Q12" s="23">
+      <c r="S12" s="23">
         <v>41</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>37</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>37</v>
       </c>
-      <c r="T12" s="23"/>
-    </row>
-    <row r="13" spans="1:20">
+      <c r="V12" s="23"/>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>213</v>
       </c>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
       <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
       <c r="P13" s="23"/>
-      <c r="S13">
+      <c r="Q13" s="23"/>
+      <c r="R13" s="23"/>
+      <c r="U13">
         <v>30</v>
       </c>
-      <c r="T13" s="23"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="V13" s="23"/>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -6212,7 +6281,7 @@
         <v>216</v>
       </c>
       <c r="G14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="H14" t="s">
         <v>216</v>
@@ -6220,10 +6289,10 @@
       <c r="I14" t="s">
         <v>216</v>
       </c>
-      <c r="K14" s="23" t="s">
+      <c r="J14" t="s">
         <v>216</v>
       </c>
-      <c r="L14" s="23" t="s">
+      <c r="K14" t="s">
         <v>216</v>
       </c>
       <c r="M14" s="23" t="s">
@@ -6247,8 +6316,14 @@
       <c r="S14" s="23" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" s="21" customFormat="1">
+      <c r="T14" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="U14" s="23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" s="21" customFormat="1">
       <c r="A16" s="21" t="s">
         <v>5</v>
       </c>
@@ -6268,51 +6343,63 @@
         <v>30.584579999999999</v>
       </c>
       <c r="G16" s="21">
+        <v>64.962770178</v>
+      </c>
+      <c r="H16" s="21">
         <v>30.721707769999998</v>
       </c>
       <c r="I16" s="21">
+        <v>30.754858800000001</v>
+      </c>
+      <c r="J16" s="21">
+        <v>13.436368399999999</v>
+      </c>
+      <c r="K16" s="21">
         <v>11.977791</v>
       </c>
-      <c r="K16" s="21">
+      <c r="M16" s="21">
         <v>30.877478</v>
       </c>
-      <c r="L16" s="21">
+      <c r="N16" s="21">
         <v>30.66</v>
       </c>
-      <c r="M16" s="21">
+      <c r="O16" s="21">
         <v>31.211466999999999</v>
       </c>
-      <c r="N16" s="21">
+      <c r="P16" s="21">
         <v>31.880268000000001</v>
       </c>
-      <c r="O16" s="21">
+      <c r="Q16" s="21">
         <v>30.716964999999998</v>
       </c>
-      <c r="P16" s="21">
+      <c r="R16" s="21">
         <v>29.746556000000002</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="S16" s="21">
         <v>29.076453999999998</v>
       </c>
-      <c r="R16" s="21">
+      <c r="T16" s="21">
         <v>29.443950000000001</v>
       </c>
-      <c r="S16" s="21">
+      <c r="U16" s="21">
         <v>11.154477999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="21" customFormat="1">
+    <row r="17" spans="1:21" s="21" customFormat="1">
       <c r="A17" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="I17" s="21">
+      <c r="J17" s="21">
+        <v>8.5977074000000009</v>
+      </c>
+      <c r="K17" s="21">
         <v>12.778447999999999</v>
       </c>
-      <c r="S17" s="21">
+      <c r="U17" s="21">
         <v>17.8</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="21" customFormat="1" ht="14" customHeight="1">
+    <row r="18" spans="1:21" s="21" customFormat="1" ht="14" customHeight="1">
       <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
@@ -6332,40 +6419,49 @@
         <v>-5.8981399999999997</v>
       </c>
       <c r="G18" s="21">
+        <v>-0.43686686800000002</v>
+      </c>
+      <c r="H18" s="21">
         <v>-4.6886315600000001</v>
       </c>
       <c r="I18" s="21">
+        <v>-3.2696827000000002</v>
+      </c>
+      <c r="J18" s="21">
+        <v>-8.0795293000000008</v>
+      </c>
+      <c r="K18" s="21">
         <v>-10.718495000000001</v>
       </c>
-      <c r="K18" s="21">
+      <c r="M18" s="21">
         <v>-3.858498</v>
       </c>
-      <c r="L18" s="21">
+      <c r="N18" s="21">
         <v>-4.7</v>
       </c>
-      <c r="M18" s="21">
+      <c r="O18" s="21">
         <v>-3.9753639999999999</v>
       </c>
-      <c r="N18" s="21">
+      <c r="P18" s="21">
         <v>-6.589467</v>
       </c>
-      <c r="O18" s="21">
+      <c r="Q18" s="21">
         <v>-4.670153</v>
       </c>
-      <c r="P18" s="21">
+      <c r="R18" s="21">
         <v>-6.3059329999999996</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="S18" s="21">
         <v>-4.2054489999999998</v>
       </c>
-      <c r="R18" s="21">
+      <c r="T18" s="21">
         <v>-4.4239769999999998</v>
       </c>
-      <c r="S18" s="21">
+      <c r="U18" s="21">
         <v>-11.179836</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="21" customFormat="1">
+    <row r="19" spans="1:21" s="21" customFormat="1">
       <c r="A19" s="21" t="s">
         <v>8</v>
       </c>
@@ -6385,40 +6481,49 @@
         <v>-1.7522850000000001</v>
       </c>
       <c r="G19" s="21">
+        <v>-0.59282655500000003</v>
+      </c>
+      <c r="H19" s="21">
         <v>-3.2544300800000001</v>
       </c>
       <c r="I19" s="21">
+        <v>-2.0773652</v>
+      </c>
+      <c r="J19" s="21">
+        <v>-0.73294579999999998</v>
+      </c>
+      <c r="K19" s="21">
         <v>-1.3810519999999999</v>
       </c>
-      <c r="K19" s="21">
+      <c r="M19" s="21">
         <v>-3.1080649999999999</v>
       </c>
-      <c r="L19" s="21">
+      <c r="N19" s="21">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="M19" s="21">
+      <c r="O19" s="21">
         <v>-3.5504150000000001</v>
       </c>
-      <c r="N19" s="21">
+      <c r="P19" s="21">
         <v>-2.3749199999999999</v>
       </c>
-      <c r="O19" s="21">
+      <c r="Q19" s="21">
         <v>-1.740626</v>
       </c>
-      <c r="P19" s="21">
+      <c r="R19" s="21">
         <v>-1.149972</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="S19" s="21">
         <v>-3.8012999999999999</v>
       </c>
-      <c r="R19" s="21">
+      <c r="T19" s="21">
         <v>-4.6329729999999998</v>
       </c>
-      <c r="S19" s="21">
+      <c r="U19" s="21">
         <v>-1.4</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="21" customFormat="1">
+    <row r="20" spans="1:21" s="21" customFormat="1">
       <c r="A20" s="21" t="s">
         <v>9</v>
       </c>
@@ -6438,111 +6543,141 @@
         <v>-7.6310460000000004</v>
       </c>
       <c r="G20" s="21">
+        <v>-0.28852171599999998</v>
+      </c>
+      <c r="H20" s="21">
         <v>-8.3550094300000008</v>
       </c>
       <c r="I20" s="21">
+        <v>-7.0728663999999997</v>
+      </c>
+      <c r="J20" s="21">
+        <v>-8.4076094999999995</v>
+      </c>
+      <c r="K20" s="21">
         <v>-9.5678230000000006</v>
       </c>
-      <c r="K20" s="21">
+      <c r="M20" s="21">
         <v>-10.069042</v>
       </c>
-      <c r="L20" s="21">
+      <c r="N20" s="21">
         <v>-8.5</v>
       </c>
-      <c r="M20" s="21">
+      <c r="O20" s="21">
         <v>-10.401221</v>
       </c>
-      <c r="N20" s="21">
+      <c r="P20" s="21">
         <v>-9.9066620000000007</v>
       </c>
-      <c r="O20" s="21">
+      <c r="Q20" s="21">
         <v>-8.6652190000000004</v>
       </c>
-      <c r="P20" s="21">
+      <c r="R20" s="21">
         <v>-9.8209820000000008</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="S20" s="21">
         <v>-10.442672999999999</v>
       </c>
-      <c r="R20" s="21">
+      <c r="T20" s="21">
         <v>-10.520892</v>
       </c>
-      <c r="S20" s="21">
+      <c r="U20" s="21">
         <v>-9.7576470000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:21">
       <c r="A21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:21">
       <c r="A22" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:21">
       <c r="A23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:21">
       <c r="A24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:21">
       <c r="A25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:21">
       <c r="A26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:21">
       <c r="A27" t="s">
         <v>210</v>
       </c>
-      <c r="I27">
+      <c r="J27">
+        <v>6.1738270000000002</v>
+      </c>
+      <c r="K27">
         <v>9.932563</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:21">
       <c r="A28" t="s">
         <v>10</v>
       </c>
       <c r="G28">
+        <v>-1.4379709999999999E-3</v>
+      </c>
+      <c r="H28">
         <v>-9.5536179999999998E-2</v>
       </c>
-      <c r="M28" s="21">
+      <c r="I28">
+        <v>0.15195020000000001</v>
+      </c>
+      <c r="O28" s="21">
         <v>1.47323</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:21">
       <c r="A29" t="s">
         <v>11</v>
       </c>
       <c r="G29">
+        <v>4.1001559999999998E-3</v>
+      </c>
+      <c r="H29">
         <v>0.85033303000000005</v>
       </c>
-      <c r="M29" s="21">
+      <c r="I29">
+        <v>1.3428956999999999</v>
+      </c>
+      <c r="O29" s="21">
         <v>1.0277529999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:21">
       <c r="A30" t="s">
         <v>12</v>
       </c>
       <c r="G30">
+        <v>-1.7003655999999999E-2</v>
+      </c>
+      <c r="H30">
         <v>-0.27255634000000001</v>
       </c>
-      <c r="M30" s="21">
+      <c r="I30">
+        <v>-0.39319349999999997</v>
+      </c>
+      <c r="O30" s="21">
         <v>-1.052503</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:21">
       <c r="A32" s="15" t="s">
         <v>972</v>
       </c>
@@ -6555,258 +6690,260 @@
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
       <c r="J32" s="15"/>
-    </row>
-    <row r="33" spans="1:17">
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+    </row>
+    <row r="33" spans="1:19">
       <c r="A33" t="s">
         <v>57</v>
       </c>
-      <c r="Q33" s="17"/>
-    </row>
-    <row r="34" spans="1:17">
+      <c r="S33" s="17"/>
+    </row>
+    <row r="34" spans="1:19">
       <c r="A34" t="s">
         <v>58</v>
       </c>
-      <c r="Q34" s="17"/>
-    </row>
-    <row r="35" spans="1:17">
+      <c r="S34" s="17"/>
+    </row>
+    <row r="35" spans="1:19">
       <c r="A35" t="s">
         <v>59</v>
       </c>
-      <c r="Q35" s="17"/>
-    </row>
-    <row r="36" spans="1:17">
+      <c r="S35" s="17"/>
+    </row>
+    <row r="36" spans="1:19">
       <c r="A36" t="s">
         <v>60</v>
       </c>
-      <c r="Q36" s="17"/>
-    </row>
-    <row r="37" spans="1:17">
+      <c r="S36" s="17"/>
+    </row>
+    <row r="37" spans="1:19">
       <c r="A37" t="s">
         <v>61</v>
       </c>
-      <c r="Q37" s="17"/>
-    </row>
-    <row r="38" spans="1:17">
+      <c r="S37" s="17"/>
+    </row>
+    <row r="38" spans="1:19">
       <c r="A38" t="s">
         <v>62</v>
       </c>
-      <c r="Q38" s="17"/>
-    </row>
-    <row r="39" spans="1:17">
+      <c r="S38" s="17"/>
+    </row>
+    <row r="39" spans="1:19">
       <c r="A39" t="s">
         <v>63</v>
       </c>
-      <c r="Q39" s="17"/>
-    </row>
-    <row r="40" spans="1:17">
+      <c r="S39" s="17"/>
+    </row>
+    <row r="40" spans="1:19">
       <c r="A40" t="s">
         <v>64</v>
       </c>
-      <c r="Q40" s="17"/>
-    </row>
-    <row r="41" spans="1:17">
+      <c r="S40" s="17"/>
+    </row>
+    <row r="41" spans="1:19">
       <c r="A41" t="s">
         <v>65</v>
       </c>
-      <c r="Q41" s="17"/>
-    </row>
-    <row r="42" spans="1:17">
+      <c r="S41" s="17"/>
+    </row>
+    <row r="42" spans="1:19">
       <c r="A42" t="s">
         <v>66</v>
       </c>
-      <c r="Q42" s="17"/>
-    </row>
-    <row r="43" spans="1:17">
+      <c r="S42" s="17"/>
+    </row>
+    <row r="43" spans="1:19">
       <c r="A43" t="s">
         <v>67</v>
       </c>
-      <c r="Q43" s="17"/>
-    </row>
-    <row r="44" spans="1:17">
+      <c r="S43" s="17"/>
+    </row>
+    <row r="44" spans="1:19">
       <c r="A44" t="s">
         <v>68</v>
       </c>
-      <c r="Q44" s="17"/>
-    </row>
-    <row r="45" spans="1:17">
+      <c r="S44" s="17"/>
+    </row>
+    <row r="45" spans="1:19">
       <c r="A45" t="s">
         <v>69</v>
       </c>
-      <c r="Q45" s="17"/>
-    </row>
-    <row r="46" spans="1:17">
+      <c r="S45" s="17"/>
+    </row>
+    <row r="46" spans="1:19">
       <c r="A46" t="s">
         <v>70</v>
       </c>
-      <c r="Q46" s="17"/>
-    </row>
-    <row r="47" spans="1:17">
+      <c r="S46" s="17"/>
+    </row>
+    <row r="47" spans="1:19">
       <c r="A47" t="s">
         <v>71</v>
       </c>
-      <c r="Q47" s="17"/>
-    </row>
-    <row r="48" spans="1:17">
+      <c r="S47" s="17"/>
+    </row>
+    <row r="48" spans="1:19">
       <c r="A48" t="s">
         <v>72</v>
       </c>
-      <c r="Q48" s="17"/>
-    </row>
-    <row r="49" spans="1:17">
+      <c r="S48" s="17"/>
+    </row>
+    <row r="49" spans="1:19">
       <c r="A49" t="s">
         <v>73</v>
       </c>
-      <c r="Q49" s="17"/>
-    </row>
-    <row r="50" spans="1:17">
+      <c r="S49" s="17"/>
+    </row>
+    <row r="50" spans="1:19">
       <c r="A50" t="s">
         <v>74</v>
       </c>
-      <c r="Q50" s="17"/>
-    </row>
-    <row r="51" spans="1:17">
+      <c r="S50" s="17"/>
+    </row>
+    <row r="51" spans="1:19">
       <c r="A51" t="s">
         <v>75</v>
       </c>
-      <c r="Q51" s="17"/>
-    </row>
-    <row r="52" spans="1:17">
+      <c r="S51" s="17"/>
+    </row>
+    <row r="52" spans="1:19">
       <c r="A52" t="s">
         <v>76</v>
       </c>
-      <c r="Q52" s="17"/>
-    </row>
-    <row r="53" spans="1:17">
+      <c r="S52" s="17"/>
+    </row>
+    <row r="53" spans="1:19">
       <c r="A53" t="s">
         <v>77</v>
       </c>
-      <c r="Q53" s="17"/>
-    </row>
-    <row r="54" spans="1:17">
+      <c r="S53" s="17"/>
+    </row>
+    <row r="54" spans="1:19">
       <c r="A54" t="s">
         <v>78</v>
       </c>
-      <c r="Q54" s="17"/>
-    </row>
-    <row r="55" spans="1:17">
+      <c r="S54" s="17"/>
+    </row>
+    <row r="55" spans="1:19">
       <c r="A55" t="s">
         <v>79</v>
       </c>
-      <c r="Q55" s="17"/>
-    </row>
-    <row r="56" spans="1:17">
+      <c r="S55" s="17"/>
+    </row>
+    <row r="56" spans="1:19">
       <c r="A56" t="s">
         <v>80</v>
       </c>
-      <c r="Q56" s="17"/>
-    </row>
-    <row r="57" spans="1:17">
+      <c r="S56" s="17"/>
+    </row>
+    <row r="57" spans="1:19">
       <c r="A57" t="s">
         <v>81</v>
       </c>
-      <c r="Q57" s="17"/>
-    </row>
-    <row r="58" spans="1:17">
+      <c r="S57" s="17"/>
+    </row>
+    <row r="58" spans="1:19">
       <c r="A58" t="s">
         <v>82</v>
       </c>
-      <c r="Q58" s="17"/>
-    </row>
-    <row r="59" spans="1:17">
+      <c r="S58" s="17"/>
+    </row>
+    <row r="59" spans="1:19">
       <c r="A59" t="s">
         <v>83</v>
       </c>
-      <c r="Q59" s="17"/>
-    </row>
-    <row r="60" spans="1:17">
+      <c r="S59" s="17"/>
+    </row>
+    <row r="60" spans="1:19">
       <c r="A60" t="s">
         <v>84</v>
       </c>
-      <c r="Q60" s="17"/>
-    </row>
-    <row r="61" spans="1:17">
+      <c r="S60" s="17"/>
+    </row>
+    <row r="61" spans="1:19">
       <c r="A61" t="s">
         <v>85</v>
       </c>
-      <c r="Q61" s="17"/>
-    </row>
-    <row r="62" spans="1:17">
+      <c r="S61" s="17"/>
+    </row>
+    <row r="62" spans="1:19">
       <c r="A62" t="s">
         <v>86</v>
       </c>
-      <c r="Q62" s="17"/>
-    </row>
-    <row r="63" spans="1:17">
+      <c r="S62" s="17"/>
+    </row>
+    <row r="63" spans="1:19">
       <c r="A63" t="s">
         <v>87</v>
       </c>
-      <c r="Q63" s="17"/>
-    </row>
-    <row r="64" spans="1:17">
+      <c r="S63" s="17"/>
+    </row>
+    <row r="64" spans="1:19">
       <c r="A64" t="s">
         <v>88</v>
       </c>
-      <c r="Q64" s="17"/>
-    </row>
-    <row r="65" spans="1:18">
+      <c r="S64" s="17"/>
+    </row>
+    <row r="65" spans="1:20">
       <c r="A65" t="s">
         <v>89</v>
       </c>
-      <c r="Q65" s="17"/>
-    </row>
-    <row r="66" spans="1:18">
+      <c r="S65" s="17"/>
+    </row>
+    <row r="66" spans="1:20">
       <c r="A66" t="s">
         <v>90</v>
       </c>
-      <c r="Q66" s="17"/>
-    </row>
-    <row r="67" spans="1:18">
+      <c r="S66" s="17"/>
+    </row>
+    <row r="67" spans="1:20">
       <c r="A67" t="s">
         <v>91</v>
       </c>
-      <c r="Q67" s="17"/>
-    </row>
-    <row r="68" spans="1:18">
+      <c r="S67" s="17"/>
+    </row>
+    <row r="68" spans="1:20">
       <c r="A68" t="s">
         <v>92</v>
       </c>
-      <c r="Q68" s="17"/>
-    </row>
-    <row r="69" spans="1:18">
+      <c r="S68" s="17"/>
+    </row>
+    <row r="69" spans="1:20">
       <c r="A69" t="s">
         <v>93</v>
       </c>
-      <c r="Q69" s="17"/>
-    </row>
-    <row r="70" spans="1:18">
+      <c r="S69" s="17"/>
+    </row>
+    <row r="70" spans="1:20">
       <c r="A70" t="s">
         <v>94</v>
       </c>
-      <c r="Q70" s="17"/>
-    </row>
-    <row r="71" spans="1:18">
-      <c r="K71" s="22"/>
-      <c r="L71" s="22"/>
+      <c r="S70" s="17"/>
+    </row>
+    <row r="71" spans="1:20">
       <c r="M71" s="22"/>
       <c r="N71" s="22"/>
       <c r="O71" s="22"/>
       <c r="P71" s="22"/>
-      <c r="Q71" s="17"/>
-      <c r="R71" s="17"/>
-    </row>
-    <row r="72" spans="1:18">
-      <c r="Q72" s="17"/>
-    </row>
-    <row r="73" spans="1:18">
-      <c r="Q73" s="17"/>
-    </row>
-    <row r="74" spans="1:18">
-      <c r="Q74" s="17"/>
-    </row>
-    <row r="75" spans="1:18">
-      <c r="Q75" s="17"/>
-    </row>
-    <row r="76" spans="1:18">
+      <c r="Q71" s="22"/>
+      <c r="R71" s="22"/>
+      <c r="S71" s="17"/>
+      <c r="T71" s="17"/>
+    </row>
+    <row r="72" spans="1:20">
+      <c r="S72" s="17"/>
+    </row>
+    <row r="73" spans="1:20">
+      <c r="S73" s="17"/>
+    </row>
+    <row r="74" spans="1:20">
+      <c r="S74" s="17"/>
+    </row>
+    <row r="75" spans="1:20">
+      <c r="S75" s="17"/>
+    </row>
+    <row r="76" spans="1:20">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -6817,733 +6954,735 @@
       <c r="H76" s="17"/>
       <c r="I76" s="17"/>
       <c r="J76" s="17"/>
-      <c r="Q76" s="17"/>
-    </row>
-    <row r="77" spans="1:18">
+      <c r="K76" s="17"/>
+      <c r="L76" s="17"/>
+      <c r="S76" s="17"/>
+    </row>
+    <row r="77" spans="1:20">
       <c r="A77" t="s">
         <v>171</v>
       </c>
-      <c r="Q77" s="17"/>
-    </row>
-    <row r="78" spans="1:18">
+      <c r="S77" s="17"/>
+    </row>
+    <row r="78" spans="1:20">
       <c r="A78" t="s">
         <v>172</v>
       </c>
-      <c r="Q78" s="17"/>
-    </row>
-    <row r="79" spans="1:18">
+      <c r="S78" s="17"/>
+    </row>
+    <row r="79" spans="1:20">
       <c r="A79" t="s">
         <v>173</v>
       </c>
-      <c r="Q79" s="17"/>
-    </row>
-    <row r="80" spans="1:18">
+      <c r="S79" s="17"/>
+    </row>
+    <row r="80" spans="1:20">
       <c r="A80" t="s">
         <v>174</v>
       </c>
-      <c r="Q80" s="17"/>
-    </row>
-    <row r="81" spans="1:17">
+      <c r="S80" s="17"/>
+    </row>
+    <row r="81" spans="1:19">
       <c r="A81" t="s">
         <v>175</v>
       </c>
-      <c r="Q81" s="17"/>
-    </row>
-    <row r="82" spans="1:17">
+      <c r="S81" s="17"/>
+    </row>
+    <row r="82" spans="1:19">
       <c r="A82" t="s">
         <v>176</v>
       </c>
-      <c r="Q82" s="17"/>
-    </row>
-    <row r="83" spans="1:17">
+      <c r="S82" s="17"/>
+    </row>
+    <row r="83" spans="1:19">
       <c r="A83" t="s">
         <v>177</v>
       </c>
-      <c r="Q83" s="17"/>
-    </row>
-    <row r="84" spans="1:17">
+      <c r="S83" s="17"/>
+    </row>
+    <row r="84" spans="1:19">
       <c r="A84" t="s">
         <v>178</v>
       </c>
-      <c r="Q84" s="17"/>
-    </row>
-    <row r="85" spans="1:17">
+      <c r="S84" s="17"/>
+    </row>
+    <row r="85" spans="1:19">
       <c r="A85" t="s">
         <v>179</v>
       </c>
-      <c r="Q85" s="17"/>
-    </row>
-    <row r="86" spans="1:17">
+      <c r="S85" s="17"/>
+    </row>
+    <row r="86" spans="1:19">
       <c r="A86" t="s">
         <v>180</v>
       </c>
-      <c r="Q86" s="17"/>
-    </row>
-    <row r="87" spans="1:17">
+      <c r="S86" s="17"/>
+    </row>
+    <row r="87" spans="1:19">
       <c r="A87" t="s">
         <v>181</v>
       </c>
-      <c r="Q87" s="17"/>
-    </row>
-    <row r="88" spans="1:17">
+      <c r="S87" s="17"/>
+    </row>
+    <row r="88" spans="1:19">
       <c r="A88" t="s">
         <v>182</v>
       </c>
-      <c r="Q88" s="17"/>
-    </row>
-    <row r="89" spans="1:17">
+      <c r="S88" s="17"/>
+    </row>
+    <row r="89" spans="1:19">
       <c r="A89" t="s">
         <v>183</v>
       </c>
-      <c r="Q89" s="17"/>
-    </row>
-    <row r="90" spans="1:17">
+      <c r="S89" s="17"/>
+    </row>
+    <row r="90" spans="1:19">
       <c r="A90" t="s">
         <v>184</v>
       </c>
-      <c r="Q90" s="17"/>
-    </row>
-    <row r="91" spans="1:17">
+      <c r="S90" s="17"/>
+    </row>
+    <row r="91" spans="1:19">
       <c r="A91" t="s">
         <v>185</v>
       </c>
-      <c r="Q91" s="17"/>
-    </row>
-    <row r="92" spans="1:17">
+      <c r="S91" s="17"/>
+    </row>
+    <row r="92" spans="1:19">
       <c r="A92" t="s">
         <v>186</v>
       </c>
-      <c r="Q92" s="17"/>
-    </row>
-    <row r="93" spans="1:17">
+      <c r="S92" s="17"/>
+    </row>
+    <row r="93" spans="1:19">
       <c r="A93" t="s">
         <v>187</v>
       </c>
-      <c r="Q93" s="17"/>
-    </row>
-    <row r="94" spans="1:17">
+      <c r="S93" s="17"/>
+    </row>
+    <row r="94" spans="1:19">
       <c r="A94" t="s">
         <v>188</v>
       </c>
-      <c r="Q94" s="17"/>
-    </row>
-    <row r="95" spans="1:17">
+      <c r="S94" s="17"/>
+    </row>
+    <row r="95" spans="1:19">
       <c r="A95" t="s">
         <v>189</v>
       </c>
-      <c r="Q95" s="17"/>
-    </row>
-    <row r="96" spans="1:17">
+      <c r="S95" s="17"/>
+    </row>
+    <row r="96" spans="1:19">
       <c r="A96" t="s">
         <v>190</v>
       </c>
-      <c r="Q96" s="17"/>
-    </row>
-    <row r="97" spans="1:17">
+      <c r="S96" s="17"/>
+    </row>
+    <row r="97" spans="1:19">
       <c r="A97" t="s">
         <v>191</v>
       </c>
-      <c r="Q97" s="17"/>
-    </row>
-    <row r="98" spans="1:17">
+      <c r="S97" s="17"/>
+    </row>
+    <row r="98" spans="1:19">
       <c r="A98" t="s">
         <v>192</v>
       </c>
-      <c r="Q98" s="17"/>
-    </row>
-    <row r="99" spans="1:17">
+      <c r="S98" s="17"/>
+    </row>
+    <row r="99" spans="1:19">
       <c r="A99" t="s">
         <v>193</v>
       </c>
-      <c r="Q99" s="17"/>
-    </row>
-    <row r="100" spans="1:17">
+      <c r="S99" s="17"/>
+    </row>
+    <row r="100" spans="1:19">
       <c r="A100" t="s">
         <v>194</v>
       </c>
-      <c r="Q100" s="17"/>
-    </row>
-    <row r="101" spans="1:17">
+      <c r="S100" s="17"/>
+    </row>
+    <row r="101" spans="1:19">
       <c r="A101" t="s">
         <v>195</v>
       </c>
-      <c r="Q101" s="17"/>
-    </row>
-    <row r="102" spans="1:17">
+      <c r="S101" s="17"/>
+    </row>
+    <row r="102" spans="1:19">
       <c r="A102" t="s">
         <v>196</v>
       </c>
-      <c r="Q102" s="17"/>
-    </row>
-    <row r="103" spans="1:17">
+      <c r="S102" s="17"/>
+    </row>
+    <row r="103" spans="1:19">
       <c r="A103" t="s">
         <v>197</v>
       </c>
-      <c r="Q103" s="17"/>
-    </row>
-    <row r="104" spans="1:17">
+      <c r="S103" s="17"/>
+    </row>
+    <row r="104" spans="1:19">
       <c r="A104" t="s">
         <v>198</v>
       </c>
-      <c r="Q104" s="17"/>
-    </row>
-    <row r="105" spans="1:17">
+      <c r="S104" s="17"/>
+    </row>
+    <row r="105" spans="1:19">
       <c r="A105" t="s">
         <v>199</v>
       </c>
-      <c r="Q105" s="17"/>
-    </row>
-    <row r="106" spans="1:17">
+      <c r="S105" s="17"/>
+    </row>
+    <row r="106" spans="1:19">
       <c r="A106" t="s">
         <v>200</v>
       </c>
-      <c r="Q106" s="17"/>
-    </row>
-    <row r="107" spans="1:17">
+      <c r="S106" s="17"/>
+    </row>
+    <row r="107" spans="1:19">
       <c r="A107" t="s">
         <v>201</v>
       </c>
-      <c r="Q107" s="17"/>
-    </row>
-    <row r="108" spans="1:17">
+      <c r="S107" s="17"/>
+    </row>
+    <row r="108" spans="1:19">
       <c r="A108" t="s">
         <v>202</v>
       </c>
-      <c r="Q108" s="17"/>
-    </row>
-    <row r="109" spans="1:17">
+      <c r="S108" s="17"/>
+    </row>
+    <row r="109" spans="1:19">
       <c r="A109" t="s">
         <v>203</v>
       </c>
-      <c r="Q109" s="17"/>
-    </row>
-    <row r="110" spans="1:17">
+      <c r="S109" s="17"/>
+    </row>
+    <row r="110" spans="1:19">
       <c r="A110" t="s">
         <v>204</v>
       </c>
-      <c r="Q110" s="17"/>
-    </row>
-    <row r="111" spans="1:17">
+      <c r="S110" s="17"/>
+    </row>
+    <row r="111" spans="1:19">
       <c r="A111" t="s">
         <v>205</v>
       </c>
-      <c r="Q111" s="17"/>
-    </row>
-    <row r="112" spans="1:17">
+      <c r="S111" s="17"/>
+    </row>
+    <row r="112" spans="1:19">
       <c r="A112" t="s">
         <v>206</v>
       </c>
-      <c r="Q112" s="17"/>
-    </row>
-    <row r="113" spans="1:17">
+      <c r="S112" s="17"/>
+    </row>
+    <row r="113" spans="1:19">
       <c r="A113" t="s">
         <v>207</v>
       </c>
-      <c r="Q113" s="17"/>
-    </row>
-    <row r="114" spans="1:17">
+      <c r="S113" s="17"/>
+    </row>
+    <row r="114" spans="1:19">
       <c r="A114" t="s">
         <v>208</v>
       </c>
-      <c r="Q114" s="17"/>
-    </row>
-    <row r="115" spans="1:17">
-      <c r="Q115" s="17"/>
-    </row>
-    <row r="116" spans="1:17">
-      <c r="Q116" s="17"/>
-    </row>
-    <row r="117" spans="1:17">
-      <c r="Q117" s="17"/>
-    </row>
-    <row r="118" spans="1:17">
-      <c r="Q118" s="17"/>
-    </row>
-    <row r="119" spans="1:17">
-      <c r="Q119" s="17"/>
-    </row>
-    <row r="120" spans="1:17">
-      <c r="Q120" s="17"/>
-    </row>
-    <row r="121" spans="1:17">
+      <c r="S114" s="17"/>
+    </row>
+    <row r="115" spans="1:19">
+      <c r="S115" s="17"/>
+    </row>
+    <row r="116" spans="1:19">
+      <c r="S116" s="17"/>
+    </row>
+    <row r="117" spans="1:19">
+      <c r="S117" s="17"/>
+    </row>
+    <row r="118" spans="1:19">
+      <c r="S118" s="17"/>
+    </row>
+    <row r="119" spans="1:19">
+      <c r="S119" s="17"/>
+    </row>
+    <row r="120" spans="1:19">
+      <c r="S120" s="17"/>
+    </row>
+    <row r="121" spans="1:19">
       <c r="A121" t="s">
         <v>133</v>
       </c>
-      <c r="Q121" s="17"/>
-    </row>
-    <row r="122" spans="1:17">
+      <c r="S121" s="17"/>
+    </row>
+    <row r="122" spans="1:19">
       <c r="A122" t="s">
         <v>134</v>
       </c>
-      <c r="Q122" s="17"/>
-    </row>
-    <row r="123" spans="1:17">
+      <c r="S122" s="17"/>
+    </row>
+    <row r="123" spans="1:19">
       <c r="A123" t="s">
         <v>135</v>
       </c>
-      <c r="Q123" s="17"/>
-    </row>
-    <row r="124" spans="1:17">
+      <c r="S123" s="17"/>
+    </row>
+    <row r="124" spans="1:19">
       <c r="A124" t="s">
         <v>136</v>
       </c>
-      <c r="Q124" s="17"/>
-    </row>
-    <row r="125" spans="1:17">
+      <c r="S124" s="17"/>
+    </row>
+    <row r="125" spans="1:19">
       <c r="A125" t="s">
         <v>137</v>
       </c>
-      <c r="Q125" s="17"/>
-    </row>
-    <row r="126" spans="1:17">
+      <c r="S125" s="17"/>
+    </row>
+    <row r="126" spans="1:19">
       <c r="A126" t="s">
         <v>138</v>
       </c>
-      <c r="Q126" s="17"/>
-    </row>
-    <row r="127" spans="1:17">
+      <c r="S126" s="17"/>
+    </row>
+    <row r="127" spans="1:19">
       <c r="A127" t="s">
         <v>139</v>
       </c>
-      <c r="Q127" s="17"/>
-    </row>
-    <row r="128" spans="1:17">
+      <c r="S127" s="17"/>
+    </row>
+    <row r="128" spans="1:19">
       <c r="A128" t="s">
         <v>140</v>
       </c>
-      <c r="Q128" s="17"/>
-    </row>
-    <row r="129" spans="1:17">
+      <c r="S128" s="17"/>
+    </row>
+    <row r="129" spans="1:19">
       <c r="A129" t="s">
         <v>141</v>
       </c>
-      <c r="Q129" s="17"/>
-    </row>
-    <row r="130" spans="1:17">
+      <c r="S129" s="17"/>
+    </row>
+    <row r="130" spans="1:19">
       <c r="A130" t="s">
         <v>142</v>
       </c>
-      <c r="Q130" s="17"/>
-    </row>
-    <row r="131" spans="1:17">
+      <c r="S130" s="17"/>
+    </row>
+    <row r="131" spans="1:19">
       <c r="A131" t="s">
         <v>143</v>
       </c>
-      <c r="Q131" s="17"/>
-    </row>
-    <row r="132" spans="1:17">
+      <c r="S131" s="17"/>
+    </row>
+    <row r="132" spans="1:19">
       <c r="A132" t="s">
         <v>144</v>
       </c>
-      <c r="Q132" s="17"/>
-    </row>
-    <row r="133" spans="1:17">
+      <c r="S132" s="17"/>
+    </row>
+    <row r="133" spans="1:19">
       <c r="A133" t="s">
         <v>145</v>
       </c>
-      <c r="Q133" s="17"/>
-    </row>
-    <row r="134" spans="1:17">
+      <c r="S133" s="17"/>
+    </row>
+    <row r="134" spans="1:19">
       <c r="A134" t="s">
         <v>146</v>
       </c>
-      <c r="Q134" s="17"/>
-    </row>
-    <row r="135" spans="1:17">
+      <c r="S134" s="17"/>
+    </row>
+    <row r="135" spans="1:19">
       <c r="A135" t="s">
         <v>147</v>
       </c>
-      <c r="Q135" s="17"/>
-    </row>
-    <row r="136" spans="1:17">
+      <c r="S135" s="17"/>
+    </row>
+    <row r="136" spans="1:19">
       <c r="A136" t="s">
         <v>148</v>
       </c>
-      <c r="Q136" s="17"/>
-    </row>
-    <row r="137" spans="1:17">
+      <c r="S136" s="17"/>
+    </row>
+    <row r="137" spans="1:19">
       <c r="A137" t="s">
         <v>149</v>
       </c>
-      <c r="Q137" s="17"/>
-    </row>
-    <row r="138" spans="1:17">
+      <c r="S137" s="17"/>
+    </row>
+    <row r="138" spans="1:19">
       <c r="A138" t="s">
         <v>150</v>
       </c>
-      <c r="Q138" s="17"/>
-    </row>
-    <row r="139" spans="1:17">
+      <c r="S138" s="17"/>
+    </row>
+    <row r="139" spans="1:19">
       <c r="A139" t="s">
         <v>151</v>
       </c>
-      <c r="Q139" s="17"/>
-    </row>
-    <row r="140" spans="1:17">
+      <c r="S139" s="17"/>
+    </row>
+    <row r="140" spans="1:19">
       <c r="A140" t="s">
         <v>152</v>
       </c>
-      <c r="Q140" s="17"/>
-    </row>
-    <row r="141" spans="1:17">
+      <c r="S140" s="17"/>
+    </row>
+    <row r="141" spans="1:19">
       <c r="A141" t="s">
         <v>153</v>
       </c>
-      <c r="Q141" s="17"/>
-    </row>
-    <row r="142" spans="1:17">
+      <c r="S141" s="17"/>
+    </row>
+    <row r="142" spans="1:19">
       <c r="A142" t="s">
         <v>154</v>
       </c>
-      <c r="Q142" s="17"/>
-    </row>
-    <row r="143" spans="1:17">
+      <c r="S142" s="17"/>
+    </row>
+    <row r="143" spans="1:19">
       <c r="A143" t="s">
         <v>155</v>
       </c>
-      <c r="Q143" s="17"/>
-    </row>
-    <row r="144" spans="1:17">
+      <c r="S143" s="17"/>
+    </row>
+    <row r="144" spans="1:19">
       <c r="A144" t="s">
         <v>156</v>
       </c>
-      <c r="Q144" s="17"/>
-    </row>
-    <row r="145" spans="1:17">
+      <c r="S144" s="17"/>
+    </row>
+    <row r="145" spans="1:19">
       <c r="A145" t="s">
         <v>157</v>
       </c>
-      <c r="Q145" s="17"/>
-    </row>
-    <row r="146" spans="1:17">
+      <c r="S145" s="17"/>
+    </row>
+    <row r="146" spans="1:19">
       <c r="A146" t="s">
         <v>158</v>
       </c>
-      <c r="Q146" s="17"/>
-    </row>
-    <row r="147" spans="1:17">
+      <c r="S146" s="17"/>
+    </row>
+    <row r="147" spans="1:19">
       <c r="A147" t="s">
         <v>159</v>
       </c>
-      <c r="Q147" s="17"/>
-    </row>
-    <row r="148" spans="1:17">
+      <c r="S147" s="17"/>
+    </row>
+    <row r="148" spans="1:19">
       <c r="A148" t="s">
         <v>160</v>
       </c>
-      <c r="Q148" s="17"/>
-    </row>
-    <row r="149" spans="1:17">
+      <c r="S148" s="17"/>
+    </row>
+    <row r="149" spans="1:19">
       <c r="A149" t="s">
         <v>161</v>
       </c>
-      <c r="Q149" s="17"/>
-    </row>
-    <row r="150" spans="1:17">
+      <c r="S149" s="17"/>
+    </row>
+    <row r="150" spans="1:19">
       <c r="A150" t="s">
         <v>162</v>
       </c>
-      <c r="Q150" s="17"/>
-    </row>
-    <row r="151" spans="1:17">
+      <c r="S150" s="17"/>
+    </row>
+    <row r="151" spans="1:19">
       <c r="A151" t="s">
         <v>163</v>
       </c>
-      <c r="Q151" s="17"/>
-    </row>
-    <row r="152" spans="1:17">
+      <c r="S151" s="17"/>
+    </row>
+    <row r="152" spans="1:19">
       <c r="A152" t="s">
         <v>164</v>
       </c>
-      <c r="Q152" s="17"/>
-    </row>
-    <row r="153" spans="1:17">
+      <c r="S152" s="17"/>
+    </row>
+    <row r="153" spans="1:19">
       <c r="A153" t="s">
         <v>165</v>
       </c>
-      <c r="Q153" s="17"/>
-    </row>
-    <row r="154" spans="1:17">
+      <c r="S153" s="17"/>
+    </row>
+    <row r="154" spans="1:19">
       <c r="A154" t="s">
         <v>166</v>
       </c>
-      <c r="Q154" s="17"/>
-    </row>
-    <row r="155" spans="1:17">
+      <c r="S154" s="17"/>
+    </row>
+    <row r="155" spans="1:19">
       <c r="A155" t="s">
         <v>167</v>
       </c>
-      <c r="Q155" s="17"/>
-    </row>
-    <row r="156" spans="1:17">
+      <c r="S155" s="17"/>
+    </row>
+    <row r="156" spans="1:19">
       <c r="A156" t="s">
         <v>168</v>
       </c>
-      <c r="Q156" s="17"/>
-    </row>
-    <row r="157" spans="1:17">
+      <c r="S156" s="17"/>
+    </row>
+    <row r="157" spans="1:19">
       <c r="A157" t="s">
         <v>169</v>
       </c>
-      <c r="Q157" s="17"/>
-    </row>
-    <row r="158" spans="1:17">
+      <c r="S157" s="17"/>
+    </row>
+    <row r="158" spans="1:19">
       <c r="A158" t="s">
         <v>170</v>
       </c>
-      <c r="Q158" s="17"/>
-    </row>
-    <row r="159" spans="1:17">
-      <c r="Q159" s="17"/>
-    </row>
-    <row r="160" spans="1:17">
-      <c r="Q160" s="17"/>
-    </row>
-    <row r="161" spans="1:17">
-      <c r="Q161" s="17"/>
-    </row>
-    <row r="162" spans="1:17">
-      <c r="Q162" s="17"/>
-    </row>
-    <row r="163" spans="1:17">
-      <c r="Q163" s="17"/>
-    </row>
-    <row r="164" spans="1:17">
-      <c r="Q164" s="17"/>
-    </row>
-    <row r="165" spans="1:17">
+      <c r="S158" s="17"/>
+    </row>
+    <row r="159" spans="1:19">
+      <c r="S159" s="17"/>
+    </row>
+    <row r="160" spans="1:19">
+      <c r="S160" s="17"/>
+    </row>
+    <row r="161" spans="1:19">
+      <c r="S161" s="17"/>
+    </row>
+    <row r="162" spans="1:19">
+      <c r="S162" s="17"/>
+    </row>
+    <row r="163" spans="1:19">
+      <c r="S163" s="17"/>
+    </row>
+    <row r="164" spans="1:19">
+      <c r="S164" s="17"/>
+    </row>
+    <row r="165" spans="1:19">
       <c r="A165" t="s">
         <v>95</v>
       </c>
-      <c r="Q165" s="17"/>
-    </row>
-    <row r="166" spans="1:17">
+      <c r="S165" s="17"/>
+    </row>
+    <row r="166" spans="1:19">
       <c r="A166" t="s">
         <v>96</v>
       </c>
-      <c r="Q166" s="17"/>
-    </row>
-    <row r="167" spans="1:17">
+      <c r="S166" s="17"/>
+    </row>
+    <row r="167" spans="1:19">
       <c r="A167" t="s">
         <v>97</v>
       </c>
-      <c r="Q167" s="17"/>
-    </row>
-    <row r="168" spans="1:17">
+      <c r="S167" s="17"/>
+    </row>
+    <row r="168" spans="1:19">
       <c r="A168" t="s">
         <v>98</v>
       </c>
-      <c r="Q168" s="17"/>
-    </row>
-    <row r="169" spans="1:17">
+      <c r="S168" s="17"/>
+    </row>
+    <row r="169" spans="1:19">
       <c r="A169" t="s">
         <v>99</v>
       </c>
-      <c r="Q169" s="17"/>
-    </row>
-    <row r="170" spans="1:17">
+      <c r="S169" s="17"/>
+    </row>
+    <row r="170" spans="1:19">
       <c r="A170" t="s">
         <v>100</v>
       </c>
-      <c r="Q170" s="17"/>
-    </row>
-    <row r="171" spans="1:17">
+      <c r="S170" s="17"/>
+    </row>
+    <row r="171" spans="1:19">
       <c r="A171" t="s">
         <v>101</v>
       </c>
-      <c r="Q171" s="17"/>
-    </row>
-    <row r="172" spans="1:17">
+      <c r="S171" s="17"/>
+    </row>
+    <row r="172" spans="1:19">
       <c r="A172" t="s">
         <v>102</v>
       </c>
-      <c r="Q172" s="17"/>
-    </row>
-    <row r="173" spans="1:17">
+      <c r="S172" s="17"/>
+    </row>
+    <row r="173" spans="1:19">
       <c r="A173" t="s">
         <v>103</v>
       </c>
-      <c r="Q173" s="17"/>
-    </row>
-    <row r="174" spans="1:17">
+      <c r="S173" s="17"/>
+    </row>
+    <row r="174" spans="1:19">
       <c r="A174" t="s">
         <v>104</v>
       </c>
-      <c r="Q174" s="17"/>
-    </row>
-    <row r="175" spans="1:17">
+      <c r="S174" s="17"/>
+    </row>
+    <row r="175" spans="1:19">
       <c r="A175" t="s">
         <v>105</v>
       </c>
-      <c r="Q175" s="17"/>
-    </row>
-    <row r="176" spans="1:17">
+      <c r="S175" s="17"/>
+    </row>
+    <row r="176" spans="1:19">
       <c r="A176" t="s">
         <v>106</v>
       </c>
-      <c r="Q176" s="17"/>
-    </row>
-    <row r="177" spans="1:17">
+      <c r="S176" s="17"/>
+    </row>
+    <row r="177" spans="1:19">
       <c r="A177" t="s">
         <v>107</v>
       </c>
-      <c r="Q177" s="17"/>
-    </row>
-    <row r="178" spans="1:17">
+      <c r="S177" s="17"/>
+    </row>
+    <row r="178" spans="1:19">
       <c r="A178" t="s">
         <v>108</v>
       </c>
-      <c r="Q178" s="17"/>
-    </row>
-    <row r="179" spans="1:17">
+      <c r="S178" s="17"/>
+    </row>
+    <row r="179" spans="1:19">
       <c r="A179" t="s">
         <v>109</v>
       </c>
-      <c r="Q179" s="17"/>
-    </row>
-    <row r="180" spans="1:17">
+      <c r="S179" s="17"/>
+    </row>
+    <row r="180" spans="1:19">
       <c r="A180" t="s">
         <v>110</v>
       </c>
-      <c r="Q180" s="17"/>
-    </row>
-    <row r="181" spans="1:17">
+      <c r="S180" s="17"/>
+    </row>
+    <row r="181" spans="1:19">
       <c r="A181" t="s">
         <v>111</v>
       </c>
-      <c r="Q181" s="17"/>
-    </row>
-    <row r="182" spans="1:17">
+      <c r="S181" s="17"/>
+    </row>
+    <row r="182" spans="1:19">
       <c r="A182" t="s">
         <v>112</v>
       </c>
-      <c r="Q182" s="17"/>
-    </row>
-    <row r="183" spans="1:17">
+      <c r="S182" s="17"/>
+    </row>
+    <row r="183" spans="1:19">
       <c r="A183" t="s">
         <v>113</v>
       </c>
-      <c r="Q183" s="17"/>
-    </row>
-    <row r="184" spans="1:17">
+      <c r="S183" s="17"/>
+    </row>
+    <row r="184" spans="1:19">
       <c r="A184" t="s">
         <v>114</v>
       </c>
-      <c r="Q184" s="17"/>
-    </row>
-    <row r="185" spans="1:17">
+      <c r="S184" s="17"/>
+    </row>
+    <row r="185" spans="1:19">
       <c r="A185" t="s">
         <v>115</v>
       </c>
-      <c r="Q185" s="17"/>
-    </row>
-    <row r="186" spans="1:17">
+      <c r="S185" s="17"/>
+    </row>
+    <row r="186" spans="1:19">
       <c r="A186" t="s">
         <v>116</v>
       </c>
-      <c r="K186" s="22"/>
-      <c r="L186" s="22"/>
       <c r="M186" s="22"/>
       <c r="N186" s="22"/>
       <c r="O186" s="22"/>
       <c r="P186" s="22"/>
-      <c r="Q186" s="17"/>
-    </row>
-    <row r="187" spans="1:17">
+      <c r="Q186" s="22"/>
+      <c r="R186" s="22"/>
+      <c r="S186" s="17"/>
+    </row>
+    <row r="187" spans="1:19">
       <c r="A187" t="s">
         <v>117</v>
       </c>
-      <c r="K187" s="22"/>
-      <c r="L187" s="22"/>
       <c r="M187" s="22"/>
       <c r="N187" s="22"/>
       <c r="O187" s="22"/>
       <c r="P187" s="22"/>
-      <c r="Q187" s="17"/>
-    </row>
-    <row r="188" spans="1:17">
+      <c r="Q187" s="22"/>
+      <c r="R187" s="22"/>
+      <c r="S187" s="17"/>
+    </row>
+    <row r="188" spans="1:19">
       <c r="A188" t="s">
         <v>118</v>
       </c>
-      <c r="K188" s="22"/>
-      <c r="L188" s="22"/>
       <c r="M188" s="22"/>
       <c r="N188" s="22"/>
       <c r="O188" s="22"/>
       <c r="P188" s="22"/>
-      <c r="Q188" s="17"/>
-    </row>
-    <row r="189" spans="1:17">
+      <c r="Q188" s="22"/>
+      <c r="R188" s="22"/>
+      <c r="S188" s="17"/>
+    </row>
+    <row r="189" spans="1:19">
       <c r="A189" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="190" spans="1:17">
+    <row r="190" spans="1:19">
       <c r="A190" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="191" spans="1:17">
+    <row r="191" spans="1:19">
       <c r="A191" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="192" spans="1:17">
+    <row r="192" spans="1:19">
       <c r="A192" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:12">
       <c r="A193" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:12">
       <c r="A194" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:12">
       <c r="A195" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:12">
       <c r="A196" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:12">
       <c r="A197" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:12">
       <c r="A198" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:12">
       <c r="A199" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:12">
       <c r="A200" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:12">
       <c r="A201" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:12">
       <c r="A202" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:12">
       <c r="A203" s="17"/>
       <c r="B203" s="17"/>
       <c r="C203" s="17"/>
@@ -7554,8 +7693,10 @@
       <c r="H203" s="17"/>
       <c r="I203" s="17"/>
       <c r="J203" s="17"/>
-    </row>
-    <row r="204" spans="1:10">
+      <c r="K203" s="17"/>
+      <c r="L203" s="17"/>
+    </row>
+    <row r="204" spans="1:12">
       <c r="A204" s="17"/>
       <c r="B204" s="17"/>
       <c r="C204" s="17"/>
@@ -7566,8 +7707,10 @@
       <c r="H204" s="17"/>
       <c r="I204" s="17"/>
       <c r="J204" s="17"/>
-    </row>
-    <row r="205" spans="1:10">
+      <c r="K204" s="17"/>
+      <c r="L204" s="17"/>
+    </row>
+    <row r="205" spans="1:12">
       <c r="A205" s="17"/>
       <c r="B205" s="17"/>
       <c r="C205" s="17"/>
@@ -7578,8 +7721,10 @@
       <c r="H205" s="17"/>
       <c r="I205" s="17"/>
       <c r="J205" s="17"/>
-    </row>
-    <row r="206" spans="1:10">
+      <c r="K205" s="17"/>
+      <c r="L205" s="17"/>
+    </row>
+    <row r="206" spans="1:12">
       <c r="A206" s="17"/>
       <c r="B206" s="17"/>
       <c r="C206" s="17"/>
@@ -7590,8 +7735,10 @@
       <c r="H206" s="17"/>
       <c r="I206" s="17"/>
       <c r="J206" s="17"/>
-    </row>
-    <row r="207" spans="1:10">
+      <c r="K206" s="17"/>
+      <c r="L206" s="17"/>
+    </row>
+    <row r="207" spans="1:12">
       <c r="A207" s="17"/>
       <c r="B207" s="17"/>
       <c r="C207" s="17"/>
@@ -7602,8 +7749,10 @@
       <c r="H207" s="17"/>
       <c r="I207" s="17"/>
       <c r="J207" s="17"/>
-    </row>
-    <row r="208" spans="1:10">
+      <c r="K207" s="17"/>
+      <c r="L207" s="17"/>
+    </row>
+    <row r="208" spans="1:12">
       <c r="A208" s="17"/>
       <c r="B208" s="17"/>
       <c r="C208" s="17"/>
@@ -7614,6 +7763,8 @@
       <c r="H208" s="17"/>
       <c r="I208" s="17"/>
       <c r="J208" s="17"/>
+      <c r="K208" s="17"/>
+      <c r="L208" s="17"/>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
@@ -7770,27 +7921,27 @@
         <v>273</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:12">
       <c r="A241" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:12">
       <c r="A242" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:12">
       <c r="A243" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:12">
       <c r="A244" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:12">
       <c r="A253" s="15" t="s">
         <v>283</v>
       </c>
@@ -7803,18 +7954,20 @@
       <c r="H253" s="15"/>
       <c r="I253" s="15"/>
       <c r="J253" s="15"/>
-    </row>
-    <row r="254" spans="1:10">
+      <c r="K253" s="15"/>
+      <c r="L253" s="15"/>
+    </row>
+    <row r="254" spans="1:12">
       <c r="A254" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:12">
       <c r="A255" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:12">
       <c r="A256" t="s">
         <v>59</v>
       </c>
@@ -11659,181 +11812,181 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1025" spans="1:17">
+    <row r="1025" spans="1:19">
       <c r="A1025" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="1026" spans="1:17">
+    <row r="1026" spans="1:19">
       <c r="A1026" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="1027" spans="1:17">
+    <row r="1027" spans="1:19">
       <c r="A1027" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="1028" spans="1:17">
+    <row r="1028" spans="1:19">
       <c r="A1028" t="s">
         <v>908</v>
       </c>
-      <c r="Q1028" s="17"/>
-    </row>
-    <row r="1029" spans="1:17">
+      <c r="S1028" s="17"/>
+    </row>
+    <row r="1029" spans="1:19">
       <c r="A1029" t="s">
         <v>909</v>
       </c>
-      <c r="Q1029" s="17"/>
-    </row>
-    <row r="1030" spans="1:17">
+      <c r="S1029" s="17"/>
+    </row>
+    <row r="1030" spans="1:19">
       <c r="A1030" t="s">
         <v>910</v>
       </c>
-      <c r="Q1030" s="17"/>
-    </row>
-    <row r="1031" spans="1:17">
+      <c r="S1030" s="17"/>
+    </row>
+    <row r="1031" spans="1:19">
       <c r="A1031" t="s">
         <v>911</v>
       </c>
-      <c r="Q1031" s="17"/>
-    </row>
-    <row r="1032" spans="1:17">
+      <c r="S1031" s="17"/>
+    </row>
+    <row r="1032" spans="1:19">
       <c r="A1032" t="s">
         <v>912</v>
       </c>
-      <c r="Q1032" s="17"/>
-    </row>
-    <row r="1033" spans="1:17">
+      <c r="S1032" s="17"/>
+    </row>
+    <row r="1033" spans="1:19">
       <c r="A1033" t="s">
         <v>913</v>
       </c>
-      <c r="Q1033" s="17"/>
-    </row>
-    <row r="1034" spans="1:17">
+      <c r="S1033" s="17"/>
+    </row>
+    <row r="1034" spans="1:19">
       <c r="A1034" t="s">
         <v>914</v>
       </c>
-      <c r="Q1034" s="17"/>
-    </row>
-    <row r="1035" spans="1:17">
+      <c r="S1034" s="17"/>
+    </row>
+    <row r="1035" spans="1:19">
       <c r="A1035" t="s">
         <v>915</v>
       </c>
-      <c r="Q1035" s="17"/>
-    </row>
-    <row r="1036" spans="1:17">
+      <c r="S1035" s="17"/>
+    </row>
+    <row r="1036" spans="1:19">
       <c r="A1036" t="s">
         <v>916</v>
       </c>
-      <c r="Q1036" s="17"/>
-    </row>
-    <row r="1037" spans="1:17">
+      <c r="S1036" s="17"/>
+    </row>
+    <row r="1037" spans="1:19">
       <c r="A1037" t="s">
         <v>917</v>
       </c>
-      <c r="Q1037" s="17"/>
-    </row>
-    <row r="1038" spans="1:17">
+      <c r="S1037" s="17"/>
+    </row>
+    <row r="1038" spans="1:19">
       <c r="A1038" t="s">
         <v>918</v>
       </c>
-      <c r="Q1038" s="17"/>
-    </row>
-    <row r="1039" spans="1:17">
+      <c r="S1038" s="17"/>
+    </row>
+    <row r="1039" spans="1:19">
       <c r="A1039" t="s">
         <v>919</v>
       </c>
-      <c r="Q1039" s="17"/>
-    </row>
-    <row r="1040" spans="1:17">
+      <c r="S1039" s="17"/>
+    </row>
+    <row r="1040" spans="1:19">
       <c r="A1040" t="s">
         <v>920</v>
       </c>
-      <c r="Q1040" s="17"/>
-    </row>
-    <row r="1041" spans="1:17">
+      <c r="S1040" s="17"/>
+    </row>
+    <row r="1041" spans="1:19">
       <c r="A1041" t="s">
         <v>921</v>
       </c>
-      <c r="Q1041" s="17"/>
-    </row>
-    <row r="1042" spans="1:17">
+      <c r="S1041" s="17"/>
+    </row>
+    <row r="1042" spans="1:19">
       <c r="A1042" t="s">
         <v>922</v>
       </c>
-      <c r="Q1042" s="17"/>
-    </row>
-    <row r="1043" spans="1:17">
+      <c r="S1042" s="17"/>
+    </row>
+    <row r="1043" spans="1:19">
       <c r="A1043" t="s">
         <v>923</v>
       </c>
-      <c r="Q1043" s="17"/>
-    </row>
-    <row r="1044" spans="1:17">
+      <c r="S1043" s="17"/>
+    </row>
+    <row r="1044" spans="1:19">
       <c r="A1044" t="s">
         <v>924</v>
       </c>
-      <c r="Q1044" s="17"/>
-    </row>
-    <row r="1045" spans="1:17">
+      <c r="S1044" s="17"/>
+    </row>
+    <row r="1045" spans="1:19">
       <c r="A1045" t="s">
         <v>925</v>
       </c>
-      <c r="Q1045" s="17"/>
-    </row>
-    <row r="1046" spans="1:17">
+      <c r="S1045" s="17"/>
+    </row>
+    <row r="1046" spans="1:19">
       <c r="A1046" t="s">
         <v>926</v>
       </c>
-      <c r="Q1046" s="17"/>
-    </row>
-    <row r="1047" spans="1:17">
+      <c r="S1046" s="17"/>
+    </row>
+    <row r="1047" spans="1:19">
       <c r="A1047" t="s">
         <v>927</v>
       </c>
-      <c r="Q1047" s="17"/>
-    </row>
-    <row r="1048" spans="1:17">
+      <c r="S1047" s="17"/>
+    </row>
+    <row r="1048" spans="1:19">
       <c r="A1048" t="s">
         <v>928</v>
       </c>
-      <c r="Q1048" s="17"/>
-    </row>
-    <row r="1049" spans="1:17">
+      <c r="S1048" s="17"/>
+    </row>
+    <row r="1049" spans="1:19">
       <c r="A1049" t="s">
         <v>929</v>
       </c>
-      <c r="Q1049" s="17"/>
-    </row>
-    <row r="1050" spans="1:17">
+      <c r="S1049" s="17"/>
+    </row>
+    <row r="1050" spans="1:19">
       <c r="A1050" t="s">
         <v>930</v>
       </c>
-      <c r="Q1050" s="17"/>
-    </row>
-    <row r="1051" spans="1:17">
+      <c r="S1050" s="17"/>
+    </row>
+    <row r="1051" spans="1:19">
       <c r="A1051" t="s">
         <v>931</v>
       </c>
-      <c r="Q1051" s="17"/>
-    </row>
-    <row r="1052" spans="1:17">
+      <c r="S1051" s="17"/>
+    </row>
+    <row r="1052" spans="1:19">
       <c r="A1052" t="s">
         <v>932</v>
       </c>
-      <c r="Q1052" s="17"/>
-    </row>
-    <row r="1053" spans="1:17">
+      <c r="S1052" s="17"/>
+    </row>
+    <row r="1053" spans="1:19">
       <c r="A1053" t="s">
         <v>933</v>
       </c>
-      <c r="Q1053" s="17"/>
-    </row>
-    <row r="1054" spans="1:17">
-      <c r="Q1054" s="17"/>
-    </row>
-    <row r="1055" spans="1:17">
+      <c r="S1053" s="17"/>
+    </row>
+    <row r="1054" spans="1:19">
+      <c r="S1054" s="17"/>
+    </row>
+    <row r="1055" spans="1:19">
       <c r="A1055" s="17" t="s">
         <v>243</v>
       </c>
@@ -11846,9 +11999,11 @@
       <c r="H1055" s="17"/>
       <c r="I1055" s="17"/>
       <c r="J1055" s="17"/>
-      <c r="Q1055" s="17"/>
-    </row>
-    <row r="1056" spans="1:17">
+      <c r="K1055" s="17"/>
+      <c r="L1055" s="17"/>
+      <c r="S1055" s="17"/>
+    </row>
+    <row r="1056" spans="1:19">
       <c r="A1056" s="17" t="s">
         <v>244</v>
       </c>
@@ -11861,9 +12016,11 @@
       <c r="H1056" s="17"/>
       <c r="I1056" s="17"/>
       <c r="J1056" s="17"/>
-      <c r="Q1056" s="17"/>
-    </row>
-    <row r="1057" spans="1:17">
+      <c r="K1056" s="17"/>
+      <c r="L1056" s="17"/>
+      <c r="S1056" s="17"/>
+    </row>
+    <row r="1057" spans="1:19">
       <c r="A1057" s="17" t="s">
         <v>245</v>
       </c>
@@ -11876,9 +12033,11 @@
       <c r="H1057" s="17"/>
       <c r="I1057" s="17"/>
       <c r="J1057" s="17"/>
-      <c r="Q1057" s="17"/>
-    </row>
-    <row r="1058" spans="1:17">
+      <c r="K1057" s="17"/>
+      <c r="L1057" s="17"/>
+      <c r="S1057" s="17"/>
+    </row>
+    <row r="1058" spans="1:19">
       <c r="A1058" s="17" t="s">
         <v>246</v>
       </c>
@@ -11891,9 +12050,11 @@
       <c r="H1058" s="17"/>
       <c r="I1058" s="17"/>
       <c r="J1058" s="17"/>
-      <c r="Q1058" s="17"/>
-    </row>
-    <row r="1059" spans="1:17">
+      <c r="K1058" s="17"/>
+      <c r="L1058" s="17"/>
+      <c r="S1058" s="17"/>
+    </row>
+    <row r="1059" spans="1:19">
       <c r="A1059" s="17" t="s">
         <v>247</v>
       </c>
@@ -11906,9 +12067,11 @@
       <c r="H1059" s="17"/>
       <c r="I1059" s="17"/>
       <c r="J1059" s="17"/>
-      <c r="Q1059" s="17"/>
-    </row>
-    <row r="1060" spans="1:17">
+      <c r="K1059" s="17"/>
+      <c r="L1059" s="17"/>
+      <c r="S1059" s="17"/>
+    </row>
+    <row r="1060" spans="1:19">
       <c r="A1060" s="17" t="s">
         <v>248</v>
       </c>
@@ -11921,9 +12084,11 @@
       <c r="H1060" s="17"/>
       <c r="I1060" s="17"/>
       <c r="J1060" s="17"/>
-      <c r="Q1060" s="17"/>
-    </row>
-    <row r="1061" spans="1:17">
+      <c r="K1060" s="17"/>
+      <c r="L1060" s="17"/>
+      <c r="S1060" s="17"/>
+    </row>
+    <row r="1061" spans="1:19">
       <c r="A1061" s="17" t="s">
         <v>249</v>
       </c>
@@ -11936,9 +12101,11 @@
       <c r="H1061" s="17"/>
       <c r="I1061" s="17"/>
       <c r="J1061" s="17"/>
-      <c r="Q1061" s="17"/>
-    </row>
-    <row r="1062" spans="1:17">
+      <c r="K1061" s="17"/>
+      <c r="L1061" s="17"/>
+      <c r="S1061" s="17"/>
+    </row>
+    <row r="1062" spans="1:19">
       <c r="A1062" s="17" t="s">
         <v>250</v>
       </c>
@@ -11951,9 +12118,11 @@
       <c r="H1062" s="17"/>
       <c r="I1062" s="17"/>
       <c r="J1062" s="17"/>
-      <c r="Q1062" s="17"/>
-    </row>
-    <row r="1063" spans="1:17">
+      <c r="K1062" s="17"/>
+      <c r="L1062" s="17"/>
+      <c r="S1062" s="17"/>
+    </row>
+    <row r="1063" spans="1:19">
       <c r="A1063" s="17" t="s">
         <v>251</v>
       </c>
@@ -11966,9 +12135,11 @@
       <c r="H1063" s="17"/>
       <c r="I1063" s="17"/>
       <c r="J1063" s="17"/>
-      <c r="Q1063" s="17"/>
-    </row>
-    <row r="1064" spans="1:17">
+      <c r="K1063" s="17"/>
+      <c r="L1063" s="17"/>
+      <c r="S1063" s="17"/>
+    </row>
+    <row r="1064" spans="1:19">
       <c r="A1064" s="17" t="s">
         <v>252</v>
       </c>
@@ -11981,9 +12152,11 @@
       <c r="H1064" s="17"/>
       <c r="I1064" s="17"/>
       <c r="J1064" s="17"/>
-      <c r="Q1064" s="17"/>
-    </row>
-    <row r="1065" spans="1:17">
+      <c r="K1064" s="17"/>
+      <c r="L1064" s="17"/>
+      <c r="S1064" s="17"/>
+    </row>
+    <row r="1065" spans="1:19">
       <c r="A1065" s="17" t="s">
         <v>253</v>
       </c>
@@ -11996,9 +12169,11 @@
       <c r="H1065" s="17"/>
       <c r="I1065" s="17"/>
       <c r="J1065" s="17"/>
-      <c r="Q1065" s="17"/>
-    </row>
-    <row r="1066" spans="1:17">
+      <c r="K1065" s="17"/>
+      <c r="L1065" s="17"/>
+      <c r="S1065" s="17"/>
+    </row>
+    <row r="1066" spans="1:19">
       <c r="A1066" s="17" t="s">
         <v>254</v>
       </c>
@@ -12011,9 +12186,11 @@
       <c r="H1066" s="17"/>
       <c r="I1066" s="17"/>
       <c r="J1066" s="17"/>
-      <c r="Q1066" s="17"/>
-    </row>
-    <row r="1067" spans="1:17">
+      <c r="K1066" s="17"/>
+      <c r="L1066" s="17"/>
+      <c r="S1066" s="17"/>
+    </row>
+    <row r="1067" spans="1:19">
       <c r="A1067" s="17" t="s">
         <v>255</v>
       </c>
@@ -12026,9 +12203,11 @@
       <c r="H1067" s="17"/>
       <c r="I1067" s="17"/>
       <c r="J1067" s="17"/>
-      <c r="Q1067" s="17"/>
-    </row>
-    <row r="1068" spans="1:17">
+      <c r="K1067" s="17"/>
+      <c r="L1067" s="17"/>
+      <c r="S1067" s="17"/>
+    </row>
+    <row r="1068" spans="1:19">
       <c r="A1068" s="17" t="s">
         <v>256</v>
       </c>
@@ -12041,14 +12220,16 @@
       <c r="H1068" s="17"/>
       <c r="I1068" s="17"/>
       <c r="J1068" s="17"/>
-      <c r="K1068"/>
-      <c r="L1068"/>
+      <c r="K1068" s="17"/>
+      <c r="L1068" s="17"/>
       <c r="M1068"/>
       <c r="N1068"/>
       <c r="O1068"/>
       <c r="P1068"/>
-    </row>
-    <row r="1069" spans="1:17">
+      <c r="Q1068"/>
+      <c r="R1068"/>
+    </row>
+    <row r="1069" spans="1:19">
       <c r="A1069" s="17" t="s">
         <v>257</v>
       </c>
@@ -12061,14 +12242,16 @@
       <c r="H1069" s="17"/>
       <c r="I1069" s="17"/>
       <c r="J1069" s="17"/>
-      <c r="K1069"/>
-      <c r="L1069"/>
+      <c r="K1069" s="17"/>
+      <c r="L1069" s="17"/>
       <c r="M1069"/>
       <c r="N1069"/>
       <c r="O1069"/>
       <c r="P1069"/>
-    </row>
-    <row r="1070" spans="1:17">
+      <c r="Q1069"/>
+      <c r="R1069"/>
+    </row>
+    <row r="1070" spans="1:19">
       <c r="A1070" s="17" t="s">
         <v>258</v>
       </c>
@@ -12081,14 +12264,16 @@
       <c r="H1070" s="17"/>
       <c r="I1070" s="17"/>
       <c r="J1070" s="17"/>
-      <c r="K1070"/>
-      <c r="L1070"/>
+      <c r="K1070" s="17"/>
+      <c r="L1070" s="17"/>
       <c r="M1070"/>
       <c r="N1070"/>
       <c r="O1070"/>
       <c r="P1070"/>
-    </row>
-    <row r="1071" spans="1:17">
+      <c r="Q1070"/>
+      <c r="R1070"/>
+    </row>
+    <row r="1071" spans="1:19">
       <c r="A1071" s="17" t="s">
         <v>259</v>
       </c>
@@ -12101,14 +12286,16 @@
       <c r="H1071" s="17"/>
       <c r="I1071" s="17"/>
       <c r="J1071" s="17"/>
-      <c r="K1071"/>
-      <c r="L1071"/>
+      <c r="K1071" s="17"/>
+      <c r="L1071" s="17"/>
       <c r="M1071"/>
       <c r="N1071"/>
       <c r="O1071"/>
       <c r="P1071"/>
-    </row>
-    <row r="1072" spans="1:17">
+      <c r="Q1071"/>
+      <c r="R1071"/>
+    </row>
+    <row r="1072" spans="1:19">
       <c r="A1072" s="17" t="s">
         <v>260</v>
       </c>
@@ -12121,14 +12308,16 @@
       <c r="H1072" s="17"/>
       <c r="I1072" s="17"/>
       <c r="J1072" s="17"/>
-      <c r="K1072"/>
-      <c r="L1072"/>
+      <c r="K1072" s="17"/>
+      <c r="L1072" s="17"/>
       <c r="M1072"/>
       <c r="N1072"/>
       <c r="O1072"/>
       <c r="P1072"/>
-    </row>
-    <row r="1073" spans="1:16">
+      <c r="Q1072"/>
+      <c r="R1072"/>
+    </row>
+    <row r="1073" spans="1:18">
       <c r="A1073" s="17" t="s">
         <v>261</v>
       </c>
@@ -12141,14 +12330,16 @@
       <c r="H1073" s="17"/>
       <c r="I1073" s="17"/>
       <c r="J1073" s="17"/>
-      <c r="K1073"/>
-      <c r="L1073"/>
+      <c r="K1073" s="17"/>
+      <c r="L1073" s="17"/>
       <c r="M1073"/>
       <c r="N1073"/>
       <c r="O1073"/>
       <c r="P1073"/>
-    </row>
-    <row r="1074" spans="1:16">
+      <c r="Q1073"/>
+      <c r="R1073"/>
+    </row>
+    <row r="1074" spans="1:18">
       <c r="A1074" s="17" t="s">
         <v>262</v>
       </c>
@@ -12161,14 +12352,16 @@
       <c r="H1074" s="17"/>
       <c r="I1074" s="17"/>
       <c r="J1074" s="17"/>
-      <c r="K1074"/>
-      <c r="L1074"/>
+      <c r="K1074" s="17"/>
+      <c r="L1074" s="17"/>
       <c r="M1074"/>
       <c r="N1074"/>
       <c r="O1074"/>
       <c r="P1074"/>
-    </row>
-    <row r="1075" spans="1:16">
+      <c r="Q1074"/>
+      <c r="R1074"/>
+    </row>
+    <row r="1075" spans="1:18">
       <c r="A1075" s="17" t="s">
         <v>263</v>
       </c>
@@ -12181,14 +12374,16 @@
       <c r="H1075" s="17"/>
       <c r="I1075" s="17"/>
       <c r="J1075" s="17"/>
-      <c r="K1075"/>
-      <c r="L1075"/>
+      <c r="K1075" s="17"/>
+      <c r="L1075" s="17"/>
       <c r="M1075"/>
       <c r="N1075"/>
       <c r="O1075"/>
       <c r="P1075"/>
-    </row>
-    <row r="1076" spans="1:16">
+      <c r="Q1075"/>
+      <c r="R1075"/>
+    </row>
+    <row r="1076" spans="1:18">
       <c r="A1076" s="17" t="s">
         <v>264</v>
       </c>
@@ -12201,14 +12396,16 @@
       <c r="H1076" s="17"/>
       <c r="I1076" s="17"/>
       <c r="J1076" s="17"/>
-      <c r="K1076"/>
-      <c r="L1076"/>
+      <c r="K1076" s="17"/>
+      <c r="L1076" s="17"/>
       <c r="M1076"/>
       <c r="N1076"/>
       <c r="O1076"/>
       <c r="P1076"/>
-    </row>
-    <row r="1077" spans="1:16">
+      <c r="Q1076"/>
+      <c r="R1076"/>
+    </row>
+    <row r="1077" spans="1:18">
       <c r="A1077" s="17" t="s">
         <v>265</v>
       </c>
@@ -12221,14 +12418,16 @@
       <c r="H1077" s="17"/>
       <c r="I1077" s="17"/>
       <c r="J1077" s="17"/>
-      <c r="K1077"/>
-      <c r="L1077"/>
+      <c r="K1077" s="17"/>
+      <c r="L1077" s="17"/>
       <c r="M1077"/>
       <c r="N1077"/>
       <c r="O1077"/>
       <c r="P1077"/>
-    </row>
-    <row r="1078" spans="1:16">
+      <c r="Q1077"/>
+      <c r="R1077"/>
+    </row>
+    <row r="1078" spans="1:18">
       <c r="A1078" s="17" t="s">
         <v>266</v>
       </c>
@@ -12241,14 +12440,16 @@
       <c r="H1078" s="17"/>
       <c r="I1078" s="17"/>
       <c r="J1078" s="17"/>
-      <c r="K1078"/>
-      <c r="L1078"/>
+      <c r="K1078" s="17"/>
+      <c r="L1078" s="17"/>
       <c r="M1078"/>
       <c r="N1078"/>
       <c r="O1078"/>
       <c r="P1078"/>
-    </row>
-    <row r="1079" spans="1:16">
+      <c r="Q1078"/>
+      <c r="R1078"/>
+    </row>
+    <row r="1079" spans="1:18">
       <c r="A1079" s="17" t="s">
         <v>267</v>
       </c>
@@ -12261,14 +12462,16 @@
       <c r="H1079" s="17"/>
       <c r="I1079" s="17"/>
       <c r="J1079" s="17"/>
-      <c r="K1079"/>
-      <c r="L1079"/>
+      <c r="K1079" s="17"/>
+      <c r="L1079" s="17"/>
       <c r="M1079"/>
       <c r="N1079"/>
       <c r="O1079"/>
       <c r="P1079"/>
-    </row>
-    <row r="1080" spans="1:16">
+      <c r="Q1079"/>
+      <c r="R1079"/>
+    </row>
+    <row r="1080" spans="1:18">
       <c r="A1080" s="17" t="s">
         <v>268</v>
       </c>
@@ -12281,14 +12484,16 @@
       <c r="H1080" s="17"/>
       <c r="I1080" s="17"/>
       <c r="J1080" s="17"/>
-      <c r="K1080"/>
-      <c r="L1080"/>
+      <c r="K1080" s="17"/>
+      <c r="L1080" s="17"/>
       <c r="M1080"/>
       <c r="N1080"/>
       <c r="O1080"/>
       <c r="P1080"/>
-    </row>
-    <row r="1081" spans="1:16">
+      <c r="Q1080"/>
+      <c r="R1080"/>
+    </row>
+    <row r="1081" spans="1:18">
       <c r="A1081" s="17" t="s">
         <v>269</v>
       </c>
@@ -12301,14 +12506,16 @@
       <c r="H1081" s="17"/>
       <c r="I1081" s="17"/>
       <c r="J1081" s="17"/>
-      <c r="K1081"/>
-      <c r="L1081"/>
+      <c r="K1081" s="17"/>
+      <c r="L1081" s="17"/>
       <c r="M1081"/>
       <c r="N1081"/>
       <c r="O1081"/>
       <c r="P1081"/>
-    </row>
-    <row r="1082" spans="1:16">
+      <c r="Q1081"/>
+      <c r="R1081"/>
+    </row>
+    <row r="1082" spans="1:18">
       <c r="A1082" s="17" t="s">
         <v>270</v>
       </c>
@@ -12321,14 +12528,16 @@
       <c r="H1082" s="17"/>
       <c r="I1082" s="17"/>
       <c r="J1082" s="17"/>
-      <c r="K1082"/>
-      <c r="L1082"/>
+      <c r="K1082" s="17"/>
+      <c r="L1082" s="17"/>
       <c r="M1082"/>
       <c r="N1082"/>
       <c r="O1082"/>
       <c r="P1082"/>
-    </row>
-    <row r="1083" spans="1:16">
+      <c r="Q1082"/>
+      <c r="R1082"/>
+    </row>
+    <row r="1083" spans="1:18">
       <c r="A1083" s="17" t="s">
         <v>271</v>
       </c>
@@ -12341,14 +12550,16 @@
       <c r="H1083" s="17"/>
       <c r="I1083" s="17"/>
       <c r="J1083" s="17"/>
-      <c r="K1083"/>
-      <c r="L1083"/>
+      <c r="K1083" s="17"/>
+      <c r="L1083" s="17"/>
       <c r="M1083"/>
       <c r="N1083"/>
       <c r="O1083"/>
       <c r="P1083"/>
-    </row>
-    <row r="1084" spans="1:16">
+      <c r="Q1083"/>
+      <c r="R1083"/>
+    </row>
+    <row r="1084" spans="1:18">
       <c r="A1084" s="17" t="s">
         <v>272</v>
       </c>
@@ -12361,14 +12572,16 @@
       <c r="H1084" s="17"/>
       <c r="I1084" s="17"/>
       <c r="J1084" s="17"/>
-      <c r="K1084"/>
-      <c r="L1084"/>
+      <c r="K1084" s="17"/>
+      <c r="L1084" s="17"/>
       <c r="M1084"/>
       <c r="N1084"/>
       <c r="O1084"/>
       <c r="P1084"/>
-    </row>
-    <row r="1085" spans="1:16">
+      <c r="Q1084"/>
+      <c r="R1084"/>
+    </row>
+    <row r="1085" spans="1:18">
       <c r="A1085" s="17" t="s">
         <v>273</v>
       </c>
@@ -12381,14 +12594,16 @@
       <c r="H1085" s="17"/>
       <c r="I1085" s="17"/>
       <c r="J1085" s="17"/>
-      <c r="K1085"/>
-      <c r="L1085"/>
+      <c r="K1085" s="17"/>
+      <c r="L1085" s="17"/>
       <c r="M1085"/>
       <c r="N1085"/>
       <c r="O1085"/>
       <c r="P1085"/>
-    </row>
-    <row r="1086" spans="1:16">
+      <c r="Q1085"/>
+      <c r="R1085"/>
+    </row>
+    <row r="1086" spans="1:18">
       <c r="A1086" s="17" t="s">
         <v>274</v>
       </c>
@@ -12401,14 +12616,16 @@
       <c r="H1086" s="17"/>
       <c r="I1086" s="17"/>
       <c r="J1086" s="17"/>
-      <c r="K1086"/>
-      <c r="L1086"/>
+      <c r="K1086" s="17"/>
+      <c r="L1086" s="17"/>
       <c r="M1086"/>
       <c r="N1086"/>
       <c r="O1086"/>
       <c r="P1086"/>
-    </row>
-    <row r="1087" spans="1:16">
+      <c r="Q1086"/>
+      <c r="R1086"/>
+    </row>
+    <row r="1087" spans="1:18">
       <c r="A1087" s="17" t="s">
         <v>275</v>
       </c>
@@ -12421,14 +12638,16 @@
       <c r="H1087" s="17"/>
       <c r="I1087" s="17"/>
       <c r="J1087" s="17"/>
-      <c r="K1087"/>
-      <c r="L1087"/>
+      <c r="K1087" s="17"/>
+      <c r="L1087" s="17"/>
       <c r="M1087"/>
       <c r="N1087"/>
       <c r="O1087"/>
       <c r="P1087"/>
-    </row>
-    <row r="1088" spans="1:16">
+      <c r="Q1087"/>
+      <c r="R1087"/>
+    </row>
+    <row r="1088" spans="1:18">
       <c r="A1088" s="17" t="s">
         <v>276</v>
       </c>
@@ -12441,14 +12660,16 @@
       <c r="H1088" s="17"/>
       <c r="I1088" s="17"/>
       <c r="J1088" s="17"/>
-      <c r="K1088"/>
-      <c r="L1088"/>
+      <c r="K1088" s="17"/>
+      <c r="L1088" s="17"/>
       <c r="M1088"/>
       <c r="N1088"/>
       <c r="O1088"/>
       <c r="P1088"/>
-    </row>
-    <row r="1089" spans="1:16">
+      <c r="Q1088"/>
+      <c r="R1088"/>
+    </row>
+    <row r="1089" spans="1:18">
       <c r="A1089" s="17" t="s">
         <v>277</v>
       </c>
@@ -12461,14 +12682,16 @@
       <c r="H1089" s="17"/>
       <c r="I1089" s="17"/>
       <c r="J1089" s="17"/>
-      <c r="K1089"/>
-      <c r="L1089"/>
+      <c r="K1089" s="17"/>
+      <c r="L1089" s="17"/>
       <c r="M1089"/>
       <c r="N1089"/>
       <c r="O1089"/>
       <c r="P1089"/>
-    </row>
-    <row r="1090" spans="1:16">
+      <c r="Q1089"/>
+      <c r="R1089"/>
+    </row>
+    <row r="1090" spans="1:18">
       <c r="A1090" s="17" t="s">
         <v>934</v>
       </c>
@@ -12481,14 +12704,16 @@
       <c r="H1090" s="17"/>
       <c r="I1090" s="17"/>
       <c r="J1090" s="17"/>
-      <c r="K1090"/>
-      <c r="L1090"/>
+      <c r="K1090" s="17"/>
+      <c r="L1090" s="17"/>
       <c r="M1090"/>
       <c r="N1090"/>
       <c r="O1090"/>
       <c r="P1090"/>
-    </row>
-    <row r="1091" spans="1:16">
+      <c r="Q1090"/>
+      <c r="R1090"/>
+    </row>
+    <row r="1091" spans="1:18">
       <c r="A1091" s="17" t="s">
         <v>935</v>
       </c>
@@ -12501,14 +12726,16 @@
       <c r="H1091" s="17"/>
       <c r="I1091" s="17"/>
       <c r="J1091" s="17"/>
-      <c r="K1091"/>
-      <c r="L1091"/>
+      <c r="K1091" s="17"/>
+      <c r="L1091" s="17"/>
       <c r="M1091"/>
       <c r="N1091"/>
       <c r="O1091"/>
       <c r="P1091"/>
-    </row>
-    <row r="1092" spans="1:16">
+      <c r="Q1091"/>
+      <c r="R1091"/>
+    </row>
+    <row r="1092" spans="1:18">
       <c r="A1092" s="17" t="s">
         <v>936</v>
       </c>
@@ -12521,14 +12748,16 @@
       <c r="H1092" s="17"/>
       <c r="I1092" s="17"/>
       <c r="J1092" s="17"/>
-      <c r="K1092"/>
-      <c r="L1092"/>
+      <c r="K1092" s="17"/>
+      <c r="L1092" s="17"/>
       <c r="M1092"/>
       <c r="N1092"/>
       <c r="O1092"/>
       <c r="P1092"/>
-    </row>
-    <row r="1093" spans="1:16">
+      <c r="Q1092"/>
+      <c r="R1092"/>
+    </row>
+    <row r="1093" spans="1:18">
       <c r="A1093" s="17" t="s">
         <v>937</v>
       </c>
@@ -12541,14 +12770,16 @@
       <c r="H1093" s="17"/>
       <c r="I1093" s="17"/>
       <c r="J1093" s="17"/>
-      <c r="K1093"/>
-      <c r="L1093"/>
+      <c r="K1093" s="17"/>
+      <c r="L1093" s="17"/>
       <c r="M1093"/>
       <c r="N1093"/>
       <c r="O1093"/>
       <c r="P1093"/>
-    </row>
-    <row r="1094" spans="1:16">
+      <c r="Q1093"/>
+      <c r="R1093"/>
+    </row>
+    <row r="1094" spans="1:18">
       <c r="A1094" s="17" t="s">
         <v>938</v>
       </c>
@@ -12561,572 +12792,574 @@
       <c r="H1094" s="17"/>
       <c r="I1094" s="17"/>
       <c r="J1094" s="17"/>
-      <c r="K1094"/>
-      <c r="L1094"/>
+      <c r="K1094" s="17"/>
+      <c r="L1094" s="17"/>
       <c r="M1094"/>
       <c r="N1094"/>
       <c r="O1094"/>
       <c r="P1094"/>
-    </row>
-    <row r="1095" spans="1:16">
-      <c r="K1095"/>
-      <c r="L1095"/>
+      <c r="Q1094"/>
+      <c r="R1094"/>
+    </row>
+    <row r="1095" spans="1:18">
       <c r="M1095"/>
       <c r="N1095"/>
       <c r="O1095"/>
       <c r="P1095"/>
-    </row>
-    <row r="1096" spans="1:16">
-      <c r="K1096"/>
-      <c r="L1096"/>
+      <c r="Q1095"/>
+      <c r="R1095"/>
+    </row>
+    <row r="1096" spans="1:18">
       <c r="M1096"/>
       <c r="N1096"/>
       <c r="O1096"/>
       <c r="P1096"/>
-    </row>
-    <row r="1097" spans="1:16">
-      <c r="K1097"/>
-      <c r="L1097"/>
+      <c r="Q1096"/>
+      <c r="R1096"/>
+    </row>
+    <row r="1097" spans="1:18">
       <c r="M1097"/>
       <c r="N1097"/>
       <c r="O1097"/>
       <c r="P1097"/>
-    </row>
-    <row r="1098" spans="1:16">
-      <c r="K1098"/>
-      <c r="L1098"/>
+      <c r="Q1097"/>
+      <c r="R1097"/>
+    </row>
+    <row r="1098" spans="1:18">
       <c r="M1098"/>
       <c r="N1098"/>
       <c r="O1098"/>
       <c r="P1098"/>
-    </row>
-    <row r="1099" spans="1:16">
-      <c r="K1099"/>
-      <c r="L1099"/>
+      <c r="Q1098"/>
+      <c r="R1098"/>
+    </row>
+    <row r="1099" spans="1:18">
       <c r="M1099"/>
       <c r="N1099"/>
       <c r="O1099"/>
       <c r="P1099"/>
-    </row>
-    <row r="1100" spans="1:16">
-      <c r="K1100"/>
-      <c r="L1100"/>
+      <c r="Q1099"/>
+      <c r="R1099"/>
+    </row>
+    <row r="1100" spans="1:18">
       <c r="M1100"/>
       <c r="N1100"/>
       <c r="O1100"/>
       <c r="P1100"/>
-    </row>
-    <row r="1101" spans="1:16">
-      <c r="K1101"/>
-      <c r="L1101"/>
+      <c r="Q1100"/>
+      <c r="R1100"/>
+    </row>
+    <row r="1101" spans="1:18">
       <c r="M1101"/>
       <c r="N1101"/>
       <c r="O1101"/>
       <c r="P1101"/>
-    </row>
-    <row r="1102" spans="1:16">
-      <c r="K1102"/>
-      <c r="L1102"/>
+      <c r="Q1101"/>
+      <c r="R1101"/>
+    </row>
+    <row r="1102" spans="1:18">
       <c r="M1102"/>
       <c r="N1102"/>
       <c r="O1102"/>
       <c r="P1102"/>
-    </row>
-    <row r="1103" spans="1:16">
-      <c r="K1103"/>
-      <c r="L1103"/>
+      <c r="Q1102"/>
+      <c r="R1102"/>
+    </row>
+    <row r="1103" spans="1:18">
       <c r="M1103"/>
       <c r="N1103"/>
       <c r="O1103"/>
       <c r="P1103"/>
-    </row>
-    <row r="1104" spans="1:16">
-      <c r="K1104"/>
-      <c r="L1104"/>
+      <c r="Q1103"/>
+      <c r="R1103"/>
+    </row>
+    <row r="1104" spans="1:18">
       <c r="M1104"/>
       <c r="N1104"/>
       <c r="O1104"/>
       <c r="P1104"/>
-    </row>
-    <row r="1105" spans="11:16">
-      <c r="K1105"/>
-      <c r="L1105"/>
+      <c r="Q1104"/>
+      <c r="R1104"/>
+    </row>
+    <row r="1105" spans="13:18">
       <c r="M1105"/>
       <c r="N1105"/>
       <c r="O1105"/>
       <c r="P1105"/>
-    </row>
-    <row r="1106" spans="11:16">
-      <c r="K1106"/>
-      <c r="L1106"/>
+      <c r="Q1105"/>
+      <c r="R1105"/>
+    </row>
+    <row r="1106" spans="13:18">
       <c r="M1106"/>
       <c r="N1106"/>
       <c r="O1106"/>
       <c r="P1106"/>
-    </row>
-    <row r="1107" spans="11:16">
-      <c r="K1107"/>
-      <c r="L1107"/>
+      <c r="Q1106"/>
+      <c r="R1106"/>
+    </row>
+    <row r="1107" spans="13:18">
       <c r="M1107"/>
       <c r="N1107"/>
       <c r="O1107"/>
       <c r="P1107"/>
-    </row>
-    <row r="1108" spans="11:16">
-      <c r="K1108"/>
-      <c r="L1108"/>
+      <c r="Q1107"/>
+      <c r="R1107"/>
+    </row>
+    <row r="1108" spans="13:18">
       <c r="M1108"/>
       <c r="N1108"/>
       <c r="O1108"/>
       <c r="P1108"/>
-    </row>
-    <row r="1109" spans="11:16">
-      <c r="K1109"/>
-      <c r="L1109"/>
+      <c r="Q1108"/>
+      <c r="R1108"/>
+    </row>
+    <row r="1109" spans="13:18">
       <c r="M1109"/>
       <c r="N1109"/>
       <c r="O1109"/>
       <c r="P1109"/>
-    </row>
-    <row r="1110" spans="11:16">
-      <c r="K1110"/>
-      <c r="L1110"/>
+      <c r="Q1109"/>
+      <c r="R1109"/>
+    </row>
+    <row r="1110" spans="13:18">
       <c r="M1110"/>
       <c r="N1110"/>
       <c r="O1110"/>
       <c r="P1110"/>
-    </row>
-    <row r="1111" spans="11:16">
-      <c r="K1111"/>
-      <c r="L1111"/>
+      <c r="Q1110"/>
+      <c r="R1110"/>
+    </row>
+    <row r="1111" spans="13:18">
       <c r="M1111"/>
       <c r="N1111"/>
       <c r="O1111"/>
       <c r="P1111"/>
-    </row>
-    <row r="1112" spans="11:16">
-      <c r="K1112"/>
-      <c r="L1112"/>
+      <c r="Q1111"/>
+      <c r="R1111"/>
+    </row>
+    <row r="1112" spans="13:18">
       <c r="M1112"/>
       <c r="N1112"/>
       <c r="O1112"/>
       <c r="P1112"/>
-    </row>
-    <row r="1113" spans="11:16">
-      <c r="K1113"/>
-      <c r="L1113"/>
+      <c r="Q1112"/>
+      <c r="R1112"/>
+    </row>
+    <row r="1113" spans="13:18">
       <c r="M1113"/>
       <c r="N1113"/>
       <c r="O1113"/>
       <c r="P1113"/>
-    </row>
-    <row r="1114" spans="11:16">
-      <c r="K1114"/>
-      <c r="L1114"/>
+      <c r="Q1113"/>
+      <c r="R1113"/>
+    </row>
+    <row r="1114" spans="13:18">
       <c r="M1114"/>
       <c r="N1114"/>
       <c r="O1114"/>
       <c r="P1114"/>
-    </row>
-    <row r="1115" spans="11:16">
-      <c r="K1115"/>
-      <c r="L1115"/>
+      <c r="Q1114"/>
+      <c r="R1114"/>
+    </row>
+    <row r="1115" spans="13:18">
       <c r="M1115"/>
       <c r="N1115"/>
       <c r="O1115"/>
       <c r="P1115"/>
-    </row>
-    <row r="1116" spans="11:16">
-      <c r="K1116"/>
-      <c r="L1116"/>
+      <c r="Q1115"/>
+      <c r="R1115"/>
+    </row>
+    <row r="1116" spans="13:18">
       <c r="M1116"/>
       <c r="N1116"/>
       <c r="O1116"/>
       <c r="P1116"/>
-    </row>
-    <row r="1117" spans="11:16">
-      <c r="K1117"/>
-      <c r="L1117"/>
+      <c r="Q1116"/>
+      <c r="R1116"/>
+    </row>
+    <row r="1117" spans="13:18">
       <c r="M1117"/>
       <c r="N1117"/>
       <c r="O1117"/>
       <c r="P1117"/>
-    </row>
-    <row r="1118" spans="11:16">
-      <c r="K1118"/>
-      <c r="L1118"/>
+      <c r="Q1117"/>
+      <c r="R1117"/>
+    </row>
+    <row r="1118" spans="13:18">
       <c r="M1118"/>
       <c r="N1118"/>
       <c r="O1118"/>
       <c r="P1118"/>
-    </row>
-    <row r="1119" spans="11:16">
-      <c r="K1119"/>
-      <c r="L1119"/>
+      <c r="Q1118"/>
+      <c r="R1118"/>
+    </row>
+    <row r="1119" spans="13:18">
       <c r="M1119"/>
       <c r="N1119"/>
       <c r="O1119"/>
       <c r="P1119"/>
-    </row>
-    <row r="1120" spans="11:16">
-      <c r="K1120"/>
-      <c r="L1120"/>
+      <c r="Q1119"/>
+      <c r="R1119"/>
+    </row>
+    <row r="1120" spans="13:18">
       <c r="M1120"/>
       <c r="N1120"/>
       <c r="O1120"/>
       <c r="P1120"/>
-    </row>
-    <row r="1121" spans="11:16">
-      <c r="K1121"/>
-      <c r="L1121"/>
+      <c r="Q1120"/>
+      <c r="R1120"/>
+    </row>
+    <row r="1121" spans="13:18">
       <c r="M1121"/>
       <c r="N1121"/>
       <c r="O1121"/>
       <c r="P1121"/>
-    </row>
-    <row r="1122" spans="11:16">
-      <c r="K1122"/>
-      <c r="L1122"/>
+      <c r="Q1121"/>
+      <c r="R1121"/>
+    </row>
+    <row r="1122" spans="13:18">
       <c r="M1122"/>
       <c r="N1122"/>
       <c r="O1122"/>
       <c r="P1122"/>
-    </row>
-    <row r="1123" spans="11:16">
-      <c r="K1123"/>
-      <c r="L1123"/>
+      <c r="Q1122"/>
+      <c r="R1122"/>
+    </row>
+    <row r="1123" spans="13:18">
       <c r="M1123"/>
       <c r="N1123"/>
       <c r="O1123"/>
       <c r="P1123"/>
-    </row>
-    <row r="1124" spans="11:16">
-      <c r="K1124"/>
-      <c r="L1124"/>
+      <c r="Q1123"/>
+      <c r="R1123"/>
+    </row>
+    <row r="1124" spans="13:18">
       <c r="M1124"/>
       <c r="N1124"/>
       <c r="O1124"/>
       <c r="P1124"/>
-    </row>
-    <row r="1125" spans="11:16">
-      <c r="K1125"/>
-      <c r="L1125"/>
+      <c r="Q1124"/>
+      <c r="R1124"/>
+    </row>
+    <row r="1125" spans="13:18">
       <c r="M1125"/>
       <c r="N1125"/>
       <c r="O1125"/>
       <c r="P1125"/>
-    </row>
-    <row r="1126" spans="11:16">
-      <c r="K1126"/>
-      <c r="L1126"/>
+      <c r="Q1125"/>
+      <c r="R1125"/>
+    </row>
+    <row r="1126" spans="13:18">
       <c r="M1126"/>
       <c r="N1126"/>
       <c r="O1126"/>
       <c r="P1126"/>
-    </row>
-    <row r="1127" spans="11:16">
-      <c r="K1127"/>
-      <c r="L1127"/>
+      <c r="Q1126"/>
+      <c r="R1126"/>
+    </row>
+    <row r="1127" spans="13:18">
       <c r="M1127"/>
       <c r="N1127"/>
       <c r="O1127"/>
       <c r="P1127"/>
-    </row>
-    <row r="1128" spans="11:16">
-      <c r="K1128"/>
-      <c r="L1128"/>
+      <c r="Q1127"/>
+      <c r="R1127"/>
+    </row>
+    <row r="1128" spans="13:18">
       <c r="M1128"/>
       <c r="N1128"/>
       <c r="O1128"/>
       <c r="P1128"/>
-    </row>
-    <row r="1129" spans="11:16">
-      <c r="K1129"/>
-      <c r="L1129"/>
+      <c r="Q1128"/>
+      <c r="R1128"/>
+    </row>
+    <row r="1129" spans="13:18">
       <c r="M1129"/>
       <c r="N1129"/>
       <c r="O1129"/>
       <c r="P1129"/>
-    </row>
-    <row r="1130" spans="11:16">
-      <c r="K1130"/>
-      <c r="L1130"/>
+      <c r="Q1129"/>
+      <c r="R1129"/>
+    </row>
+    <row r="1130" spans="13:18">
       <c r="M1130"/>
       <c r="N1130"/>
       <c r="O1130"/>
       <c r="P1130"/>
-    </row>
-    <row r="1131" spans="11:16">
-      <c r="K1131"/>
-      <c r="L1131"/>
+      <c r="Q1130"/>
+      <c r="R1130"/>
+    </row>
+    <row r="1131" spans="13:18">
       <c r="M1131"/>
       <c r="N1131"/>
       <c r="O1131"/>
       <c r="P1131"/>
-    </row>
-    <row r="1132" spans="11:16">
-      <c r="K1132"/>
-      <c r="L1132"/>
+      <c r="Q1131"/>
+      <c r="R1131"/>
+    </row>
+    <row r="1132" spans="13:18">
       <c r="M1132"/>
       <c r="N1132"/>
       <c r="O1132"/>
       <c r="P1132"/>
-    </row>
-    <row r="1133" spans="11:16">
-      <c r="K1133"/>
-      <c r="L1133"/>
+      <c r="Q1132"/>
+      <c r="R1132"/>
+    </row>
+    <row r="1133" spans="13:18">
       <c r="M1133"/>
       <c r="N1133"/>
       <c r="O1133"/>
       <c r="P1133"/>
-    </row>
-    <row r="1134" spans="11:16">
-      <c r="K1134"/>
-      <c r="L1134"/>
+      <c r="Q1133"/>
+      <c r="R1133"/>
+    </row>
+    <row r="1134" spans="13:18">
       <c r="M1134"/>
       <c r="N1134"/>
       <c r="O1134"/>
       <c r="P1134"/>
-    </row>
-    <row r="1135" spans="11:16">
-      <c r="K1135"/>
-      <c r="L1135"/>
+      <c r="Q1134"/>
+      <c r="R1134"/>
+    </row>
+    <row r="1135" spans="13:18">
       <c r="M1135"/>
       <c r="N1135"/>
       <c r="O1135"/>
       <c r="P1135"/>
-    </row>
-    <row r="1136" spans="11:16">
-      <c r="K1136"/>
-      <c r="L1136"/>
+      <c r="Q1135"/>
+      <c r="R1135"/>
+    </row>
+    <row r="1136" spans="13:18">
       <c r="M1136"/>
       <c r="N1136"/>
       <c r="O1136"/>
       <c r="P1136"/>
-    </row>
-    <row r="1137" spans="11:16">
-      <c r="K1137"/>
-      <c r="L1137"/>
+      <c r="Q1136"/>
+      <c r="R1136"/>
+    </row>
+    <row r="1137" spans="13:18">
       <c r="M1137"/>
       <c r="N1137"/>
       <c r="O1137"/>
       <c r="P1137"/>
-    </row>
-    <row r="1138" spans="11:16">
-      <c r="K1138"/>
-      <c r="L1138"/>
+      <c r="Q1137"/>
+      <c r="R1137"/>
+    </row>
+    <row r="1138" spans="13:18">
       <c r="M1138"/>
       <c r="N1138"/>
       <c r="O1138"/>
       <c r="P1138"/>
-    </row>
-    <row r="1139" spans="11:16">
-      <c r="K1139"/>
-      <c r="L1139"/>
+      <c r="Q1138"/>
+      <c r="R1138"/>
+    </row>
+    <row r="1139" spans="13:18">
       <c r="M1139"/>
       <c r="N1139"/>
       <c r="O1139"/>
       <c r="P1139"/>
-    </row>
-    <row r="1140" spans="11:16">
-      <c r="K1140"/>
-      <c r="L1140"/>
+      <c r="Q1139"/>
+      <c r="R1139"/>
+    </row>
+    <row r="1140" spans="13:18">
       <c r="M1140"/>
       <c r="N1140"/>
       <c r="O1140"/>
       <c r="P1140"/>
-    </row>
-    <row r="1141" spans="11:16">
-      <c r="K1141"/>
-      <c r="L1141"/>
+      <c r="Q1140"/>
+      <c r="R1140"/>
+    </row>
+    <row r="1141" spans="13:18">
       <c r="M1141"/>
       <c r="N1141"/>
       <c r="O1141"/>
       <c r="P1141"/>
-    </row>
-    <row r="1142" spans="11:16">
-      <c r="K1142"/>
-      <c r="L1142"/>
+      <c r="Q1141"/>
+      <c r="R1141"/>
+    </row>
+    <row r="1142" spans="13:18">
       <c r="M1142"/>
       <c r="N1142"/>
       <c r="O1142"/>
       <c r="P1142"/>
-    </row>
-    <row r="1143" spans="11:16">
-      <c r="K1143"/>
-      <c r="L1143"/>
+      <c r="Q1142"/>
+      <c r="R1142"/>
+    </row>
+    <row r="1143" spans="13:18">
       <c r="M1143"/>
       <c r="N1143"/>
       <c r="O1143"/>
       <c r="P1143"/>
-    </row>
-    <row r="1144" spans="11:16">
-      <c r="K1144"/>
-      <c r="L1144"/>
+      <c r="Q1143"/>
+      <c r="R1143"/>
+    </row>
+    <row r="1144" spans="13:18">
       <c r="M1144"/>
       <c r="N1144"/>
       <c r="O1144"/>
       <c r="P1144"/>
-    </row>
-    <row r="1145" spans="11:16">
-      <c r="K1145"/>
-      <c r="L1145"/>
+      <c r="Q1144"/>
+      <c r="R1144"/>
+    </row>
+    <row r="1145" spans="13:18">
       <c r="M1145"/>
       <c r="N1145"/>
       <c r="O1145"/>
       <c r="P1145"/>
-    </row>
-    <row r="1146" spans="11:16">
-      <c r="K1146"/>
-      <c r="L1146"/>
+      <c r="Q1145"/>
+      <c r="R1145"/>
+    </row>
+    <row r="1146" spans="13:18">
       <c r="M1146"/>
       <c r="N1146"/>
       <c r="O1146"/>
       <c r="P1146"/>
-    </row>
-    <row r="1147" spans="11:16">
-      <c r="K1147"/>
-      <c r="L1147"/>
+      <c r="Q1146"/>
+      <c r="R1146"/>
+    </row>
+    <row r="1147" spans="13:18">
       <c r="M1147"/>
       <c r="N1147"/>
       <c r="O1147"/>
       <c r="P1147"/>
-    </row>
-    <row r="1148" spans="11:16">
-      <c r="K1148"/>
-      <c r="L1148"/>
+      <c r="Q1147"/>
+      <c r="R1147"/>
+    </row>
+    <row r="1148" spans="13:18">
       <c r="M1148"/>
       <c r="N1148"/>
       <c r="O1148"/>
       <c r="P1148"/>
-    </row>
-    <row r="1149" spans="11:16">
-      <c r="K1149"/>
-      <c r="L1149"/>
+      <c r="Q1148"/>
+      <c r="R1148"/>
+    </row>
+    <row r="1149" spans="13:18">
       <c r="M1149"/>
       <c r="N1149"/>
       <c r="O1149"/>
       <c r="P1149"/>
-    </row>
-    <row r="1150" spans="11:16">
-      <c r="K1150"/>
-      <c r="L1150"/>
+      <c r="Q1149"/>
+      <c r="R1149"/>
+    </row>
+    <row r="1150" spans="13:18">
       <c r="M1150"/>
       <c r="N1150"/>
       <c r="O1150"/>
       <c r="P1150"/>
-    </row>
-    <row r="1151" spans="11:16">
-      <c r="K1151"/>
-      <c r="L1151"/>
+      <c r="Q1150"/>
+      <c r="R1150"/>
+    </row>
+    <row r="1151" spans="13:18">
       <c r="M1151"/>
       <c r="N1151"/>
       <c r="O1151"/>
       <c r="P1151"/>
-    </row>
-    <row r="1152" spans="11:16">
-      <c r="K1152"/>
-      <c r="L1152"/>
+      <c r="Q1151"/>
+      <c r="R1151"/>
+    </row>
+    <row r="1152" spans="13:18">
       <c r="M1152"/>
       <c r="N1152"/>
       <c r="O1152"/>
       <c r="P1152"/>
-    </row>
-    <row r="1153" spans="11:16">
-      <c r="K1153"/>
-      <c r="L1153"/>
+      <c r="Q1152"/>
+      <c r="R1152"/>
+    </row>
+    <row r="1153" spans="13:18">
       <c r="M1153"/>
       <c r="N1153"/>
       <c r="O1153"/>
       <c r="P1153"/>
-    </row>
-    <row r="1154" spans="11:16">
-      <c r="K1154"/>
-      <c r="L1154"/>
+      <c r="Q1153"/>
+      <c r="R1153"/>
+    </row>
+    <row r="1154" spans="13:18">
       <c r="M1154"/>
       <c r="N1154"/>
       <c r="O1154"/>
       <c r="P1154"/>
-    </row>
-    <row r="1155" spans="11:16">
-      <c r="K1155"/>
-      <c r="L1155"/>
+      <c r="Q1154"/>
+      <c r="R1154"/>
+    </row>
+    <row r="1155" spans="13:18">
       <c r="M1155"/>
       <c r="N1155"/>
       <c r="O1155"/>
       <c r="P1155"/>
-    </row>
-    <row r="1156" spans="11:16">
-      <c r="K1156"/>
-      <c r="L1156"/>
+      <c r="Q1155"/>
+      <c r="R1155"/>
+    </row>
+    <row r="1156" spans="13:18">
       <c r="M1156"/>
       <c r="N1156"/>
       <c r="O1156"/>
       <c r="P1156"/>
-    </row>
-    <row r="1157" spans="11:16">
-      <c r="K1157"/>
-      <c r="L1157"/>
+      <c r="Q1156"/>
+      <c r="R1156"/>
+    </row>
+    <row r="1157" spans="13:18">
       <c r="M1157"/>
       <c r="N1157"/>
       <c r="O1157"/>
       <c r="P1157"/>
-    </row>
-    <row r="1158" spans="11:16">
-      <c r="K1158"/>
-      <c r="L1158"/>
+      <c r="Q1157"/>
+      <c r="R1157"/>
+    </row>
+    <row r="1158" spans="13:18">
       <c r="M1158"/>
       <c r="N1158"/>
       <c r="O1158"/>
       <c r="P1158"/>
-    </row>
-    <row r="1159" spans="11:16">
-      <c r="K1159"/>
-      <c r="L1159"/>
+      <c r="Q1158"/>
+      <c r="R1158"/>
+    </row>
+    <row r="1159" spans="13:18">
       <c r="M1159"/>
       <c r="N1159"/>
       <c r="O1159"/>
       <c r="P1159"/>
-    </row>
-    <row r="1160" spans="11:16">
-      <c r="K1160"/>
-      <c r="L1160"/>
+      <c r="Q1159"/>
+      <c r="R1159"/>
+    </row>
+    <row r="1160" spans="13:18">
       <c r="M1160"/>
       <c r="N1160"/>
       <c r="O1160"/>
       <c r="P1160"/>
-    </row>
-    <row r="1161" spans="11:16">
-      <c r="K1161"/>
-      <c r="L1161"/>
+      <c r="Q1160"/>
+      <c r="R1160"/>
+    </row>
+    <row r="1161" spans="13:18">
       <c r="M1161"/>
       <c r="N1161"/>
       <c r="O1161"/>
       <c r="P1161"/>
-    </row>
-    <row r="1162" spans="11:16">
-      <c r="K1162"/>
-      <c r="L1162"/>
+      <c r="Q1161"/>
+      <c r="R1161"/>
+    </row>
+    <row r="1162" spans="13:18">
       <c r="M1162"/>
       <c r="N1162"/>
       <c r="O1162"/>
       <c r="P1162"/>
-    </row>
-    <row r="1163" spans="11:16">
-      <c r="K1163"/>
-      <c r="L1163"/>
+      <c r="Q1162"/>
+      <c r="R1162"/>
+    </row>
+    <row r="1163" spans="13:18">
       <c r="M1163"/>
       <c r="N1163"/>
       <c r="O1163"/>
       <c r="P1163"/>
-    </row>
-    <row r="1164" spans="11:16">
-      <c r="K1164"/>
-      <c r="L1164"/>
+      <c r="Q1163"/>
+      <c r="R1163"/>
+    </row>
+    <row r="1164" spans="13:18">
       <c r="M1164"/>
       <c r="N1164"/>
       <c r="O1164"/>
       <c r="P1164"/>
+      <c r="Q1164"/>
+      <c r="R1164"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Plotting code now works with and without z-score
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7480" yWindow="2320" windowWidth="25600" windowHeight="16000" tabRatio="902" activeTab="3"/>
+    <workbookView xWindow="7420" yWindow="580" windowWidth="25600" windowHeight="16000" tabRatio="902" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4095" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4100" uniqueCount="1070">
   <si>
     <t>param</t>
   </si>
@@ -3497,8 +3497,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="387">
+  <cellStyleXfs count="389">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3957,7 +3959,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="387">
+  <cellStyles count="389">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4151,6 +4153,7 @@
     <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4344,6 +4347,7 @@
     <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5705,29 +5709,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC1164"/>
+  <dimension ref="A1:AD1164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="12" width="17.1640625" customWidth="1"/>
-    <col min="13" max="18" width="18.5" style="21" customWidth="1"/>
-    <col min="19" max="19" width="17.1640625" customWidth="1"/>
-    <col min="20" max="20" width="15" customWidth="1"/>
-    <col min="21" max="21" width="13.5" customWidth="1"/>
-    <col min="22" max="22" width="13.6640625" customWidth="1"/>
-    <col min="23" max="23" width="13.1640625" customWidth="1"/>
-    <col min="24" max="24" width="11.83203125" customWidth="1"/>
-    <col min="25" max="25" width="15.5" customWidth="1"/>
-    <col min="26" max="26" width="12.6640625" customWidth="1"/>
-    <col min="27" max="27" width="14.33203125" customWidth="1"/>
-    <col min="28" max="29" width="10.83203125" style="19"/>
+    <col min="1" max="13" width="17.1640625" customWidth="1"/>
+    <col min="14" max="19" width="18.5" style="21" customWidth="1"/>
+    <col min="20" max="20" width="17.1640625" customWidth="1"/>
+    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="22" max="22" width="13.5" customWidth="1"/>
+    <col min="23" max="23" width="13.6640625" customWidth="1"/>
+    <col min="24" max="24" width="13.1640625" customWidth="1"/>
+    <col min="25" max="25" width="11.83203125" customWidth="1"/>
+    <col min="26" max="26" width="15.5" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" customWidth="1"/>
+    <col min="29" max="30" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="18" customFormat="1">
+    <row r="1" spans="1:23" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
         <v>212</v>
       </c>
@@ -5746,8 +5750,8 @@
       <c r="F1" t="s">
         <v>1054</v>
       </c>
-      <c r="G1" s="18" t="s">
-        <v>1</v>
+      <c r="G1" t="s">
+        <v>1054</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>1</v>
@@ -5756,25 +5760,25 @@
         <v>1</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>976</v>
+        <v>1</v>
       </c>
       <c r="K1" s="18" t="s">
         <v>976</v>
       </c>
-      <c r="L1"/>
-      <c r="M1" t="s">
+      <c r="L1" s="18" t="s">
+        <v>976</v>
+      </c>
+      <c r="M1"/>
+      <c r="N1" t="s">
         <v>992</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>1054</v>
       </c>
-      <c r="O1" s="18" t="s">
+      <c r="P1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="P1" s="17" t="s">
-        <v>992</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="17" t="s">
         <v>992</v>
       </c>
       <c r="R1" t="s">
@@ -5783,14 +5787,17 @@
       <c r="S1" t="s">
         <v>992</v>
       </c>
-      <c r="T1" s="18" t="s">
+      <c r="T1" t="s">
+        <v>992</v>
+      </c>
+      <c r="U1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="V1" s="18" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="18" customFormat="1">
+    <row r="2" spans="1:23" s="18" customFormat="1">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -5804,12 +5811,13 @@
       <c r="L2"/>
       <c r="M2"/>
       <c r="N2"/>
-      <c r="P2" s="17"/>
-      <c r="Q2"/>
+      <c r="O2"/>
+      <c r="Q2" s="17"/>
       <c r="R2"/>
       <c r="S2"/>
-    </row>
-    <row r="3" spans="1:22" s="40" customFormat="1">
+      <c r="T2"/>
+    </row>
+    <row r="3" spans="1:23" s="40" customFormat="1">
       <c r="A3" s="40" t="s">
         <v>1066</v>
       </c>
@@ -5828,12 +5836,13 @@
       <c r="L3" s="41"/>
       <c r="M3" s="41"/>
       <c r="N3" s="41"/>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="41"/>
+      <c r="O3" s="41"/>
+      <c r="Q3" s="42"/>
       <c r="R3" s="41"/>
       <c r="S3" s="41"/>
-    </row>
-    <row r="4" spans="1:22">
+      <c r="T3" s="41"/>
+    </row>
+    <row r="4" spans="1:23">
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -5845,10 +5854,11 @@
       <c r="J4" s="21"/>
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
-      <c r="P4" s="22"/>
-      <c r="S4" s="21"/>
-    </row>
-    <row r="5" spans="1:22">
+      <c r="M4" s="21"/>
+      <c r="Q4" s="22"/>
+      <c r="T4" s="21"/>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -5882,27 +5892,27 @@
       <c r="K5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21" t="s">
+      <c r="L5" s="21" t="s">
         <v>1032</v>
       </c>
+      <c r="M5" s="21"/>
       <c r="N5" s="21" t="s">
         <v>1032</v>
       </c>
       <c r="O5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="P5" s="22" t="s">
+      <c r="P5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="Q5" s="22" t="s">
         <v>1034</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="R5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="S5" s="22" t="s">
         <v>1034</v>
-      </c>
-      <c r="S5" s="21" t="s">
-        <v>1032</v>
       </c>
       <c r="T5" s="21" t="s">
         <v>1032</v>
@@ -5910,9 +5920,12 @@
       <c r="U5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="V5" s="21"/>
-    </row>
-    <row r="6" spans="1:22">
+      <c r="V5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="W5" s="21"/>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
         <v>221</v>
       </c>
@@ -5946,37 +5959,40 @@
       <c r="K6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="L6" s="21"/>
-      <c r="M6" s="21" t="s">
+      <c r="L6" s="21" t="s">
         <v>1031</v>
       </c>
+      <c r="M6" s="21"/>
       <c r="N6" s="21" t="s">
         <v>1031</v>
       </c>
       <c r="O6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="P6" s="22" t="s">
+      <c r="P6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="Q6" s="21" t="s">
-        <v>1035</v>
+      <c r="Q6" s="22" t="s">
+        <v>1031</v>
       </c>
       <c r="R6" s="21" t="s">
         <v>1035</v>
       </c>
       <c r="S6" s="21" t="s">
+        <v>1035</v>
+      </c>
+      <c r="T6" s="21" t="s">
         <v>1033</v>
-      </c>
-      <c r="T6" s="22" t="s">
-        <v>1036</v>
       </c>
       <c r="U6" s="22" t="s">
         <v>1036</v>
       </c>
-      <c r="V6" s="21"/>
-    </row>
-    <row r="7" spans="1:22">
+      <c r="V6" s="22" t="s">
+        <v>1036</v>
+      </c>
+      <c r="W6" s="21"/>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
         <v>280</v>
       </c>
@@ -5992,16 +6008,14 @@
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
-      <c r="J7" t="s">
+      <c r="J7" s="21"/>
+      <c r="K7" t="s">
         <v>1069</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="L7" s="21" t="s">
         <v>1068</v>
       </c>
-      <c r="L7" s="21"/>
-      <c r="M7" s="21" t="s">
-        <v>281</v>
-      </c>
+      <c r="M7" s="21"/>
       <c r="N7" s="21" t="s">
         <v>281</v>
       </c>
@@ -6026,14 +6040,14 @@
       <c r="U7" s="21" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="8" spans="1:22">
+      <c r="V7" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
         <v>224</v>
       </c>
-      <c r="M8" s="21" t="s">
-        <v>1064</v>
-      </c>
       <c r="N8" s="21" t="s">
         <v>1064</v>
       </c>
@@ -6055,11 +6069,14 @@
       <c r="T8" s="21" t="s">
         <v>1064</v>
       </c>
-      <c r="U8" t="s">
+      <c r="U8" s="21" t="s">
+        <v>1064</v>
+      </c>
+      <c r="V8" t="s">
         <v>1065</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
         <v>1063</v>
       </c>
@@ -6091,12 +6108,12 @@
         <v>1056</v>
       </c>
       <c r="K9" s="21" t="s">
+        <v>1056</v>
+      </c>
+      <c r="L9" s="21" t="s">
         <v>1062</v>
       </c>
-      <c r="L9" s="21"/>
-      <c r="M9" s="21" t="s">
-        <v>1062</v>
-      </c>
+      <c r="M9" s="21"/>
       <c r="N9" s="21" t="s">
         <v>1062</v>
       </c>
@@ -6121,8 +6138,11 @@
       <c r="U9" s="21" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="11" spans="1:22">
+      <c r="V9" s="21" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
         <v>214</v>
       </c>
@@ -6148,16 +6168,16 @@
         <v>1524</v>
       </c>
       <c r="I11">
-        <v>2497</v>
+        <v>1524</v>
       </c>
       <c r="J11">
         <v>2497</v>
       </c>
       <c r="K11">
+        <v>2497</v>
+      </c>
+      <c r="L11">
         <v>1524</v>
-      </c>
-      <c r="M11" s="23">
-        <v>1556</v>
       </c>
       <c r="N11" s="23">
         <v>1556</v>
@@ -6166,25 +6186,28 @@
         <v>1556</v>
       </c>
       <c r="P11" s="23">
+        <v>1556</v>
+      </c>
+      <c r="Q11" s="23">
         <v>1097</v>
       </c>
-      <c r="Q11" s="23">
+      <c r="R11" s="23">
         <v>2651</v>
       </c>
-      <c r="R11" s="23">
+      <c r="S11" s="23">
         <v>2112</v>
       </c>
-      <c r="S11" s="23">
+      <c r="T11" s="23">
         <v>1953</v>
-      </c>
-      <c r="T11">
-        <v>1556</v>
       </c>
       <c r="U11">
         <v>1556</v>
       </c>
-    </row>
-    <row r="12" spans="1:22">
+      <c r="V11">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
         <v>211</v>
       </c>
@@ -6210,15 +6233,15 @@
         <v>37</v>
       </c>
       <c r="I12">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="J12">
         <v>199</v>
       </c>
       <c r="K12">
-        <v>37</v>
-      </c>
-      <c r="M12" s="23">
+        <v>199</v>
+      </c>
+      <c r="L12">
         <v>37</v>
       </c>
       <c r="N12" s="23">
@@ -6228,40 +6251,43 @@
         <v>37</v>
       </c>
       <c r="P12" s="23">
+        <v>37</v>
+      </c>
+      <c r="Q12" s="23">
         <v>25</v>
       </c>
-      <c r="Q12" s="23">
+      <c r="R12" s="23">
         <v>200</v>
       </c>
-      <c r="R12" s="23">
+      <c r="S12" s="23">
         <v>179</v>
       </c>
-      <c r="S12" s="23">
+      <c r="T12" s="23">
         <v>41</v>
-      </c>
-      <c r="T12">
-        <v>37</v>
       </c>
       <c r="U12">
         <v>37</v>
       </c>
-      <c r="V12" s="23"/>
-    </row>
-    <row r="13" spans="1:22">
+      <c r="V12">
+        <v>37</v>
+      </c>
+      <c r="W12" s="23"/>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
         <v>213</v>
       </c>
-      <c r="M13" s="23"/>
       <c r="N13" s="23"/>
-      <c r="P13" s="23"/>
+      <c r="O13" s="23"/>
       <c r="Q13" s="23"/>
       <c r="R13" s="23"/>
-      <c r="U13">
+      <c r="S13" s="23"/>
+      <c r="V13">
         <v>30</v>
       </c>
-      <c r="V13" s="23"/>
-    </row>
-    <row r="14" spans="1:22">
+      <c r="W13" s="23"/>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -6284,7 +6310,7 @@
         <v>214</v>
       </c>
       <c r="H14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I14" t="s">
         <v>216</v>
@@ -6295,7 +6321,7 @@
       <c r="K14" t="s">
         <v>216</v>
       </c>
-      <c r="M14" s="23" t="s">
+      <c r="L14" t="s">
         <v>216</v>
       </c>
       <c r="N14" s="23" t="s">
@@ -6322,8 +6348,11 @@
       <c r="U14" s="23" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" s="21" customFormat="1">
+      <c r="V14" s="23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" s="21" customFormat="1">
       <c r="A16" s="21" t="s">
         <v>5</v>
       </c>
@@ -6343,63 +6372,66 @@
         <v>30.584579999999999</v>
       </c>
       <c r="G16" s="21">
+        <v>64.010794300000001</v>
+      </c>
+      <c r="H16" s="21">
         <v>64.962770178</v>
       </c>
-      <c r="H16" s="21">
+      <c r="I16" s="21">
         <v>30.721707769999998</v>
       </c>
-      <c r="I16" s="21">
+      <c r="J16" s="21">
         <v>30.754858800000001</v>
       </c>
-      <c r="J16" s="21">
+      <c r="K16" s="21">
         <v>13.436368399999999</v>
       </c>
-      <c r="K16" s="21">
+      <c r="L16" s="21">
         <v>11.977791</v>
       </c>
-      <c r="M16" s="21">
+      <c r="N16" s="21">
         <v>30.877478</v>
       </c>
-      <c r="N16" s="21">
+      <c r="O16" s="21">
         <v>30.66</v>
       </c>
-      <c r="O16" s="21">
+      <c r="P16" s="21">
         <v>31.211466999999999</v>
       </c>
-      <c r="P16" s="21">
+      <c r="Q16" s="21">
         <v>31.880268000000001</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="R16" s="21">
         <v>30.716964999999998</v>
       </c>
-      <c r="R16" s="21">
+      <c r="S16" s="21">
         <v>29.746556000000002</v>
       </c>
-      <c r="S16" s="21">
+      <c r="T16" s="21">
         <v>29.076453999999998</v>
       </c>
-      <c r="T16" s="21">
+      <c r="U16" s="21">
         <v>29.443950000000001</v>
       </c>
-      <c r="U16" s="21">
+      <c r="V16" s="21">
         <v>11.154477999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="21" customFormat="1">
+    <row r="17" spans="1:22" s="21" customFormat="1">
       <c r="A17" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="J17" s="21">
+      <c r="K17" s="21">
         <v>8.5977074000000009</v>
       </c>
-      <c r="K17" s="21">
+      <c r="L17" s="21">
         <v>12.778447999999999</v>
       </c>
-      <c r="U17" s="21">
+      <c r="V17" s="21">
         <v>17.8</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="21" customFormat="1" ht="14" customHeight="1">
+    <row r="18" spans="1:22" s="21" customFormat="1" ht="14" customHeight="1">
       <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
@@ -6419,49 +6451,52 @@
         <v>-5.8981399999999997</v>
       </c>
       <c r="G18" s="21">
+        <v>-0.98127699999999995</v>
+      </c>
+      <c r="H18" s="21">
         <v>-0.43686686800000002</v>
       </c>
-      <c r="H18" s="21">
+      <c r="I18" s="21">
         <v>-4.6886315600000001</v>
       </c>
-      <c r="I18" s="21">
+      <c r="J18" s="21">
         <v>-3.2696827000000002</v>
       </c>
-      <c r="J18" s="21">
+      <c r="K18" s="21">
         <v>-8.0795293000000008</v>
       </c>
-      <c r="K18" s="21">
+      <c r="L18" s="21">
         <v>-10.718495000000001</v>
       </c>
-      <c r="M18" s="21">
+      <c r="N18" s="21">
         <v>-3.858498</v>
       </c>
-      <c r="N18" s="21">
+      <c r="O18" s="21">
         <v>-4.7</v>
       </c>
-      <c r="O18" s="21">
+      <c r="P18" s="21">
         <v>-3.9753639999999999</v>
       </c>
-      <c r="P18" s="21">
+      <c r="Q18" s="21">
         <v>-6.589467</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="R18" s="21">
         <v>-4.670153</v>
       </c>
-      <c r="R18" s="21">
+      <c r="S18" s="21">
         <v>-6.3059329999999996</v>
       </c>
-      <c r="S18" s="21">
+      <c r="T18" s="21">
         <v>-4.2054489999999998</v>
       </c>
-      <c r="T18" s="21">
+      <c r="U18" s="21">
         <v>-4.4239769999999998</v>
       </c>
-      <c r="U18" s="21">
+      <c r="V18" s="21">
         <v>-11.179836</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="21" customFormat="1">
+    <row r="19" spans="1:22" s="21" customFormat="1">
       <c r="A19" s="21" t="s">
         <v>8</v>
       </c>
@@ -6481,49 +6516,52 @@
         <v>-1.7522850000000001</v>
       </c>
       <c r="G19" s="21">
+        <v>-0.32169579999999998</v>
+      </c>
+      <c r="H19" s="21">
         <v>-0.59282655500000003</v>
       </c>
-      <c r="H19" s="21">
+      <c r="I19" s="21">
         <v>-3.2544300800000001</v>
       </c>
-      <c r="I19" s="21">
+      <c r="J19" s="21">
         <v>-2.0773652</v>
       </c>
-      <c r="J19" s="21">
+      <c r="K19" s="21">
         <v>-0.73294579999999998</v>
       </c>
-      <c r="K19" s="21">
+      <c r="L19" s="21">
         <v>-1.3810519999999999</v>
       </c>
-      <c r="M19" s="21">
+      <c r="N19" s="21">
         <v>-3.1080649999999999</v>
       </c>
-      <c r="N19" s="21">
+      <c r="O19" s="21">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="O19" s="21">
+      <c r="P19" s="21">
         <v>-3.5504150000000001</v>
       </c>
-      <c r="P19" s="21">
+      <c r="Q19" s="21">
         <v>-2.3749199999999999</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="R19" s="21">
         <v>-1.740626</v>
       </c>
-      <c r="R19" s="21">
+      <c r="S19" s="21">
         <v>-1.149972</v>
       </c>
-      <c r="S19" s="21">
+      <c r="T19" s="21">
         <v>-3.8012999999999999</v>
       </c>
-      <c r="T19" s="21">
+      <c r="U19" s="21">
         <v>-4.6329729999999998</v>
       </c>
-      <c r="U19" s="21">
+      <c r="V19" s="21">
         <v>-1.4</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="21" customFormat="1">
+    <row r="20" spans="1:22" s="21" customFormat="1">
       <c r="A20" s="21" t="s">
         <v>9</v>
       </c>
@@ -6543,141 +6581,144 @@
         <v>-7.6310460000000004</v>
       </c>
       <c r="G20" s="21">
+        <v>-0.22312940000000001</v>
+      </c>
+      <c r="H20" s="21">
         <v>-0.28852171599999998</v>
       </c>
-      <c r="H20" s="21">
+      <c r="I20" s="21">
         <v>-8.3550094300000008</v>
       </c>
-      <c r="I20" s="21">
+      <c r="J20" s="21">
         <v>-7.0728663999999997</v>
       </c>
-      <c r="J20" s="21">
+      <c r="K20" s="21">
         <v>-8.4076094999999995</v>
       </c>
-      <c r="K20" s="21">
+      <c r="L20" s="21">
         <v>-9.5678230000000006</v>
       </c>
-      <c r="M20" s="21">
+      <c r="N20" s="21">
         <v>-10.069042</v>
       </c>
-      <c r="N20" s="21">
+      <c r="O20" s="21">
         <v>-8.5</v>
       </c>
-      <c r="O20" s="21">
+      <c r="P20" s="21">
         <v>-10.401221</v>
       </c>
-      <c r="P20" s="21">
+      <c r="Q20" s="21">
         <v>-9.9066620000000007</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="R20" s="21">
         <v>-8.6652190000000004</v>
       </c>
-      <c r="R20" s="21">
+      <c r="S20" s="21">
         <v>-9.8209820000000008</v>
       </c>
-      <c r="S20" s="21">
+      <c r="T20" s="21">
         <v>-10.442672999999999</v>
       </c>
-      <c r="T20" s="21">
+      <c r="U20" s="21">
         <v>-10.520892</v>
       </c>
-      <c r="U20" s="21">
+      <c r="V20" s="21">
         <v>-9.7576470000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:21">
+    <row r="21" spans="1:22">
       <c r="A21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:21">
+    <row r="22" spans="1:22">
       <c r="A22" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:21">
+    <row r="23" spans="1:22">
       <c r="A23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:21">
+    <row r="24" spans="1:22">
       <c r="A24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:21">
+    <row r="25" spans="1:22">
       <c r="A25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:21">
+    <row r="26" spans="1:22">
       <c r="A26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:21">
+    <row r="27" spans="1:22">
       <c r="A27" t="s">
         <v>210</v>
       </c>
-      <c r="J27">
+      <c r="K27">
         <v>6.1738270000000002</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>9.932563</v>
       </c>
     </row>
-    <row r="28" spans="1:21">
+    <row r="28" spans="1:22">
       <c r="A28" t="s">
         <v>10</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>-1.4379709999999999E-3</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>-9.5536179999999998E-2</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>0.15195020000000001</v>
       </c>
-      <c r="O28" s="21">
+      <c r="P28" s="21">
         <v>1.47323</v>
       </c>
     </row>
-    <row r="29" spans="1:21">
+    <row r="29" spans="1:22">
       <c r="A29" t="s">
         <v>11</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>4.1001559999999998E-3</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>0.85033303000000005</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>1.3428956999999999</v>
       </c>
-      <c r="O29" s="21">
+      <c r="P29" s="21">
         <v>1.0277529999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:21">
+    <row r="30" spans="1:22">
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>-1.7003655999999999E-2</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>-0.27255634000000001</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>-0.39319349999999997</v>
       </c>
-      <c r="O30" s="21">
+      <c r="P30" s="21">
         <v>-1.052503</v>
       </c>
     </row>
-    <row r="32" spans="1:21">
+    <row r="32" spans="1:22">
       <c r="A32" s="15" t="s">
         <v>972</v>
       </c>
@@ -6692,258 +6733,259 @@
       <c r="J32" s="15"/>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
-    </row>
-    <row r="33" spans="1:19">
+      <c r="M32" s="15"/>
+    </row>
+    <row r="33" spans="1:20">
       <c r="A33" t="s">
         <v>57</v>
       </c>
-      <c r="S33" s="17"/>
-    </row>
-    <row r="34" spans="1:19">
+      <c r="T33" s="17"/>
+    </row>
+    <row r="34" spans="1:20">
       <c r="A34" t="s">
         <v>58</v>
       </c>
-      <c r="S34" s="17"/>
-    </row>
-    <row r="35" spans="1:19">
+      <c r="T34" s="17"/>
+    </row>
+    <row r="35" spans="1:20">
       <c r="A35" t="s">
         <v>59</v>
       </c>
-      <c r="S35" s="17"/>
-    </row>
-    <row r="36" spans="1:19">
+      <c r="T35" s="17"/>
+    </row>
+    <row r="36" spans="1:20">
       <c r="A36" t="s">
         <v>60</v>
       </c>
-      <c r="S36" s="17"/>
-    </row>
-    <row r="37" spans="1:19">
+      <c r="T36" s="17"/>
+    </row>
+    <row r="37" spans="1:20">
       <c r="A37" t="s">
         <v>61</v>
       </c>
-      <c r="S37" s="17"/>
-    </row>
-    <row r="38" spans="1:19">
+      <c r="T37" s="17"/>
+    </row>
+    <row r="38" spans="1:20">
       <c r="A38" t="s">
         <v>62</v>
       </c>
-      <c r="S38" s="17"/>
-    </row>
-    <row r="39" spans="1:19">
+      <c r="T38" s="17"/>
+    </row>
+    <row r="39" spans="1:20">
       <c r="A39" t="s">
         <v>63</v>
       </c>
-      <c r="S39" s="17"/>
-    </row>
-    <row r="40" spans="1:19">
+      <c r="T39" s="17"/>
+    </row>
+    <row r="40" spans="1:20">
       <c r="A40" t="s">
         <v>64</v>
       </c>
-      <c r="S40" s="17"/>
-    </row>
-    <row r="41" spans="1:19">
+      <c r="T40" s="17"/>
+    </row>
+    <row r="41" spans="1:20">
       <c r="A41" t="s">
         <v>65</v>
       </c>
-      <c r="S41" s="17"/>
-    </row>
-    <row r="42" spans="1:19">
+      <c r="T41" s="17"/>
+    </row>
+    <row r="42" spans="1:20">
       <c r="A42" t="s">
         <v>66</v>
       </c>
-      <c r="S42" s="17"/>
-    </row>
-    <row r="43" spans="1:19">
+      <c r="T42" s="17"/>
+    </row>
+    <row r="43" spans="1:20">
       <c r="A43" t="s">
         <v>67</v>
       </c>
-      <c r="S43" s="17"/>
-    </row>
-    <row r="44" spans="1:19">
+      <c r="T43" s="17"/>
+    </row>
+    <row r="44" spans="1:20">
       <c r="A44" t="s">
         <v>68</v>
       </c>
-      <c r="S44" s="17"/>
-    </row>
-    <row r="45" spans="1:19">
+      <c r="T44" s="17"/>
+    </row>
+    <row r="45" spans="1:20">
       <c r="A45" t="s">
         <v>69</v>
       </c>
-      <c r="S45" s="17"/>
-    </row>
-    <row r="46" spans="1:19">
+      <c r="T45" s="17"/>
+    </row>
+    <row r="46" spans="1:20">
       <c r="A46" t="s">
         <v>70</v>
       </c>
-      <c r="S46" s="17"/>
-    </row>
-    <row r="47" spans="1:19">
+      <c r="T46" s="17"/>
+    </row>
+    <row r="47" spans="1:20">
       <c r="A47" t="s">
         <v>71</v>
       </c>
-      <c r="S47" s="17"/>
-    </row>
-    <row r="48" spans="1:19">
+      <c r="T47" s="17"/>
+    </row>
+    <row r="48" spans="1:20">
       <c r="A48" t="s">
         <v>72</v>
       </c>
-      <c r="S48" s="17"/>
-    </row>
-    <row r="49" spans="1:19">
+      <c r="T48" s="17"/>
+    </row>
+    <row r="49" spans="1:20">
       <c r="A49" t="s">
         <v>73</v>
       </c>
-      <c r="S49" s="17"/>
-    </row>
-    <row r="50" spans="1:19">
+      <c r="T49" s="17"/>
+    </row>
+    <row r="50" spans="1:20">
       <c r="A50" t="s">
         <v>74</v>
       </c>
-      <c r="S50" s="17"/>
-    </row>
-    <row r="51" spans="1:19">
+      <c r="T50" s="17"/>
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51" t="s">
         <v>75</v>
       </c>
-      <c r="S51" s="17"/>
-    </row>
-    <row r="52" spans="1:19">
+      <c r="T51" s="17"/>
+    </row>
+    <row r="52" spans="1:20">
       <c r="A52" t="s">
         <v>76</v>
       </c>
-      <c r="S52" s="17"/>
-    </row>
-    <row r="53" spans="1:19">
+      <c r="T52" s="17"/>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" t="s">
         <v>77</v>
       </c>
-      <c r="S53" s="17"/>
-    </row>
-    <row r="54" spans="1:19">
+      <c r="T53" s="17"/>
+    </row>
+    <row r="54" spans="1:20">
       <c r="A54" t="s">
         <v>78</v>
       </c>
-      <c r="S54" s="17"/>
-    </row>
-    <row r="55" spans="1:19">
+      <c r="T54" s="17"/>
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55" t="s">
         <v>79</v>
       </c>
-      <c r="S55" s="17"/>
-    </row>
-    <row r="56" spans="1:19">
+      <c r="T55" s="17"/>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56" t="s">
         <v>80</v>
       </c>
-      <c r="S56" s="17"/>
-    </row>
-    <row r="57" spans="1:19">
+      <c r="T56" s="17"/>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57" t="s">
         <v>81</v>
       </c>
-      <c r="S57" s="17"/>
-    </row>
-    <row r="58" spans="1:19">
+      <c r="T57" s="17"/>
+    </row>
+    <row r="58" spans="1:20">
       <c r="A58" t="s">
         <v>82</v>
       </c>
-      <c r="S58" s="17"/>
-    </row>
-    <row r="59" spans="1:19">
+      <c r="T58" s="17"/>
+    </row>
+    <row r="59" spans="1:20">
       <c r="A59" t="s">
         <v>83</v>
       </c>
-      <c r="S59" s="17"/>
-    </row>
-    <row r="60" spans="1:19">
+      <c r="T59" s="17"/>
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60" t="s">
         <v>84</v>
       </c>
-      <c r="S60" s="17"/>
-    </row>
-    <row r="61" spans="1:19">
+      <c r="T60" s="17"/>
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61" t="s">
         <v>85</v>
       </c>
-      <c r="S61" s="17"/>
-    </row>
-    <row r="62" spans="1:19">
+      <c r="T61" s="17"/>
+    </row>
+    <row r="62" spans="1:20">
       <c r="A62" t="s">
         <v>86</v>
       </c>
-      <c r="S62" s="17"/>
-    </row>
-    <row r="63" spans="1:19">
+      <c r="T62" s="17"/>
+    </row>
+    <row r="63" spans="1:20">
       <c r="A63" t="s">
         <v>87</v>
       </c>
-      <c r="S63" s="17"/>
-    </row>
-    <row r="64" spans="1:19">
+      <c r="T63" s="17"/>
+    </row>
+    <row r="64" spans="1:20">
       <c r="A64" t="s">
         <v>88</v>
       </c>
-      <c r="S64" s="17"/>
-    </row>
-    <row r="65" spans="1:20">
+      <c r="T64" s="17"/>
+    </row>
+    <row r="65" spans="1:21">
       <c r="A65" t="s">
         <v>89</v>
       </c>
-      <c r="S65" s="17"/>
-    </row>
-    <row r="66" spans="1:20">
+      <c r="T65" s="17"/>
+    </row>
+    <row r="66" spans="1:21">
       <c r="A66" t="s">
         <v>90</v>
       </c>
-      <c r="S66" s="17"/>
-    </row>
-    <row r="67" spans="1:20">
+      <c r="T66" s="17"/>
+    </row>
+    <row r="67" spans="1:21">
       <c r="A67" t="s">
         <v>91</v>
       </c>
-      <c r="S67" s="17"/>
-    </row>
-    <row r="68" spans="1:20">
+      <c r="T67" s="17"/>
+    </row>
+    <row r="68" spans="1:21">
       <c r="A68" t="s">
         <v>92</v>
       </c>
-      <c r="S68" s="17"/>
-    </row>
-    <row r="69" spans="1:20">
+      <c r="T68" s="17"/>
+    </row>
+    <row r="69" spans="1:21">
       <c r="A69" t="s">
         <v>93</v>
       </c>
-      <c r="S69" s="17"/>
-    </row>
-    <row r="70" spans="1:20">
+      <c r="T69" s="17"/>
+    </row>
+    <row r="70" spans="1:21">
       <c r="A70" t="s">
         <v>94</v>
       </c>
-      <c r="S70" s="17"/>
-    </row>
-    <row r="71" spans="1:20">
-      <c r="M71" s="22"/>
+      <c r="T70" s="17"/>
+    </row>
+    <row r="71" spans="1:21">
       <c r="N71" s="22"/>
       <c r="O71" s="22"/>
       <c r="P71" s="22"/>
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
-      <c r="S71" s="17"/>
+      <c r="S71" s="22"/>
       <c r="T71" s="17"/>
-    </row>
-    <row r="72" spans="1:20">
-      <c r="S72" s="17"/>
-    </row>
-    <row r="73" spans="1:20">
-      <c r="S73" s="17"/>
-    </row>
-    <row r="74" spans="1:20">
-      <c r="S74" s="17"/>
-    </row>
-    <row r="75" spans="1:20">
-      <c r="S75" s="17"/>
-    </row>
-    <row r="76" spans="1:20">
+      <c r="U71" s="17"/>
+    </row>
+    <row r="72" spans="1:21">
+      <c r="T72" s="17"/>
+    </row>
+    <row r="73" spans="1:21">
+      <c r="T73" s="17"/>
+    </row>
+    <row r="74" spans="1:21">
+      <c r="T74" s="17"/>
+    </row>
+    <row r="75" spans="1:21">
+      <c r="T75" s="17"/>
+    </row>
+    <row r="76" spans="1:21">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -6956,733 +6998,734 @@
       <c r="J76" s="17"/>
       <c r="K76" s="17"/>
       <c r="L76" s="17"/>
-      <c r="S76" s="17"/>
-    </row>
-    <row r="77" spans="1:20">
+      <c r="M76" s="17"/>
+      <c r="T76" s="17"/>
+    </row>
+    <row r="77" spans="1:21">
       <c r="A77" t="s">
         <v>171</v>
       </c>
-      <c r="S77" s="17"/>
-    </row>
-    <row r="78" spans="1:20">
+      <c r="T77" s="17"/>
+    </row>
+    <row r="78" spans="1:21">
       <c r="A78" t="s">
         <v>172</v>
       </c>
-      <c r="S78" s="17"/>
-    </row>
-    <row r="79" spans="1:20">
+      <c r="T78" s="17"/>
+    </row>
+    <row r="79" spans="1:21">
       <c r="A79" t="s">
         <v>173</v>
       </c>
-      <c r="S79" s="17"/>
-    </row>
-    <row r="80" spans="1:20">
+      <c r="T79" s="17"/>
+    </row>
+    <row r="80" spans="1:21">
       <c r="A80" t="s">
         <v>174</v>
       </c>
-      <c r="S80" s="17"/>
-    </row>
-    <row r="81" spans="1:19">
+      <c r="T80" s="17"/>
+    </row>
+    <row r="81" spans="1:20">
       <c r="A81" t="s">
         <v>175</v>
       </c>
-      <c r="S81" s="17"/>
-    </row>
-    <row r="82" spans="1:19">
+      <c r="T81" s="17"/>
+    </row>
+    <row r="82" spans="1:20">
       <c r="A82" t="s">
         <v>176</v>
       </c>
-      <c r="S82" s="17"/>
-    </row>
-    <row r="83" spans="1:19">
+      <c r="T82" s="17"/>
+    </row>
+    <row r="83" spans="1:20">
       <c r="A83" t="s">
         <v>177</v>
       </c>
-      <c r="S83" s="17"/>
-    </row>
-    <row r="84" spans="1:19">
+      <c r="T83" s="17"/>
+    </row>
+    <row r="84" spans="1:20">
       <c r="A84" t="s">
         <v>178</v>
       </c>
-      <c r="S84" s="17"/>
-    </row>
-    <row r="85" spans="1:19">
+      <c r="T84" s="17"/>
+    </row>
+    <row r="85" spans="1:20">
       <c r="A85" t="s">
         <v>179</v>
       </c>
-      <c r="S85" s="17"/>
-    </row>
-    <row r="86" spans="1:19">
+      <c r="T85" s="17"/>
+    </row>
+    <row r="86" spans="1:20">
       <c r="A86" t="s">
         <v>180</v>
       </c>
-      <c r="S86" s="17"/>
-    </row>
-    <row r="87" spans="1:19">
+      <c r="T86" s="17"/>
+    </row>
+    <row r="87" spans="1:20">
       <c r="A87" t="s">
         <v>181</v>
       </c>
-      <c r="S87" s="17"/>
-    </row>
-    <row r="88" spans="1:19">
+      <c r="T87" s="17"/>
+    </row>
+    <row r="88" spans="1:20">
       <c r="A88" t="s">
         <v>182</v>
       </c>
-      <c r="S88" s="17"/>
-    </row>
-    <row r="89" spans="1:19">
+      <c r="T88" s="17"/>
+    </row>
+    <row r="89" spans="1:20">
       <c r="A89" t="s">
         <v>183</v>
       </c>
-      <c r="S89" s="17"/>
-    </row>
-    <row r="90" spans="1:19">
+      <c r="T89" s="17"/>
+    </row>
+    <row r="90" spans="1:20">
       <c r="A90" t="s">
         <v>184</v>
       </c>
-      <c r="S90" s="17"/>
-    </row>
-    <row r="91" spans="1:19">
+      <c r="T90" s="17"/>
+    </row>
+    <row r="91" spans="1:20">
       <c r="A91" t="s">
         <v>185</v>
       </c>
-      <c r="S91" s="17"/>
-    </row>
-    <row r="92" spans="1:19">
+      <c r="T91" s="17"/>
+    </row>
+    <row r="92" spans="1:20">
       <c r="A92" t="s">
         <v>186</v>
       </c>
-      <c r="S92" s="17"/>
-    </row>
-    <row r="93" spans="1:19">
+      <c r="T92" s="17"/>
+    </row>
+    <row r="93" spans="1:20">
       <c r="A93" t="s">
         <v>187</v>
       </c>
-      <c r="S93" s="17"/>
-    </row>
-    <row r="94" spans="1:19">
+      <c r="T93" s="17"/>
+    </row>
+    <row r="94" spans="1:20">
       <c r="A94" t="s">
         <v>188</v>
       </c>
-      <c r="S94" s="17"/>
-    </row>
-    <row r="95" spans="1:19">
+      <c r="T94" s="17"/>
+    </row>
+    <row r="95" spans="1:20">
       <c r="A95" t="s">
         <v>189</v>
       </c>
-      <c r="S95" s="17"/>
-    </row>
-    <row r="96" spans="1:19">
+      <c r="T95" s="17"/>
+    </row>
+    <row r="96" spans="1:20">
       <c r="A96" t="s">
         <v>190</v>
       </c>
-      <c r="S96" s="17"/>
-    </row>
-    <row r="97" spans="1:19">
+      <c r="T96" s="17"/>
+    </row>
+    <row r="97" spans="1:20">
       <c r="A97" t="s">
         <v>191</v>
       </c>
-      <c r="S97" s="17"/>
-    </row>
-    <row r="98" spans="1:19">
+      <c r="T97" s="17"/>
+    </row>
+    <row r="98" spans="1:20">
       <c r="A98" t="s">
         <v>192</v>
       </c>
-      <c r="S98" s="17"/>
-    </row>
-    <row r="99" spans="1:19">
+      <c r="T98" s="17"/>
+    </row>
+    <row r="99" spans="1:20">
       <c r="A99" t="s">
         <v>193</v>
       </c>
-      <c r="S99" s="17"/>
-    </row>
-    <row r="100" spans="1:19">
+      <c r="T99" s="17"/>
+    </row>
+    <row r="100" spans="1:20">
       <c r="A100" t="s">
         <v>194</v>
       </c>
-      <c r="S100" s="17"/>
-    </row>
-    <row r="101" spans="1:19">
+      <c r="T100" s="17"/>
+    </row>
+    <row r="101" spans="1:20">
       <c r="A101" t="s">
         <v>195</v>
       </c>
-      <c r="S101" s="17"/>
-    </row>
-    <row r="102" spans="1:19">
+      <c r="T101" s="17"/>
+    </row>
+    <row r="102" spans="1:20">
       <c r="A102" t="s">
         <v>196</v>
       </c>
-      <c r="S102" s="17"/>
-    </row>
-    <row r="103" spans="1:19">
+      <c r="T102" s="17"/>
+    </row>
+    <row r="103" spans="1:20">
       <c r="A103" t="s">
         <v>197</v>
       </c>
-      <c r="S103" s="17"/>
-    </row>
-    <row r="104" spans="1:19">
+      <c r="T103" s="17"/>
+    </row>
+    <row r="104" spans="1:20">
       <c r="A104" t="s">
         <v>198</v>
       </c>
-      <c r="S104" s="17"/>
-    </row>
-    <row r="105" spans="1:19">
+      <c r="T104" s="17"/>
+    </row>
+    <row r="105" spans="1:20">
       <c r="A105" t="s">
         <v>199</v>
       </c>
-      <c r="S105" s="17"/>
-    </row>
-    <row r="106" spans="1:19">
+      <c r="T105" s="17"/>
+    </row>
+    <row r="106" spans="1:20">
       <c r="A106" t="s">
         <v>200</v>
       </c>
-      <c r="S106" s="17"/>
-    </row>
-    <row r="107" spans="1:19">
+      <c r="T106" s="17"/>
+    </row>
+    <row r="107" spans="1:20">
       <c r="A107" t="s">
         <v>201</v>
       </c>
-      <c r="S107" s="17"/>
-    </row>
-    <row r="108" spans="1:19">
+      <c r="T107" s="17"/>
+    </row>
+    <row r="108" spans="1:20">
       <c r="A108" t="s">
         <v>202</v>
       </c>
-      <c r="S108" s="17"/>
-    </row>
-    <row r="109" spans="1:19">
+      <c r="T108" s="17"/>
+    </row>
+    <row r="109" spans="1:20">
       <c r="A109" t="s">
         <v>203</v>
       </c>
-      <c r="S109" s="17"/>
-    </row>
-    <row r="110" spans="1:19">
+      <c r="T109" s="17"/>
+    </row>
+    <row r="110" spans="1:20">
       <c r="A110" t="s">
         <v>204</v>
       </c>
-      <c r="S110" s="17"/>
-    </row>
-    <row r="111" spans="1:19">
+      <c r="T110" s="17"/>
+    </row>
+    <row r="111" spans="1:20">
       <c r="A111" t="s">
         <v>205</v>
       </c>
-      <c r="S111" s="17"/>
-    </row>
-    <row r="112" spans="1:19">
+      <c r="T111" s="17"/>
+    </row>
+    <row r="112" spans="1:20">
       <c r="A112" t="s">
         <v>206</v>
       </c>
-      <c r="S112" s="17"/>
-    </row>
-    <row r="113" spans="1:19">
+      <c r="T112" s="17"/>
+    </row>
+    <row r="113" spans="1:20">
       <c r="A113" t="s">
         <v>207</v>
       </c>
-      <c r="S113" s="17"/>
-    </row>
-    <row r="114" spans="1:19">
+      <c r="T113" s="17"/>
+    </row>
+    <row r="114" spans="1:20">
       <c r="A114" t="s">
         <v>208</v>
       </c>
-      <c r="S114" s="17"/>
-    </row>
-    <row r="115" spans="1:19">
-      <c r="S115" s="17"/>
-    </row>
-    <row r="116" spans="1:19">
-      <c r="S116" s="17"/>
-    </row>
-    <row r="117" spans="1:19">
-      <c r="S117" s="17"/>
-    </row>
-    <row r="118" spans="1:19">
-      <c r="S118" s="17"/>
-    </row>
-    <row r="119" spans="1:19">
-      <c r="S119" s="17"/>
-    </row>
-    <row r="120" spans="1:19">
-      <c r="S120" s="17"/>
-    </row>
-    <row r="121" spans="1:19">
+      <c r="T114" s="17"/>
+    </row>
+    <row r="115" spans="1:20">
+      <c r="T115" s="17"/>
+    </row>
+    <row r="116" spans="1:20">
+      <c r="T116" s="17"/>
+    </row>
+    <row r="117" spans="1:20">
+      <c r="T117" s="17"/>
+    </row>
+    <row r="118" spans="1:20">
+      <c r="T118" s="17"/>
+    </row>
+    <row r="119" spans="1:20">
+      <c r="T119" s="17"/>
+    </row>
+    <row r="120" spans="1:20">
+      <c r="T120" s="17"/>
+    </row>
+    <row r="121" spans="1:20">
       <c r="A121" t="s">
         <v>133</v>
       </c>
-      <c r="S121" s="17"/>
-    </row>
-    <row r="122" spans="1:19">
+      <c r="T121" s="17"/>
+    </row>
+    <row r="122" spans="1:20">
       <c r="A122" t="s">
         <v>134</v>
       </c>
-      <c r="S122" s="17"/>
-    </row>
-    <row r="123" spans="1:19">
+      <c r="T122" s="17"/>
+    </row>
+    <row r="123" spans="1:20">
       <c r="A123" t="s">
         <v>135</v>
       </c>
-      <c r="S123" s="17"/>
-    </row>
-    <row r="124" spans="1:19">
+      <c r="T123" s="17"/>
+    </row>
+    <row r="124" spans="1:20">
       <c r="A124" t="s">
         <v>136</v>
       </c>
-      <c r="S124" s="17"/>
-    </row>
-    <row r="125" spans="1:19">
+      <c r="T124" s="17"/>
+    </row>
+    <row r="125" spans="1:20">
       <c r="A125" t="s">
         <v>137</v>
       </c>
-      <c r="S125" s="17"/>
-    </row>
-    <row r="126" spans="1:19">
+      <c r="T125" s="17"/>
+    </row>
+    <row r="126" spans="1:20">
       <c r="A126" t="s">
         <v>138</v>
       </c>
-      <c r="S126" s="17"/>
-    </row>
-    <row r="127" spans="1:19">
+      <c r="T126" s="17"/>
+    </row>
+    <row r="127" spans="1:20">
       <c r="A127" t="s">
         <v>139</v>
       </c>
-      <c r="S127" s="17"/>
-    </row>
-    <row r="128" spans="1:19">
+      <c r="T127" s="17"/>
+    </row>
+    <row r="128" spans="1:20">
       <c r="A128" t="s">
         <v>140</v>
       </c>
-      <c r="S128" s="17"/>
-    </row>
-    <row r="129" spans="1:19">
+      <c r="T128" s="17"/>
+    </row>
+    <row r="129" spans="1:20">
       <c r="A129" t="s">
         <v>141</v>
       </c>
-      <c r="S129" s="17"/>
-    </row>
-    <row r="130" spans="1:19">
+      <c r="T129" s="17"/>
+    </row>
+    <row r="130" spans="1:20">
       <c r="A130" t="s">
         <v>142</v>
       </c>
-      <c r="S130" s="17"/>
-    </row>
-    <row r="131" spans="1:19">
+      <c r="T130" s="17"/>
+    </row>
+    <row r="131" spans="1:20">
       <c r="A131" t="s">
         <v>143</v>
       </c>
-      <c r="S131" s="17"/>
-    </row>
-    <row r="132" spans="1:19">
+      <c r="T131" s="17"/>
+    </row>
+    <row r="132" spans="1:20">
       <c r="A132" t="s">
         <v>144</v>
       </c>
-      <c r="S132" s="17"/>
-    </row>
-    <row r="133" spans="1:19">
+      <c r="T132" s="17"/>
+    </row>
+    <row r="133" spans="1:20">
       <c r="A133" t="s">
         <v>145</v>
       </c>
-      <c r="S133" s="17"/>
-    </row>
-    <row r="134" spans="1:19">
+      <c r="T133" s="17"/>
+    </row>
+    <row r="134" spans="1:20">
       <c r="A134" t="s">
         <v>146</v>
       </c>
-      <c r="S134" s="17"/>
-    </row>
-    <row r="135" spans="1:19">
+      <c r="T134" s="17"/>
+    </row>
+    <row r="135" spans="1:20">
       <c r="A135" t="s">
         <v>147</v>
       </c>
-      <c r="S135" s="17"/>
-    </row>
-    <row r="136" spans="1:19">
+      <c r="T135" s="17"/>
+    </row>
+    <row r="136" spans="1:20">
       <c r="A136" t="s">
         <v>148</v>
       </c>
-      <c r="S136" s="17"/>
-    </row>
-    <row r="137" spans="1:19">
+      <c r="T136" s="17"/>
+    </row>
+    <row r="137" spans="1:20">
       <c r="A137" t="s">
         <v>149</v>
       </c>
-      <c r="S137" s="17"/>
-    </row>
-    <row r="138" spans="1:19">
+      <c r="T137" s="17"/>
+    </row>
+    <row r="138" spans="1:20">
       <c r="A138" t="s">
         <v>150</v>
       </c>
-      <c r="S138" s="17"/>
-    </row>
-    <row r="139" spans="1:19">
+      <c r="T138" s="17"/>
+    </row>
+    <row r="139" spans="1:20">
       <c r="A139" t="s">
         <v>151</v>
       </c>
-      <c r="S139" s="17"/>
-    </row>
-    <row r="140" spans="1:19">
+      <c r="T139" s="17"/>
+    </row>
+    <row r="140" spans="1:20">
       <c r="A140" t="s">
         <v>152</v>
       </c>
-      <c r="S140" s="17"/>
-    </row>
-    <row r="141" spans="1:19">
+      <c r="T140" s="17"/>
+    </row>
+    <row r="141" spans="1:20">
       <c r="A141" t="s">
         <v>153</v>
       </c>
-      <c r="S141" s="17"/>
-    </row>
-    <row r="142" spans="1:19">
+      <c r="T141" s="17"/>
+    </row>
+    <row r="142" spans="1:20">
       <c r="A142" t="s">
         <v>154</v>
       </c>
-      <c r="S142" s="17"/>
-    </row>
-    <row r="143" spans="1:19">
+      <c r="T142" s="17"/>
+    </row>
+    <row r="143" spans="1:20">
       <c r="A143" t="s">
         <v>155</v>
       </c>
-      <c r="S143" s="17"/>
-    </row>
-    <row r="144" spans="1:19">
+      <c r="T143" s="17"/>
+    </row>
+    <row r="144" spans="1:20">
       <c r="A144" t="s">
         <v>156</v>
       </c>
-      <c r="S144" s="17"/>
-    </row>
-    <row r="145" spans="1:19">
+      <c r="T144" s="17"/>
+    </row>
+    <row r="145" spans="1:20">
       <c r="A145" t="s">
         <v>157</v>
       </c>
-      <c r="S145" s="17"/>
-    </row>
-    <row r="146" spans="1:19">
+      <c r="T145" s="17"/>
+    </row>
+    <row r="146" spans="1:20">
       <c r="A146" t="s">
         <v>158</v>
       </c>
-      <c r="S146" s="17"/>
-    </row>
-    <row r="147" spans="1:19">
+      <c r="T146" s="17"/>
+    </row>
+    <row r="147" spans="1:20">
       <c r="A147" t="s">
         <v>159</v>
       </c>
-      <c r="S147" s="17"/>
-    </row>
-    <row r="148" spans="1:19">
+      <c r="T147" s="17"/>
+    </row>
+    <row r="148" spans="1:20">
       <c r="A148" t="s">
         <v>160</v>
       </c>
-      <c r="S148" s="17"/>
-    </row>
-    <row r="149" spans="1:19">
+      <c r="T148" s="17"/>
+    </row>
+    <row r="149" spans="1:20">
       <c r="A149" t="s">
         <v>161</v>
       </c>
-      <c r="S149" s="17"/>
-    </row>
-    <row r="150" spans="1:19">
+      <c r="T149" s="17"/>
+    </row>
+    <row r="150" spans="1:20">
       <c r="A150" t="s">
         <v>162</v>
       </c>
-      <c r="S150" s="17"/>
-    </row>
-    <row r="151" spans="1:19">
+      <c r="T150" s="17"/>
+    </row>
+    <row r="151" spans="1:20">
       <c r="A151" t="s">
         <v>163</v>
       </c>
-      <c r="S151" s="17"/>
-    </row>
-    <row r="152" spans="1:19">
+      <c r="T151" s="17"/>
+    </row>
+    <row r="152" spans="1:20">
       <c r="A152" t="s">
         <v>164</v>
       </c>
-      <c r="S152" s="17"/>
-    </row>
-    <row r="153" spans="1:19">
+      <c r="T152" s="17"/>
+    </row>
+    <row r="153" spans="1:20">
       <c r="A153" t="s">
         <v>165</v>
       </c>
-      <c r="S153" s="17"/>
-    </row>
-    <row r="154" spans="1:19">
+      <c r="T153" s="17"/>
+    </row>
+    <row r="154" spans="1:20">
       <c r="A154" t="s">
         <v>166</v>
       </c>
-      <c r="S154" s="17"/>
-    </row>
-    <row r="155" spans="1:19">
+      <c r="T154" s="17"/>
+    </row>
+    <row r="155" spans="1:20">
       <c r="A155" t="s">
         <v>167</v>
       </c>
-      <c r="S155" s="17"/>
-    </row>
-    <row r="156" spans="1:19">
+      <c r="T155" s="17"/>
+    </row>
+    <row r="156" spans="1:20">
       <c r="A156" t="s">
         <v>168</v>
       </c>
-      <c r="S156" s="17"/>
-    </row>
-    <row r="157" spans="1:19">
+      <c r="T156" s="17"/>
+    </row>
+    <row r="157" spans="1:20">
       <c r="A157" t="s">
         <v>169</v>
       </c>
-      <c r="S157" s="17"/>
-    </row>
-    <row r="158" spans="1:19">
+      <c r="T157" s="17"/>
+    </row>
+    <row r="158" spans="1:20">
       <c r="A158" t="s">
         <v>170</v>
       </c>
-      <c r="S158" s="17"/>
-    </row>
-    <row r="159" spans="1:19">
-      <c r="S159" s="17"/>
-    </row>
-    <row r="160" spans="1:19">
-      <c r="S160" s="17"/>
-    </row>
-    <row r="161" spans="1:19">
-      <c r="S161" s="17"/>
-    </row>
-    <row r="162" spans="1:19">
-      <c r="S162" s="17"/>
-    </row>
-    <row r="163" spans="1:19">
-      <c r="S163" s="17"/>
-    </row>
-    <row r="164" spans="1:19">
-      <c r="S164" s="17"/>
-    </row>
-    <row r="165" spans="1:19">
+      <c r="T158" s="17"/>
+    </row>
+    <row r="159" spans="1:20">
+      <c r="T159" s="17"/>
+    </row>
+    <row r="160" spans="1:20">
+      <c r="T160" s="17"/>
+    </row>
+    <row r="161" spans="1:20">
+      <c r="T161" s="17"/>
+    </row>
+    <row r="162" spans="1:20">
+      <c r="T162" s="17"/>
+    </row>
+    <row r="163" spans="1:20">
+      <c r="T163" s="17"/>
+    </row>
+    <row r="164" spans="1:20">
+      <c r="T164" s="17"/>
+    </row>
+    <row r="165" spans="1:20">
       <c r="A165" t="s">
         <v>95</v>
       </c>
-      <c r="S165" s="17"/>
-    </row>
-    <row r="166" spans="1:19">
+      <c r="T165" s="17"/>
+    </row>
+    <row r="166" spans="1:20">
       <c r="A166" t="s">
         <v>96</v>
       </c>
-      <c r="S166" s="17"/>
-    </row>
-    <row r="167" spans="1:19">
+      <c r="T166" s="17"/>
+    </row>
+    <row r="167" spans="1:20">
       <c r="A167" t="s">
         <v>97</v>
       </c>
-      <c r="S167" s="17"/>
-    </row>
-    <row r="168" spans="1:19">
+      <c r="T167" s="17"/>
+    </row>
+    <row r="168" spans="1:20">
       <c r="A168" t="s">
         <v>98</v>
       </c>
-      <c r="S168" s="17"/>
-    </row>
-    <row r="169" spans="1:19">
+      <c r="T168" s="17"/>
+    </row>
+    <row r="169" spans="1:20">
       <c r="A169" t="s">
         <v>99</v>
       </c>
-      <c r="S169" s="17"/>
-    </row>
-    <row r="170" spans="1:19">
+      <c r="T169" s="17"/>
+    </row>
+    <row r="170" spans="1:20">
       <c r="A170" t="s">
         <v>100</v>
       </c>
-      <c r="S170" s="17"/>
-    </row>
-    <row r="171" spans="1:19">
+      <c r="T170" s="17"/>
+    </row>
+    <row r="171" spans="1:20">
       <c r="A171" t="s">
         <v>101</v>
       </c>
-      <c r="S171" s="17"/>
-    </row>
-    <row r="172" spans="1:19">
+      <c r="T171" s="17"/>
+    </row>
+    <row r="172" spans="1:20">
       <c r="A172" t="s">
         <v>102</v>
       </c>
-      <c r="S172" s="17"/>
-    </row>
-    <row r="173" spans="1:19">
+      <c r="T172" s="17"/>
+    </row>
+    <row r="173" spans="1:20">
       <c r="A173" t="s">
         <v>103</v>
       </c>
-      <c r="S173" s="17"/>
-    </row>
-    <row r="174" spans="1:19">
+      <c r="T173" s="17"/>
+    </row>
+    <row r="174" spans="1:20">
       <c r="A174" t="s">
         <v>104</v>
       </c>
-      <c r="S174" s="17"/>
-    </row>
-    <row r="175" spans="1:19">
+      <c r="T174" s="17"/>
+    </row>
+    <row r="175" spans="1:20">
       <c r="A175" t="s">
         <v>105</v>
       </c>
-      <c r="S175" s="17"/>
-    </row>
-    <row r="176" spans="1:19">
+      <c r="T175" s="17"/>
+    </row>
+    <row r="176" spans="1:20">
       <c r="A176" t="s">
         <v>106</v>
       </c>
-      <c r="S176" s="17"/>
-    </row>
-    <row r="177" spans="1:19">
+      <c r="T176" s="17"/>
+    </row>
+    <row r="177" spans="1:20">
       <c r="A177" t="s">
         <v>107</v>
       </c>
-      <c r="S177" s="17"/>
-    </row>
-    <row r="178" spans="1:19">
+      <c r="T177" s="17"/>
+    </row>
+    <row r="178" spans="1:20">
       <c r="A178" t="s">
         <v>108</v>
       </c>
-      <c r="S178" s="17"/>
-    </row>
-    <row r="179" spans="1:19">
+      <c r="T178" s="17"/>
+    </row>
+    <row r="179" spans="1:20">
       <c r="A179" t="s">
         <v>109</v>
       </c>
-      <c r="S179" s="17"/>
-    </row>
-    <row r="180" spans="1:19">
+      <c r="T179" s="17"/>
+    </row>
+    <row r="180" spans="1:20">
       <c r="A180" t="s">
         <v>110</v>
       </c>
-      <c r="S180" s="17"/>
-    </row>
-    <row r="181" spans="1:19">
+      <c r="T180" s="17"/>
+    </row>
+    <row r="181" spans="1:20">
       <c r="A181" t="s">
         <v>111</v>
       </c>
-      <c r="S181" s="17"/>
-    </row>
-    <row r="182" spans="1:19">
+      <c r="T181" s="17"/>
+    </row>
+    <row r="182" spans="1:20">
       <c r="A182" t="s">
         <v>112</v>
       </c>
-      <c r="S182" s="17"/>
-    </row>
-    <row r="183" spans="1:19">
+      <c r="T182" s="17"/>
+    </row>
+    <row r="183" spans="1:20">
       <c r="A183" t="s">
         <v>113</v>
       </c>
-      <c r="S183" s="17"/>
-    </row>
-    <row r="184" spans="1:19">
+      <c r="T183" s="17"/>
+    </row>
+    <row r="184" spans="1:20">
       <c r="A184" t="s">
         <v>114</v>
       </c>
-      <c r="S184" s="17"/>
-    </row>
-    <row r="185" spans="1:19">
+      <c r="T184" s="17"/>
+    </row>
+    <row r="185" spans="1:20">
       <c r="A185" t="s">
         <v>115</v>
       </c>
-      <c r="S185" s="17"/>
-    </row>
-    <row r="186" spans="1:19">
+      <c r="T185" s="17"/>
+    </row>
+    <row r="186" spans="1:20">
       <c r="A186" t="s">
         <v>116</v>
       </c>
-      <c r="M186" s="22"/>
       <c r="N186" s="22"/>
       <c r="O186" s="22"/>
       <c r="P186" s="22"/>
       <c r="Q186" s="22"/>
       <c r="R186" s="22"/>
-      <c r="S186" s="17"/>
-    </row>
-    <row r="187" spans="1:19">
+      <c r="S186" s="22"/>
+      <c r="T186" s="17"/>
+    </row>
+    <row r="187" spans="1:20">
       <c r="A187" t="s">
         <v>117</v>
       </c>
-      <c r="M187" s="22"/>
       <c r="N187" s="22"/>
       <c r="O187" s="22"/>
       <c r="P187" s="22"/>
       <c r="Q187" s="22"/>
       <c r="R187" s="22"/>
-      <c r="S187" s="17"/>
-    </row>
-    <row r="188" spans="1:19">
+      <c r="S187" s="22"/>
+      <c r="T187" s="17"/>
+    </row>
+    <row r="188" spans="1:20">
       <c r="A188" t="s">
         <v>118</v>
       </c>
-      <c r="M188" s="22"/>
       <c r="N188" s="22"/>
       <c r="O188" s="22"/>
       <c r="P188" s="22"/>
       <c r="Q188" s="22"/>
       <c r="R188" s="22"/>
-      <c r="S188" s="17"/>
-    </row>
-    <row r="189" spans="1:19">
+      <c r="S188" s="22"/>
+      <c r="T188" s="17"/>
+    </row>
+    <row r="189" spans="1:20">
       <c r="A189" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="190" spans="1:19">
+    <row r="190" spans="1:20">
       <c r="A190" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="191" spans="1:19">
+    <row r="191" spans="1:20">
       <c r="A191" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="192" spans="1:19">
+    <row r="192" spans="1:20">
       <c r="A192" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="193" spans="1:12">
+    <row r="193" spans="1:13">
       <c r="A193" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="194" spans="1:12">
+    <row r="194" spans="1:13">
       <c r="A194" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="195" spans="1:12">
+    <row r="195" spans="1:13">
       <c r="A195" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="196" spans="1:12">
+    <row r="196" spans="1:13">
       <c r="A196" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="197" spans="1:12">
+    <row r="197" spans="1:13">
       <c r="A197" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="198" spans="1:12">
+    <row r="198" spans="1:13">
       <c r="A198" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="199" spans="1:12">
+    <row r="199" spans="1:13">
       <c r="A199" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="200" spans="1:12">
+    <row r="200" spans="1:13">
       <c r="A200" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="201" spans="1:12">
+    <row r="201" spans="1:13">
       <c r="A201" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="202" spans="1:12">
+    <row r="202" spans="1:13">
       <c r="A202" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="203" spans="1:12">
+    <row r="203" spans="1:13">
       <c r="A203" s="17"/>
       <c r="B203" s="17"/>
       <c r="C203" s="17"/>
@@ -7695,8 +7738,9 @@
       <c r="J203" s="17"/>
       <c r="K203" s="17"/>
       <c r="L203" s="17"/>
-    </row>
-    <row r="204" spans="1:12">
+      <c r="M203" s="17"/>
+    </row>
+    <row r="204" spans="1:13">
       <c r="A204" s="17"/>
       <c r="B204" s="17"/>
       <c r="C204" s="17"/>
@@ -7709,8 +7753,9 @@
       <c r="J204" s="17"/>
       <c r="K204" s="17"/>
       <c r="L204" s="17"/>
-    </row>
-    <row r="205" spans="1:12">
+      <c r="M204" s="17"/>
+    </row>
+    <row r="205" spans="1:13">
       <c r="A205" s="17"/>
       <c r="B205" s="17"/>
       <c r="C205" s="17"/>
@@ -7723,8 +7768,9 @@
       <c r="J205" s="17"/>
       <c r="K205" s="17"/>
       <c r="L205" s="17"/>
-    </row>
-    <row r="206" spans="1:12">
+      <c r="M205" s="17"/>
+    </row>
+    <row r="206" spans="1:13">
       <c r="A206" s="17"/>
       <c r="B206" s="17"/>
       <c r="C206" s="17"/>
@@ -7737,8 +7783,9 @@
       <c r="J206" s="17"/>
       <c r="K206" s="17"/>
       <c r="L206" s="17"/>
-    </row>
-    <row r="207" spans="1:12">
+      <c r="M206" s="17"/>
+    </row>
+    <row r="207" spans="1:13">
       <c r="A207" s="17"/>
       <c r="B207" s="17"/>
       <c r="C207" s="17"/>
@@ -7751,8 +7798,9 @@
       <c r="J207" s="17"/>
       <c r="K207" s="17"/>
       <c r="L207" s="17"/>
-    </row>
-    <row r="208" spans="1:12">
+      <c r="M207" s="17"/>
+    </row>
+    <row r="208" spans="1:13">
       <c r="A208" s="17"/>
       <c r="B208" s="17"/>
       <c r="C208" s="17"/>
@@ -7765,6 +7813,7 @@
       <c r="J208" s="17"/>
       <c r="K208" s="17"/>
       <c r="L208" s="17"/>
+      <c r="M208" s="17"/>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
@@ -7921,27 +7970,27 @@
         <v>273</v>
       </c>
     </row>
-    <row r="241" spans="1:12">
+    <row r="241" spans="1:13">
       <c r="A241" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="242" spans="1:12">
+    <row r="242" spans="1:13">
       <c r="A242" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="243" spans="1:12">
+    <row r="243" spans="1:13">
       <c r="A243" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="244" spans="1:12">
+    <row r="244" spans="1:13">
       <c r="A244" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="253" spans="1:12">
+    <row r="253" spans="1:13">
       <c r="A253" s="15" t="s">
         <v>283</v>
       </c>
@@ -7956,18 +8005,19 @@
       <c r="J253" s="15"/>
       <c r="K253" s="15"/>
       <c r="L253" s="15"/>
-    </row>
-    <row r="254" spans="1:12">
+      <c r="M253" s="15"/>
+    </row>
+    <row r="254" spans="1:13">
       <c r="A254" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="255" spans="1:12">
+    <row r="255" spans="1:13">
       <c r="A255" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="256" spans="1:12">
+    <row r="256" spans="1:13">
       <c r="A256" t="s">
         <v>59</v>
       </c>
@@ -11812,181 +11862,181 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1025" spans="1:19">
+    <row r="1025" spans="1:20">
       <c r="A1025" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="1026" spans="1:19">
+    <row r="1026" spans="1:20">
       <c r="A1026" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="1027" spans="1:19">
+    <row r="1027" spans="1:20">
       <c r="A1027" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="1028" spans="1:19">
+    <row r="1028" spans="1:20">
       <c r="A1028" t="s">
         <v>908</v>
       </c>
-      <c r="S1028" s="17"/>
-    </row>
-    <row r="1029" spans="1:19">
+      <c r="T1028" s="17"/>
+    </row>
+    <row r="1029" spans="1:20">
       <c r="A1029" t="s">
         <v>909</v>
       </c>
-      <c r="S1029" s="17"/>
-    </row>
-    <row r="1030" spans="1:19">
+      <c r="T1029" s="17"/>
+    </row>
+    <row r="1030" spans="1:20">
       <c r="A1030" t="s">
         <v>910</v>
       </c>
-      <c r="S1030" s="17"/>
-    </row>
-    <row r="1031" spans="1:19">
+      <c r="T1030" s="17"/>
+    </row>
+    <row r="1031" spans="1:20">
       <c r="A1031" t="s">
         <v>911</v>
       </c>
-      <c r="S1031" s="17"/>
-    </row>
-    <row r="1032" spans="1:19">
+      <c r="T1031" s="17"/>
+    </row>
+    <row r="1032" spans="1:20">
       <c r="A1032" t="s">
         <v>912</v>
       </c>
-      <c r="S1032" s="17"/>
-    </row>
-    <row r="1033" spans="1:19">
+      <c r="T1032" s="17"/>
+    </row>
+    <row r="1033" spans="1:20">
       <c r="A1033" t="s">
         <v>913</v>
       </c>
-      <c r="S1033" s="17"/>
-    </row>
-    <row r="1034" spans="1:19">
+      <c r="T1033" s="17"/>
+    </row>
+    <row r="1034" spans="1:20">
       <c r="A1034" t="s">
         <v>914</v>
       </c>
-      <c r="S1034" s="17"/>
-    </row>
-    <row r="1035" spans="1:19">
+      <c r="T1034" s="17"/>
+    </row>
+    <row r="1035" spans="1:20">
       <c r="A1035" t="s">
         <v>915</v>
       </c>
-      <c r="S1035" s="17"/>
-    </row>
-    <row r="1036" spans="1:19">
+      <c r="T1035" s="17"/>
+    </row>
+    <row r="1036" spans="1:20">
       <c r="A1036" t="s">
         <v>916</v>
       </c>
-      <c r="S1036" s="17"/>
-    </row>
-    <row r="1037" spans="1:19">
+      <c r="T1036" s="17"/>
+    </row>
+    <row r="1037" spans="1:20">
       <c r="A1037" t="s">
         <v>917</v>
       </c>
-      <c r="S1037" s="17"/>
-    </row>
-    <row r="1038" spans="1:19">
+      <c r="T1037" s="17"/>
+    </row>
+    <row r="1038" spans="1:20">
       <c r="A1038" t="s">
         <v>918</v>
       </c>
-      <c r="S1038" s="17"/>
-    </row>
-    <row r="1039" spans="1:19">
+      <c r="T1038" s="17"/>
+    </row>
+    <row r="1039" spans="1:20">
       <c r="A1039" t="s">
         <v>919</v>
       </c>
-      <c r="S1039" s="17"/>
-    </row>
-    <row r="1040" spans="1:19">
+      <c r="T1039" s="17"/>
+    </row>
+    <row r="1040" spans="1:20">
       <c r="A1040" t="s">
         <v>920</v>
       </c>
-      <c r="S1040" s="17"/>
-    </row>
-    <row r="1041" spans="1:19">
+      <c r="T1040" s="17"/>
+    </row>
+    <row r="1041" spans="1:20">
       <c r="A1041" t="s">
         <v>921</v>
       </c>
-      <c r="S1041" s="17"/>
-    </row>
-    <row r="1042" spans="1:19">
+      <c r="T1041" s="17"/>
+    </row>
+    <row r="1042" spans="1:20">
       <c r="A1042" t="s">
         <v>922</v>
       </c>
-      <c r="S1042" s="17"/>
-    </row>
-    <row r="1043" spans="1:19">
+      <c r="T1042" s="17"/>
+    </row>
+    <row r="1043" spans="1:20">
       <c r="A1043" t="s">
         <v>923</v>
       </c>
-      <c r="S1043" s="17"/>
-    </row>
-    <row r="1044" spans="1:19">
+      <c r="T1043" s="17"/>
+    </row>
+    <row r="1044" spans="1:20">
       <c r="A1044" t="s">
         <v>924</v>
       </c>
-      <c r="S1044" s="17"/>
-    </row>
-    <row r="1045" spans="1:19">
+      <c r="T1044" s="17"/>
+    </row>
+    <row r="1045" spans="1:20">
       <c r="A1045" t="s">
         <v>925</v>
       </c>
-      <c r="S1045" s="17"/>
-    </row>
-    <row r="1046" spans="1:19">
+      <c r="T1045" s="17"/>
+    </row>
+    <row r="1046" spans="1:20">
       <c r="A1046" t="s">
         <v>926</v>
       </c>
-      <c r="S1046" s="17"/>
-    </row>
-    <row r="1047" spans="1:19">
+      <c r="T1046" s="17"/>
+    </row>
+    <row r="1047" spans="1:20">
       <c r="A1047" t="s">
         <v>927</v>
       </c>
-      <c r="S1047" s="17"/>
-    </row>
-    <row r="1048" spans="1:19">
+      <c r="T1047" s="17"/>
+    </row>
+    <row r="1048" spans="1:20">
       <c r="A1048" t="s">
         <v>928</v>
       </c>
-      <c r="S1048" s="17"/>
-    </row>
-    <row r="1049" spans="1:19">
+      <c r="T1048" s="17"/>
+    </row>
+    <row r="1049" spans="1:20">
       <c r="A1049" t="s">
         <v>929</v>
       </c>
-      <c r="S1049" s="17"/>
-    </row>
-    <row r="1050" spans="1:19">
+      <c r="T1049" s="17"/>
+    </row>
+    <row r="1050" spans="1:20">
       <c r="A1050" t="s">
         <v>930</v>
       </c>
-      <c r="S1050" s="17"/>
-    </row>
-    <row r="1051" spans="1:19">
+      <c r="T1050" s="17"/>
+    </row>
+    <row r="1051" spans="1:20">
       <c r="A1051" t="s">
         <v>931</v>
       </c>
-      <c r="S1051" s="17"/>
-    </row>
-    <row r="1052" spans="1:19">
+      <c r="T1051" s="17"/>
+    </row>
+    <row r="1052" spans="1:20">
       <c r="A1052" t="s">
         <v>932</v>
       </c>
-      <c r="S1052" s="17"/>
-    </row>
-    <row r="1053" spans="1:19">
+      <c r="T1052" s="17"/>
+    </row>
+    <row r="1053" spans="1:20">
       <c r="A1053" t="s">
         <v>933</v>
       </c>
-      <c r="S1053" s="17"/>
-    </row>
-    <row r="1054" spans="1:19">
-      <c r="S1054" s="17"/>
-    </row>
-    <row r="1055" spans="1:19">
+      <c r="T1053" s="17"/>
+    </row>
+    <row r="1054" spans="1:20">
+      <c r="T1054" s="17"/>
+    </row>
+    <row r="1055" spans="1:20">
       <c r="A1055" s="17" t="s">
         <v>243</v>
       </c>
@@ -12001,9 +12051,10 @@
       <c r="J1055" s="17"/>
       <c r="K1055" s="17"/>
       <c r="L1055" s="17"/>
-      <c r="S1055" s="17"/>
-    </row>
-    <row r="1056" spans="1:19">
+      <c r="M1055" s="17"/>
+      <c r="T1055" s="17"/>
+    </row>
+    <row r="1056" spans="1:20">
       <c r="A1056" s="17" t="s">
         <v>244</v>
       </c>
@@ -12018,9 +12069,10 @@
       <c r="J1056" s="17"/>
       <c r="K1056" s="17"/>
       <c r="L1056" s="17"/>
-      <c r="S1056" s="17"/>
-    </row>
-    <row r="1057" spans="1:19">
+      <c r="M1056" s="17"/>
+      <c r="T1056" s="17"/>
+    </row>
+    <row r="1057" spans="1:20">
       <c r="A1057" s="17" t="s">
         <v>245</v>
       </c>
@@ -12035,9 +12087,10 @@
       <c r="J1057" s="17"/>
       <c r="K1057" s="17"/>
       <c r="L1057" s="17"/>
-      <c r="S1057" s="17"/>
-    </row>
-    <row r="1058" spans="1:19">
+      <c r="M1057" s="17"/>
+      <c r="T1057" s="17"/>
+    </row>
+    <row r="1058" spans="1:20">
       <c r="A1058" s="17" t="s">
         <v>246</v>
       </c>
@@ -12052,9 +12105,10 @@
       <c r="J1058" s="17"/>
       <c r="K1058" s="17"/>
       <c r="L1058" s="17"/>
-      <c r="S1058" s="17"/>
-    </row>
-    <row r="1059" spans="1:19">
+      <c r="M1058" s="17"/>
+      <c r="T1058" s="17"/>
+    </row>
+    <row r="1059" spans="1:20">
       <c r="A1059" s="17" t="s">
         <v>247</v>
       </c>
@@ -12069,9 +12123,10 @@
       <c r="J1059" s="17"/>
       <c r="K1059" s="17"/>
       <c r="L1059" s="17"/>
-      <c r="S1059" s="17"/>
-    </row>
-    <row r="1060" spans="1:19">
+      <c r="M1059" s="17"/>
+      <c r="T1059" s="17"/>
+    </row>
+    <row r="1060" spans="1:20">
       <c r="A1060" s="17" t="s">
         <v>248</v>
       </c>
@@ -12086,9 +12141,10 @@
       <c r="J1060" s="17"/>
       <c r="K1060" s="17"/>
       <c r="L1060" s="17"/>
-      <c r="S1060" s="17"/>
-    </row>
-    <row r="1061" spans="1:19">
+      <c r="M1060" s="17"/>
+      <c r="T1060" s="17"/>
+    </row>
+    <row r="1061" spans="1:20">
       <c r="A1061" s="17" t="s">
         <v>249</v>
       </c>
@@ -12103,9 +12159,10 @@
       <c r="J1061" s="17"/>
       <c r="K1061" s="17"/>
       <c r="L1061" s="17"/>
-      <c r="S1061" s="17"/>
-    </row>
-    <row r="1062" spans="1:19">
+      <c r="M1061" s="17"/>
+      <c r="T1061" s="17"/>
+    </row>
+    <row r="1062" spans="1:20">
       <c r="A1062" s="17" t="s">
         <v>250</v>
       </c>
@@ -12120,9 +12177,10 @@
       <c r="J1062" s="17"/>
       <c r="K1062" s="17"/>
       <c r="L1062" s="17"/>
-      <c r="S1062" s="17"/>
-    </row>
-    <row r="1063" spans="1:19">
+      <c r="M1062" s="17"/>
+      <c r="T1062" s="17"/>
+    </row>
+    <row r="1063" spans="1:20">
       <c r="A1063" s="17" t="s">
         <v>251</v>
       </c>
@@ -12137,9 +12195,10 @@
       <c r="J1063" s="17"/>
       <c r="K1063" s="17"/>
       <c r="L1063" s="17"/>
-      <c r="S1063" s="17"/>
-    </row>
-    <row r="1064" spans="1:19">
+      <c r="M1063" s="17"/>
+      <c r="T1063" s="17"/>
+    </row>
+    <row r="1064" spans="1:20">
       <c r="A1064" s="17" t="s">
         <v>252</v>
       </c>
@@ -12154,9 +12213,10 @@
       <c r="J1064" s="17"/>
       <c r="K1064" s="17"/>
       <c r="L1064" s="17"/>
-      <c r="S1064" s="17"/>
-    </row>
-    <row r="1065" spans="1:19">
+      <c r="M1064" s="17"/>
+      <c r="T1064" s="17"/>
+    </row>
+    <row r="1065" spans="1:20">
       <c r="A1065" s="17" t="s">
         <v>253</v>
       </c>
@@ -12171,9 +12231,10 @@
       <c r="J1065" s="17"/>
       <c r="K1065" s="17"/>
       <c r="L1065" s="17"/>
-      <c r="S1065" s="17"/>
-    </row>
-    <row r="1066" spans="1:19">
+      <c r="M1065" s="17"/>
+      <c r="T1065" s="17"/>
+    </row>
+    <row r="1066" spans="1:20">
       <c r="A1066" s="17" t="s">
         <v>254</v>
       </c>
@@ -12188,9 +12249,10 @@
       <c r="J1066" s="17"/>
       <c r="K1066" s="17"/>
       <c r="L1066" s="17"/>
-      <c r="S1066" s="17"/>
-    </row>
-    <row r="1067" spans="1:19">
+      <c r="M1066" s="17"/>
+      <c r="T1066" s="17"/>
+    </row>
+    <row r="1067" spans="1:20">
       <c r="A1067" s="17" t="s">
         <v>255</v>
       </c>
@@ -12205,9 +12267,10 @@
       <c r="J1067" s="17"/>
       <c r="K1067" s="17"/>
       <c r="L1067" s="17"/>
-      <c r="S1067" s="17"/>
-    </row>
-    <row r="1068" spans="1:19">
+      <c r="M1067" s="17"/>
+      <c r="T1067" s="17"/>
+    </row>
+    <row r="1068" spans="1:20">
       <c r="A1068" s="17" t="s">
         <v>256</v>
       </c>
@@ -12222,14 +12285,15 @@
       <c r="J1068" s="17"/>
       <c r="K1068" s="17"/>
       <c r="L1068" s="17"/>
-      <c r="M1068"/>
+      <c r="M1068" s="17"/>
       <c r="N1068"/>
       <c r="O1068"/>
       <c r="P1068"/>
       <c r="Q1068"/>
       <c r="R1068"/>
-    </row>
-    <row r="1069" spans="1:19">
+      <c r="S1068"/>
+    </row>
+    <row r="1069" spans="1:20">
       <c r="A1069" s="17" t="s">
         <v>257</v>
       </c>
@@ -12244,14 +12308,15 @@
       <c r="J1069" s="17"/>
       <c r="K1069" s="17"/>
       <c r="L1069" s="17"/>
-      <c r="M1069"/>
+      <c r="M1069" s="17"/>
       <c r="N1069"/>
       <c r="O1069"/>
       <c r="P1069"/>
       <c r="Q1069"/>
       <c r="R1069"/>
-    </row>
-    <row r="1070" spans="1:19">
+      <c r="S1069"/>
+    </row>
+    <row r="1070" spans="1:20">
       <c r="A1070" s="17" t="s">
         <v>258</v>
       </c>
@@ -12266,14 +12331,15 @@
       <c r="J1070" s="17"/>
       <c r="K1070" s="17"/>
       <c r="L1070" s="17"/>
-      <c r="M1070"/>
+      <c r="M1070" s="17"/>
       <c r="N1070"/>
       <c r="O1070"/>
       <c r="P1070"/>
       <c r="Q1070"/>
       <c r="R1070"/>
-    </row>
-    <row r="1071" spans="1:19">
+      <c r="S1070"/>
+    </row>
+    <row r="1071" spans="1:20">
       <c r="A1071" s="17" t="s">
         <v>259</v>
       </c>
@@ -12288,14 +12354,15 @@
       <c r="J1071" s="17"/>
       <c r="K1071" s="17"/>
       <c r="L1071" s="17"/>
-      <c r="M1071"/>
+      <c r="M1071" s="17"/>
       <c r="N1071"/>
       <c r="O1071"/>
       <c r="P1071"/>
       <c r="Q1071"/>
       <c r="R1071"/>
-    </row>
-    <row r="1072" spans="1:19">
+      <c r="S1071"/>
+    </row>
+    <row r="1072" spans="1:20">
       <c r="A1072" s="17" t="s">
         <v>260</v>
       </c>
@@ -12310,14 +12377,15 @@
       <c r="J1072" s="17"/>
       <c r="K1072" s="17"/>
       <c r="L1072" s="17"/>
-      <c r="M1072"/>
+      <c r="M1072" s="17"/>
       <c r="N1072"/>
       <c r="O1072"/>
       <c r="P1072"/>
       <c r="Q1072"/>
       <c r="R1072"/>
-    </row>
-    <row r="1073" spans="1:18">
+      <c r="S1072"/>
+    </row>
+    <row r="1073" spans="1:19">
       <c r="A1073" s="17" t="s">
         <v>261</v>
       </c>
@@ -12332,14 +12400,15 @@
       <c r="J1073" s="17"/>
       <c r="K1073" s="17"/>
       <c r="L1073" s="17"/>
-      <c r="M1073"/>
+      <c r="M1073" s="17"/>
       <c r="N1073"/>
       <c r="O1073"/>
       <c r="P1073"/>
       <c r="Q1073"/>
       <c r="R1073"/>
-    </row>
-    <row r="1074" spans="1:18">
+      <c r="S1073"/>
+    </row>
+    <row r="1074" spans="1:19">
       <c r="A1074" s="17" t="s">
         <v>262</v>
       </c>
@@ -12354,14 +12423,15 @@
       <c r="J1074" s="17"/>
       <c r="K1074" s="17"/>
       <c r="L1074" s="17"/>
-      <c r="M1074"/>
+      <c r="M1074" s="17"/>
       <c r="N1074"/>
       <c r="O1074"/>
       <c r="P1074"/>
       <c r="Q1074"/>
       <c r="R1074"/>
-    </row>
-    <row r="1075" spans="1:18">
+      <c r="S1074"/>
+    </row>
+    <row r="1075" spans="1:19">
       <c r="A1075" s="17" t="s">
         <v>263</v>
       </c>
@@ -12376,14 +12446,15 @@
       <c r="J1075" s="17"/>
       <c r="K1075" s="17"/>
       <c r="L1075" s="17"/>
-      <c r="M1075"/>
+      <c r="M1075" s="17"/>
       <c r="N1075"/>
       <c r="O1075"/>
       <c r="P1075"/>
       <c r="Q1075"/>
       <c r="R1075"/>
-    </row>
-    <row r="1076" spans="1:18">
+      <c r="S1075"/>
+    </row>
+    <row r="1076" spans="1:19">
       <c r="A1076" s="17" t="s">
         <v>264</v>
       </c>
@@ -12398,14 +12469,15 @@
       <c r="J1076" s="17"/>
       <c r="K1076" s="17"/>
       <c r="L1076" s="17"/>
-      <c r="M1076"/>
+      <c r="M1076" s="17"/>
       <c r="N1076"/>
       <c r="O1076"/>
       <c r="P1076"/>
       <c r="Q1076"/>
       <c r="R1076"/>
-    </row>
-    <row r="1077" spans="1:18">
+      <c r="S1076"/>
+    </row>
+    <row r="1077" spans="1:19">
       <c r="A1077" s="17" t="s">
         <v>265</v>
       </c>
@@ -12420,14 +12492,15 @@
       <c r="J1077" s="17"/>
       <c r="K1077" s="17"/>
       <c r="L1077" s="17"/>
-      <c r="M1077"/>
+      <c r="M1077" s="17"/>
       <c r="N1077"/>
       <c r="O1077"/>
       <c r="P1077"/>
       <c r="Q1077"/>
       <c r="R1077"/>
-    </row>
-    <row r="1078" spans="1:18">
+      <c r="S1077"/>
+    </row>
+    <row r="1078" spans="1:19">
       <c r="A1078" s="17" t="s">
         <v>266</v>
       </c>
@@ -12442,14 +12515,15 @@
       <c r="J1078" s="17"/>
       <c r="K1078" s="17"/>
       <c r="L1078" s="17"/>
-      <c r="M1078"/>
+      <c r="M1078" s="17"/>
       <c r="N1078"/>
       <c r="O1078"/>
       <c r="P1078"/>
       <c r="Q1078"/>
       <c r="R1078"/>
-    </row>
-    <row r="1079" spans="1:18">
+      <c r="S1078"/>
+    </row>
+    <row r="1079" spans="1:19">
       <c r="A1079" s="17" t="s">
         <v>267</v>
       </c>
@@ -12464,14 +12538,15 @@
       <c r="J1079" s="17"/>
       <c r="K1079" s="17"/>
       <c r="L1079" s="17"/>
-      <c r="M1079"/>
+      <c r="M1079" s="17"/>
       <c r="N1079"/>
       <c r="O1079"/>
       <c r="P1079"/>
       <c r="Q1079"/>
       <c r="R1079"/>
-    </row>
-    <row r="1080" spans="1:18">
+      <c r="S1079"/>
+    </row>
+    <row r="1080" spans="1:19">
       <c r="A1080" s="17" t="s">
         <v>268</v>
       </c>
@@ -12486,14 +12561,15 @@
       <c r="J1080" s="17"/>
       <c r="K1080" s="17"/>
       <c r="L1080" s="17"/>
-      <c r="M1080"/>
+      <c r="M1080" s="17"/>
       <c r="N1080"/>
       <c r="O1080"/>
       <c r="P1080"/>
       <c r="Q1080"/>
       <c r="R1080"/>
-    </row>
-    <row r="1081" spans="1:18">
+      <c r="S1080"/>
+    </row>
+    <row r="1081" spans="1:19">
       <c r="A1081" s="17" t="s">
         <v>269</v>
       </c>
@@ -12508,14 +12584,15 @@
       <c r="J1081" s="17"/>
       <c r="K1081" s="17"/>
       <c r="L1081" s="17"/>
-      <c r="M1081"/>
+      <c r="M1081" s="17"/>
       <c r="N1081"/>
       <c r="O1081"/>
       <c r="P1081"/>
       <c r="Q1081"/>
       <c r="R1081"/>
-    </row>
-    <row r="1082" spans="1:18">
+      <c r="S1081"/>
+    </row>
+    <row r="1082" spans="1:19">
       <c r="A1082" s="17" t="s">
         <v>270</v>
       </c>
@@ -12530,14 +12607,15 @@
       <c r="J1082" s="17"/>
       <c r="K1082" s="17"/>
       <c r="L1082" s="17"/>
-      <c r="M1082"/>
+      <c r="M1082" s="17"/>
       <c r="N1082"/>
       <c r="O1082"/>
       <c r="P1082"/>
       <c r="Q1082"/>
       <c r="R1082"/>
-    </row>
-    <row r="1083" spans="1:18">
+      <c r="S1082"/>
+    </row>
+    <row r="1083" spans="1:19">
       <c r="A1083" s="17" t="s">
         <v>271</v>
       </c>
@@ -12552,14 +12630,15 @@
       <c r="J1083" s="17"/>
       <c r="K1083" s="17"/>
       <c r="L1083" s="17"/>
-      <c r="M1083"/>
+      <c r="M1083" s="17"/>
       <c r="N1083"/>
       <c r="O1083"/>
       <c r="P1083"/>
       <c r="Q1083"/>
       <c r="R1083"/>
-    </row>
-    <row r="1084" spans="1:18">
+      <c r="S1083"/>
+    </row>
+    <row r="1084" spans="1:19">
       <c r="A1084" s="17" t="s">
         <v>272</v>
       </c>
@@ -12574,14 +12653,15 @@
       <c r="J1084" s="17"/>
       <c r="K1084" s="17"/>
       <c r="L1084" s="17"/>
-      <c r="M1084"/>
+      <c r="M1084" s="17"/>
       <c r="N1084"/>
       <c r="O1084"/>
       <c r="P1084"/>
       <c r="Q1084"/>
       <c r="R1084"/>
-    </row>
-    <row r="1085" spans="1:18">
+      <c r="S1084"/>
+    </row>
+    <row r="1085" spans="1:19">
       <c r="A1085" s="17" t="s">
         <v>273</v>
       </c>
@@ -12596,14 +12676,15 @@
       <c r="J1085" s="17"/>
       <c r="K1085" s="17"/>
       <c r="L1085" s="17"/>
-      <c r="M1085"/>
+      <c r="M1085" s="17"/>
       <c r="N1085"/>
       <c r="O1085"/>
       <c r="P1085"/>
       <c r="Q1085"/>
       <c r="R1085"/>
-    </row>
-    <row r="1086" spans="1:18">
+      <c r="S1085"/>
+    </row>
+    <row r="1086" spans="1:19">
       <c r="A1086" s="17" t="s">
         <v>274</v>
       </c>
@@ -12618,14 +12699,15 @@
       <c r="J1086" s="17"/>
       <c r="K1086" s="17"/>
       <c r="L1086" s="17"/>
-      <c r="M1086"/>
+      <c r="M1086" s="17"/>
       <c r="N1086"/>
       <c r="O1086"/>
       <c r="P1086"/>
       <c r="Q1086"/>
       <c r="R1086"/>
-    </row>
-    <row r="1087" spans="1:18">
+      <c r="S1086"/>
+    </row>
+    <row r="1087" spans="1:19">
       <c r="A1087" s="17" t="s">
         <v>275</v>
       </c>
@@ -12640,14 +12722,15 @@
       <c r="J1087" s="17"/>
       <c r="K1087" s="17"/>
       <c r="L1087" s="17"/>
-      <c r="M1087"/>
+      <c r="M1087" s="17"/>
       <c r="N1087"/>
       <c r="O1087"/>
       <c r="P1087"/>
       <c r="Q1087"/>
       <c r="R1087"/>
-    </row>
-    <row r="1088" spans="1:18">
+      <c r="S1087"/>
+    </row>
+    <row r="1088" spans="1:19">
       <c r="A1088" s="17" t="s">
         <v>276</v>
       </c>
@@ -12662,14 +12745,15 @@
       <c r="J1088" s="17"/>
       <c r="K1088" s="17"/>
       <c r="L1088" s="17"/>
-      <c r="M1088"/>
+      <c r="M1088" s="17"/>
       <c r="N1088"/>
       <c r="O1088"/>
       <c r="P1088"/>
       <c r="Q1088"/>
       <c r="R1088"/>
-    </row>
-    <row r="1089" spans="1:18">
+      <c r="S1088"/>
+    </row>
+    <row r="1089" spans="1:19">
       <c r="A1089" s="17" t="s">
         <v>277</v>
       </c>
@@ -12684,14 +12768,15 @@
       <c r="J1089" s="17"/>
       <c r="K1089" s="17"/>
       <c r="L1089" s="17"/>
-      <c r="M1089"/>
+      <c r="M1089" s="17"/>
       <c r="N1089"/>
       <c r="O1089"/>
       <c r="P1089"/>
       <c r="Q1089"/>
       <c r="R1089"/>
-    </row>
-    <row r="1090" spans="1:18">
+      <c r="S1089"/>
+    </row>
+    <row r="1090" spans="1:19">
       <c r="A1090" s="17" t="s">
         <v>934</v>
       </c>
@@ -12706,14 +12791,15 @@
       <c r="J1090" s="17"/>
       <c r="K1090" s="17"/>
       <c r="L1090" s="17"/>
-      <c r="M1090"/>
+      <c r="M1090" s="17"/>
       <c r="N1090"/>
       <c r="O1090"/>
       <c r="P1090"/>
       <c r="Q1090"/>
       <c r="R1090"/>
-    </row>
-    <row r="1091" spans="1:18">
+      <c r="S1090"/>
+    </row>
+    <row r="1091" spans="1:19">
       <c r="A1091" s="17" t="s">
         <v>935</v>
       </c>
@@ -12728,14 +12814,15 @@
       <c r="J1091" s="17"/>
       <c r="K1091" s="17"/>
       <c r="L1091" s="17"/>
-      <c r="M1091"/>
+      <c r="M1091" s="17"/>
       <c r="N1091"/>
       <c r="O1091"/>
       <c r="P1091"/>
       <c r="Q1091"/>
       <c r="R1091"/>
-    </row>
-    <row r="1092" spans="1:18">
+      <c r="S1091"/>
+    </row>
+    <row r="1092" spans="1:19">
       <c r="A1092" s="17" t="s">
         <v>936</v>
       </c>
@@ -12750,14 +12837,15 @@
       <c r="J1092" s="17"/>
       <c r="K1092" s="17"/>
       <c r="L1092" s="17"/>
-      <c r="M1092"/>
+      <c r="M1092" s="17"/>
       <c r="N1092"/>
       <c r="O1092"/>
       <c r="P1092"/>
       <c r="Q1092"/>
       <c r="R1092"/>
-    </row>
-    <row r="1093" spans="1:18">
+      <c r="S1092"/>
+    </row>
+    <row r="1093" spans="1:19">
       <c r="A1093" s="17" t="s">
         <v>937</v>
       </c>
@@ -12772,14 +12860,15 @@
       <c r="J1093" s="17"/>
       <c r="K1093" s="17"/>
       <c r="L1093" s="17"/>
-      <c r="M1093"/>
+      <c r="M1093" s="17"/>
       <c r="N1093"/>
       <c r="O1093"/>
       <c r="P1093"/>
       <c r="Q1093"/>
       <c r="R1093"/>
-    </row>
-    <row r="1094" spans="1:18">
+      <c r="S1093"/>
+    </row>
+    <row r="1094" spans="1:19">
       <c r="A1094" s="17" t="s">
         <v>938</v>
       </c>
@@ -12794,572 +12883,573 @@
       <c r="J1094" s="17"/>
       <c r="K1094" s="17"/>
       <c r="L1094" s="17"/>
-      <c r="M1094"/>
+      <c r="M1094" s="17"/>
       <c r="N1094"/>
       <c r="O1094"/>
       <c r="P1094"/>
       <c r="Q1094"/>
       <c r="R1094"/>
-    </row>
-    <row r="1095" spans="1:18">
-      <c r="M1095"/>
+      <c r="S1094"/>
+    </row>
+    <row r="1095" spans="1:19">
       <c r="N1095"/>
       <c r="O1095"/>
       <c r="P1095"/>
       <c r="Q1095"/>
       <c r="R1095"/>
-    </row>
-    <row r="1096" spans="1:18">
-      <c r="M1096"/>
+      <c r="S1095"/>
+    </row>
+    <row r="1096" spans="1:19">
       <c r="N1096"/>
       <c r="O1096"/>
       <c r="P1096"/>
       <c r="Q1096"/>
       <c r="R1096"/>
-    </row>
-    <row r="1097" spans="1:18">
-      <c r="M1097"/>
+      <c r="S1096"/>
+    </row>
+    <row r="1097" spans="1:19">
       <c r="N1097"/>
       <c r="O1097"/>
       <c r="P1097"/>
       <c r="Q1097"/>
       <c r="R1097"/>
-    </row>
-    <row r="1098" spans="1:18">
-      <c r="M1098"/>
+      <c r="S1097"/>
+    </row>
+    <row r="1098" spans="1:19">
       <c r="N1098"/>
       <c r="O1098"/>
       <c r="P1098"/>
       <c r="Q1098"/>
       <c r="R1098"/>
-    </row>
-    <row r="1099" spans="1:18">
-      <c r="M1099"/>
+      <c r="S1098"/>
+    </row>
+    <row r="1099" spans="1:19">
       <c r="N1099"/>
       <c r="O1099"/>
       <c r="P1099"/>
       <c r="Q1099"/>
       <c r="R1099"/>
-    </row>
-    <row r="1100" spans="1:18">
-      <c r="M1100"/>
+      <c r="S1099"/>
+    </row>
+    <row r="1100" spans="1:19">
       <c r="N1100"/>
       <c r="O1100"/>
       <c r="P1100"/>
       <c r="Q1100"/>
       <c r="R1100"/>
-    </row>
-    <row r="1101" spans="1:18">
-      <c r="M1101"/>
+      <c r="S1100"/>
+    </row>
+    <row r="1101" spans="1:19">
       <c r="N1101"/>
       <c r="O1101"/>
       <c r="P1101"/>
       <c r="Q1101"/>
       <c r="R1101"/>
-    </row>
-    <row r="1102" spans="1:18">
-      <c r="M1102"/>
+      <c r="S1101"/>
+    </row>
+    <row r="1102" spans="1:19">
       <c r="N1102"/>
       <c r="O1102"/>
       <c r="P1102"/>
       <c r="Q1102"/>
       <c r="R1102"/>
-    </row>
-    <row r="1103" spans="1:18">
-      <c r="M1103"/>
+      <c r="S1102"/>
+    </row>
+    <row r="1103" spans="1:19">
       <c r="N1103"/>
       <c r="O1103"/>
       <c r="P1103"/>
       <c r="Q1103"/>
       <c r="R1103"/>
-    </row>
-    <row r="1104" spans="1:18">
-      <c r="M1104"/>
+      <c r="S1103"/>
+    </row>
+    <row r="1104" spans="1:19">
       <c r="N1104"/>
       <c r="O1104"/>
       <c r="P1104"/>
       <c r="Q1104"/>
       <c r="R1104"/>
-    </row>
-    <row r="1105" spans="13:18">
-      <c r="M1105"/>
+      <c r="S1104"/>
+    </row>
+    <row r="1105" spans="14:19">
       <c r="N1105"/>
       <c r="O1105"/>
       <c r="P1105"/>
       <c r="Q1105"/>
       <c r="R1105"/>
-    </row>
-    <row r="1106" spans="13:18">
-      <c r="M1106"/>
+      <c r="S1105"/>
+    </row>
+    <row r="1106" spans="14:19">
       <c r="N1106"/>
       <c r="O1106"/>
       <c r="P1106"/>
       <c r="Q1106"/>
       <c r="R1106"/>
-    </row>
-    <row r="1107" spans="13:18">
-      <c r="M1107"/>
+      <c r="S1106"/>
+    </row>
+    <row r="1107" spans="14:19">
       <c r="N1107"/>
       <c r="O1107"/>
       <c r="P1107"/>
       <c r="Q1107"/>
       <c r="R1107"/>
-    </row>
-    <row r="1108" spans="13:18">
-      <c r="M1108"/>
+      <c r="S1107"/>
+    </row>
+    <row r="1108" spans="14:19">
       <c r="N1108"/>
       <c r="O1108"/>
       <c r="P1108"/>
       <c r="Q1108"/>
       <c r="R1108"/>
-    </row>
-    <row r="1109" spans="13:18">
-      <c r="M1109"/>
+      <c r="S1108"/>
+    </row>
+    <row r="1109" spans="14:19">
       <c r="N1109"/>
       <c r="O1109"/>
       <c r="P1109"/>
       <c r="Q1109"/>
       <c r="R1109"/>
-    </row>
-    <row r="1110" spans="13:18">
-      <c r="M1110"/>
+      <c r="S1109"/>
+    </row>
+    <row r="1110" spans="14:19">
       <c r="N1110"/>
       <c r="O1110"/>
       <c r="P1110"/>
       <c r="Q1110"/>
       <c r="R1110"/>
-    </row>
-    <row r="1111" spans="13:18">
-      <c r="M1111"/>
+      <c r="S1110"/>
+    </row>
+    <row r="1111" spans="14:19">
       <c r="N1111"/>
       <c r="O1111"/>
       <c r="P1111"/>
       <c r="Q1111"/>
       <c r="R1111"/>
-    </row>
-    <row r="1112" spans="13:18">
-      <c r="M1112"/>
+      <c r="S1111"/>
+    </row>
+    <row r="1112" spans="14:19">
       <c r="N1112"/>
       <c r="O1112"/>
       <c r="P1112"/>
       <c r="Q1112"/>
       <c r="R1112"/>
-    </row>
-    <row r="1113" spans="13:18">
-      <c r="M1113"/>
+      <c r="S1112"/>
+    </row>
+    <row r="1113" spans="14:19">
       <c r="N1113"/>
       <c r="O1113"/>
       <c r="P1113"/>
       <c r="Q1113"/>
       <c r="R1113"/>
-    </row>
-    <row r="1114" spans="13:18">
-      <c r="M1114"/>
+      <c r="S1113"/>
+    </row>
+    <row r="1114" spans="14:19">
       <c r="N1114"/>
       <c r="O1114"/>
       <c r="P1114"/>
       <c r="Q1114"/>
       <c r="R1114"/>
-    </row>
-    <row r="1115" spans="13:18">
-      <c r="M1115"/>
+      <c r="S1114"/>
+    </row>
+    <row r="1115" spans="14:19">
       <c r="N1115"/>
       <c r="O1115"/>
       <c r="P1115"/>
       <c r="Q1115"/>
       <c r="R1115"/>
-    </row>
-    <row r="1116" spans="13:18">
-      <c r="M1116"/>
+      <c r="S1115"/>
+    </row>
+    <row r="1116" spans="14:19">
       <c r="N1116"/>
       <c r="O1116"/>
       <c r="P1116"/>
       <c r="Q1116"/>
       <c r="R1116"/>
-    </row>
-    <row r="1117" spans="13:18">
-      <c r="M1117"/>
+      <c r="S1116"/>
+    </row>
+    <row r="1117" spans="14:19">
       <c r="N1117"/>
       <c r="O1117"/>
       <c r="P1117"/>
       <c r="Q1117"/>
       <c r="R1117"/>
-    </row>
-    <row r="1118" spans="13:18">
-      <c r="M1118"/>
+      <c r="S1117"/>
+    </row>
+    <row r="1118" spans="14:19">
       <c r="N1118"/>
       <c r="O1118"/>
       <c r="P1118"/>
       <c r="Q1118"/>
       <c r="R1118"/>
-    </row>
-    <row r="1119" spans="13:18">
-      <c r="M1119"/>
+      <c r="S1118"/>
+    </row>
+    <row r="1119" spans="14:19">
       <c r="N1119"/>
       <c r="O1119"/>
       <c r="P1119"/>
       <c r="Q1119"/>
       <c r="R1119"/>
-    </row>
-    <row r="1120" spans="13:18">
-      <c r="M1120"/>
+      <c r="S1119"/>
+    </row>
+    <row r="1120" spans="14:19">
       <c r="N1120"/>
       <c r="O1120"/>
       <c r="P1120"/>
       <c r="Q1120"/>
       <c r="R1120"/>
-    </row>
-    <row r="1121" spans="13:18">
-      <c r="M1121"/>
+      <c r="S1120"/>
+    </row>
+    <row r="1121" spans="14:19">
       <c r="N1121"/>
       <c r="O1121"/>
       <c r="P1121"/>
       <c r="Q1121"/>
       <c r="R1121"/>
-    </row>
-    <row r="1122" spans="13:18">
-      <c r="M1122"/>
+      <c r="S1121"/>
+    </row>
+    <row r="1122" spans="14:19">
       <c r="N1122"/>
       <c r="O1122"/>
       <c r="P1122"/>
       <c r="Q1122"/>
       <c r="R1122"/>
-    </row>
-    <row r="1123" spans="13:18">
-      <c r="M1123"/>
+      <c r="S1122"/>
+    </row>
+    <row r="1123" spans="14:19">
       <c r="N1123"/>
       <c r="O1123"/>
       <c r="P1123"/>
       <c r="Q1123"/>
       <c r="R1123"/>
-    </row>
-    <row r="1124" spans="13:18">
-      <c r="M1124"/>
+      <c r="S1123"/>
+    </row>
+    <row r="1124" spans="14:19">
       <c r="N1124"/>
       <c r="O1124"/>
       <c r="P1124"/>
       <c r="Q1124"/>
       <c r="R1124"/>
-    </row>
-    <row r="1125" spans="13:18">
-      <c r="M1125"/>
+      <c r="S1124"/>
+    </row>
+    <row r="1125" spans="14:19">
       <c r="N1125"/>
       <c r="O1125"/>
       <c r="P1125"/>
       <c r="Q1125"/>
       <c r="R1125"/>
-    </row>
-    <row r="1126" spans="13:18">
-      <c r="M1126"/>
+      <c r="S1125"/>
+    </row>
+    <row r="1126" spans="14:19">
       <c r="N1126"/>
       <c r="O1126"/>
       <c r="P1126"/>
       <c r="Q1126"/>
       <c r="R1126"/>
-    </row>
-    <row r="1127" spans="13:18">
-      <c r="M1127"/>
+      <c r="S1126"/>
+    </row>
+    <row r="1127" spans="14:19">
       <c r="N1127"/>
       <c r="O1127"/>
       <c r="P1127"/>
       <c r="Q1127"/>
       <c r="R1127"/>
-    </row>
-    <row r="1128" spans="13:18">
-      <c r="M1128"/>
+      <c r="S1127"/>
+    </row>
+    <row r="1128" spans="14:19">
       <c r="N1128"/>
       <c r="O1128"/>
       <c r="P1128"/>
       <c r="Q1128"/>
       <c r="R1128"/>
-    </row>
-    <row r="1129" spans="13:18">
-      <c r="M1129"/>
+      <c r="S1128"/>
+    </row>
+    <row r="1129" spans="14:19">
       <c r="N1129"/>
       <c r="O1129"/>
       <c r="P1129"/>
       <c r="Q1129"/>
       <c r="R1129"/>
-    </row>
-    <row r="1130" spans="13:18">
-      <c r="M1130"/>
+      <c r="S1129"/>
+    </row>
+    <row r="1130" spans="14:19">
       <c r="N1130"/>
       <c r="O1130"/>
       <c r="P1130"/>
       <c r="Q1130"/>
       <c r="R1130"/>
-    </row>
-    <row r="1131" spans="13:18">
-      <c r="M1131"/>
+      <c r="S1130"/>
+    </row>
+    <row r="1131" spans="14:19">
       <c r="N1131"/>
       <c r="O1131"/>
       <c r="P1131"/>
       <c r="Q1131"/>
       <c r="R1131"/>
-    </row>
-    <row r="1132" spans="13:18">
-      <c r="M1132"/>
+      <c r="S1131"/>
+    </row>
+    <row r="1132" spans="14:19">
       <c r="N1132"/>
       <c r="O1132"/>
       <c r="P1132"/>
       <c r="Q1132"/>
       <c r="R1132"/>
-    </row>
-    <row r="1133" spans="13:18">
-      <c r="M1133"/>
+      <c r="S1132"/>
+    </row>
+    <row r="1133" spans="14:19">
       <c r="N1133"/>
       <c r="O1133"/>
       <c r="P1133"/>
       <c r="Q1133"/>
       <c r="R1133"/>
-    </row>
-    <row r="1134" spans="13:18">
-      <c r="M1134"/>
+      <c r="S1133"/>
+    </row>
+    <row r="1134" spans="14:19">
       <c r="N1134"/>
       <c r="O1134"/>
       <c r="P1134"/>
       <c r="Q1134"/>
       <c r="R1134"/>
-    </row>
-    <row r="1135" spans="13:18">
-      <c r="M1135"/>
+      <c r="S1134"/>
+    </row>
+    <row r="1135" spans="14:19">
       <c r="N1135"/>
       <c r="O1135"/>
       <c r="P1135"/>
       <c r="Q1135"/>
       <c r="R1135"/>
-    </row>
-    <row r="1136" spans="13:18">
-      <c r="M1136"/>
+      <c r="S1135"/>
+    </row>
+    <row r="1136" spans="14:19">
       <c r="N1136"/>
       <c r="O1136"/>
       <c r="P1136"/>
       <c r="Q1136"/>
       <c r="R1136"/>
-    </row>
-    <row r="1137" spans="13:18">
-      <c r="M1137"/>
+      <c r="S1136"/>
+    </row>
+    <row r="1137" spans="14:19">
       <c r="N1137"/>
       <c r="O1137"/>
       <c r="P1137"/>
       <c r="Q1137"/>
       <c r="R1137"/>
-    </row>
-    <row r="1138" spans="13:18">
-      <c r="M1138"/>
+      <c r="S1137"/>
+    </row>
+    <row r="1138" spans="14:19">
       <c r="N1138"/>
       <c r="O1138"/>
       <c r="P1138"/>
       <c r="Q1138"/>
       <c r="R1138"/>
-    </row>
-    <row r="1139" spans="13:18">
-      <c r="M1139"/>
+      <c r="S1138"/>
+    </row>
+    <row r="1139" spans="14:19">
       <c r="N1139"/>
       <c r="O1139"/>
       <c r="P1139"/>
       <c r="Q1139"/>
       <c r="R1139"/>
-    </row>
-    <row r="1140" spans="13:18">
-      <c r="M1140"/>
+      <c r="S1139"/>
+    </row>
+    <row r="1140" spans="14:19">
       <c r="N1140"/>
       <c r="O1140"/>
       <c r="P1140"/>
       <c r="Q1140"/>
       <c r="R1140"/>
-    </row>
-    <row r="1141" spans="13:18">
-      <c r="M1141"/>
+      <c r="S1140"/>
+    </row>
+    <row r="1141" spans="14:19">
       <c r="N1141"/>
       <c r="O1141"/>
       <c r="P1141"/>
       <c r="Q1141"/>
       <c r="R1141"/>
-    </row>
-    <row r="1142" spans="13:18">
-      <c r="M1142"/>
+      <c r="S1141"/>
+    </row>
+    <row r="1142" spans="14:19">
       <c r="N1142"/>
       <c r="O1142"/>
       <c r="P1142"/>
       <c r="Q1142"/>
       <c r="R1142"/>
-    </row>
-    <row r="1143" spans="13:18">
-      <c r="M1143"/>
+      <c r="S1142"/>
+    </row>
+    <row r="1143" spans="14:19">
       <c r="N1143"/>
       <c r="O1143"/>
       <c r="P1143"/>
       <c r="Q1143"/>
       <c r="R1143"/>
-    </row>
-    <row r="1144" spans="13:18">
-      <c r="M1144"/>
+      <c r="S1143"/>
+    </row>
+    <row r="1144" spans="14:19">
       <c r="N1144"/>
       <c r="O1144"/>
       <c r="P1144"/>
       <c r="Q1144"/>
       <c r="R1144"/>
-    </row>
-    <row r="1145" spans="13:18">
-      <c r="M1145"/>
+      <c r="S1144"/>
+    </row>
+    <row r="1145" spans="14:19">
       <c r="N1145"/>
       <c r="O1145"/>
       <c r="P1145"/>
       <c r="Q1145"/>
       <c r="R1145"/>
-    </row>
-    <row r="1146" spans="13:18">
-      <c r="M1146"/>
+      <c r="S1145"/>
+    </row>
+    <row r="1146" spans="14:19">
       <c r="N1146"/>
       <c r="O1146"/>
       <c r="P1146"/>
       <c r="Q1146"/>
       <c r="R1146"/>
-    </row>
-    <row r="1147" spans="13:18">
-      <c r="M1147"/>
+      <c r="S1146"/>
+    </row>
+    <row r="1147" spans="14:19">
       <c r="N1147"/>
       <c r="O1147"/>
       <c r="P1147"/>
       <c r="Q1147"/>
       <c r="R1147"/>
-    </row>
-    <row r="1148" spans="13:18">
-      <c r="M1148"/>
+      <c r="S1147"/>
+    </row>
+    <row r="1148" spans="14:19">
       <c r="N1148"/>
       <c r="O1148"/>
       <c r="P1148"/>
       <c r="Q1148"/>
       <c r="R1148"/>
-    </row>
-    <row r="1149" spans="13:18">
-      <c r="M1149"/>
+      <c r="S1148"/>
+    </row>
+    <row r="1149" spans="14:19">
       <c r="N1149"/>
       <c r="O1149"/>
       <c r="P1149"/>
       <c r="Q1149"/>
       <c r="R1149"/>
-    </row>
-    <row r="1150" spans="13:18">
-      <c r="M1150"/>
+      <c r="S1149"/>
+    </row>
+    <row r="1150" spans="14:19">
       <c r="N1150"/>
       <c r="O1150"/>
       <c r="P1150"/>
       <c r="Q1150"/>
       <c r="R1150"/>
-    </row>
-    <row r="1151" spans="13:18">
-      <c r="M1151"/>
+      <c r="S1150"/>
+    </row>
+    <row r="1151" spans="14:19">
       <c r="N1151"/>
       <c r="O1151"/>
       <c r="P1151"/>
       <c r="Q1151"/>
       <c r="R1151"/>
-    </row>
-    <row r="1152" spans="13:18">
-      <c r="M1152"/>
+      <c r="S1151"/>
+    </row>
+    <row r="1152" spans="14:19">
       <c r="N1152"/>
       <c r="O1152"/>
       <c r="P1152"/>
       <c r="Q1152"/>
       <c r="R1152"/>
-    </row>
-    <row r="1153" spans="13:18">
-      <c r="M1153"/>
+      <c r="S1152"/>
+    </row>
+    <row r="1153" spans="14:19">
       <c r="N1153"/>
       <c r="O1153"/>
       <c r="P1153"/>
       <c r="Q1153"/>
       <c r="R1153"/>
-    </row>
-    <row r="1154" spans="13:18">
-      <c r="M1154"/>
+      <c r="S1153"/>
+    </row>
+    <row r="1154" spans="14:19">
       <c r="N1154"/>
       <c r="O1154"/>
       <c r="P1154"/>
       <c r="Q1154"/>
       <c r="R1154"/>
-    </row>
-    <row r="1155" spans="13:18">
-      <c r="M1155"/>
+      <c r="S1154"/>
+    </row>
+    <row r="1155" spans="14:19">
       <c r="N1155"/>
       <c r="O1155"/>
       <c r="P1155"/>
       <c r="Q1155"/>
       <c r="R1155"/>
-    </row>
-    <row r="1156" spans="13:18">
-      <c r="M1156"/>
+      <c r="S1155"/>
+    </row>
+    <row r="1156" spans="14:19">
       <c r="N1156"/>
       <c r="O1156"/>
       <c r="P1156"/>
       <c r="Q1156"/>
       <c r="R1156"/>
-    </row>
-    <row r="1157" spans="13:18">
-      <c r="M1157"/>
+      <c r="S1156"/>
+    </row>
+    <row r="1157" spans="14:19">
       <c r="N1157"/>
       <c r="O1157"/>
       <c r="P1157"/>
       <c r="Q1157"/>
       <c r="R1157"/>
-    </row>
-    <row r="1158" spans="13:18">
-      <c r="M1158"/>
+      <c r="S1157"/>
+    </row>
+    <row r="1158" spans="14:19">
       <c r="N1158"/>
       <c r="O1158"/>
       <c r="P1158"/>
       <c r="Q1158"/>
       <c r="R1158"/>
-    </row>
-    <row r="1159" spans="13:18">
-      <c r="M1159"/>
+      <c r="S1158"/>
+    </row>
+    <row r="1159" spans="14:19">
       <c r="N1159"/>
       <c r="O1159"/>
       <c r="P1159"/>
       <c r="Q1159"/>
       <c r="R1159"/>
-    </row>
-    <row r="1160" spans="13:18">
-      <c r="M1160"/>
+      <c r="S1159"/>
+    </row>
+    <row r="1160" spans="14:19">
       <c r="N1160"/>
       <c r="O1160"/>
       <c r="P1160"/>
       <c r="Q1160"/>
       <c r="R1160"/>
-    </row>
-    <row r="1161" spans="13:18">
-      <c r="M1161"/>
+      <c r="S1160"/>
+    </row>
+    <row r="1161" spans="14:19">
       <c r="N1161"/>
       <c r="O1161"/>
       <c r="P1161"/>
       <c r="Q1161"/>
       <c r="R1161"/>
-    </row>
-    <row r="1162" spans="13:18">
-      <c r="M1162"/>
+      <c r="S1161"/>
+    </row>
+    <row r="1162" spans="14:19">
       <c r="N1162"/>
       <c r="O1162"/>
       <c r="P1162"/>
       <c r="Q1162"/>
       <c r="R1162"/>
-    </row>
-    <row r="1163" spans="13:18">
-      <c r="M1163"/>
+      <c r="S1162"/>
+    </row>
+    <row r="1163" spans="14:19">
       <c r="N1163"/>
       <c r="O1163"/>
       <c r="P1163"/>
       <c r="Q1163"/>
       <c r="R1163"/>
-    </row>
-    <row r="1164" spans="13:18">
-      <c r="M1164"/>
+      <c r="S1163"/>
+    </row>
+    <row r="1164" spans="14:19">
       <c r="N1164"/>
       <c r="O1164"/>
       <c r="P1164"/>
       <c r="Q1164"/>
       <c r="R1164"/>
+      <c r="S1164"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Adding in model with crops
Adds 200+ rows but only one species when we use chill portions ....
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4100" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4107" uniqueCount="1070">
   <si>
     <t>param</t>
   </si>
@@ -3497,8 +3497,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="389">
+  <cellStyleXfs count="391">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3959,7 +3961,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="389">
+  <cellStyles count="391">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4154,6 +4156,7 @@
     <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4348,6 +4351,7 @@
     <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5709,29 +5713,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD1164"/>
+  <dimension ref="A1:AE1164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="13" width="17.1640625" customWidth="1"/>
-    <col min="14" max="19" width="18.5" style="21" customWidth="1"/>
-    <col min="20" max="20" width="17.1640625" customWidth="1"/>
-    <col min="21" max="21" width="15" customWidth="1"/>
-    <col min="22" max="22" width="13.5" customWidth="1"/>
-    <col min="23" max="23" width="13.6640625" customWidth="1"/>
-    <col min="24" max="24" width="13.1640625" customWidth="1"/>
-    <col min="25" max="25" width="11.83203125" customWidth="1"/>
-    <col min="26" max="26" width="15.5" customWidth="1"/>
-    <col min="27" max="27" width="12.6640625" customWidth="1"/>
-    <col min="28" max="28" width="14.33203125" customWidth="1"/>
-    <col min="29" max="30" width="10.83203125" style="19"/>
+    <col min="1" max="14" width="17.1640625" customWidth="1"/>
+    <col min="15" max="20" width="18.5" style="21" customWidth="1"/>
+    <col min="21" max="21" width="17.1640625" customWidth="1"/>
+    <col min="22" max="22" width="15" customWidth="1"/>
+    <col min="23" max="23" width="13.5" customWidth="1"/>
+    <col min="24" max="24" width="13.6640625" customWidth="1"/>
+    <col min="25" max="25" width="13.1640625" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" customWidth="1"/>
+    <col min="27" max="27" width="15.5" customWidth="1"/>
+    <col min="28" max="28" width="12.6640625" customWidth="1"/>
+    <col min="29" max="29" width="14.33203125" customWidth="1"/>
+    <col min="30" max="31" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="18" customFormat="1">
+    <row r="1" spans="1:24" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
         <v>212</v>
       </c>
@@ -5748,13 +5752,13 @@
         <v>992</v>
       </c>
       <c r="F1" t="s">
-        <v>1054</v>
+        <v>992</v>
       </c>
       <c r="G1" t="s">
         <v>1054</v>
       </c>
-      <c r="H1" s="18" t="s">
-        <v>1</v>
+      <c r="H1" t="s">
+        <v>1054</v>
       </c>
       <c r="I1" s="18" t="s">
         <v>1</v>
@@ -5763,25 +5767,25 @@
         <v>1</v>
       </c>
       <c r="K1" s="18" t="s">
-        <v>976</v>
+        <v>1</v>
       </c>
       <c r="L1" s="18" t="s">
         <v>976</v>
       </c>
-      <c r="M1"/>
-      <c r="N1" t="s">
+      <c r="M1" s="18" t="s">
+        <v>976</v>
+      </c>
+      <c r="N1"/>
+      <c r="O1" t="s">
         <v>992</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>1054</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="17" t="s">
-        <v>992</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="R1" s="17" t="s">
         <v>992</v>
       </c>
       <c r="S1" t="s">
@@ -5790,14 +5794,17 @@
       <c r="T1" t="s">
         <v>992</v>
       </c>
-      <c r="U1" s="18" t="s">
+      <c r="U1" t="s">
+        <v>992</v>
+      </c>
+      <c r="V1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="W1" s="18" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="18" customFormat="1">
+    <row r="2" spans="1:24" s="18" customFormat="1">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -5812,12 +5819,13 @@
       <c r="M2"/>
       <c r="N2"/>
       <c r="O2"/>
-      <c r="Q2" s="17"/>
-      <c r="R2"/>
+      <c r="P2"/>
+      <c r="R2" s="17"/>
       <c r="S2"/>
       <c r="T2"/>
-    </row>
-    <row r="3" spans="1:23" s="40" customFormat="1">
+      <c r="U2"/>
+    </row>
+    <row r="3" spans="1:24" s="40" customFormat="1">
       <c r="A3" s="40" t="s">
         <v>1066</v>
       </c>
@@ -5825,7 +5833,9 @@
       <c r="C3" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="D3" s="41"/>
+      <c r="D3" s="41" t="s">
+        <v>216</v>
+      </c>
       <c r="E3" s="41"/>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
@@ -5837,12 +5847,13 @@
       <c r="M3" s="41"/>
       <c r="N3" s="41"/>
       <c r="O3" s="41"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="41"/>
+      <c r="P3" s="41"/>
+      <c r="R3" s="42"/>
       <c r="S3" s="41"/>
       <c r="T3" s="41"/>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="U3" s="41"/>
+    </row>
+    <row r="4" spans="1:24">
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -5855,10 +5866,11 @@
       <c r="K4" s="21"/>
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
-      <c r="Q4" s="22"/>
-      <c r="T4" s="21"/>
-    </row>
-    <row r="5" spans="1:23">
+      <c r="N4" s="21"/>
+      <c r="R4" s="22"/>
+      <c r="U4" s="21"/>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -5895,27 +5907,27 @@
       <c r="L5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21" t="s">
+      <c r="M5" s="21" t="s">
         <v>1032</v>
       </c>
+      <c r="N5" s="21"/>
       <c r="O5" s="21" t="s">
         <v>1032</v>
       </c>
       <c r="P5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="Q5" s="22" t="s">
+      <c r="Q5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="R5" s="22" t="s">
         <v>1034</v>
       </c>
-      <c r="R5" s="21" t="s">
+      <c r="S5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="S5" s="22" t="s">
+      <c r="T5" s="22" t="s">
         <v>1034</v>
-      </c>
-      <c r="T5" s="21" t="s">
-        <v>1032</v>
       </c>
       <c r="U5" s="21" t="s">
         <v>1032</v>
@@ -5923,9 +5935,12 @@
       <c r="V5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="W5" s="21"/>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="W5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="X5" s="21"/>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
         <v>221</v>
       </c>
@@ -5936,13 +5951,13 @@
         <v>1031</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>1067</v>
+        <v>1033</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>1031</v>
+        <v>1067</v>
       </c>
       <c r="G6" s="21" t="s">
         <v>1031</v>
@@ -5962,37 +5977,40 @@
       <c r="L6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21" t="s">
+      <c r="M6" s="21" t="s">
         <v>1031</v>
       </c>
+      <c r="N6" s="21"/>
       <c r="O6" s="21" t="s">
         <v>1031</v>
       </c>
       <c r="P6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="Q6" s="22" t="s">
+      <c r="Q6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="R6" s="21" t="s">
-        <v>1035</v>
+      <c r="R6" s="22" t="s">
+        <v>1031</v>
       </c>
       <c r="S6" s="21" t="s">
         <v>1035</v>
       </c>
       <c r="T6" s="21" t="s">
+        <v>1035</v>
+      </c>
+      <c r="U6" s="21" t="s">
         <v>1033</v>
-      </c>
-      <c r="U6" s="22" t="s">
-        <v>1036</v>
       </c>
       <c r="V6" s="22" t="s">
         <v>1036</v>
       </c>
-      <c r="W6" s="21"/>
-    </row>
-    <row r="7" spans="1:23">
+      <c r="W6" s="22" t="s">
+        <v>1036</v>
+      </c>
+      <c r="X6" s="21"/>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
         <v>280</v>
       </c>
@@ -6002,23 +6020,23 @@
       <c r="C7" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="D7" s="21"/>
+      <c r="D7" s="21" t="s">
+        <v>281</v>
+      </c>
       <c r="E7" s="21"/>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
-      <c r="K7" t="s">
+      <c r="K7" s="21"/>
+      <c r="L7" t="s">
         <v>1069</v>
       </c>
-      <c r="L7" s="21" t="s">
+      <c r="M7" s="21" t="s">
         <v>1068</v>
       </c>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21" t="s">
-        <v>281</v>
-      </c>
+      <c r="N7" s="21"/>
       <c r="O7" s="21" t="s">
         <v>281</v>
       </c>
@@ -6043,14 +6061,14 @@
       <c r="V7" s="21" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="W7" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
         <v>224</v>
       </c>
-      <c r="N8" s="21" t="s">
-        <v>1064</v>
-      </c>
       <c r="O8" s="21" t="s">
         <v>1064</v>
       </c>
@@ -6072,11 +6090,14 @@
       <c r="U8" s="21" t="s">
         <v>1064</v>
       </c>
-      <c r="V8" t="s">
+      <c r="V8" s="21" t="s">
+        <v>1064</v>
+      </c>
+      <c r="W8" t="s">
         <v>1065</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:24">
       <c r="A9" t="s">
         <v>1063</v>
       </c>
@@ -6111,12 +6132,12 @@
         <v>1056</v>
       </c>
       <c r="L9" s="21" t="s">
+        <v>1056</v>
+      </c>
+      <c r="M9" s="21" t="s">
         <v>1062</v>
       </c>
-      <c r="M9" s="21"/>
-      <c r="N9" s="21" t="s">
-        <v>1062</v>
-      </c>
+      <c r="N9" s="21"/>
       <c r="O9" s="21" t="s">
         <v>1062</v>
       </c>
@@ -6141,8 +6162,11 @@
       <c r="V9" s="21" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="W9" s="21" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" t="s">
         <v>214</v>
       </c>
@@ -6153,13 +6177,13 @@
         <v>1524</v>
       </c>
       <c r="D11">
-        <v>2497</v>
+        <v>1775</v>
       </c>
       <c r="E11">
         <v>2497</v>
       </c>
       <c r="F11">
-        <v>1524</v>
+        <v>2497</v>
       </c>
       <c r="G11">
         <v>1524</v>
@@ -6171,16 +6195,16 @@
         <v>1524</v>
       </c>
       <c r="J11">
-        <v>2497</v>
+        <v>1524</v>
       </c>
       <c r="K11">
         <v>2497</v>
       </c>
       <c r="L11">
+        <v>2497</v>
+      </c>
+      <c r="M11">
         <v>1524</v>
-      </c>
-      <c r="N11" s="23">
-        <v>1556</v>
       </c>
       <c r="O11" s="23">
         <v>1556</v>
@@ -6189,25 +6213,28 @@
         <v>1556</v>
       </c>
       <c r="Q11" s="23">
+        <v>1556</v>
+      </c>
+      <c r="R11" s="23">
         <v>1097</v>
       </c>
-      <c r="R11" s="23">
+      <c r="S11" s="23">
         <v>2651</v>
       </c>
-      <c r="S11" s="23">
+      <c r="T11" s="23">
         <v>2112</v>
       </c>
-      <c r="T11" s="23">
+      <c r="U11" s="23">
         <v>1953</v>
-      </c>
-      <c r="U11">
-        <v>1556</v>
       </c>
       <c r="V11">
         <v>1556</v>
       </c>
-    </row>
-    <row r="12" spans="1:23">
+      <c r="W11">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" t="s">
         <v>211</v>
       </c>
@@ -6218,13 +6245,13 @@
         <v>37</v>
       </c>
       <c r="D12">
-        <v>199</v>
+        <v>38</v>
       </c>
       <c r="E12">
         <v>199</v>
       </c>
       <c r="F12">
-        <v>37</v>
+        <v>199</v>
       </c>
       <c r="G12">
         <v>37</v>
@@ -6236,15 +6263,15 @@
         <v>37</v>
       </c>
       <c r="J12">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="K12">
         <v>199</v>
       </c>
       <c r="L12">
-        <v>37</v>
-      </c>
-      <c r="N12" s="23">
+        <v>199</v>
+      </c>
+      <c r="M12">
         <v>37</v>
       </c>
       <c r="O12" s="23">
@@ -6254,40 +6281,43 @@
         <v>37</v>
       </c>
       <c r="Q12" s="23">
+        <v>37</v>
+      </c>
+      <c r="R12" s="23">
         <v>25</v>
       </c>
-      <c r="R12" s="23">
+      <c r="S12" s="23">
         <v>200</v>
       </c>
-      <c r="S12" s="23">
+      <c r="T12" s="23">
         <v>179</v>
       </c>
-      <c r="T12" s="23">
+      <c r="U12" s="23">
         <v>41</v>
-      </c>
-      <c r="U12">
-        <v>37</v>
       </c>
       <c r="V12">
         <v>37</v>
       </c>
-      <c r="W12" s="23"/>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="W12">
+        <v>37</v>
+      </c>
+      <c r="X12" s="23"/>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" t="s">
         <v>213</v>
       </c>
-      <c r="N13" s="23"/>
       <c r="O13" s="23"/>
-      <c r="Q13" s="23"/>
+      <c r="P13" s="23"/>
       <c r="R13" s="23"/>
       <c r="S13" s="23"/>
-      <c r="V13">
+      <c r="T13" s="23"/>
+      <c r="W13">
         <v>30</v>
       </c>
-      <c r="W13" s="23"/>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="X13" s="23"/>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -6298,22 +6328,22 @@
         <v>216</v>
       </c>
       <c r="D14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" t="s">
         <v>214</v>
-      </c>
-      <c r="E14" t="s">
-        <v>216</v>
       </c>
       <c r="F14" t="s">
         <v>216</v>
       </c>
       <c r="G14" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="H14" t="s">
         <v>214</v>
       </c>
       <c r="I14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J14" t="s">
         <v>216</v>
@@ -6324,7 +6354,7 @@
       <c r="L14" t="s">
         <v>216</v>
       </c>
-      <c r="N14" s="23" t="s">
+      <c r="M14" t="s">
         <v>216</v>
       </c>
       <c r="O14" s="23" t="s">
@@ -6351,8 +6381,11 @@
       <c r="V14" s="23" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" s="21" customFormat="1">
+      <c r="W14" s="23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" s="21" customFormat="1">
       <c r="A16" s="21" t="s">
         <v>5</v>
       </c>
@@ -6363,75 +6396,78 @@
         <v>30.654658000000001</v>
       </c>
       <c r="D16" s="21">
+        <v>28.90391</v>
+      </c>
+      <c r="E16" s="21">
         <v>62.459069999999997</v>
       </c>
-      <c r="E16" s="21">
+      <c r="F16" s="21">
         <v>30.738227999999999</v>
       </c>
-      <c r="F16" s="21">
+      <c r="G16" s="21">
         <v>30.584579999999999</v>
       </c>
-      <c r="G16" s="21">
+      <c r="H16" s="21">
         <v>64.010794300000001</v>
       </c>
-      <c r="H16" s="21">
+      <c r="I16" s="21">
         <v>64.962770178</v>
       </c>
-      <c r="I16" s="21">
+      <c r="J16" s="21">
         <v>30.721707769999998</v>
       </c>
-      <c r="J16" s="21">
+      <c r="K16" s="21">
         <v>30.754858800000001</v>
       </c>
-      <c r="K16" s="21">
+      <c r="L16" s="21">
         <v>13.436368399999999</v>
       </c>
-      <c r="L16" s="21">
+      <c r="M16" s="21">
         <v>11.977791</v>
       </c>
-      <c r="N16" s="21">
+      <c r="O16" s="21">
         <v>30.877478</v>
       </c>
-      <c r="O16" s="21">
+      <c r="P16" s="21">
         <v>30.66</v>
       </c>
-      <c r="P16" s="21">
+      <c r="Q16" s="21">
         <v>31.211466999999999</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="R16" s="21">
         <v>31.880268000000001</v>
       </c>
-      <c r="R16" s="21">
+      <c r="S16" s="21">
         <v>30.716964999999998</v>
       </c>
-      <c r="S16" s="21">
+      <c r="T16" s="21">
         <v>29.746556000000002</v>
       </c>
-      <c r="T16" s="21">
+      <c r="U16" s="21">
         <v>29.076453999999998</v>
       </c>
-      <c r="U16" s="21">
+      <c r="V16" s="21">
         <v>29.443950000000001</v>
       </c>
-      <c r="V16" s="21">
+      <c r="W16" s="21">
         <v>11.154477999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:22" s="21" customFormat="1">
+    <row r="17" spans="1:23" s="21" customFormat="1">
       <c r="A17" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="K17" s="21">
+      <c r="L17" s="21">
         <v>8.5977074000000009</v>
       </c>
-      <c r="L17" s="21">
+      <c r="M17" s="21">
         <v>12.778447999999999</v>
       </c>
-      <c r="V17" s="21">
+      <c r="W17" s="21">
         <v>17.8</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="21" customFormat="1" ht="14" customHeight="1">
+    <row r="18" spans="1:23" s="21" customFormat="1" ht="14" customHeight="1">
       <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
@@ -6442,61 +6478,64 @@
         <v>-4.640949</v>
       </c>
       <c r="D18" s="21">
+        <v>-4.0439959999999999</v>
+      </c>
+      <c r="E18" s="21">
         <v>-0.66238750000000002</v>
       </c>
-      <c r="E18" s="21">
+      <c r="F18" s="21">
         <v>-3.1059860000000001</v>
       </c>
-      <c r="F18" s="21">
+      <c r="G18" s="21">
         <v>-5.8981399999999997</v>
       </c>
-      <c r="G18" s="21">
+      <c r="H18" s="21">
         <v>-0.98127699999999995</v>
       </c>
-      <c r="H18" s="21">
+      <c r="I18" s="21">
         <v>-0.43686686800000002</v>
       </c>
-      <c r="I18" s="21">
+      <c r="J18" s="21">
         <v>-4.6886315600000001</v>
       </c>
-      <c r="J18" s="21">
+      <c r="K18" s="21">
         <v>-3.2696827000000002</v>
       </c>
-      <c r="K18" s="21">
+      <c r="L18" s="21">
         <v>-8.0795293000000008</v>
       </c>
-      <c r="L18" s="21">
+      <c r="M18" s="21">
         <v>-10.718495000000001</v>
       </c>
-      <c r="N18" s="21">
+      <c r="O18" s="21">
         <v>-3.858498</v>
       </c>
-      <c r="O18" s="21">
+      <c r="P18" s="21">
         <v>-4.7</v>
       </c>
-      <c r="P18" s="21">
+      <c r="Q18" s="21">
         <v>-3.9753639999999999</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="R18" s="21">
         <v>-6.589467</v>
       </c>
-      <c r="R18" s="21">
+      <c r="S18" s="21">
         <v>-4.670153</v>
       </c>
-      <c r="S18" s="21">
+      <c r="T18" s="21">
         <v>-6.3059329999999996</v>
       </c>
-      <c r="T18" s="21">
+      <c r="U18" s="21">
         <v>-4.2054489999999998</v>
       </c>
-      <c r="U18" s="21">
+      <c r="V18" s="21">
         <v>-4.4239769999999998</v>
       </c>
-      <c r="V18" s="21">
+      <c r="W18" s="21">
         <v>-11.179836</v>
       </c>
     </row>
-    <row r="19" spans="1:22" s="21" customFormat="1">
+    <row r="19" spans="1:23" s="21" customFormat="1">
       <c r="A19" s="21" t="s">
         <v>8</v>
       </c>
@@ -6507,61 +6546,64 @@
         <v>-2.9664130000000002</v>
       </c>
       <c r="D19" s="21">
+        <v>-3.5158939999999999</v>
+      </c>
+      <c r="E19" s="21">
         <v>-0.30074129999999999</v>
       </c>
-      <c r="E19" s="21">
+      <c r="F19" s="21">
         <v>-1.8089200000000001</v>
       </c>
-      <c r="F19" s="21">
+      <c r="G19" s="21">
         <v>-1.7522850000000001</v>
       </c>
-      <c r="G19" s="21">
+      <c r="H19" s="21">
         <v>-0.32169579999999998</v>
       </c>
-      <c r="H19" s="21">
+      <c r="I19" s="21">
         <v>-0.59282655500000003</v>
       </c>
-      <c r="I19" s="21">
+      <c r="J19" s="21">
         <v>-3.2544300800000001</v>
       </c>
-      <c r="J19" s="21">
+      <c r="K19" s="21">
         <v>-2.0773652</v>
       </c>
-      <c r="K19" s="21">
+      <c r="L19" s="21">
         <v>-0.73294579999999998</v>
       </c>
-      <c r="L19" s="21">
+      <c r="M19" s="21">
         <v>-1.3810519999999999</v>
       </c>
-      <c r="N19" s="21">
+      <c r="O19" s="21">
         <v>-3.1080649999999999</v>
       </c>
-      <c r="O19" s="21">
+      <c r="P19" s="21">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="P19" s="21">
+      <c r="Q19" s="21">
         <v>-3.5504150000000001</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="R19" s="21">
         <v>-2.3749199999999999</v>
       </c>
-      <c r="R19" s="21">
+      <c r="S19" s="21">
         <v>-1.740626</v>
       </c>
-      <c r="S19" s="21">
+      <c r="T19" s="21">
         <v>-1.149972</v>
       </c>
-      <c r="T19" s="21">
+      <c r="U19" s="21">
         <v>-3.8012999999999999</v>
       </c>
-      <c r="U19" s="21">
+      <c r="V19" s="21">
         <v>-4.6329729999999998</v>
       </c>
-      <c r="V19" s="21">
+      <c r="W19" s="21">
         <v>-1.4</v>
       </c>
     </row>
-    <row r="20" spans="1:22" s="21" customFormat="1">
+    <row r="20" spans="1:23" s="21" customFormat="1">
       <c r="A20" s="21" t="s">
         <v>9</v>
       </c>
@@ -6572,153 +6614,156 @@
         <v>-8.3231070000000003</v>
       </c>
       <c r="D20" s="21">
+        <v>-8.3347940000000005</v>
+      </c>
+      <c r="E20" s="21">
         <v>-0.2393874</v>
       </c>
-      <c r="E20" s="21">
+      <c r="F20" s="21">
         <v>-7.3253700000000004</v>
       </c>
-      <c r="F20" s="21">
+      <c r="G20" s="21">
         <v>-7.6310460000000004</v>
       </c>
-      <c r="G20" s="21">
+      <c r="H20" s="21">
         <v>-0.22312940000000001</v>
       </c>
-      <c r="H20" s="21">
+      <c r="I20" s="21">
         <v>-0.28852171599999998</v>
       </c>
-      <c r="I20" s="21">
+      <c r="J20" s="21">
         <v>-8.3550094300000008</v>
       </c>
-      <c r="J20" s="21">
+      <c r="K20" s="21">
         <v>-7.0728663999999997</v>
       </c>
-      <c r="K20" s="21">
+      <c r="L20" s="21">
         <v>-8.4076094999999995</v>
       </c>
-      <c r="L20" s="21">
+      <c r="M20" s="21">
         <v>-9.5678230000000006</v>
       </c>
-      <c r="N20" s="21">
+      <c r="O20" s="21">
         <v>-10.069042</v>
       </c>
-      <c r="O20" s="21">
+      <c r="P20" s="21">
         <v>-8.5</v>
       </c>
-      <c r="P20" s="21">
+      <c r="Q20" s="21">
         <v>-10.401221</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="R20" s="21">
         <v>-9.9066620000000007</v>
       </c>
-      <c r="R20" s="21">
+      <c r="S20" s="21">
         <v>-8.6652190000000004</v>
       </c>
-      <c r="S20" s="21">
+      <c r="T20" s="21">
         <v>-9.8209820000000008</v>
       </c>
-      <c r="T20" s="21">
+      <c r="U20" s="21">
         <v>-10.442672999999999</v>
       </c>
-      <c r="U20" s="21">
+      <c r="V20" s="21">
         <v>-10.520892</v>
       </c>
-      <c r="V20" s="21">
+      <c r="W20" s="21">
         <v>-9.7576470000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:22">
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
         <v>210</v>
       </c>
-      <c r="K27">
+      <c r="L27">
         <v>6.1738270000000002</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>9.932563</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
         <v>10</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>-1.4379709999999999E-3</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>-9.5536179999999998E-2</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>0.15195020000000001</v>
       </c>
-      <c r="P28" s="21">
+      <c r="Q28" s="21">
         <v>1.47323</v>
       </c>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
         <v>11</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>4.1001559999999998E-3</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>0.85033303000000005</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>1.3428956999999999</v>
       </c>
-      <c r="P29" s="21">
+      <c r="Q29" s="21">
         <v>1.0277529999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:22">
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>-1.7003655999999999E-2</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>-0.27255634000000001</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>-0.39319349999999997</v>
       </c>
-      <c r="P30" s="21">
+      <c r="Q30" s="21">
         <v>-1.052503</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:23">
       <c r="A32" s="15" t="s">
         <v>972</v>
       </c>
@@ -6734,258 +6779,259 @@
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
-    </row>
-    <row r="33" spans="1:20">
+      <c r="N32" s="15"/>
+    </row>
+    <row r="33" spans="1:21">
       <c r="A33" t="s">
         <v>57</v>
       </c>
-      <c r="T33" s="17"/>
-    </row>
-    <row r="34" spans="1:20">
+      <c r="U33" s="17"/>
+    </row>
+    <row r="34" spans="1:21">
       <c r="A34" t="s">
         <v>58</v>
       </c>
-      <c r="T34" s="17"/>
-    </row>
-    <row r="35" spans="1:20">
+      <c r="U34" s="17"/>
+    </row>
+    <row r="35" spans="1:21">
       <c r="A35" t="s">
         <v>59</v>
       </c>
-      <c r="T35" s="17"/>
-    </row>
-    <row r="36" spans="1:20">
+      <c r="U35" s="17"/>
+    </row>
+    <row r="36" spans="1:21">
       <c r="A36" t="s">
         <v>60</v>
       </c>
-      <c r="T36" s="17"/>
-    </row>
-    <row r="37" spans="1:20">
+      <c r="U36" s="17"/>
+    </row>
+    <row r="37" spans="1:21">
       <c r="A37" t="s">
         <v>61</v>
       </c>
-      <c r="T37" s="17"/>
-    </row>
-    <row r="38" spans="1:20">
+      <c r="U37" s="17"/>
+    </row>
+    <row r="38" spans="1:21">
       <c r="A38" t="s">
         <v>62</v>
       </c>
-      <c r="T38" s="17"/>
-    </row>
-    <row r="39" spans="1:20">
+      <c r="U38" s="17"/>
+    </row>
+    <row r="39" spans="1:21">
       <c r="A39" t="s">
         <v>63</v>
       </c>
-      <c r="T39" s="17"/>
-    </row>
-    <row r="40" spans="1:20">
+      <c r="U39" s="17"/>
+    </row>
+    <row r="40" spans="1:21">
       <c r="A40" t="s">
         <v>64</v>
       </c>
-      <c r="T40" s="17"/>
-    </row>
-    <row r="41" spans="1:20">
+      <c r="U40" s="17"/>
+    </row>
+    <row r="41" spans="1:21">
       <c r="A41" t="s">
         <v>65</v>
       </c>
-      <c r="T41" s="17"/>
-    </row>
-    <row r="42" spans="1:20">
+      <c r="U41" s="17"/>
+    </row>
+    <row r="42" spans="1:21">
       <c r="A42" t="s">
         <v>66</v>
       </c>
-      <c r="T42" s="17"/>
-    </row>
-    <row r="43" spans="1:20">
+      <c r="U42" s="17"/>
+    </row>
+    <row r="43" spans="1:21">
       <c r="A43" t="s">
         <v>67</v>
       </c>
-      <c r="T43" s="17"/>
-    </row>
-    <row r="44" spans="1:20">
+      <c r="U43" s="17"/>
+    </row>
+    <row r="44" spans="1:21">
       <c r="A44" t="s">
         <v>68</v>
       </c>
-      <c r="T44" s="17"/>
-    </row>
-    <row r="45" spans="1:20">
+      <c r="U44" s="17"/>
+    </row>
+    <row r="45" spans="1:21">
       <c r="A45" t="s">
         <v>69</v>
       </c>
-      <c r="T45" s="17"/>
-    </row>
-    <row r="46" spans="1:20">
+      <c r="U45" s="17"/>
+    </row>
+    <row r="46" spans="1:21">
       <c r="A46" t="s">
         <v>70</v>
       </c>
-      <c r="T46" s="17"/>
-    </row>
-    <row r="47" spans="1:20">
+      <c r="U46" s="17"/>
+    </row>
+    <row r="47" spans="1:21">
       <c r="A47" t="s">
         <v>71</v>
       </c>
-      <c r="T47" s="17"/>
-    </row>
-    <row r="48" spans="1:20">
+      <c r="U47" s="17"/>
+    </row>
+    <row r="48" spans="1:21">
       <c r="A48" t="s">
         <v>72</v>
       </c>
-      <c r="T48" s="17"/>
-    </row>
-    <row r="49" spans="1:20">
+      <c r="U48" s="17"/>
+    </row>
+    <row r="49" spans="1:21">
       <c r="A49" t="s">
         <v>73</v>
       </c>
-      <c r="T49" s="17"/>
-    </row>
-    <row r="50" spans="1:20">
+      <c r="U49" s="17"/>
+    </row>
+    <row r="50" spans="1:21">
       <c r="A50" t="s">
         <v>74</v>
       </c>
-      <c r="T50" s="17"/>
-    </row>
-    <row r="51" spans="1:20">
+      <c r="U50" s="17"/>
+    </row>
+    <row r="51" spans="1:21">
       <c r="A51" t="s">
         <v>75</v>
       </c>
-      <c r="T51" s="17"/>
-    </row>
-    <row r="52" spans="1:20">
+      <c r="U51" s="17"/>
+    </row>
+    <row r="52" spans="1:21">
       <c r="A52" t="s">
         <v>76</v>
       </c>
-      <c r="T52" s="17"/>
-    </row>
-    <row r="53" spans="1:20">
+      <c r="U52" s="17"/>
+    </row>
+    <row r="53" spans="1:21">
       <c r="A53" t="s">
         <v>77</v>
       </c>
-      <c r="T53" s="17"/>
-    </row>
-    <row r="54" spans="1:20">
+      <c r="U53" s="17"/>
+    </row>
+    <row r="54" spans="1:21">
       <c r="A54" t="s">
         <v>78</v>
       </c>
-      <c r="T54" s="17"/>
-    </row>
-    <row r="55" spans="1:20">
+      <c r="U54" s="17"/>
+    </row>
+    <row r="55" spans="1:21">
       <c r="A55" t="s">
         <v>79</v>
       </c>
-      <c r="T55" s="17"/>
-    </row>
-    <row r="56" spans="1:20">
+      <c r="U55" s="17"/>
+    </row>
+    <row r="56" spans="1:21">
       <c r="A56" t="s">
         <v>80</v>
       </c>
-      <c r="T56" s="17"/>
-    </row>
-    <row r="57" spans="1:20">
+      <c r="U56" s="17"/>
+    </row>
+    <row r="57" spans="1:21">
       <c r="A57" t="s">
         <v>81</v>
       </c>
-      <c r="T57" s="17"/>
-    </row>
-    <row r="58" spans="1:20">
+      <c r="U57" s="17"/>
+    </row>
+    <row r="58" spans="1:21">
       <c r="A58" t="s">
         <v>82</v>
       </c>
-      <c r="T58" s="17"/>
-    </row>
-    <row r="59" spans="1:20">
+      <c r="U58" s="17"/>
+    </row>
+    <row r="59" spans="1:21">
       <c r="A59" t="s">
         <v>83</v>
       </c>
-      <c r="T59" s="17"/>
-    </row>
-    <row r="60" spans="1:20">
+      <c r="U59" s="17"/>
+    </row>
+    <row r="60" spans="1:21">
       <c r="A60" t="s">
         <v>84</v>
       </c>
-      <c r="T60" s="17"/>
-    </row>
-    <row r="61" spans="1:20">
+      <c r="U60" s="17"/>
+    </row>
+    <row r="61" spans="1:21">
       <c r="A61" t="s">
         <v>85</v>
       </c>
-      <c r="T61" s="17"/>
-    </row>
-    <row r="62" spans="1:20">
+      <c r="U61" s="17"/>
+    </row>
+    <row r="62" spans="1:21">
       <c r="A62" t="s">
         <v>86</v>
       </c>
-      <c r="T62" s="17"/>
-    </row>
-    <row r="63" spans="1:20">
+      <c r="U62" s="17"/>
+    </row>
+    <row r="63" spans="1:21">
       <c r="A63" t="s">
         <v>87</v>
       </c>
-      <c r="T63" s="17"/>
-    </row>
-    <row r="64" spans="1:20">
+      <c r="U63" s="17"/>
+    </row>
+    <row r="64" spans="1:21">
       <c r="A64" t="s">
         <v>88</v>
       </c>
-      <c r="T64" s="17"/>
-    </row>
-    <row r="65" spans="1:21">
+      <c r="U64" s="17"/>
+    </row>
+    <row r="65" spans="1:22">
       <c r="A65" t="s">
         <v>89</v>
       </c>
-      <c r="T65" s="17"/>
-    </row>
-    <row r="66" spans="1:21">
+      <c r="U65" s="17"/>
+    </row>
+    <row r="66" spans="1:22">
       <c r="A66" t="s">
         <v>90</v>
       </c>
-      <c r="T66" s="17"/>
-    </row>
-    <row r="67" spans="1:21">
+      <c r="U66" s="17"/>
+    </row>
+    <row r="67" spans="1:22">
       <c r="A67" t="s">
         <v>91</v>
       </c>
-      <c r="T67" s="17"/>
-    </row>
-    <row r="68" spans="1:21">
+      <c r="U67" s="17"/>
+    </row>
+    <row r="68" spans="1:22">
       <c r="A68" t="s">
         <v>92</v>
       </c>
-      <c r="T68" s="17"/>
-    </row>
-    <row r="69" spans="1:21">
+      <c r="U68" s="17"/>
+    </row>
+    <row r="69" spans="1:22">
       <c r="A69" t="s">
         <v>93</v>
       </c>
-      <c r="T69" s="17"/>
-    </row>
-    <row r="70" spans="1:21">
+      <c r="U69" s="17"/>
+    </row>
+    <row r="70" spans="1:22">
       <c r="A70" t="s">
         <v>94</v>
       </c>
-      <c r="T70" s="17"/>
-    </row>
-    <row r="71" spans="1:21">
-      <c r="N71" s="22"/>
+      <c r="U70" s="17"/>
+    </row>
+    <row r="71" spans="1:22">
       <c r="O71" s="22"/>
       <c r="P71" s="22"/>
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="22"/>
-      <c r="T71" s="17"/>
+      <c r="T71" s="22"/>
       <c r="U71" s="17"/>
-    </row>
-    <row r="72" spans="1:21">
-      <c r="T72" s="17"/>
-    </row>
-    <row r="73" spans="1:21">
-      <c r="T73" s="17"/>
-    </row>
-    <row r="74" spans="1:21">
-      <c r="T74" s="17"/>
-    </row>
-    <row r="75" spans="1:21">
-      <c r="T75" s="17"/>
-    </row>
-    <row r="76" spans="1:21">
+      <c r="V71" s="17"/>
+    </row>
+    <row r="72" spans="1:22">
+      <c r="U72" s="17"/>
+    </row>
+    <row r="73" spans="1:22">
+      <c r="U73" s="17"/>
+    </row>
+    <row r="74" spans="1:22">
+      <c r="U74" s="17"/>
+    </row>
+    <row r="75" spans="1:22">
+      <c r="U75" s="17"/>
+    </row>
+    <row r="76" spans="1:22">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -6999,733 +7045,734 @@
       <c r="K76" s="17"/>
       <c r="L76" s="17"/>
       <c r="M76" s="17"/>
-      <c r="T76" s="17"/>
-    </row>
-    <row r="77" spans="1:21">
+      <c r="N76" s="17"/>
+      <c r="U76" s="17"/>
+    </row>
+    <row r="77" spans="1:22">
       <c r="A77" t="s">
         <v>171</v>
       </c>
-      <c r="T77" s="17"/>
-    </row>
-    <row r="78" spans="1:21">
+      <c r="U77" s="17"/>
+    </row>
+    <row r="78" spans="1:22">
       <c r="A78" t="s">
         <v>172</v>
       </c>
-      <c r="T78" s="17"/>
-    </row>
-    <row r="79" spans="1:21">
+      <c r="U78" s="17"/>
+    </row>
+    <row r="79" spans="1:22">
       <c r="A79" t="s">
         <v>173</v>
       </c>
-      <c r="T79" s="17"/>
-    </row>
-    <row r="80" spans="1:21">
+      <c r="U79" s="17"/>
+    </row>
+    <row r="80" spans="1:22">
       <c r="A80" t="s">
         <v>174</v>
       </c>
-      <c r="T80" s="17"/>
-    </row>
-    <row r="81" spans="1:20">
+      <c r="U80" s="17"/>
+    </row>
+    <row r="81" spans="1:21">
       <c r="A81" t="s">
         <v>175</v>
       </c>
-      <c r="T81" s="17"/>
-    </row>
-    <row r="82" spans="1:20">
+      <c r="U81" s="17"/>
+    </row>
+    <row r="82" spans="1:21">
       <c r="A82" t="s">
         <v>176</v>
       </c>
-      <c r="T82" s="17"/>
-    </row>
-    <row r="83" spans="1:20">
+      <c r="U82" s="17"/>
+    </row>
+    <row r="83" spans="1:21">
       <c r="A83" t="s">
         <v>177</v>
       </c>
-      <c r="T83" s="17"/>
-    </row>
-    <row r="84" spans="1:20">
+      <c r="U83" s="17"/>
+    </row>
+    <row r="84" spans="1:21">
       <c r="A84" t="s">
         <v>178</v>
       </c>
-      <c r="T84" s="17"/>
-    </row>
-    <row r="85" spans="1:20">
+      <c r="U84" s="17"/>
+    </row>
+    <row r="85" spans="1:21">
       <c r="A85" t="s">
         <v>179</v>
       </c>
-      <c r="T85" s="17"/>
-    </row>
-    <row r="86" spans="1:20">
+      <c r="U85" s="17"/>
+    </row>
+    <row r="86" spans="1:21">
       <c r="A86" t="s">
         <v>180</v>
       </c>
-      <c r="T86" s="17"/>
-    </row>
-    <row r="87" spans="1:20">
+      <c r="U86" s="17"/>
+    </row>
+    <row r="87" spans="1:21">
       <c r="A87" t="s">
         <v>181</v>
       </c>
-      <c r="T87" s="17"/>
-    </row>
-    <row r="88" spans="1:20">
+      <c r="U87" s="17"/>
+    </row>
+    <row r="88" spans="1:21">
       <c r="A88" t="s">
         <v>182</v>
       </c>
-      <c r="T88" s="17"/>
-    </row>
-    <row r="89" spans="1:20">
+      <c r="U88" s="17"/>
+    </row>
+    <row r="89" spans="1:21">
       <c r="A89" t="s">
         <v>183</v>
       </c>
-      <c r="T89" s="17"/>
-    </row>
-    <row r="90" spans="1:20">
+      <c r="U89" s="17"/>
+    </row>
+    <row r="90" spans="1:21">
       <c r="A90" t="s">
         <v>184</v>
       </c>
-      <c r="T90" s="17"/>
-    </row>
-    <row r="91" spans="1:20">
+      <c r="U90" s="17"/>
+    </row>
+    <row r="91" spans="1:21">
       <c r="A91" t="s">
         <v>185</v>
       </c>
-      <c r="T91" s="17"/>
-    </row>
-    <row r="92" spans="1:20">
+      <c r="U91" s="17"/>
+    </row>
+    <row r="92" spans="1:21">
       <c r="A92" t="s">
         <v>186</v>
       </c>
-      <c r="T92" s="17"/>
-    </row>
-    <row r="93" spans="1:20">
+      <c r="U92" s="17"/>
+    </row>
+    <row r="93" spans="1:21">
       <c r="A93" t="s">
         <v>187</v>
       </c>
-      <c r="T93" s="17"/>
-    </row>
-    <row r="94" spans="1:20">
+      <c r="U93" s="17"/>
+    </row>
+    <row r="94" spans="1:21">
       <c r="A94" t="s">
         <v>188</v>
       </c>
-      <c r="T94" s="17"/>
-    </row>
-    <row r="95" spans="1:20">
+      <c r="U94" s="17"/>
+    </row>
+    <row r="95" spans="1:21">
       <c r="A95" t="s">
         <v>189</v>
       </c>
-      <c r="T95" s="17"/>
-    </row>
-    <row r="96" spans="1:20">
+      <c r="U95" s="17"/>
+    </row>
+    <row r="96" spans="1:21">
       <c r="A96" t="s">
         <v>190</v>
       </c>
-      <c r="T96" s="17"/>
-    </row>
-    <row r="97" spans="1:20">
+      <c r="U96" s="17"/>
+    </row>
+    <row r="97" spans="1:21">
       <c r="A97" t="s">
         <v>191</v>
       </c>
-      <c r="T97" s="17"/>
-    </row>
-    <row r="98" spans="1:20">
+      <c r="U97" s="17"/>
+    </row>
+    <row r="98" spans="1:21">
       <c r="A98" t="s">
         <v>192</v>
       </c>
-      <c r="T98" s="17"/>
-    </row>
-    <row r="99" spans="1:20">
+      <c r="U98" s="17"/>
+    </row>
+    <row r="99" spans="1:21">
       <c r="A99" t="s">
         <v>193</v>
       </c>
-      <c r="T99" s="17"/>
-    </row>
-    <row r="100" spans="1:20">
+      <c r="U99" s="17"/>
+    </row>
+    <row r="100" spans="1:21">
       <c r="A100" t="s">
         <v>194</v>
       </c>
-      <c r="T100" s="17"/>
-    </row>
-    <row r="101" spans="1:20">
+      <c r="U100" s="17"/>
+    </row>
+    <row r="101" spans="1:21">
       <c r="A101" t="s">
         <v>195</v>
       </c>
-      <c r="T101" s="17"/>
-    </row>
-    <row r="102" spans="1:20">
+      <c r="U101" s="17"/>
+    </row>
+    <row r="102" spans="1:21">
       <c r="A102" t="s">
         <v>196</v>
       </c>
-      <c r="T102" s="17"/>
-    </row>
-    <row r="103" spans="1:20">
+      <c r="U102" s="17"/>
+    </row>
+    <row r="103" spans="1:21">
       <c r="A103" t="s">
         <v>197</v>
       </c>
-      <c r="T103" s="17"/>
-    </row>
-    <row r="104" spans="1:20">
+      <c r="U103" s="17"/>
+    </row>
+    <row r="104" spans="1:21">
       <c r="A104" t="s">
         <v>198</v>
       </c>
-      <c r="T104" s="17"/>
-    </row>
-    <row r="105" spans="1:20">
+      <c r="U104" s="17"/>
+    </row>
+    <row r="105" spans="1:21">
       <c r="A105" t="s">
         <v>199</v>
       </c>
-      <c r="T105" s="17"/>
-    </row>
-    <row r="106" spans="1:20">
+      <c r="U105" s="17"/>
+    </row>
+    <row r="106" spans="1:21">
       <c r="A106" t="s">
         <v>200</v>
       </c>
-      <c r="T106" s="17"/>
-    </row>
-    <row r="107" spans="1:20">
+      <c r="U106" s="17"/>
+    </row>
+    <row r="107" spans="1:21">
       <c r="A107" t="s">
         <v>201</v>
       </c>
-      <c r="T107" s="17"/>
-    </row>
-    <row r="108" spans="1:20">
+      <c r="U107" s="17"/>
+    </row>
+    <row r="108" spans="1:21">
       <c r="A108" t="s">
         <v>202</v>
       </c>
-      <c r="T108" s="17"/>
-    </row>
-    <row r="109" spans="1:20">
+      <c r="U108" s="17"/>
+    </row>
+    <row r="109" spans="1:21">
       <c r="A109" t="s">
         <v>203</v>
       </c>
-      <c r="T109" s="17"/>
-    </row>
-    <row r="110" spans="1:20">
+      <c r="U109" s="17"/>
+    </row>
+    <row r="110" spans="1:21">
       <c r="A110" t="s">
         <v>204</v>
       </c>
-      <c r="T110" s="17"/>
-    </row>
-    <row r="111" spans="1:20">
+      <c r="U110" s="17"/>
+    </row>
+    <row r="111" spans="1:21">
       <c r="A111" t="s">
         <v>205</v>
       </c>
-      <c r="T111" s="17"/>
-    </row>
-    <row r="112" spans="1:20">
+      <c r="U111" s="17"/>
+    </row>
+    <row r="112" spans="1:21">
       <c r="A112" t="s">
         <v>206</v>
       </c>
-      <c r="T112" s="17"/>
-    </row>
-    <row r="113" spans="1:20">
+      <c r="U112" s="17"/>
+    </row>
+    <row r="113" spans="1:21">
       <c r="A113" t="s">
         <v>207</v>
       </c>
-      <c r="T113" s="17"/>
-    </row>
-    <row r="114" spans="1:20">
+      <c r="U113" s="17"/>
+    </row>
+    <row r="114" spans="1:21">
       <c r="A114" t="s">
         <v>208</v>
       </c>
-      <c r="T114" s="17"/>
-    </row>
-    <row r="115" spans="1:20">
-      <c r="T115" s="17"/>
-    </row>
-    <row r="116" spans="1:20">
-      <c r="T116" s="17"/>
-    </row>
-    <row r="117" spans="1:20">
-      <c r="T117" s="17"/>
-    </row>
-    <row r="118" spans="1:20">
-      <c r="T118" s="17"/>
-    </row>
-    <row r="119" spans="1:20">
-      <c r="T119" s="17"/>
-    </row>
-    <row r="120" spans="1:20">
-      <c r="T120" s="17"/>
-    </row>
-    <row r="121" spans="1:20">
+      <c r="U114" s="17"/>
+    </row>
+    <row r="115" spans="1:21">
+      <c r="U115" s="17"/>
+    </row>
+    <row r="116" spans="1:21">
+      <c r="U116" s="17"/>
+    </row>
+    <row r="117" spans="1:21">
+      <c r="U117" s="17"/>
+    </row>
+    <row r="118" spans="1:21">
+      <c r="U118" s="17"/>
+    </row>
+    <row r="119" spans="1:21">
+      <c r="U119" s="17"/>
+    </row>
+    <row r="120" spans="1:21">
+      <c r="U120" s="17"/>
+    </row>
+    <row r="121" spans="1:21">
       <c r="A121" t="s">
         <v>133</v>
       </c>
-      <c r="T121" s="17"/>
-    </row>
-    <row r="122" spans="1:20">
+      <c r="U121" s="17"/>
+    </row>
+    <row r="122" spans="1:21">
       <c r="A122" t="s">
         <v>134</v>
       </c>
-      <c r="T122" s="17"/>
-    </row>
-    <row r="123" spans="1:20">
+      <c r="U122" s="17"/>
+    </row>
+    <row r="123" spans="1:21">
       <c r="A123" t="s">
         <v>135</v>
       </c>
-      <c r="T123" s="17"/>
-    </row>
-    <row r="124" spans="1:20">
+      <c r="U123" s="17"/>
+    </row>
+    <row r="124" spans="1:21">
       <c r="A124" t="s">
         <v>136</v>
       </c>
-      <c r="T124" s="17"/>
-    </row>
-    <row r="125" spans="1:20">
+      <c r="U124" s="17"/>
+    </row>
+    <row r="125" spans="1:21">
       <c r="A125" t="s">
         <v>137</v>
       </c>
-      <c r="T125" s="17"/>
-    </row>
-    <row r="126" spans="1:20">
+      <c r="U125" s="17"/>
+    </row>
+    <row r="126" spans="1:21">
       <c r="A126" t="s">
         <v>138</v>
       </c>
-      <c r="T126" s="17"/>
-    </row>
-    <row r="127" spans="1:20">
+      <c r="U126" s="17"/>
+    </row>
+    <row r="127" spans="1:21">
       <c r="A127" t="s">
         <v>139</v>
       </c>
-      <c r="T127" s="17"/>
-    </row>
-    <row r="128" spans="1:20">
+      <c r="U127" s="17"/>
+    </row>
+    <row r="128" spans="1:21">
       <c r="A128" t="s">
         <v>140</v>
       </c>
-      <c r="T128" s="17"/>
-    </row>
-    <row r="129" spans="1:20">
+      <c r="U128" s="17"/>
+    </row>
+    <row r="129" spans="1:21">
       <c r="A129" t="s">
         <v>141</v>
       </c>
-      <c r="T129" s="17"/>
-    </row>
-    <row r="130" spans="1:20">
+      <c r="U129" s="17"/>
+    </row>
+    <row r="130" spans="1:21">
       <c r="A130" t="s">
         <v>142</v>
       </c>
-      <c r="T130" s="17"/>
-    </row>
-    <row r="131" spans="1:20">
+      <c r="U130" s="17"/>
+    </row>
+    <row r="131" spans="1:21">
       <c r="A131" t="s">
         <v>143</v>
       </c>
-      <c r="T131" s="17"/>
-    </row>
-    <row r="132" spans="1:20">
+      <c r="U131" s="17"/>
+    </row>
+    <row r="132" spans="1:21">
       <c r="A132" t="s">
         <v>144</v>
       </c>
-      <c r="T132" s="17"/>
-    </row>
-    <row r="133" spans="1:20">
+      <c r="U132" s="17"/>
+    </row>
+    <row r="133" spans="1:21">
       <c r="A133" t="s">
         <v>145</v>
       </c>
-      <c r="T133" s="17"/>
-    </row>
-    <row r="134" spans="1:20">
+      <c r="U133" s="17"/>
+    </row>
+    <row r="134" spans="1:21">
       <c r="A134" t="s">
         <v>146</v>
       </c>
-      <c r="T134" s="17"/>
-    </row>
-    <row r="135" spans="1:20">
+      <c r="U134" s="17"/>
+    </row>
+    <row r="135" spans="1:21">
       <c r="A135" t="s">
         <v>147</v>
       </c>
-      <c r="T135" s="17"/>
-    </row>
-    <row r="136" spans="1:20">
+      <c r="U135" s="17"/>
+    </row>
+    <row r="136" spans="1:21">
       <c r="A136" t="s">
         <v>148</v>
       </c>
-      <c r="T136" s="17"/>
-    </row>
-    <row r="137" spans="1:20">
+      <c r="U136" s="17"/>
+    </row>
+    <row r="137" spans="1:21">
       <c r="A137" t="s">
         <v>149</v>
       </c>
-      <c r="T137" s="17"/>
-    </row>
-    <row r="138" spans="1:20">
+      <c r="U137" s="17"/>
+    </row>
+    <row r="138" spans="1:21">
       <c r="A138" t="s">
         <v>150</v>
       </c>
-      <c r="T138" s="17"/>
-    </row>
-    <row r="139" spans="1:20">
+      <c r="U138" s="17"/>
+    </row>
+    <row r="139" spans="1:21">
       <c r="A139" t="s">
         <v>151</v>
       </c>
-      <c r="T139" s="17"/>
-    </row>
-    <row r="140" spans="1:20">
+      <c r="U139" s="17"/>
+    </row>
+    <row r="140" spans="1:21">
       <c r="A140" t="s">
         <v>152</v>
       </c>
-      <c r="T140" s="17"/>
-    </row>
-    <row r="141" spans="1:20">
+      <c r="U140" s="17"/>
+    </row>
+    <row r="141" spans="1:21">
       <c r="A141" t="s">
         <v>153</v>
       </c>
-      <c r="T141" s="17"/>
-    </row>
-    <row r="142" spans="1:20">
+      <c r="U141" s="17"/>
+    </row>
+    <row r="142" spans="1:21">
       <c r="A142" t="s">
         <v>154</v>
       </c>
-      <c r="T142" s="17"/>
-    </row>
-    <row r="143" spans="1:20">
+      <c r="U142" s="17"/>
+    </row>
+    <row r="143" spans="1:21">
       <c r="A143" t="s">
         <v>155</v>
       </c>
-      <c r="T143" s="17"/>
-    </row>
-    <row r="144" spans="1:20">
+      <c r="U143" s="17"/>
+    </row>
+    <row r="144" spans="1:21">
       <c r="A144" t="s">
         <v>156</v>
       </c>
-      <c r="T144" s="17"/>
-    </row>
-    <row r="145" spans="1:20">
+      <c r="U144" s="17"/>
+    </row>
+    <row r="145" spans="1:21">
       <c r="A145" t="s">
         <v>157</v>
       </c>
-      <c r="T145" s="17"/>
-    </row>
-    <row r="146" spans="1:20">
+      <c r="U145" s="17"/>
+    </row>
+    <row r="146" spans="1:21">
       <c r="A146" t="s">
         <v>158</v>
       </c>
-      <c r="T146" s="17"/>
-    </row>
-    <row r="147" spans="1:20">
+      <c r="U146" s="17"/>
+    </row>
+    <row r="147" spans="1:21">
       <c r="A147" t="s">
         <v>159</v>
       </c>
-      <c r="T147" s="17"/>
-    </row>
-    <row r="148" spans="1:20">
+      <c r="U147" s="17"/>
+    </row>
+    <row r="148" spans="1:21">
       <c r="A148" t="s">
         <v>160</v>
       </c>
-      <c r="T148" s="17"/>
-    </row>
-    <row r="149" spans="1:20">
+      <c r="U148" s="17"/>
+    </row>
+    <row r="149" spans="1:21">
       <c r="A149" t="s">
         <v>161</v>
       </c>
-      <c r="T149" s="17"/>
-    </row>
-    <row r="150" spans="1:20">
+      <c r="U149" s="17"/>
+    </row>
+    <row r="150" spans="1:21">
       <c r="A150" t="s">
         <v>162</v>
       </c>
-      <c r="T150" s="17"/>
-    </row>
-    <row r="151" spans="1:20">
+      <c r="U150" s="17"/>
+    </row>
+    <row r="151" spans="1:21">
       <c r="A151" t="s">
         <v>163</v>
       </c>
-      <c r="T151" s="17"/>
-    </row>
-    <row r="152" spans="1:20">
+      <c r="U151" s="17"/>
+    </row>
+    <row r="152" spans="1:21">
       <c r="A152" t="s">
         <v>164</v>
       </c>
-      <c r="T152" s="17"/>
-    </row>
-    <row r="153" spans="1:20">
+      <c r="U152" s="17"/>
+    </row>
+    <row r="153" spans="1:21">
       <c r="A153" t="s">
         <v>165</v>
       </c>
-      <c r="T153" s="17"/>
-    </row>
-    <row r="154" spans="1:20">
+      <c r="U153" s="17"/>
+    </row>
+    <row r="154" spans="1:21">
       <c r="A154" t="s">
         <v>166</v>
       </c>
-      <c r="T154" s="17"/>
-    </row>
-    <row r="155" spans="1:20">
+      <c r="U154" s="17"/>
+    </row>
+    <row r="155" spans="1:21">
       <c r="A155" t="s">
         <v>167</v>
       </c>
-      <c r="T155" s="17"/>
-    </row>
-    <row r="156" spans="1:20">
+      <c r="U155" s="17"/>
+    </row>
+    <row r="156" spans="1:21">
       <c r="A156" t="s">
         <v>168</v>
       </c>
-      <c r="T156" s="17"/>
-    </row>
-    <row r="157" spans="1:20">
+      <c r="U156" s="17"/>
+    </row>
+    <row r="157" spans="1:21">
       <c r="A157" t="s">
         <v>169</v>
       </c>
-      <c r="T157" s="17"/>
-    </row>
-    <row r="158" spans="1:20">
+      <c r="U157" s="17"/>
+    </row>
+    <row r="158" spans="1:21">
       <c r="A158" t="s">
         <v>170</v>
       </c>
-      <c r="T158" s="17"/>
-    </row>
-    <row r="159" spans="1:20">
-      <c r="T159" s="17"/>
-    </row>
-    <row r="160" spans="1:20">
-      <c r="T160" s="17"/>
-    </row>
-    <row r="161" spans="1:20">
-      <c r="T161" s="17"/>
-    </row>
-    <row r="162" spans="1:20">
-      <c r="T162" s="17"/>
-    </row>
-    <row r="163" spans="1:20">
-      <c r="T163" s="17"/>
-    </row>
-    <row r="164" spans="1:20">
-      <c r="T164" s="17"/>
-    </row>
-    <row r="165" spans="1:20">
+      <c r="U158" s="17"/>
+    </row>
+    <row r="159" spans="1:21">
+      <c r="U159" s="17"/>
+    </row>
+    <row r="160" spans="1:21">
+      <c r="U160" s="17"/>
+    </row>
+    <row r="161" spans="1:21">
+      <c r="U161" s="17"/>
+    </row>
+    <row r="162" spans="1:21">
+      <c r="U162" s="17"/>
+    </row>
+    <row r="163" spans="1:21">
+      <c r="U163" s="17"/>
+    </row>
+    <row r="164" spans="1:21">
+      <c r="U164" s="17"/>
+    </row>
+    <row r="165" spans="1:21">
       <c r="A165" t="s">
         <v>95</v>
       </c>
-      <c r="T165" s="17"/>
-    </row>
-    <row r="166" spans="1:20">
+      <c r="U165" s="17"/>
+    </row>
+    <row r="166" spans="1:21">
       <c r="A166" t="s">
         <v>96</v>
       </c>
-      <c r="T166" s="17"/>
-    </row>
-    <row r="167" spans="1:20">
+      <c r="U166" s="17"/>
+    </row>
+    <row r="167" spans="1:21">
       <c r="A167" t="s">
         <v>97</v>
       </c>
-      <c r="T167" s="17"/>
-    </row>
-    <row r="168" spans="1:20">
+      <c r="U167" s="17"/>
+    </row>
+    <row r="168" spans="1:21">
       <c r="A168" t="s">
         <v>98</v>
       </c>
-      <c r="T168" s="17"/>
-    </row>
-    <row r="169" spans="1:20">
+      <c r="U168" s="17"/>
+    </row>
+    <row r="169" spans="1:21">
       <c r="A169" t="s">
         <v>99</v>
       </c>
-      <c r="T169" s="17"/>
-    </row>
-    <row r="170" spans="1:20">
+      <c r="U169" s="17"/>
+    </row>
+    <row r="170" spans="1:21">
       <c r="A170" t="s">
         <v>100</v>
       </c>
-      <c r="T170" s="17"/>
-    </row>
-    <row r="171" spans="1:20">
+      <c r="U170" s="17"/>
+    </row>
+    <row r="171" spans="1:21">
       <c r="A171" t="s">
         <v>101</v>
       </c>
-      <c r="T171" s="17"/>
-    </row>
-    <row r="172" spans="1:20">
+      <c r="U171" s="17"/>
+    </row>
+    <row r="172" spans="1:21">
       <c r="A172" t="s">
         <v>102</v>
       </c>
-      <c r="T172" s="17"/>
-    </row>
-    <row r="173" spans="1:20">
+      <c r="U172" s="17"/>
+    </row>
+    <row r="173" spans="1:21">
       <c r="A173" t="s">
         <v>103</v>
       </c>
-      <c r="T173" s="17"/>
-    </row>
-    <row r="174" spans="1:20">
+      <c r="U173" s="17"/>
+    </row>
+    <row r="174" spans="1:21">
       <c r="A174" t="s">
         <v>104</v>
       </c>
-      <c r="T174" s="17"/>
-    </row>
-    <row r="175" spans="1:20">
+      <c r="U174" s="17"/>
+    </row>
+    <row r="175" spans="1:21">
       <c r="A175" t="s">
         <v>105</v>
       </c>
-      <c r="T175" s="17"/>
-    </row>
-    <row r="176" spans="1:20">
+      <c r="U175" s="17"/>
+    </row>
+    <row r="176" spans="1:21">
       <c r="A176" t="s">
         <v>106</v>
       </c>
-      <c r="T176" s="17"/>
-    </row>
-    <row r="177" spans="1:20">
+      <c r="U176" s="17"/>
+    </row>
+    <row r="177" spans="1:21">
       <c r="A177" t="s">
         <v>107</v>
       </c>
-      <c r="T177" s="17"/>
-    </row>
-    <row r="178" spans="1:20">
+      <c r="U177" s="17"/>
+    </row>
+    <row r="178" spans="1:21">
       <c r="A178" t="s">
         <v>108</v>
       </c>
-      <c r="T178" s="17"/>
-    </row>
-    <row r="179" spans="1:20">
+      <c r="U178" s="17"/>
+    </row>
+    <row r="179" spans="1:21">
       <c r="A179" t="s">
         <v>109</v>
       </c>
-      <c r="T179" s="17"/>
-    </row>
-    <row r="180" spans="1:20">
+      <c r="U179" s="17"/>
+    </row>
+    <row r="180" spans="1:21">
       <c r="A180" t="s">
         <v>110</v>
       </c>
-      <c r="T180" s="17"/>
-    </row>
-    <row r="181" spans="1:20">
+      <c r="U180" s="17"/>
+    </row>
+    <row r="181" spans="1:21">
       <c r="A181" t="s">
         <v>111</v>
       </c>
-      <c r="T181" s="17"/>
-    </row>
-    <row r="182" spans="1:20">
+      <c r="U181" s="17"/>
+    </row>
+    <row r="182" spans="1:21">
       <c r="A182" t="s">
         <v>112</v>
       </c>
-      <c r="T182" s="17"/>
-    </row>
-    <row r="183" spans="1:20">
+      <c r="U182" s="17"/>
+    </row>
+    <row r="183" spans="1:21">
       <c r="A183" t="s">
         <v>113</v>
       </c>
-      <c r="T183" s="17"/>
-    </row>
-    <row r="184" spans="1:20">
+      <c r="U183" s="17"/>
+    </row>
+    <row r="184" spans="1:21">
       <c r="A184" t="s">
         <v>114</v>
       </c>
-      <c r="T184" s="17"/>
-    </row>
-    <row r="185" spans="1:20">
+      <c r="U184" s="17"/>
+    </row>
+    <row r="185" spans="1:21">
       <c r="A185" t="s">
         <v>115</v>
       </c>
-      <c r="T185" s="17"/>
-    </row>
-    <row r="186" spans="1:20">
+      <c r="U185" s="17"/>
+    </row>
+    <row r="186" spans="1:21">
       <c r="A186" t="s">
         <v>116</v>
       </c>
-      <c r="N186" s="22"/>
       <c r="O186" s="22"/>
       <c r="P186" s="22"/>
       <c r="Q186" s="22"/>
       <c r="R186" s="22"/>
       <c r="S186" s="22"/>
-      <c r="T186" s="17"/>
-    </row>
-    <row r="187" spans="1:20">
+      <c r="T186" s="22"/>
+      <c r="U186" s="17"/>
+    </row>
+    <row r="187" spans="1:21">
       <c r="A187" t="s">
         <v>117</v>
       </c>
-      <c r="N187" s="22"/>
       <c r="O187" s="22"/>
       <c r="P187" s="22"/>
       <c r="Q187" s="22"/>
       <c r="R187" s="22"/>
       <c r="S187" s="22"/>
-      <c r="T187" s="17"/>
-    </row>
-    <row r="188" spans="1:20">
+      <c r="T187" s="22"/>
+      <c r="U187" s="17"/>
+    </row>
+    <row r="188" spans="1:21">
       <c r="A188" t="s">
         <v>118</v>
       </c>
-      <c r="N188" s="22"/>
       <c r="O188" s="22"/>
       <c r="P188" s="22"/>
       <c r="Q188" s="22"/>
       <c r="R188" s="22"/>
       <c r="S188" s="22"/>
-      <c r="T188" s="17"/>
-    </row>
-    <row r="189" spans="1:20">
+      <c r="T188" s="22"/>
+      <c r="U188" s="17"/>
+    </row>
+    <row r="189" spans="1:21">
       <c r="A189" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="190" spans="1:20">
+    <row r="190" spans="1:21">
       <c r="A190" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="191" spans="1:20">
+    <row r="191" spans="1:21">
       <c r="A191" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="192" spans="1:20">
+    <row r="192" spans="1:21">
       <c r="A192" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:14">
       <c r="A193" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:14">
       <c r="A194" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:14">
       <c r="A195" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:14">
       <c r="A196" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:14">
       <c r="A197" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:14">
       <c r="A198" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:14">
       <c r="A199" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:14">
       <c r="A200" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:14">
       <c r="A201" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:14">
       <c r="A202" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:14">
       <c r="A203" s="17"/>
       <c r="B203" s="17"/>
       <c r="C203" s="17"/>
@@ -7739,8 +7786,9 @@
       <c r="K203" s="17"/>
       <c r="L203" s="17"/>
       <c r="M203" s="17"/>
-    </row>
-    <row r="204" spans="1:13">
+      <c r="N203" s="17"/>
+    </row>
+    <row r="204" spans="1:14">
       <c r="A204" s="17"/>
       <c r="B204" s="17"/>
       <c r="C204" s="17"/>
@@ -7754,8 +7802,9 @@
       <c r="K204" s="17"/>
       <c r="L204" s="17"/>
       <c r="M204" s="17"/>
-    </row>
-    <row r="205" spans="1:13">
+      <c r="N204" s="17"/>
+    </row>
+    <row r="205" spans="1:14">
       <c r="A205" s="17"/>
       <c r="B205" s="17"/>
       <c r="C205" s="17"/>
@@ -7769,8 +7818,9 @@
       <c r="K205" s="17"/>
       <c r="L205" s="17"/>
       <c r="M205" s="17"/>
-    </row>
-    <row r="206" spans="1:13">
+      <c r="N205" s="17"/>
+    </row>
+    <row r="206" spans="1:14">
       <c r="A206" s="17"/>
       <c r="B206" s="17"/>
       <c r="C206" s="17"/>
@@ -7784,8 +7834,9 @@
       <c r="K206" s="17"/>
       <c r="L206" s="17"/>
       <c r="M206" s="17"/>
-    </row>
-    <row r="207" spans="1:13">
+      <c r="N206" s="17"/>
+    </row>
+    <row r="207" spans="1:14">
       <c r="A207" s="17"/>
       <c r="B207" s="17"/>
       <c r="C207" s="17"/>
@@ -7799,8 +7850,9 @@
       <c r="K207" s="17"/>
       <c r="L207" s="17"/>
       <c r="M207" s="17"/>
-    </row>
-    <row r="208" spans="1:13">
+      <c r="N207" s="17"/>
+    </row>
+    <row r="208" spans="1:14">
       <c r="A208" s="17"/>
       <c r="B208" s="17"/>
       <c r="C208" s="17"/>
@@ -7814,6 +7866,7 @@
       <c r="K208" s="17"/>
       <c r="L208" s="17"/>
       <c r="M208" s="17"/>
+      <c r="N208" s="17"/>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
@@ -7970,27 +8023,27 @@
         <v>273</v>
       </c>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:14">
       <c r="A241" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="242" spans="1:13">
+    <row r="242" spans="1:14">
       <c r="A242" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:14">
       <c r="A243" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:14">
       <c r="A244" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:14">
       <c r="A253" s="15" t="s">
         <v>283</v>
       </c>
@@ -8006,18 +8059,19 @@
       <c r="K253" s="15"/>
       <c r="L253" s="15"/>
       <c r="M253" s="15"/>
-    </row>
-    <row r="254" spans="1:13">
+      <c r="N253" s="15"/>
+    </row>
+    <row r="254" spans="1:14">
       <c r="A254" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:14">
       <c r="A255" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:14">
       <c r="A256" t="s">
         <v>59</v>
       </c>
@@ -11862,181 +11916,181 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1025" spans="1:20">
+    <row r="1025" spans="1:21">
       <c r="A1025" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="1026" spans="1:20">
+    <row r="1026" spans="1:21">
       <c r="A1026" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="1027" spans="1:20">
+    <row r="1027" spans="1:21">
       <c r="A1027" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="1028" spans="1:20">
+    <row r="1028" spans="1:21">
       <c r="A1028" t="s">
         <v>908</v>
       </c>
-      <c r="T1028" s="17"/>
-    </row>
-    <row r="1029" spans="1:20">
+      <c r="U1028" s="17"/>
+    </row>
+    <row r="1029" spans="1:21">
       <c r="A1029" t="s">
         <v>909</v>
       </c>
-      <c r="T1029" s="17"/>
-    </row>
-    <row r="1030" spans="1:20">
+      <c r="U1029" s="17"/>
+    </row>
+    <row r="1030" spans="1:21">
       <c r="A1030" t="s">
         <v>910</v>
       </c>
-      <c r="T1030" s="17"/>
-    </row>
-    <row r="1031" spans="1:20">
+      <c r="U1030" s="17"/>
+    </row>
+    <row r="1031" spans="1:21">
       <c r="A1031" t="s">
         <v>911</v>
       </c>
-      <c r="T1031" s="17"/>
-    </row>
-    <row r="1032" spans="1:20">
+      <c r="U1031" s="17"/>
+    </row>
+    <row r="1032" spans="1:21">
       <c r="A1032" t="s">
         <v>912</v>
       </c>
-      <c r="T1032" s="17"/>
-    </row>
-    <row r="1033" spans="1:20">
+      <c r="U1032" s="17"/>
+    </row>
+    <row r="1033" spans="1:21">
       <c r="A1033" t="s">
         <v>913</v>
       </c>
-      <c r="T1033" s="17"/>
-    </row>
-    <row r="1034" spans="1:20">
+      <c r="U1033" s="17"/>
+    </row>
+    <row r="1034" spans="1:21">
       <c r="A1034" t="s">
         <v>914</v>
       </c>
-      <c r="T1034" s="17"/>
-    </row>
-    <row r="1035" spans="1:20">
+      <c r="U1034" s="17"/>
+    </row>
+    <row r="1035" spans="1:21">
       <c r="A1035" t="s">
         <v>915</v>
       </c>
-      <c r="T1035" s="17"/>
-    </row>
-    <row r="1036" spans="1:20">
+      <c r="U1035" s="17"/>
+    </row>
+    <row r="1036" spans="1:21">
       <c r="A1036" t="s">
         <v>916</v>
       </c>
-      <c r="T1036" s="17"/>
-    </row>
-    <row r="1037" spans="1:20">
+      <c r="U1036" s="17"/>
+    </row>
+    <row r="1037" spans="1:21">
       <c r="A1037" t="s">
         <v>917</v>
       </c>
-      <c r="T1037" s="17"/>
-    </row>
-    <row r="1038" spans="1:20">
+      <c r="U1037" s="17"/>
+    </row>
+    <row r="1038" spans="1:21">
       <c r="A1038" t="s">
         <v>918</v>
       </c>
-      <c r="T1038" s="17"/>
-    </row>
-    <row r="1039" spans="1:20">
+      <c r="U1038" s="17"/>
+    </row>
+    <row r="1039" spans="1:21">
       <c r="A1039" t="s">
         <v>919</v>
       </c>
-      <c r="T1039" s="17"/>
-    </row>
-    <row r="1040" spans="1:20">
+      <c r="U1039" s="17"/>
+    </row>
+    <row r="1040" spans="1:21">
       <c r="A1040" t="s">
         <v>920</v>
       </c>
-      <c r="T1040" s="17"/>
-    </row>
-    <row r="1041" spans="1:20">
+      <c r="U1040" s="17"/>
+    </row>
+    <row r="1041" spans="1:21">
       <c r="A1041" t="s">
         <v>921</v>
       </c>
-      <c r="T1041" s="17"/>
-    </row>
-    <row r="1042" spans="1:20">
+      <c r="U1041" s="17"/>
+    </row>
+    <row r="1042" spans="1:21">
       <c r="A1042" t="s">
         <v>922</v>
       </c>
-      <c r="T1042" s="17"/>
-    </row>
-    <row r="1043" spans="1:20">
+      <c r="U1042" s="17"/>
+    </row>
+    <row r="1043" spans="1:21">
       <c r="A1043" t="s">
         <v>923</v>
       </c>
-      <c r="T1043" s="17"/>
-    </row>
-    <row r="1044" spans="1:20">
+      <c r="U1043" s="17"/>
+    </row>
+    <row r="1044" spans="1:21">
       <c r="A1044" t="s">
         <v>924</v>
       </c>
-      <c r="T1044" s="17"/>
-    </row>
-    <row r="1045" spans="1:20">
+      <c r="U1044" s="17"/>
+    </row>
+    <row r="1045" spans="1:21">
       <c r="A1045" t="s">
         <v>925</v>
       </c>
-      <c r="T1045" s="17"/>
-    </row>
-    <row r="1046" spans="1:20">
+      <c r="U1045" s="17"/>
+    </row>
+    <row r="1046" spans="1:21">
       <c r="A1046" t="s">
         <v>926</v>
       </c>
-      <c r="T1046" s="17"/>
-    </row>
-    <row r="1047" spans="1:20">
+      <c r="U1046" s="17"/>
+    </row>
+    <row r="1047" spans="1:21">
       <c r="A1047" t="s">
         <v>927</v>
       </c>
-      <c r="T1047" s="17"/>
-    </row>
-    <row r="1048" spans="1:20">
+      <c r="U1047" s="17"/>
+    </row>
+    <row r="1048" spans="1:21">
       <c r="A1048" t="s">
         <v>928</v>
       </c>
-      <c r="T1048" s="17"/>
-    </row>
-    <row r="1049" spans="1:20">
+      <c r="U1048" s="17"/>
+    </row>
+    <row r="1049" spans="1:21">
       <c r="A1049" t="s">
         <v>929</v>
       </c>
-      <c r="T1049" s="17"/>
-    </row>
-    <row r="1050" spans="1:20">
+      <c r="U1049" s="17"/>
+    </row>
+    <row r="1050" spans="1:21">
       <c r="A1050" t="s">
         <v>930</v>
       </c>
-      <c r="T1050" s="17"/>
-    </row>
-    <row r="1051" spans="1:20">
+      <c r="U1050" s="17"/>
+    </row>
+    <row r="1051" spans="1:21">
       <c r="A1051" t="s">
         <v>931</v>
       </c>
-      <c r="T1051" s="17"/>
-    </row>
-    <row r="1052" spans="1:20">
+      <c r="U1051" s="17"/>
+    </row>
+    <row r="1052" spans="1:21">
       <c r="A1052" t="s">
         <v>932</v>
       </c>
-      <c r="T1052" s="17"/>
-    </row>
-    <row r="1053" spans="1:20">
+      <c r="U1052" s="17"/>
+    </row>
+    <row r="1053" spans="1:21">
       <c r="A1053" t="s">
         <v>933</v>
       </c>
-      <c r="T1053" s="17"/>
-    </row>
-    <row r="1054" spans="1:20">
-      <c r="T1054" s="17"/>
-    </row>
-    <row r="1055" spans="1:20">
+      <c r="U1053" s="17"/>
+    </row>
+    <row r="1054" spans="1:21">
+      <c r="U1054" s="17"/>
+    </row>
+    <row r="1055" spans="1:21">
       <c r="A1055" s="17" t="s">
         <v>243</v>
       </c>
@@ -12052,9 +12106,10 @@
       <c r="K1055" s="17"/>
       <c r="L1055" s="17"/>
       <c r="M1055" s="17"/>
-      <c r="T1055" s="17"/>
-    </row>
-    <row r="1056" spans="1:20">
+      <c r="N1055" s="17"/>
+      <c r="U1055" s="17"/>
+    </row>
+    <row r="1056" spans="1:21">
       <c r="A1056" s="17" t="s">
         <v>244</v>
       </c>
@@ -12070,9 +12125,10 @@
       <c r="K1056" s="17"/>
       <c r="L1056" s="17"/>
       <c r="M1056" s="17"/>
-      <c r="T1056" s="17"/>
-    </row>
-    <row r="1057" spans="1:20">
+      <c r="N1056" s="17"/>
+      <c r="U1056" s="17"/>
+    </row>
+    <row r="1057" spans="1:21">
       <c r="A1057" s="17" t="s">
         <v>245</v>
       </c>
@@ -12088,9 +12144,10 @@
       <c r="K1057" s="17"/>
       <c r="L1057" s="17"/>
       <c r="M1057" s="17"/>
-      <c r="T1057" s="17"/>
-    </row>
-    <row r="1058" spans="1:20">
+      <c r="N1057" s="17"/>
+      <c r="U1057" s="17"/>
+    </row>
+    <row r="1058" spans="1:21">
       <c r="A1058" s="17" t="s">
         <v>246</v>
       </c>
@@ -12106,9 +12163,10 @@
       <c r="K1058" s="17"/>
       <c r="L1058" s="17"/>
       <c r="M1058" s="17"/>
-      <c r="T1058" s="17"/>
-    </row>
-    <row r="1059" spans="1:20">
+      <c r="N1058" s="17"/>
+      <c r="U1058" s="17"/>
+    </row>
+    <row r="1059" spans="1:21">
       <c r="A1059" s="17" t="s">
         <v>247</v>
       </c>
@@ -12124,9 +12182,10 @@
       <c r="K1059" s="17"/>
       <c r="L1059" s="17"/>
       <c r="M1059" s="17"/>
-      <c r="T1059" s="17"/>
-    </row>
-    <row r="1060" spans="1:20">
+      <c r="N1059" s="17"/>
+      <c r="U1059" s="17"/>
+    </row>
+    <row r="1060" spans="1:21">
       <c r="A1060" s="17" t="s">
         <v>248</v>
       </c>
@@ -12142,9 +12201,10 @@
       <c r="K1060" s="17"/>
       <c r="L1060" s="17"/>
       <c r="M1060" s="17"/>
-      <c r="T1060" s="17"/>
-    </row>
-    <row r="1061" spans="1:20">
+      <c r="N1060" s="17"/>
+      <c r="U1060" s="17"/>
+    </row>
+    <row r="1061" spans="1:21">
       <c r="A1061" s="17" t="s">
         <v>249</v>
       </c>
@@ -12160,9 +12220,10 @@
       <c r="K1061" s="17"/>
       <c r="L1061" s="17"/>
       <c r="M1061" s="17"/>
-      <c r="T1061" s="17"/>
-    </row>
-    <row r="1062" spans="1:20">
+      <c r="N1061" s="17"/>
+      <c r="U1061" s="17"/>
+    </row>
+    <row r="1062" spans="1:21">
       <c r="A1062" s="17" t="s">
         <v>250</v>
       </c>
@@ -12178,9 +12239,10 @@
       <c r="K1062" s="17"/>
       <c r="L1062" s="17"/>
       <c r="M1062" s="17"/>
-      <c r="T1062" s="17"/>
-    </row>
-    <row r="1063" spans="1:20">
+      <c r="N1062" s="17"/>
+      <c r="U1062" s="17"/>
+    </row>
+    <row r="1063" spans="1:21">
       <c r="A1063" s="17" t="s">
         <v>251</v>
       </c>
@@ -12196,9 +12258,10 @@
       <c r="K1063" s="17"/>
       <c r="L1063" s="17"/>
       <c r="M1063" s="17"/>
-      <c r="T1063" s="17"/>
-    </row>
-    <row r="1064" spans="1:20">
+      <c r="N1063" s="17"/>
+      <c r="U1063" s="17"/>
+    </row>
+    <row r="1064" spans="1:21">
       <c r="A1064" s="17" t="s">
         <v>252</v>
       </c>
@@ -12214,9 +12277,10 @@
       <c r="K1064" s="17"/>
       <c r="L1064" s="17"/>
       <c r="M1064" s="17"/>
-      <c r="T1064" s="17"/>
-    </row>
-    <row r="1065" spans="1:20">
+      <c r="N1064" s="17"/>
+      <c r="U1064" s="17"/>
+    </row>
+    <row r="1065" spans="1:21">
       <c r="A1065" s="17" t="s">
         <v>253</v>
       </c>
@@ -12232,9 +12296,10 @@
       <c r="K1065" s="17"/>
       <c r="L1065" s="17"/>
       <c r="M1065" s="17"/>
-      <c r="T1065" s="17"/>
-    </row>
-    <row r="1066" spans="1:20">
+      <c r="N1065" s="17"/>
+      <c r="U1065" s="17"/>
+    </row>
+    <row r="1066" spans="1:21">
       <c r="A1066" s="17" t="s">
         <v>254</v>
       </c>
@@ -12250,9 +12315,10 @@
       <c r="K1066" s="17"/>
       <c r="L1066" s="17"/>
       <c r="M1066" s="17"/>
-      <c r="T1066" s="17"/>
-    </row>
-    <row r="1067" spans="1:20">
+      <c r="N1066" s="17"/>
+      <c r="U1066" s="17"/>
+    </row>
+    <row r="1067" spans="1:21">
       <c r="A1067" s="17" t="s">
         <v>255</v>
       </c>
@@ -12268,9 +12334,10 @@
       <c r="K1067" s="17"/>
       <c r="L1067" s="17"/>
       <c r="M1067" s="17"/>
-      <c r="T1067" s="17"/>
-    </row>
-    <row r="1068" spans="1:20">
+      <c r="N1067" s="17"/>
+      <c r="U1067" s="17"/>
+    </row>
+    <row r="1068" spans="1:21">
       <c r="A1068" s="17" t="s">
         <v>256</v>
       </c>
@@ -12286,14 +12353,15 @@
       <c r="K1068" s="17"/>
       <c r="L1068" s="17"/>
       <c r="M1068" s="17"/>
-      <c r="N1068"/>
+      <c r="N1068" s="17"/>
       <c r="O1068"/>
       <c r="P1068"/>
       <c r="Q1068"/>
       <c r="R1068"/>
       <c r="S1068"/>
-    </row>
-    <row r="1069" spans="1:20">
+      <c r="T1068"/>
+    </row>
+    <row r="1069" spans="1:21">
       <c r="A1069" s="17" t="s">
         <v>257</v>
       </c>
@@ -12309,14 +12377,15 @@
       <c r="K1069" s="17"/>
       <c r="L1069" s="17"/>
       <c r="M1069" s="17"/>
-      <c r="N1069"/>
+      <c r="N1069" s="17"/>
       <c r="O1069"/>
       <c r="P1069"/>
       <c r="Q1069"/>
       <c r="R1069"/>
       <c r="S1069"/>
-    </row>
-    <row r="1070" spans="1:20">
+      <c r="T1069"/>
+    </row>
+    <row r="1070" spans="1:21">
       <c r="A1070" s="17" t="s">
         <v>258</v>
       </c>
@@ -12332,14 +12401,15 @@
       <c r="K1070" s="17"/>
       <c r="L1070" s="17"/>
       <c r="M1070" s="17"/>
-      <c r="N1070"/>
+      <c r="N1070" s="17"/>
       <c r="O1070"/>
       <c r="P1070"/>
       <c r="Q1070"/>
       <c r="R1070"/>
       <c r="S1070"/>
-    </row>
-    <row r="1071" spans="1:20">
+      <c r="T1070"/>
+    </row>
+    <row r="1071" spans="1:21">
       <c r="A1071" s="17" t="s">
         <v>259</v>
       </c>
@@ -12355,14 +12425,15 @@
       <c r="K1071" s="17"/>
       <c r="L1071" s="17"/>
       <c r="M1071" s="17"/>
-      <c r="N1071"/>
+      <c r="N1071" s="17"/>
       <c r="O1071"/>
       <c r="P1071"/>
       <c r="Q1071"/>
       <c r="R1071"/>
       <c r="S1071"/>
-    </row>
-    <row r="1072" spans="1:20">
+      <c r="T1071"/>
+    </row>
+    <row r="1072" spans="1:21">
       <c r="A1072" s="17" t="s">
         <v>260</v>
       </c>
@@ -12378,14 +12449,15 @@
       <c r="K1072" s="17"/>
       <c r="L1072" s="17"/>
       <c r="M1072" s="17"/>
-      <c r="N1072"/>
+      <c r="N1072" s="17"/>
       <c r="O1072"/>
       <c r="P1072"/>
       <c r="Q1072"/>
       <c r="R1072"/>
       <c r="S1072"/>
-    </row>
-    <row r="1073" spans="1:19">
+      <c r="T1072"/>
+    </row>
+    <row r="1073" spans="1:20">
       <c r="A1073" s="17" t="s">
         <v>261</v>
       </c>
@@ -12401,14 +12473,15 @@
       <c r="K1073" s="17"/>
       <c r="L1073" s="17"/>
       <c r="M1073" s="17"/>
-      <c r="N1073"/>
+      <c r="N1073" s="17"/>
       <c r="O1073"/>
       <c r="P1073"/>
       <c r="Q1073"/>
       <c r="R1073"/>
       <c r="S1073"/>
-    </row>
-    <row r="1074" spans="1:19">
+      <c r="T1073"/>
+    </row>
+    <row r="1074" spans="1:20">
       <c r="A1074" s="17" t="s">
         <v>262</v>
       </c>
@@ -12424,14 +12497,15 @@
       <c r="K1074" s="17"/>
       <c r="L1074" s="17"/>
       <c r="M1074" s="17"/>
-      <c r="N1074"/>
+      <c r="N1074" s="17"/>
       <c r="O1074"/>
       <c r="P1074"/>
       <c r="Q1074"/>
       <c r="R1074"/>
       <c r="S1074"/>
-    </row>
-    <row r="1075" spans="1:19">
+      <c r="T1074"/>
+    </row>
+    <row r="1075" spans="1:20">
       <c r="A1075" s="17" t="s">
         <v>263</v>
       </c>
@@ -12447,14 +12521,15 @@
       <c r="K1075" s="17"/>
       <c r="L1075" s="17"/>
       <c r="M1075" s="17"/>
-      <c r="N1075"/>
+      <c r="N1075" s="17"/>
       <c r="O1075"/>
       <c r="P1075"/>
       <c r="Q1075"/>
       <c r="R1075"/>
       <c r="S1075"/>
-    </row>
-    <row r="1076" spans="1:19">
+      <c r="T1075"/>
+    </row>
+    <row r="1076" spans="1:20">
       <c r="A1076" s="17" t="s">
         <v>264</v>
       </c>
@@ -12470,14 +12545,15 @@
       <c r="K1076" s="17"/>
       <c r="L1076" s="17"/>
       <c r="M1076" s="17"/>
-      <c r="N1076"/>
+      <c r="N1076" s="17"/>
       <c r="O1076"/>
       <c r="P1076"/>
       <c r="Q1076"/>
       <c r="R1076"/>
       <c r="S1076"/>
-    </row>
-    <row r="1077" spans="1:19">
+      <c r="T1076"/>
+    </row>
+    <row r="1077" spans="1:20">
       <c r="A1077" s="17" t="s">
         <v>265</v>
       </c>
@@ -12493,14 +12569,15 @@
       <c r="K1077" s="17"/>
       <c r="L1077" s="17"/>
       <c r="M1077" s="17"/>
-      <c r="N1077"/>
+      <c r="N1077" s="17"/>
       <c r="O1077"/>
       <c r="P1077"/>
       <c r="Q1077"/>
       <c r="R1077"/>
       <c r="S1077"/>
-    </row>
-    <row r="1078" spans="1:19">
+      <c r="T1077"/>
+    </row>
+    <row r="1078" spans="1:20">
       <c r="A1078" s="17" t="s">
         <v>266</v>
       </c>
@@ -12516,14 +12593,15 @@
       <c r="K1078" s="17"/>
       <c r="L1078" s="17"/>
       <c r="M1078" s="17"/>
-      <c r="N1078"/>
+      <c r="N1078" s="17"/>
       <c r="O1078"/>
       <c r="P1078"/>
       <c r="Q1078"/>
       <c r="R1078"/>
       <c r="S1078"/>
-    </row>
-    <row r="1079" spans="1:19">
+      <c r="T1078"/>
+    </row>
+    <row r="1079" spans="1:20">
       <c r="A1079" s="17" t="s">
         <v>267</v>
       </c>
@@ -12539,14 +12617,15 @@
       <c r="K1079" s="17"/>
       <c r="L1079" s="17"/>
       <c r="M1079" s="17"/>
-      <c r="N1079"/>
+      <c r="N1079" s="17"/>
       <c r="O1079"/>
       <c r="P1079"/>
       <c r="Q1079"/>
       <c r="R1079"/>
       <c r="S1079"/>
-    </row>
-    <row r="1080" spans="1:19">
+      <c r="T1079"/>
+    </row>
+    <row r="1080" spans="1:20">
       <c r="A1080" s="17" t="s">
         <v>268</v>
       </c>
@@ -12562,14 +12641,15 @@
       <c r="K1080" s="17"/>
       <c r="L1080" s="17"/>
       <c r="M1080" s="17"/>
-      <c r="N1080"/>
+      <c r="N1080" s="17"/>
       <c r="O1080"/>
       <c r="P1080"/>
       <c r="Q1080"/>
       <c r="R1080"/>
       <c r="S1080"/>
-    </row>
-    <row r="1081" spans="1:19">
+      <c r="T1080"/>
+    </row>
+    <row r="1081" spans="1:20">
       <c r="A1081" s="17" t="s">
         <v>269</v>
       </c>
@@ -12585,14 +12665,15 @@
       <c r="K1081" s="17"/>
       <c r="L1081" s="17"/>
       <c r="M1081" s="17"/>
-      <c r="N1081"/>
+      <c r="N1081" s="17"/>
       <c r="O1081"/>
       <c r="P1081"/>
       <c r="Q1081"/>
       <c r="R1081"/>
       <c r="S1081"/>
-    </row>
-    <row r="1082" spans="1:19">
+      <c r="T1081"/>
+    </row>
+    <row r="1082" spans="1:20">
       <c r="A1082" s="17" t="s">
         <v>270</v>
       </c>
@@ -12608,14 +12689,15 @@
       <c r="K1082" s="17"/>
       <c r="L1082" s="17"/>
       <c r="M1082" s="17"/>
-      <c r="N1082"/>
+      <c r="N1082" s="17"/>
       <c r="O1082"/>
       <c r="P1082"/>
       <c r="Q1082"/>
       <c r="R1082"/>
       <c r="S1082"/>
-    </row>
-    <row r="1083" spans="1:19">
+      <c r="T1082"/>
+    </row>
+    <row r="1083" spans="1:20">
       <c r="A1083" s="17" t="s">
         <v>271</v>
       </c>
@@ -12631,14 +12713,15 @@
       <c r="K1083" s="17"/>
       <c r="L1083" s="17"/>
       <c r="M1083" s="17"/>
-      <c r="N1083"/>
+      <c r="N1083" s="17"/>
       <c r="O1083"/>
       <c r="P1083"/>
       <c r="Q1083"/>
       <c r="R1083"/>
       <c r="S1083"/>
-    </row>
-    <row r="1084" spans="1:19">
+      <c r="T1083"/>
+    </row>
+    <row r="1084" spans="1:20">
       <c r="A1084" s="17" t="s">
         <v>272</v>
       </c>
@@ -12654,14 +12737,15 @@
       <c r="K1084" s="17"/>
       <c r="L1084" s="17"/>
       <c r="M1084" s="17"/>
-      <c r="N1084"/>
+      <c r="N1084" s="17"/>
       <c r="O1084"/>
       <c r="P1084"/>
       <c r="Q1084"/>
       <c r="R1084"/>
       <c r="S1084"/>
-    </row>
-    <row r="1085" spans="1:19">
+      <c r="T1084"/>
+    </row>
+    <row r="1085" spans="1:20">
       <c r="A1085" s="17" t="s">
         <v>273</v>
       </c>
@@ -12677,14 +12761,15 @@
       <c r="K1085" s="17"/>
       <c r="L1085" s="17"/>
       <c r="M1085" s="17"/>
-      <c r="N1085"/>
+      <c r="N1085" s="17"/>
       <c r="O1085"/>
       <c r="P1085"/>
       <c r="Q1085"/>
       <c r="R1085"/>
       <c r="S1085"/>
-    </row>
-    <row r="1086" spans="1:19">
+      <c r="T1085"/>
+    </row>
+    <row r="1086" spans="1:20">
       <c r="A1086" s="17" t="s">
         <v>274</v>
       </c>
@@ -12700,14 +12785,15 @@
       <c r="K1086" s="17"/>
       <c r="L1086" s="17"/>
       <c r="M1086" s="17"/>
-      <c r="N1086"/>
+      <c r="N1086" s="17"/>
       <c r="O1086"/>
       <c r="P1086"/>
       <c r="Q1086"/>
       <c r="R1086"/>
       <c r="S1086"/>
-    </row>
-    <row r="1087" spans="1:19">
+      <c r="T1086"/>
+    </row>
+    <row r="1087" spans="1:20">
       <c r="A1087" s="17" t="s">
         <v>275</v>
       </c>
@@ -12723,14 +12809,15 @@
       <c r="K1087" s="17"/>
       <c r="L1087" s="17"/>
       <c r="M1087" s="17"/>
-      <c r="N1087"/>
+      <c r="N1087" s="17"/>
       <c r="O1087"/>
       <c r="P1087"/>
       <c r="Q1087"/>
       <c r="R1087"/>
       <c r="S1087"/>
-    </row>
-    <row r="1088" spans="1:19">
+      <c r="T1087"/>
+    </row>
+    <row r="1088" spans="1:20">
       <c r="A1088" s="17" t="s">
         <v>276</v>
       </c>
@@ -12746,14 +12833,15 @@
       <c r="K1088" s="17"/>
       <c r="L1088" s="17"/>
       <c r="M1088" s="17"/>
-      <c r="N1088"/>
+      <c r="N1088" s="17"/>
       <c r="O1088"/>
       <c r="P1088"/>
       <c r="Q1088"/>
       <c r="R1088"/>
       <c r="S1088"/>
-    </row>
-    <row r="1089" spans="1:19">
+      <c r="T1088"/>
+    </row>
+    <row r="1089" spans="1:20">
       <c r="A1089" s="17" t="s">
         <v>277</v>
       </c>
@@ -12769,14 +12857,15 @@
       <c r="K1089" s="17"/>
       <c r="L1089" s="17"/>
       <c r="M1089" s="17"/>
-      <c r="N1089"/>
+      <c r="N1089" s="17"/>
       <c r="O1089"/>
       <c r="P1089"/>
       <c r="Q1089"/>
       <c r="R1089"/>
       <c r="S1089"/>
-    </row>
-    <row r="1090" spans="1:19">
+      <c r="T1089"/>
+    </row>
+    <row r="1090" spans="1:20">
       <c r="A1090" s="17" t="s">
         <v>934</v>
       </c>
@@ -12792,14 +12881,15 @@
       <c r="K1090" s="17"/>
       <c r="L1090" s="17"/>
       <c r="M1090" s="17"/>
-      <c r="N1090"/>
+      <c r="N1090" s="17"/>
       <c r="O1090"/>
       <c r="P1090"/>
       <c r="Q1090"/>
       <c r="R1090"/>
       <c r="S1090"/>
-    </row>
-    <row r="1091" spans="1:19">
+      <c r="T1090"/>
+    </row>
+    <row r="1091" spans="1:20">
       <c r="A1091" s="17" t="s">
         <v>935</v>
       </c>
@@ -12815,14 +12905,15 @@
       <c r="K1091" s="17"/>
       <c r="L1091" s="17"/>
       <c r="M1091" s="17"/>
-      <c r="N1091"/>
+      <c r="N1091" s="17"/>
       <c r="O1091"/>
       <c r="P1091"/>
       <c r="Q1091"/>
       <c r="R1091"/>
       <c r="S1091"/>
-    </row>
-    <row r="1092" spans="1:19">
+      <c r="T1091"/>
+    </row>
+    <row r="1092" spans="1:20">
       <c r="A1092" s="17" t="s">
         <v>936</v>
       </c>
@@ -12838,14 +12929,15 @@
       <c r="K1092" s="17"/>
       <c r="L1092" s="17"/>
       <c r="M1092" s="17"/>
-      <c r="N1092"/>
+      <c r="N1092" s="17"/>
       <c r="O1092"/>
       <c r="P1092"/>
       <c r="Q1092"/>
       <c r="R1092"/>
       <c r="S1092"/>
-    </row>
-    <row r="1093" spans="1:19">
+      <c r="T1092"/>
+    </row>
+    <row r="1093" spans="1:20">
       <c r="A1093" s="17" t="s">
         <v>937</v>
       </c>
@@ -12861,14 +12953,15 @@
       <c r="K1093" s="17"/>
       <c r="L1093" s="17"/>
       <c r="M1093" s="17"/>
-      <c r="N1093"/>
+      <c r="N1093" s="17"/>
       <c r="O1093"/>
       <c r="P1093"/>
       <c r="Q1093"/>
       <c r="R1093"/>
       <c r="S1093"/>
-    </row>
-    <row r="1094" spans="1:19">
+      <c r="T1093"/>
+    </row>
+    <row r="1094" spans="1:20">
       <c r="A1094" s="17" t="s">
         <v>938</v>
       </c>
@@ -12884,572 +12977,573 @@
       <c r="K1094" s="17"/>
       <c r="L1094" s="17"/>
       <c r="M1094" s="17"/>
-      <c r="N1094"/>
+      <c r="N1094" s="17"/>
       <c r="O1094"/>
       <c r="P1094"/>
       <c r="Q1094"/>
       <c r="R1094"/>
       <c r="S1094"/>
-    </row>
-    <row r="1095" spans="1:19">
-      <c r="N1095"/>
+      <c r="T1094"/>
+    </row>
+    <row r="1095" spans="1:20">
       <c r="O1095"/>
       <c r="P1095"/>
       <c r="Q1095"/>
       <c r="R1095"/>
       <c r="S1095"/>
-    </row>
-    <row r="1096" spans="1:19">
-      <c r="N1096"/>
+      <c r="T1095"/>
+    </row>
+    <row r="1096" spans="1:20">
       <c r="O1096"/>
       <c r="P1096"/>
       <c r="Q1096"/>
       <c r="R1096"/>
       <c r="S1096"/>
-    </row>
-    <row r="1097" spans="1:19">
-      <c r="N1097"/>
+      <c r="T1096"/>
+    </row>
+    <row r="1097" spans="1:20">
       <c r="O1097"/>
       <c r="P1097"/>
       <c r="Q1097"/>
       <c r="R1097"/>
       <c r="S1097"/>
-    </row>
-    <row r="1098" spans="1:19">
-      <c r="N1098"/>
+      <c r="T1097"/>
+    </row>
+    <row r="1098" spans="1:20">
       <c r="O1098"/>
       <c r="P1098"/>
       <c r="Q1098"/>
       <c r="R1098"/>
       <c r="S1098"/>
-    </row>
-    <row r="1099" spans="1:19">
-      <c r="N1099"/>
+      <c r="T1098"/>
+    </row>
+    <row r="1099" spans="1:20">
       <c r="O1099"/>
       <c r="P1099"/>
       <c r="Q1099"/>
       <c r="R1099"/>
       <c r="S1099"/>
-    </row>
-    <row r="1100" spans="1:19">
-      <c r="N1100"/>
+      <c r="T1099"/>
+    </row>
+    <row r="1100" spans="1:20">
       <c r="O1100"/>
       <c r="P1100"/>
       <c r="Q1100"/>
       <c r="R1100"/>
       <c r="S1100"/>
-    </row>
-    <row r="1101" spans="1:19">
-      <c r="N1101"/>
+      <c r="T1100"/>
+    </row>
+    <row r="1101" spans="1:20">
       <c r="O1101"/>
       <c r="P1101"/>
       <c r="Q1101"/>
       <c r="R1101"/>
       <c r="S1101"/>
-    </row>
-    <row r="1102" spans="1:19">
-      <c r="N1102"/>
+      <c r="T1101"/>
+    </row>
+    <row r="1102" spans="1:20">
       <c r="O1102"/>
       <c r="P1102"/>
       <c r="Q1102"/>
       <c r="R1102"/>
       <c r="S1102"/>
-    </row>
-    <row r="1103" spans="1:19">
-      <c r="N1103"/>
+      <c r="T1102"/>
+    </row>
+    <row r="1103" spans="1:20">
       <c r="O1103"/>
       <c r="P1103"/>
       <c r="Q1103"/>
       <c r="R1103"/>
       <c r="S1103"/>
-    </row>
-    <row r="1104" spans="1:19">
-      <c r="N1104"/>
+      <c r="T1103"/>
+    </row>
+    <row r="1104" spans="1:20">
       <c r="O1104"/>
       <c r="P1104"/>
       <c r="Q1104"/>
       <c r="R1104"/>
       <c r="S1104"/>
-    </row>
-    <row r="1105" spans="14:19">
-      <c r="N1105"/>
+      <c r="T1104"/>
+    </row>
+    <row r="1105" spans="15:20">
       <c r="O1105"/>
       <c r="P1105"/>
       <c r="Q1105"/>
       <c r="R1105"/>
       <c r="S1105"/>
-    </row>
-    <row r="1106" spans="14:19">
-      <c r="N1106"/>
+      <c r="T1105"/>
+    </row>
+    <row r="1106" spans="15:20">
       <c r="O1106"/>
       <c r="P1106"/>
       <c r="Q1106"/>
       <c r="R1106"/>
       <c r="S1106"/>
-    </row>
-    <row r="1107" spans="14:19">
-      <c r="N1107"/>
+      <c r="T1106"/>
+    </row>
+    <row r="1107" spans="15:20">
       <c r="O1107"/>
       <c r="P1107"/>
       <c r="Q1107"/>
       <c r="R1107"/>
       <c r="S1107"/>
-    </row>
-    <row r="1108" spans="14:19">
-      <c r="N1108"/>
+      <c r="T1107"/>
+    </row>
+    <row r="1108" spans="15:20">
       <c r="O1108"/>
       <c r="P1108"/>
       <c r="Q1108"/>
       <c r="R1108"/>
       <c r="S1108"/>
-    </row>
-    <row r="1109" spans="14:19">
-      <c r="N1109"/>
+      <c r="T1108"/>
+    </row>
+    <row r="1109" spans="15:20">
       <c r="O1109"/>
       <c r="P1109"/>
       <c r="Q1109"/>
       <c r="R1109"/>
       <c r="S1109"/>
-    </row>
-    <row r="1110" spans="14:19">
-      <c r="N1110"/>
+      <c r="T1109"/>
+    </row>
+    <row r="1110" spans="15:20">
       <c r="O1110"/>
       <c r="P1110"/>
       <c r="Q1110"/>
       <c r="R1110"/>
       <c r="S1110"/>
-    </row>
-    <row r="1111" spans="14:19">
-      <c r="N1111"/>
+      <c r="T1110"/>
+    </row>
+    <row r="1111" spans="15:20">
       <c r="O1111"/>
       <c r="P1111"/>
       <c r="Q1111"/>
       <c r="R1111"/>
       <c r="S1111"/>
-    </row>
-    <row r="1112" spans="14:19">
-      <c r="N1112"/>
+      <c r="T1111"/>
+    </row>
+    <row r="1112" spans="15:20">
       <c r="O1112"/>
       <c r="P1112"/>
       <c r="Q1112"/>
       <c r="R1112"/>
       <c r="S1112"/>
-    </row>
-    <row r="1113" spans="14:19">
-      <c r="N1113"/>
+      <c r="T1112"/>
+    </row>
+    <row r="1113" spans="15:20">
       <c r="O1113"/>
       <c r="P1113"/>
       <c r="Q1113"/>
       <c r="R1113"/>
       <c r="S1113"/>
-    </row>
-    <row r="1114" spans="14:19">
-      <c r="N1114"/>
+      <c r="T1113"/>
+    </row>
+    <row r="1114" spans="15:20">
       <c r="O1114"/>
       <c r="P1114"/>
       <c r="Q1114"/>
       <c r="R1114"/>
       <c r="S1114"/>
-    </row>
-    <row r="1115" spans="14:19">
-      <c r="N1115"/>
+      <c r="T1114"/>
+    </row>
+    <row r="1115" spans="15:20">
       <c r="O1115"/>
       <c r="P1115"/>
       <c r="Q1115"/>
       <c r="R1115"/>
       <c r="S1115"/>
-    </row>
-    <row r="1116" spans="14:19">
-      <c r="N1116"/>
+      <c r="T1115"/>
+    </row>
+    <row r="1116" spans="15:20">
       <c r="O1116"/>
       <c r="P1116"/>
       <c r="Q1116"/>
       <c r="R1116"/>
       <c r="S1116"/>
-    </row>
-    <row r="1117" spans="14:19">
-      <c r="N1117"/>
+      <c r="T1116"/>
+    </row>
+    <row r="1117" spans="15:20">
       <c r="O1117"/>
       <c r="P1117"/>
       <c r="Q1117"/>
       <c r="R1117"/>
       <c r="S1117"/>
-    </row>
-    <row r="1118" spans="14:19">
-      <c r="N1118"/>
+      <c r="T1117"/>
+    </row>
+    <row r="1118" spans="15:20">
       <c r="O1118"/>
       <c r="P1118"/>
       <c r="Q1118"/>
       <c r="R1118"/>
       <c r="S1118"/>
-    </row>
-    <row r="1119" spans="14:19">
-      <c r="N1119"/>
+      <c r="T1118"/>
+    </row>
+    <row r="1119" spans="15:20">
       <c r="O1119"/>
       <c r="P1119"/>
       <c r="Q1119"/>
       <c r="R1119"/>
       <c r="S1119"/>
-    </row>
-    <row r="1120" spans="14:19">
-      <c r="N1120"/>
+      <c r="T1119"/>
+    </row>
+    <row r="1120" spans="15:20">
       <c r="O1120"/>
       <c r="P1120"/>
       <c r="Q1120"/>
       <c r="R1120"/>
       <c r="S1120"/>
-    </row>
-    <row r="1121" spans="14:19">
-      <c r="N1121"/>
+      <c r="T1120"/>
+    </row>
+    <row r="1121" spans="15:20">
       <c r="O1121"/>
       <c r="P1121"/>
       <c r="Q1121"/>
       <c r="R1121"/>
       <c r="S1121"/>
-    </row>
-    <row r="1122" spans="14:19">
-      <c r="N1122"/>
+      <c r="T1121"/>
+    </row>
+    <row r="1122" spans="15:20">
       <c r="O1122"/>
       <c r="P1122"/>
       <c r="Q1122"/>
       <c r="R1122"/>
       <c r="S1122"/>
-    </row>
-    <row r="1123" spans="14:19">
-      <c r="N1123"/>
+      <c r="T1122"/>
+    </row>
+    <row r="1123" spans="15:20">
       <c r="O1123"/>
       <c r="P1123"/>
       <c r="Q1123"/>
       <c r="R1123"/>
       <c r="S1123"/>
-    </row>
-    <row r="1124" spans="14:19">
-      <c r="N1124"/>
+      <c r="T1123"/>
+    </row>
+    <row r="1124" spans="15:20">
       <c r="O1124"/>
       <c r="P1124"/>
       <c r="Q1124"/>
       <c r="R1124"/>
       <c r="S1124"/>
-    </row>
-    <row r="1125" spans="14:19">
-      <c r="N1125"/>
+      <c r="T1124"/>
+    </row>
+    <row r="1125" spans="15:20">
       <c r="O1125"/>
       <c r="P1125"/>
       <c r="Q1125"/>
       <c r="R1125"/>
       <c r="S1125"/>
-    </row>
-    <row r="1126" spans="14:19">
-      <c r="N1126"/>
+      <c r="T1125"/>
+    </row>
+    <row r="1126" spans="15:20">
       <c r="O1126"/>
       <c r="P1126"/>
       <c r="Q1126"/>
       <c r="R1126"/>
       <c r="S1126"/>
-    </row>
-    <row r="1127" spans="14:19">
-      <c r="N1127"/>
+      <c r="T1126"/>
+    </row>
+    <row r="1127" spans="15:20">
       <c r="O1127"/>
       <c r="P1127"/>
       <c r="Q1127"/>
       <c r="R1127"/>
       <c r="S1127"/>
-    </row>
-    <row r="1128" spans="14:19">
-      <c r="N1128"/>
+      <c r="T1127"/>
+    </row>
+    <row r="1128" spans="15:20">
       <c r="O1128"/>
       <c r="P1128"/>
       <c r="Q1128"/>
       <c r="R1128"/>
       <c r="S1128"/>
-    </row>
-    <row r="1129" spans="14:19">
-      <c r="N1129"/>
+      <c r="T1128"/>
+    </row>
+    <row r="1129" spans="15:20">
       <c r="O1129"/>
       <c r="P1129"/>
       <c r="Q1129"/>
       <c r="R1129"/>
       <c r="S1129"/>
-    </row>
-    <row r="1130" spans="14:19">
-      <c r="N1130"/>
+      <c r="T1129"/>
+    </row>
+    <row r="1130" spans="15:20">
       <c r="O1130"/>
       <c r="P1130"/>
       <c r="Q1130"/>
       <c r="R1130"/>
       <c r="S1130"/>
-    </row>
-    <row r="1131" spans="14:19">
-      <c r="N1131"/>
+      <c r="T1130"/>
+    </row>
+    <row r="1131" spans="15:20">
       <c r="O1131"/>
       <c r="P1131"/>
       <c r="Q1131"/>
       <c r="R1131"/>
       <c r="S1131"/>
-    </row>
-    <row r="1132" spans="14:19">
-      <c r="N1132"/>
+      <c r="T1131"/>
+    </row>
+    <row r="1132" spans="15:20">
       <c r="O1132"/>
       <c r="P1132"/>
       <c r="Q1132"/>
       <c r="R1132"/>
       <c r="S1132"/>
-    </row>
-    <row r="1133" spans="14:19">
-      <c r="N1133"/>
+      <c r="T1132"/>
+    </row>
+    <row r="1133" spans="15:20">
       <c r="O1133"/>
       <c r="P1133"/>
       <c r="Q1133"/>
       <c r="R1133"/>
       <c r="S1133"/>
-    </row>
-    <row r="1134" spans="14:19">
-      <c r="N1134"/>
+      <c r="T1133"/>
+    </row>
+    <row r="1134" spans="15:20">
       <c r="O1134"/>
       <c r="P1134"/>
       <c r="Q1134"/>
       <c r="R1134"/>
       <c r="S1134"/>
-    </row>
-    <row r="1135" spans="14:19">
-      <c r="N1135"/>
+      <c r="T1134"/>
+    </row>
+    <row r="1135" spans="15:20">
       <c r="O1135"/>
       <c r="P1135"/>
       <c r="Q1135"/>
       <c r="R1135"/>
       <c r="S1135"/>
-    </row>
-    <row r="1136" spans="14:19">
-      <c r="N1136"/>
+      <c r="T1135"/>
+    </row>
+    <row r="1136" spans="15:20">
       <c r="O1136"/>
       <c r="P1136"/>
       <c r="Q1136"/>
       <c r="R1136"/>
       <c r="S1136"/>
-    </row>
-    <row r="1137" spans="14:19">
-      <c r="N1137"/>
+      <c r="T1136"/>
+    </row>
+    <row r="1137" spans="15:20">
       <c r="O1137"/>
       <c r="P1137"/>
       <c r="Q1137"/>
       <c r="R1137"/>
       <c r="S1137"/>
-    </row>
-    <row r="1138" spans="14:19">
-      <c r="N1138"/>
+      <c r="T1137"/>
+    </row>
+    <row r="1138" spans="15:20">
       <c r="O1138"/>
       <c r="P1138"/>
       <c r="Q1138"/>
       <c r="R1138"/>
       <c r="S1138"/>
-    </row>
-    <row r="1139" spans="14:19">
-      <c r="N1139"/>
+      <c r="T1138"/>
+    </row>
+    <row r="1139" spans="15:20">
       <c r="O1139"/>
       <c r="P1139"/>
       <c r="Q1139"/>
       <c r="R1139"/>
       <c r="S1139"/>
-    </row>
-    <row r="1140" spans="14:19">
-      <c r="N1140"/>
+      <c r="T1139"/>
+    </row>
+    <row r="1140" spans="15:20">
       <c r="O1140"/>
       <c r="P1140"/>
       <c r="Q1140"/>
       <c r="R1140"/>
       <c r="S1140"/>
-    </row>
-    <row r="1141" spans="14:19">
-      <c r="N1141"/>
+      <c r="T1140"/>
+    </row>
+    <row r="1141" spans="15:20">
       <c r="O1141"/>
       <c r="P1141"/>
       <c r="Q1141"/>
       <c r="R1141"/>
       <c r="S1141"/>
-    </row>
-    <row r="1142" spans="14:19">
-      <c r="N1142"/>
+      <c r="T1141"/>
+    </row>
+    <row r="1142" spans="15:20">
       <c r="O1142"/>
       <c r="P1142"/>
       <c r="Q1142"/>
       <c r="R1142"/>
       <c r="S1142"/>
-    </row>
-    <row r="1143" spans="14:19">
-      <c r="N1143"/>
+      <c r="T1142"/>
+    </row>
+    <row r="1143" spans="15:20">
       <c r="O1143"/>
       <c r="P1143"/>
       <c r="Q1143"/>
       <c r="R1143"/>
       <c r="S1143"/>
-    </row>
-    <row r="1144" spans="14:19">
-      <c r="N1144"/>
+      <c r="T1143"/>
+    </row>
+    <row r="1144" spans="15:20">
       <c r="O1144"/>
       <c r="P1144"/>
       <c r="Q1144"/>
       <c r="R1144"/>
       <c r="S1144"/>
-    </row>
-    <row r="1145" spans="14:19">
-      <c r="N1145"/>
+      <c r="T1144"/>
+    </row>
+    <row r="1145" spans="15:20">
       <c r="O1145"/>
       <c r="P1145"/>
       <c r="Q1145"/>
       <c r="R1145"/>
       <c r="S1145"/>
-    </row>
-    <row r="1146" spans="14:19">
-      <c r="N1146"/>
+      <c r="T1145"/>
+    </row>
+    <row r="1146" spans="15:20">
       <c r="O1146"/>
       <c r="P1146"/>
       <c r="Q1146"/>
       <c r="R1146"/>
       <c r="S1146"/>
-    </row>
-    <row r="1147" spans="14:19">
-      <c r="N1147"/>
+      <c r="T1146"/>
+    </row>
+    <row r="1147" spans="15:20">
       <c r="O1147"/>
       <c r="P1147"/>
       <c r="Q1147"/>
       <c r="R1147"/>
       <c r="S1147"/>
-    </row>
-    <row r="1148" spans="14:19">
-      <c r="N1148"/>
+      <c r="T1147"/>
+    </row>
+    <row r="1148" spans="15:20">
       <c r="O1148"/>
       <c r="P1148"/>
       <c r="Q1148"/>
       <c r="R1148"/>
       <c r="S1148"/>
-    </row>
-    <row r="1149" spans="14:19">
-      <c r="N1149"/>
+      <c r="T1148"/>
+    </row>
+    <row r="1149" spans="15:20">
       <c r="O1149"/>
       <c r="P1149"/>
       <c r="Q1149"/>
       <c r="R1149"/>
       <c r="S1149"/>
-    </row>
-    <row r="1150" spans="14:19">
-      <c r="N1150"/>
+      <c r="T1149"/>
+    </row>
+    <row r="1150" spans="15:20">
       <c r="O1150"/>
       <c r="P1150"/>
       <c r="Q1150"/>
       <c r="R1150"/>
       <c r="S1150"/>
-    </row>
-    <row r="1151" spans="14:19">
-      <c r="N1151"/>
+      <c r="T1150"/>
+    </row>
+    <row r="1151" spans="15:20">
       <c r="O1151"/>
       <c r="P1151"/>
       <c r="Q1151"/>
       <c r="R1151"/>
       <c r="S1151"/>
-    </row>
-    <row r="1152" spans="14:19">
-      <c r="N1152"/>
+      <c r="T1151"/>
+    </row>
+    <row r="1152" spans="15:20">
       <c r="O1152"/>
       <c r="P1152"/>
       <c r="Q1152"/>
       <c r="R1152"/>
       <c r="S1152"/>
-    </row>
-    <row r="1153" spans="14:19">
-      <c r="N1153"/>
+      <c r="T1152"/>
+    </row>
+    <row r="1153" spans="15:20">
       <c r="O1153"/>
       <c r="P1153"/>
       <c r="Q1153"/>
       <c r="R1153"/>
       <c r="S1153"/>
-    </row>
-    <row r="1154" spans="14:19">
-      <c r="N1154"/>
+      <c r="T1153"/>
+    </row>
+    <row r="1154" spans="15:20">
       <c r="O1154"/>
       <c r="P1154"/>
       <c r="Q1154"/>
       <c r="R1154"/>
       <c r="S1154"/>
-    </row>
-    <row r="1155" spans="14:19">
-      <c r="N1155"/>
+      <c r="T1154"/>
+    </row>
+    <row r="1155" spans="15:20">
       <c r="O1155"/>
       <c r="P1155"/>
       <c r="Q1155"/>
       <c r="R1155"/>
       <c r="S1155"/>
-    </row>
-    <row r="1156" spans="14:19">
-      <c r="N1156"/>
+      <c r="T1155"/>
+    </row>
+    <row r="1156" spans="15:20">
       <c r="O1156"/>
       <c r="P1156"/>
       <c r="Q1156"/>
       <c r="R1156"/>
       <c r="S1156"/>
-    </row>
-    <row r="1157" spans="14:19">
-      <c r="N1157"/>
+      <c r="T1156"/>
+    </row>
+    <row r="1157" spans="15:20">
       <c r="O1157"/>
       <c r="P1157"/>
       <c r="Q1157"/>
       <c r="R1157"/>
       <c r="S1157"/>
-    </row>
-    <row r="1158" spans="14:19">
-      <c r="N1158"/>
+      <c r="T1157"/>
+    </row>
+    <row r="1158" spans="15:20">
       <c r="O1158"/>
       <c r="P1158"/>
       <c r="Q1158"/>
       <c r="R1158"/>
       <c r="S1158"/>
-    </row>
-    <row r="1159" spans="14:19">
-      <c r="N1159"/>
+      <c r="T1158"/>
+    </row>
+    <row r="1159" spans="15:20">
       <c r="O1159"/>
       <c r="P1159"/>
       <c r="Q1159"/>
       <c r="R1159"/>
       <c r="S1159"/>
-    </row>
-    <row r="1160" spans="14:19">
-      <c r="N1160"/>
+      <c r="T1159"/>
+    </row>
+    <row r="1160" spans="15:20">
       <c r="O1160"/>
       <c r="P1160"/>
       <c r="Q1160"/>
       <c r="R1160"/>
       <c r="S1160"/>
-    </row>
-    <row r="1161" spans="14:19">
-      <c r="N1161"/>
+      <c r="T1160"/>
+    </row>
+    <row r="1161" spans="15:20">
       <c r="O1161"/>
       <c r="P1161"/>
       <c r="Q1161"/>
       <c r="R1161"/>
       <c r="S1161"/>
-    </row>
-    <row r="1162" spans="14:19">
-      <c r="N1162"/>
+      <c r="T1161"/>
+    </row>
+    <row r="1162" spans="15:20">
       <c r="O1162"/>
       <c r="P1162"/>
       <c r="Q1162"/>
       <c r="R1162"/>
       <c r="S1162"/>
-    </row>
-    <row r="1163" spans="14:19">
-      <c r="N1163"/>
+      <c r="T1162"/>
+    </row>
+    <row r="1163" spans="15:20">
       <c r="O1163"/>
       <c r="P1163"/>
       <c r="Q1163"/>
       <c r="R1163"/>
       <c r="S1163"/>
-    </row>
-    <row r="1164" spans="14:19">
-      <c r="N1164"/>
+      <c r="T1163"/>
+    </row>
+    <row r="1164" spans="15:20">
       <c r="O1164"/>
       <c r="P1164"/>
       <c r="Q1164"/>
       <c r="R1164"/>
       <c r="S1164"/>
+      <c r="T1164"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Teeny tiny update to show which plots are done
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4107" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4108" uniqueCount="1070">
   <si>
     <t>param</t>
   </si>
@@ -5716,7 +5716,7 @@
   <dimension ref="A1:AE1164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5829,7 +5829,9 @@
       <c r="A3" s="40" t="s">
         <v>1066</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="41" t="s">
+        <v>216</v>
+      </c>
       <c r="C3" s="41" t="s">
         <v>216</v>
       </c>

</xml_diff>

<commit_message>
Updating the results with utah units
Chillports is still the better model
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4108" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4117" uniqueCount="1072">
   <si>
     <t>param</t>
   </si>
@@ -3313,6 +3313,12 @@
   </si>
   <si>
     <t>many (&gt;5K) divegernt transitions; intercept chains wandering</t>
+  </si>
+  <si>
+    <t>rsq is 0.56</t>
+  </si>
+  <si>
+    <t>rsq is 0.59</t>
   </si>
 </sst>
 </file>
@@ -3497,8 +3503,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="391">
+  <cellStyleXfs count="395">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3961,7 +3971,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="391">
+  <cellStyles count="395">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4157,6 +4167,8 @@
     <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4352,6 +4364,8 @@
     <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5713,29 +5727,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE1164"/>
+  <dimension ref="A1:AF1164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="14" width="17.1640625" customWidth="1"/>
-    <col min="15" max="20" width="18.5" style="21" customWidth="1"/>
-    <col min="21" max="21" width="17.1640625" customWidth="1"/>
-    <col min="22" max="22" width="15" customWidth="1"/>
-    <col min="23" max="23" width="13.5" customWidth="1"/>
-    <col min="24" max="24" width="13.6640625" customWidth="1"/>
-    <col min="25" max="25" width="13.1640625" customWidth="1"/>
-    <col min="26" max="26" width="11.83203125" customWidth="1"/>
-    <col min="27" max="27" width="15.5" customWidth="1"/>
-    <col min="28" max="28" width="12.6640625" customWidth="1"/>
-    <col min="29" max="29" width="14.33203125" customWidth="1"/>
-    <col min="30" max="31" width="10.83203125" style="19"/>
+    <col min="1" max="15" width="17.1640625" customWidth="1"/>
+    <col min="16" max="21" width="18.5" style="21" customWidth="1"/>
+    <col min="22" max="22" width="17.1640625" customWidth="1"/>
+    <col min="23" max="23" width="15" customWidth="1"/>
+    <col min="24" max="24" width="13.5" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="13.1640625" customWidth="1"/>
+    <col min="27" max="27" width="11.83203125" customWidth="1"/>
+    <col min="28" max="28" width="15.5" customWidth="1"/>
+    <col min="29" max="29" width="12.6640625" customWidth="1"/>
+    <col min="30" max="30" width="14.33203125" customWidth="1"/>
+    <col min="31" max="32" width="10.83203125" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="18" customFormat="1">
+    <row r="1" spans="1:25" s="18" customFormat="1">
       <c r="A1" s="18" t="s">
         <v>212</v>
       </c>
@@ -5755,13 +5769,13 @@
         <v>992</v>
       </c>
       <c r="G1" t="s">
-        <v>1054</v>
+        <v>992</v>
       </c>
       <c r="H1" t="s">
         <v>1054</v>
       </c>
-      <c r="I1" s="18" t="s">
-        <v>1</v>
+      <c r="I1" t="s">
+        <v>1054</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>1</v>
@@ -5770,25 +5784,25 @@
         <v>1</v>
       </c>
       <c r="L1" s="18" t="s">
-        <v>976</v>
+        <v>1</v>
       </c>
       <c r="M1" s="18" t="s">
         <v>976</v>
       </c>
-      <c r="N1"/>
-      <c r="O1" t="s">
+      <c r="N1" s="18" t="s">
+        <v>976</v>
+      </c>
+      <c r="O1"/>
+      <c r="P1" t="s">
         <v>992</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>1054</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="R1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="17" t="s">
-        <v>992</v>
-      </c>
-      <c r="S1" t="s">
+      <c r="S1" s="17" t="s">
         <v>992</v>
       </c>
       <c r="T1" t="s">
@@ -5797,14 +5811,17 @@
       <c r="U1" t="s">
         <v>992</v>
       </c>
-      <c r="V1" s="18" t="s">
+      <c r="V1" t="s">
+        <v>992</v>
+      </c>
+      <c r="W1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="W1" s="18" t="s">
+      <c r="X1" s="18" t="s">
         <v>976</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="18" customFormat="1">
+    <row r="2" spans="1:25" s="18" customFormat="1">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -5820,12 +5837,13 @@
       <c r="N2"/>
       <c r="O2"/>
       <c r="P2"/>
-      <c r="R2" s="17"/>
-      <c r="S2"/>
+      <c r="Q2"/>
+      <c r="S2" s="17"/>
       <c r="T2"/>
       <c r="U2"/>
-    </row>
-    <row r="3" spans="1:24" s="40" customFormat="1">
+      <c r="V2"/>
+    </row>
+    <row r="3" spans="1:25" s="40" customFormat="1">
       <c r="A3" s="40" t="s">
         <v>1066</v>
       </c>
@@ -5838,7 +5856,9 @@
       <c r="D3" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="E3" s="41"/>
+      <c r="E3" s="41" t="s">
+        <v>216</v>
+      </c>
       <c r="F3" s="41"/>
       <c r="G3" s="41"/>
       <c r="H3" s="41"/>
@@ -5850,12 +5870,13 @@
       <c r="N3" s="41"/>
       <c r="O3" s="41"/>
       <c r="P3" s="41"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="41"/>
+      <c r="Q3" s="41"/>
+      <c r="S3" s="42"/>
       <c r="T3" s="41"/>
       <c r="U3" s="41"/>
-    </row>
-    <row r="4" spans="1:24">
+      <c r="V3" s="41"/>
+    </row>
+    <row r="4" spans="1:25">
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
       <c r="D4" s="21"/>
@@ -5869,10 +5890,11 @@
       <c r="L4" s="21"/>
       <c r="M4" s="21"/>
       <c r="N4" s="21"/>
-      <c r="R4" s="22"/>
-      <c r="U4" s="21"/>
-    </row>
-    <row r="5" spans="1:24">
+      <c r="O4" s="21"/>
+      <c r="S4" s="22"/>
+      <c r="V4" s="21"/>
+    </row>
+    <row r="5" spans="1:25">
       <c r="A5" t="s">
         <v>217</v>
       </c>
@@ -5912,27 +5934,27 @@
       <c r="M5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21" t="s">
+      <c r="N5" s="21" t="s">
         <v>1032</v>
       </c>
+      <c r="O5" s="21"/>
       <c r="P5" s="21" t="s">
         <v>1032</v>
       </c>
       <c r="Q5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="R5" s="22" t="s">
+      <c r="R5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="S5" s="22" t="s">
         <v>1034</v>
       </c>
-      <c r="S5" s="21" t="s">
+      <c r="T5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="T5" s="22" t="s">
+      <c r="U5" s="22" t="s">
         <v>1034</v>
-      </c>
-      <c r="U5" s="21" t="s">
-        <v>1032</v>
       </c>
       <c r="V5" s="21" t="s">
         <v>1032</v>
@@ -5940,9 +5962,12 @@
       <c r="W5" s="21" t="s">
         <v>1032</v>
       </c>
-      <c r="X5" s="21"/>
-    </row>
-    <row r="6" spans="1:24">
+      <c r="X5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="Y5" s="21"/>
+    </row>
+    <row r="6" spans="1:25">
       <c r="A6" t="s">
         <v>221</v>
       </c>
@@ -5956,13 +5981,13 @@
         <v>1033</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>1067</v>
+        <v>1031</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>1067</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>1031</v>
+        <v>1067</v>
       </c>
       <c r="H6" s="21" t="s">
         <v>1031</v>
@@ -5982,37 +6007,40 @@
       <c r="M6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21" t="s">
+      <c r="N6" s="21" t="s">
         <v>1031</v>
       </c>
+      <c r="O6" s="21"/>
       <c r="P6" s="21" t="s">
         <v>1031</v>
       </c>
       <c r="Q6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="R6" s="22" t="s">
+      <c r="R6" s="21" t="s">
         <v>1031</v>
       </c>
-      <c r="S6" s="21" t="s">
-        <v>1035</v>
+      <c r="S6" s="22" t="s">
+        <v>1031</v>
       </c>
       <c r="T6" s="21" t="s">
         <v>1035</v>
       </c>
       <c r="U6" s="21" t="s">
+        <v>1035</v>
+      </c>
+      <c r="V6" s="21" t="s">
         <v>1033</v>
-      </c>
-      <c r="V6" s="22" t="s">
-        <v>1036</v>
       </c>
       <c r="W6" s="22" t="s">
         <v>1036</v>
       </c>
-      <c r="X6" s="21"/>
-    </row>
-    <row r="7" spans="1:24">
+      <c r="X6" s="22" t="s">
+        <v>1036</v>
+      </c>
+      <c r="Y6" s="21"/>
+    </row>
+    <row r="7" spans="1:25">
       <c r="A7" t="s">
         <v>280</v>
       </c>
@@ -6025,23 +6053,23 @@
       <c r="D7" s="21" t="s">
         <v>281</v>
       </c>
-      <c r="E7" s="21"/>
+      <c r="E7" s="21" t="s">
+        <v>281</v>
+      </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
       <c r="J7" s="21"/>
       <c r="K7" s="21"/>
-      <c r="L7" t="s">
+      <c r="L7" s="21"/>
+      <c r="M7" t="s">
         <v>1069</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="N7" s="21" t="s">
         <v>1068</v>
       </c>
-      <c r="N7" s="21"/>
-      <c r="O7" s="21" t="s">
-        <v>281</v>
-      </c>
+      <c r="O7" s="21"/>
       <c r="P7" s="21" t="s">
         <v>281</v>
       </c>
@@ -6066,13 +6094,19 @@
       <c r="W7" s="21" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="8" spans="1:24">
+      <c r="X7" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25">
       <c r="A8" t="s">
         <v>224</v>
       </c>
-      <c r="O8" s="21" t="s">
-        <v>1064</v>
+      <c r="C8" s="21" t="s">
+        <v>1071</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>1070</v>
       </c>
       <c r="P8" s="21" t="s">
         <v>1064</v>
@@ -6095,11 +6129,14 @@
       <c r="V8" s="21" t="s">
         <v>1064</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="21" t="s">
+        <v>1064</v>
+      </c>
+      <c r="X8" t="s">
         <v>1065</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:25">
       <c r="A9" t="s">
         <v>1063</v>
       </c>
@@ -6113,7 +6150,7 @@
         <v>1056</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>1056</v>
+        <v>1062</v>
       </c>
       <c r="F9" s="21" t="s">
         <v>1056</v>
@@ -6137,12 +6174,12 @@
         <v>1056</v>
       </c>
       <c r="M9" s="21" t="s">
+        <v>1056</v>
+      </c>
+      <c r="N9" s="21" t="s">
         <v>1062</v>
       </c>
-      <c r="N9" s="21"/>
-      <c r="O9" s="21" t="s">
-        <v>1062</v>
-      </c>
+      <c r="O9" s="21"/>
       <c r="P9" s="21" t="s">
         <v>1062</v>
       </c>
@@ -6167,8 +6204,11 @@
       <c r="W9" s="21" t="s">
         <v>1062</v>
       </c>
-    </row>
-    <row r="11" spans="1:24">
+      <c r="X9" s="21" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25">
       <c r="A11" t="s">
         <v>214</v>
       </c>
@@ -6182,13 +6222,13 @@
         <v>1775</v>
       </c>
       <c r="E11">
-        <v>2497</v>
+        <v>1524</v>
       </c>
       <c r="F11">
         <v>2497</v>
       </c>
       <c r="G11">
-        <v>1524</v>
+        <v>2497</v>
       </c>
       <c r="H11">
         <v>1524</v>
@@ -6200,16 +6240,16 @@
         <v>1524</v>
       </c>
       <c r="K11">
-        <v>2497</v>
+        <v>1524</v>
       </c>
       <c r="L11">
         <v>2497</v>
       </c>
       <c r="M11">
+        <v>2497</v>
+      </c>
+      <c r="N11">
         <v>1524</v>
-      </c>
-      <c r="O11" s="23">
-        <v>1556</v>
       </c>
       <c r="P11" s="23">
         <v>1556</v>
@@ -6218,25 +6258,28 @@
         <v>1556</v>
       </c>
       <c r="R11" s="23">
+        <v>1556</v>
+      </c>
+      <c r="S11" s="23">
         <v>1097</v>
       </c>
-      <c r="S11" s="23">
+      <c r="T11" s="23">
         <v>2651</v>
       </c>
-      <c r="T11" s="23">
+      <c r="U11" s="23">
         <v>2112</v>
       </c>
-      <c r="U11" s="23">
+      <c r="V11" s="23">
         <v>1953</v>
-      </c>
-      <c r="V11">
-        <v>1556</v>
       </c>
       <c r="W11">
         <v>1556</v>
       </c>
-    </row>
-    <row r="12" spans="1:24">
+      <c r="X11">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25">
       <c r="A12" t="s">
         <v>211</v>
       </c>
@@ -6250,13 +6293,13 @@
         <v>38</v>
       </c>
       <c r="E12">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="F12">
         <v>199</v>
       </c>
       <c r="G12">
-        <v>37</v>
+        <v>199</v>
       </c>
       <c r="H12">
         <v>37</v>
@@ -6268,15 +6311,15 @@
         <v>37</v>
       </c>
       <c r="K12">
-        <v>199</v>
+        <v>37</v>
       </c>
       <c r="L12">
         <v>199</v>
       </c>
       <c r="M12">
-        <v>37</v>
-      </c>
-      <c r="O12" s="23">
+        <v>199</v>
+      </c>
+      <c r="N12">
         <v>37</v>
       </c>
       <c r="P12" s="23">
@@ -6286,40 +6329,43 @@
         <v>37</v>
       </c>
       <c r="R12" s="23">
+        <v>37</v>
+      </c>
+      <c r="S12" s="23">
         <v>25</v>
       </c>
-      <c r="S12" s="23">
+      <c r="T12" s="23">
         <v>200</v>
       </c>
-      <c r="T12" s="23">
+      <c r="U12" s="23">
         <v>179</v>
       </c>
-      <c r="U12" s="23">
+      <c r="V12" s="23">
         <v>41</v>
-      </c>
-      <c r="V12">
-        <v>37</v>
       </c>
       <c r="W12">
         <v>37</v>
       </c>
-      <c r="X12" s="23"/>
-    </row>
-    <row r="13" spans="1:24">
+      <c r="X12">
+        <v>37</v>
+      </c>
+      <c r="Y12" s="23"/>
+    </row>
+    <row r="13" spans="1:25">
       <c r="A13" t="s">
         <v>213</v>
       </c>
-      <c r="O13" s="23"/>
       <c r="P13" s="23"/>
-      <c r="R13" s="23"/>
+      <c r="Q13" s="23"/>
       <c r="S13" s="23"/>
       <c r="T13" s="23"/>
-      <c r="W13">
+      <c r="U13" s="23"/>
+      <c r="X13">
         <v>30</v>
       </c>
-      <c r="X13" s="23"/>
-    </row>
-    <row r="14" spans="1:24">
+      <c r="Y13" s="23"/>
+    </row>
+    <row r="14" spans="1:25">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -6333,22 +6379,22 @@
         <v>216</v>
       </c>
       <c r="E14" t="s">
+        <v>216</v>
+      </c>
+      <c r="F14" t="s">
         <v>214</v>
-      </c>
-      <c r="F14" t="s">
-        <v>216</v>
       </c>
       <c r="G14" t="s">
         <v>216</v>
       </c>
       <c r="H14" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="I14" t="s">
         <v>214</v>
       </c>
       <c r="J14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="K14" t="s">
         <v>216</v>
@@ -6359,7 +6405,7 @@
       <c r="M14" t="s">
         <v>216</v>
       </c>
-      <c r="O14" s="23" t="s">
+      <c r="N14" t="s">
         <v>216</v>
       </c>
       <c r="P14" s="23" t="s">
@@ -6386,8 +6432,11 @@
       <c r="W14" s="23" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="16" spans="1:24" s="21" customFormat="1">
+      <c r="X14" s="23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" s="21" customFormat="1">
       <c r="A16" s="21" t="s">
         <v>5</v>
       </c>
@@ -6401,75 +6450,78 @@
         <v>28.90391</v>
       </c>
       <c r="E16" s="21">
+        <v>30.067322000000001</v>
+      </c>
+      <c r="F16" s="21">
         <v>62.459069999999997</v>
       </c>
-      <c r="F16" s="21">
+      <c r="G16" s="21">
         <v>30.738227999999999</v>
       </c>
-      <c r="G16" s="21">
+      <c r="H16" s="21">
         <v>30.584579999999999</v>
       </c>
-      <c r="H16" s="21">
+      <c r="I16" s="21">
         <v>64.010794300000001</v>
       </c>
-      <c r="I16" s="21">
+      <c r="J16" s="21">
         <v>64.962770178</v>
       </c>
-      <c r="J16" s="21">
+      <c r="K16" s="21">
         <v>30.721707769999998</v>
       </c>
-      <c r="K16" s="21">
+      <c r="L16" s="21">
         <v>30.754858800000001</v>
       </c>
-      <c r="L16" s="21">
+      <c r="M16" s="21">
         <v>13.436368399999999</v>
       </c>
-      <c r="M16" s="21">
+      <c r="N16" s="21">
         <v>11.977791</v>
       </c>
-      <c r="O16" s="21">
+      <c r="P16" s="21">
         <v>30.877478</v>
       </c>
-      <c r="P16" s="21">
+      <c r="Q16" s="21">
         <v>30.66</v>
       </c>
-      <c r="Q16" s="21">
+      <c r="R16" s="21">
         <v>31.211466999999999</v>
       </c>
-      <c r="R16" s="21">
+      <c r="S16" s="21">
         <v>31.880268000000001</v>
       </c>
-      <c r="S16" s="21">
+      <c r="T16" s="21">
         <v>30.716964999999998</v>
       </c>
-      <c r="T16" s="21">
+      <c r="U16" s="21">
         <v>29.746556000000002</v>
       </c>
-      <c r="U16" s="21">
+      <c r="V16" s="21">
         <v>29.076453999999998</v>
       </c>
-      <c r="V16" s="21">
+      <c r="W16" s="21">
         <v>29.443950000000001</v>
       </c>
-      <c r="W16" s="21">
+      <c r="X16" s="21">
         <v>11.154477999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:23" s="21" customFormat="1">
+    <row r="17" spans="1:24" s="21" customFormat="1">
       <c r="A17" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="L17" s="21">
+      <c r="M17" s="21">
         <v>8.5977074000000009</v>
       </c>
-      <c r="M17" s="21">
+      <c r="N17" s="21">
         <v>12.778447999999999</v>
       </c>
-      <c r="W17" s="21">
+      <c r="X17" s="21">
         <v>17.8</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="21" customFormat="1" ht="14" customHeight="1">
+    <row r="18" spans="1:24" s="21" customFormat="1" ht="14" customHeight="1">
       <c r="A18" s="21" t="s">
         <v>7</v>
       </c>
@@ -6483,61 +6535,64 @@
         <v>-4.0439959999999999</v>
       </c>
       <c r="E18" s="21">
+        <v>-3.986354</v>
+      </c>
+      <c r="F18" s="21">
         <v>-0.66238750000000002</v>
       </c>
-      <c r="F18" s="21">
+      <c r="G18" s="21">
         <v>-3.1059860000000001</v>
       </c>
-      <c r="G18" s="21">
+      <c r="H18" s="21">
         <v>-5.8981399999999997</v>
       </c>
-      <c r="H18" s="21">
+      <c r="I18" s="21">
         <v>-0.98127699999999995</v>
       </c>
-      <c r="I18" s="21">
+      <c r="J18" s="21">
         <v>-0.43686686800000002</v>
       </c>
-      <c r="J18" s="21">
+      <c r="K18" s="21">
         <v>-4.6886315600000001</v>
       </c>
-      <c r="K18" s="21">
+      <c r="L18" s="21">
         <v>-3.2696827000000002</v>
       </c>
-      <c r="L18" s="21">
+      <c r="M18" s="21">
         <v>-8.0795293000000008</v>
       </c>
-      <c r="M18" s="21">
+      <c r="N18" s="21">
         <v>-10.718495000000001</v>
       </c>
-      <c r="O18" s="21">
+      <c r="P18" s="21">
         <v>-3.858498</v>
       </c>
-      <c r="P18" s="21">
+      <c r="Q18" s="21">
         <v>-4.7</v>
       </c>
-      <c r="Q18" s="21">
+      <c r="R18" s="21">
         <v>-3.9753639999999999</v>
       </c>
-      <c r="R18" s="21">
+      <c r="S18" s="21">
         <v>-6.589467</v>
       </c>
-      <c r="S18" s="21">
+      <c r="T18" s="21">
         <v>-4.670153</v>
       </c>
-      <c r="T18" s="21">
+      <c r="U18" s="21">
         <v>-6.3059329999999996</v>
       </c>
-      <c r="U18" s="21">
+      <c r="V18" s="21">
         <v>-4.2054489999999998</v>
       </c>
-      <c r="V18" s="21">
+      <c r="W18" s="21">
         <v>-4.4239769999999998</v>
       </c>
-      <c r="W18" s="21">
+      <c r="X18" s="21">
         <v>-11.179836</v>
       </c>
     </row>
-    <row r="19" spans="1:23" s="21" customFormat="1">
+    <row r="19" spans="1:24" s="21" customFormat="1">
       <c r="A19" s="21" t="s">
         <v>8</v>
       </c>
@@ -6551,61 +6606,64 @@
         <v>-3.5158939999999999</v>
       </c>
       <c r="E19" s="21">
+        <v>-2.940315</v>
+      </c>
+      <c r="F19" s="21">
         <v>-0.30074129999999999</v>
       </c>
-      <c r="F19" s="21">
+      <c r="G19" s="21">
         <v>-1.8089200000000001</v>
       </c>
-      <c r="G19" s="21">
+      <c r="H19" s="21">
         <v>-1.7522850000000001</v>
       </c>
-      <c r="H19" s="21">
+      <c r="I19" s="21">
         <v>-0.32169579999999998</v>
       </c>
-      <c r="I19" s="21">
+      <c r="J19" s="21">
         <v>-0.59282655500000003</v>
       </c>
-      <c r="J19" s="21">
+      <c r="K19" s="21">
         <v>-3.2544300800000001</v>
       </c>
-      <c r="K19" s="21">
+      <c r="L19" s="21">
         <v>-2.0773652</v>
       </c>
-      <c r="L19" s="21">
+      <c r="M19" s="21">
         <v>-0.73294579999999998</v>
       </c>
-      <c r="M19" s="21">
+      <c r="N19" s="21">
         <v>-1.3810519999999999</v>
       </c>
-      <c r="O19" s="21">
+      <c r="P19" s="21">
         <v>-3.1080649999999999</v>
       </c>
-      <c r="P19" s="21">
+      <c r="Q19" s="21">
         <v>-2.2999999999999998</v>
       </c>
-      <c r="Q19" s="21">
+      <c r="R19" s="21">
         <v>-3.5504150000000001</v>
       </c>
-      <c r="R19" s="21">
+      <c r="S19" s="21">
         <v>-2.3749199999999999</v>
       </c>
-      <c r="S19" s="21">
+      <c r="T19" s="21">
         <v>-1.740626</v>
       </c>
-      <c r="T19" s="21">
+      <c r="U19" s="21">
         <v>-1.149972</v>
       </c>
-      <c r="U19" s="21">
+      <c r="V19" s="21">
         <v>-3.8012999999999999</v>
       </c>
-      <c r="V19" s="21">
+      <c r="W19" s="21">
         <v>-4.6329729999999998</v>
       </c>
-      <c r="W19" s="21">
+      <c r="X19" s="21">
         <v>-1.4</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="21" customFormat="1">
+    <row r="20" spans="1:24" s="21" customFormat="1">
       <c r="A20" s="21" t="s">
         <v>9</v>
       </c>
@@ -6619,153 +6677,156 @@
         <v>-8.3347940000000005</v>
       </c>
       <c r="E20" s="21">
+        <v>-8.9357970000000009</v>
+      </c>
+      <c r="F20" s="21">
         <v>-0.2393874</v>
       </c>
-      <c r="F20" s="21">
+      <c r="G20" s="21">
         <v>-7.3253700000000004</v>
       </c>
-      <c r="G20" s="21">
+      <c r="H20" s="21">
         <v>-7.6310460000000004</v>
       </c>
-      <c r="H20" s="21">
+      <c r="I20" s="21">
         <v>-0.22312940000000001</v>
       </c>
-      <c r="I20" s="21">
+      <c r="J20" s="21">
         <v>-0.28852171599999998</v>
       </c>
-      <c r="J20" s="21">
+      <c r="K20" s="21">
         <v>-8.3550094300000008</v>
       </c>
-      <c r="K20" s="21">
+      <c r="L20" s="21">
         <v>-7.0728663999999997</v>
       </c>
-      <c r="L20" s="21">
+      <c r="M20" s="21">
         <v>-8.4076094999999995</v>
       </c>
-      <c r="M20" s="21">
+      <c r="N20" s="21">
         <v>-9.5678230000000006</v>
       </c>
-      <c r="O20" s="21">
+      <c r="P20" s="21">
         <v>-10.069042</v>
       </c>
-      <c r="P20" s="21">
+      <c r="Q20" s="21">
         <v>-8.5</v>
       </c>
-      <c r="Q20" s="21">
+      <c r="R20" s="21">
         <v>-10.401221</v>
       </c>
-      <c r="R20" s="21">
+      <c r="S20" s="21">
         <v>-9.9066620000000007</v>
       </c>
-      <c r="S20" s="21">
+      <c r="T20" s="21">
         <v>-8.6652190000000004</v>
       </c>
-      <c r="T20" s="21">
+      <c r="U20" s="21">
         <v>-9.8209820000000008</v>
       </c>
-      <c r="U20" s="21">
+      <c r="V20" s="21">
         <v>-10.442672999999999</v>
       </c>
-      <c r="V20" s="21">
+      <c r="W20" s="21">
         <v>-10.520892</v>
       </c>
-      <c r="W20" s="21">
+      <c r="X20" s="21">
         <v>-9.7576470000000004</v>
       </c>
     </row>
-    <row r="21" spans="1:23">
+    <row r="21" spans="1:24">
       <c r="A21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:23">
+    <row r="22" spans="1:24">
       <c r="A22" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="23" spans="1:23">
+    <row r="23" spans="1:24">
       <c r="A23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:23">
+    <row r="24" spans="1:24">
       <c r="A24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:23">
+    <row r="25" spans="1:24">
       <c r="A25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:23">
+    <row r="26" spans="1:24">
       <c r="A26" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:23">
+    <row r="27" spans="1:24">
       <c r="A27" t="s">
         <v>210</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>6.1738270000000002</v>
       </c>
-      <c r="M27">
+      <c r="N27">
         <v>9.932563</v>
       </c>
     </row>
-    <row r="28" spans="1:23">
+    <row r="28" spans="1:24">
       <c r="A28" t="s">
         <v>10</v>
       </c>
-      <c r="I28">
+      <c r="J28">
         <v>-1.4379709999999999E-3</v>
       </c>
-      <c r="J28">
+      <c r="K28">
         <v>-9.5536179999999998E-2</v>
       </c>
-      <c r="K28">
+      <c r="L28">
         <v>0.15195020000000001</v>
       </c>
-      <c r="Q28" s="21">
+      <c r="R28" s="21">
         <v>1.47323</v>
       </c>
     </row>
-    <row r="29" spans="1:23">
+    <row r="29" spans="1:24">
       <c r="A29" t="s">
         <v>11</v>
       </c>
-      <c r="I29">
+      <c r="J29">
         <v>4.1001559999999998E-3</v>
       </c>
-      <c r="J29">
+      <c r="K29">
         <v>0.85033303000000005</v>
       </c>
-      <c r="K29">
+      <c r="L29">
         <v>1.3428956999999999</v>
       </c>
-      <c r="Q29" s="21">
+      <c r="R29" s="21">
         <v>1.0277529999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:23">
+    <row r="30" spans="1:24">
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="I30">
+      <c r="J30">
         <v>-1.7003655999999999E-2</v>
       </c>
-      <c r="J30">
+      <c r="K30">
         <v>-0.27255634000000001</v>
       </c>
-      <c r="K30">
+      <c r="L30">
         <v>-0.39319349999999997</v>
       </c>
-      <c r="Q30" s="21">
+      <c r="R30" s="21">
         <v>-1.052503</v>
       </c>
     </row>
-    <row r="32" spans="1:23">
+    <row r="32" spans="1:24">
       <c r="A32" s="15" t="s">
         <v>972</v>
       </c>
@@ -6782,258 +6843,259 @@
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
       <c r="N32" s="15"/>
-    </row>
-    <row r="33" spans="1:21">
+      <c r="O32" s="15"/>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" t="s">
         <v>57</v>
       </c>
-      <c r="U33" s="17"/>
-    </row>
-    <row r="34" spans="1:21">
+      <c r="V33" s="17"/>
+    </row>
+    <row r="34" spans="1:22">
       <c r="A34" t="s">
         <v>58</v>
       </c>
-      <c r="U34" s="17"/>
-    </row>
-    <row r="35" spans="1:21">
+      <c r="V34" s="17"/>
+    </row>
+    <row r="35" spans="1:22">
       <c r="A35" t="s">
         <v>59</v>
       </c>
-      <c r="U35" s="17"/>
-    </row>
-    <row r="36" spans="1:21">
+      <c r="V35" s="17"/>
+    </row>
+    <row r="36" spans="1:22">
       <c r="A36" t="s">
         <v>60</v>
       </c>
-      <c r="U36" s="17"/>
-    </row>
-    <row r="37" spans="1:21">
+      <c r="V36" s="17"/>
+    </row>
+    <row r="37" spans="1:22">
       <c r="A37" t="s">
         <v>61</v>
       </c>
-      <c r="U37" s="17"/>
-    </row>
-    <row r="38" spans="1:21">
+      <c r="V37" s="17"/>
+    </row>
+    <row r="38" spans="1:22">
       <c r="A38" t="s">
         <v>62</v>
       </c>
-      <c r="U38" s="17"/>
-    </row>
-    <row r="39" spans="1:21">
+      <c r="V38" s="17"/>
+    </row>
+    <row r="39" spans="1:22">
       <c r="A39" t="s">
         <v>63</v>
       </c>
-      <c r="U39" s="17"/>
-    </row>
-    <row r="40" spans="1:21">
+      <c r="V39" s="17"/>
+    </row>
+    <row r="40" spans="1:22">
       <c r="A40" t="s">
         <v>64</v>
       </c>
-      <c r="U40" s="17"/>
-    </row>
-    <row r="41" spans="1:21">
+      <c r="V40" s="17"/>
+    </row>
+    <row r="41" spans="1:22">
       <c r="A41" t="s">
         <v>65</v>
       </c>
-      <c r="U41" s="17"/>
-    </row>
-    <row r="42" spans="1:21">
+      <c r="V41" s="17"/>
+    </row>
+    <row r="42" spans="1:22">
       <c r="A42" t="s">
         <v>66</v>
       </c>
-      <c r="U42" s="17"/>
-    </row>
-    <row r="43" spans="1:21">
+      <c r="V42" s="17"/>
+    </row>
+    <row r="43" spans="1:22">
       <c r="A43" t="s">
         <v>67</v>
       </c>
-      <c r="U43" s="17"/>
-    </row>
-    <row r="44" spans="1:21">
+      <c r="V43" s="17"/>
+    </row>
+    <row r="44" spans="1:22">
       <c r="A44" t="s">
         <v>68</v>
       </c>
-      <c r="U44" s="17"/>
-    </row>
-    <row r="45" spans="1:21">
+      <c r="V44" s="17"/>
+    </row>
+    <row r="45" spans="1:22">
       <c r="A45" t="s">
         <v>69</v>
       </c>
-      <c r="U45" s="17"/>
-    </row>
-    <row r="46" spans="1:21">
+      <c r="V45" s="17"/>
+    </row>
+    <row r="46" spans="1:22">
       <c r="A46" t="s">
         <v>70</v>
       </c>
-      <c r="U46" s="17"/>
-    </row>
-    <row r="47" spans="1:21">
+      <c r="V46" s="17"/>
+    </row>
+    <row r="47" spans="1:22">
       <c r="A47" t="s">
         <v>71</v>
       </c>
-      <c r="U47" s="17"/>
-    </row>
-    <row r="48" spans="1:21">
+      <c r="V47" s="17"/>
+    </row>
+    <row r="48" spans="1:22">
       <c r="A48" t="s">
         <v>72</v>
       </c>
-      <c r="U48" s="17"/>
-    </row>
-    <row r="49" spans="1:21">
+      <c r="V48" s="17"/>
+    </row>
+    <row r="49" spans="1:22">
       <c r="A49" t="s">
         <v>73</v>
       </c>
-      <c r="U49" s="17"/>
-    </row>
-    <row r="50" spans="1:21">
+      <c r="V49" s="17"/>
+    </row>
+    <row r="50" spans="1:22">
       <c r="A50" t="s">
         <v>74</v>
       </c>
-      <c r="U50" s="17"/>
-    </row>
-    <row r="51" spans="1:21">
+      <c r="V50" s="17"/>
+    </row>
+    <row r="51" spans="1:22">
       <c r="A51" t="s">
         <v>75</v>
       </c>
-      <c r="U51" s="17"/>
-    </row>
-    <row r="52" spans="1:21">
+      <c r="V51" s="17"/>
+    </row>
+    <row r="52" spans="1:22">
       <c r="A52" t="s">
         <v>76</v>
       </c>
-      <c r="U52" s="17"/>
-    </row>
-    <row r="53" spans="1:21">
+      <c r="V52" s="17"/>
+    </row>
+    <row r="53" spans="1:22">
       <c r="A53" t="s">
         <v>77</v>
       </c>
-      <c r="U53" s="17"/>
-    </row>
-    <row r="54" spans="1:21">
+      <c r="V53" s="17"/>
+    </row>
+    <row r="54" spans="1:22">
       <c r="A54" t="s">
         <v>78</v>
       </c>
-      <c r="U54" s="17"/>
-    </row>
-    <row r="55" spans="1:21">
+      <c r="V54" s="17"/>
+    </row>
+    <row r="55" spans="1:22">
       <c r="A55" t="s">
         <v>79</v>
       </c>
-      <c r="U55" s="17"/>
-    </row>
-    <row r="56" spans="1:21">
+      <c r="V55" s="17"/>
+    </row>
+    <row r="56" spans="1:22">
       <c r="A56" t="s">
         <v>80</v>
       </c>
-      <c r="U56" s="17"/>
-    </row>
-    <row r="57" spans="1:21">
+      <c r="V56" s="17"/>
+    </row>
+    <row r="57" spans="1:22">
       <c r="A57" t="s">
         <v>81</v>
       </c>
-      <c r="U57" s="17"/>
-    </row>
-    <row r="58" spans="1:21">
+      <c r="V57" s="17"/>
+    </row>
+    <row r="58" spans="1:22">
       <c r="A58" t="s">
         <v>82</v>
       </c>
-      <c r="U58" s="17"/>
-    </row>
-    <row r="59" spans="1:21">
+      <c r="V58" s="17"/>
+    </row>
+    <row r="59" spans="1:22">
       <c r="A59" t="s">
         <v>83</v>
       </c>
-      <c r="U59" s="17"/>
-    </row>
-    <row r="60" spans="1:21">
+      <c r="V59" s="17"/>
+    </row>
+    <row r="60" spans="1:22">
       <c r="A60" t="s">
         <v>84</v>
       </c>
-      <c r="U60" s="17"/>
-    </row>
-    <row r="61" spans="1:21">
+      <c r="V60" s="17"/>
+    </row>
+    <row r="61" spans="1:22">
       <c r="A61" t="s">
         <v>85</v>
       </c>
-      <c r="U61" s="17"/>
-    </row>
-    <row r="62" spans="1:21">
+      <c r="V61" s="17"/>
+    </row>
+    <row r="62" spans="1:22">
       <c r="A62" t="s">
         <v>86</v>
       </c>
-      <c r="U62" s="17"/>
-    </row>
-    <row r="63" spans="1:21">
+      <c r="V62" s="17"/>
+    </row>
+    <row r="63" spans="1:22">
       <c r="A63" t="s">
         <v>87</v>
       </c>
-      <c r="U63" s="17"/>
-    </row>
-    <row r="64" spans="1:21">
+      <c r="V63" s="17"/>
+    </row>
+    <row r="64" spans="1:22">
       <c r="A64" t="s">
         <v>88</v>
       </c>
-      <c r="U64" s="17"/>
-    </row>
-    <row r="65" spans="1:22">
+      <c r="V64" s="17"/>
+    </row>
+    <row r="65" spans="1:23">
       <c r="A65" t="s">
         <v>89</v>
       </c>
-      <c r="U65" s="17"/>
-    </row>
-    <row r="66" spans="1:22">
+      <c r="V65" s="17"/>
+    </row>
+    <row r="66" spans="1:23">
       <c r="A66" t="s">
         <v>90</v>
       </c>
-      <c r="U66" s="17"/>
-    </row>
-    <row r="67" spans="1:22">
+      <c r="V66" s="17"/>
+    </row>
+    <row r="67" spans="1:23">
       <c r="A67" t="s">
         <v>91</v>
       </c>
-      <c r="U67" s="17"/>
-    </row>
-    <row r="68" spans="1:22">
+      <c r="V67" s="17"/>
+    </row>
+    <row r="68" spans="1:23">
       <c r="A68" t="s">
         <v>92</v>
       </c>
-      <c r="U68" s="17"/>
-    </row>
-    <row r="69" spans="1:22">
+      <c r="V68" s="17"/>
+    </row>
+    <row r="69" spans="1:23">
       <c r="A69" t="s">
         <v>93</v>
       </c>
-      <c r="U69" s="17"/>
-    </row>
-    <row r="70" spans="1:22">
+      <c r="V69" s="17"/>
+    </row>
+    <row r="70" spans="1:23">
       <c r="A70" t="s">
         <v>94</v>
       </c>
-      <c r="U70" s="17"/>
-    </row>
-    <row r="71" spans="1:22">
-      <c r="O71" s="22"/>
+      <c r="V70" s="17"/>
+    </row>
+    <row r="71" spans="1:23">
       <c r="P71" s="22"/>
       <c r="Q71" s="22"/>
       <c r="R71" s="22"/>
       <c r="S71" s="22"/>
       <c r="T71" s="22"/>
-      <c r="U71" s="17"/>
+      <c r="U71" s="22"/>
       <c r="V71" s="17"/>
-    </row>
-    <row r="72" spans="1:22">
-      <c r="U72" s="17"/>
-    </row>
-    <row r="73" spans="1:22">
-      <c r="U73" s="17"/>
-    </row>
-    <row r="74" spans="1:22">
-      <c r="U74" s="17"/>
-    </row>
-    <row r="75" spans="1:22">
-      <c r="U75" s="17"/>
-    </row>
-    <row r="76" spans="1:22">
+      <c r="W71" s="17"/>
+    </row>
+    <row r="72" spans="1:23">
+      <c r="V72" s="17"/>
+    </row>
+    <row r="73" spans="1:23">
+      <c r="V73" s="17"/>
+    </row>
+    <row r="74" spans="1:23">
+      <c r="V74" s="17"/>
+    </row>
+    <row r="75" spans="1:23">
+      <c r="V75" s="17"/>
+    </row>
+    <row r="76" spans="1:23">
       <c r="A76" s="17"/>
       <c r="B76" s="17"/>
       <c r="C76" s="17"/>
@@ -7048,733 +7110,734 @@
       <c r="L76" s="17"/>
       <c r="M76" s="17"/>
       <c r="N76" s="17"/>
-      <c r="U76" s="17"/>
-    </row>
-    <row r="77" spans="1:22">
+      <c r="O76" s="17"/>
+      <c r="V76" s="17"/>
+    </row>
+    <row r="77" spans="1:23">
       <c r="A77" t="s">
         <v>171</v>
       </c>
-      <c r="U77" s="17"/>
-    </row>
-    <row r="78" spans="1:22">
+      <c r="V77" s="17"/>
+    </row>
+    <row r="78" spans="1:23">
       <c r="A78" t="s">
         <v>172</v>
       </c>
-      <c r="U78" s="17"/>
-    </row>
-    <row r="79" spans="1:22">
+      <c r="V78" s="17"/>
+    </row>
+    <row r="79" spans="1:23">
       <c r="A79" t="s">
         <v>173</v>
       </c>
-      <c r="U79" s="17"/>
-    </row>
-    <row r="80" spans="1:22">
+      <c r="V79" s="17"/>
+    </row>
+    <row r="80" spans="1:23">
       <c r="A80" t="s">
         <v>174</v>
       </c>
-      <c r="U80" s="17"/>
-    </row>
-    <row r="81" spans="1:21">
+      <c r="V80" s="17"/>
+    </row>
+    <row r="81" spans="1:22">
       <c r="A81" t="s">
         <v>175</v>
       </c>
-      <c r="U81" s="17"/>
-    </row>
-    <row r="82" spans="1:21">
+      <c r="V81" s="17"/>
+    </row>
+    <row r="82" spans="1:22">
       <c r="A82" t="s">
         <v>176</v>
       </c>
-      <c r="U82" s="17"/>
-    </row>
-    <row r="83" spans="1:21">
+      <c r="V82" s="17"/>
+    </row>
+    <row r="83" spans="1:22">
       <c r="A83" t="s">
         <v>177</v>
       </c>
-      <c r="U83" s="17"/>
-    </row>
-    <row r="84" spans="1:21">
+      <c r="V83" s="17"/>
+    </row>
+    <row r="84" spans="1:22">
       <c r="A84" t="s">
         <v>178</v>
       </c>
-      <c r="U84" s="17"/>
-    </row>
-    <row r="85" spans="1:21">
+      <c r="V84" s="17"/>
+    </row>
+    <row r="85" spans="1:22">
       <c r="A85" t="s">
         <v>179</v>
       </c>
-      <c r="U85" s="17"/>
-    </row>
-    <row r="86" spans="1:21">
+      <c r="V85" s="17"/>
+    </row>
+    <row r="86" spans="1:22">
       <c r="A86" t="s">
         <v>180</v>
       </c>
-      <c r="U86" s="17"/>
-    </row>
-    <row r="87" spans="1:21">
+      <c r="V86" s="17"/>
+    </row>
+    <row r="87" spans="1:22">
       <c r="A87" t="s">
         <v>181</v>
       </c>
-      <c r="U87" s="17"/>
-    </row>
-    <row r="88" spans="1:21">
+      <c r="V87" s="17"/>
+    </row>
+    <row r="88" spans="1:22">
       <c r="A88" t="s">
         <v>182</v>
       </c>
-      <c r="U88" s="17"/>
-    </row>
-    <row r="89" spans="1:21">
+      <c r="V88" s="17"/>
+    </row>
+    <row r="89" spans="1:22">
       <c r="A89" t="s">
         <v>183</v>
       </c>
-      <c r="U89" s="17"/>
-    </row>
-    <row r="90" spans="1:21">
+      <c r="V89" s="17"/>
+    </row>
+    <row r="90" spans="1:22">
       <c r="A90" t="s">
         <v>184</v>
       </c>
-      <c r="U90" s="17"/>
-    </row>
-    <row r="91" spans="1:21">
+      <c r="V90" s="17"/>
+    </row>
+    <row r="91" spans="1:22">
       <c r="A91" t="s">
         <v>185</v>
       </c>
-      <c r="U91" s="17"/>
-    </row>
-    <row r="92" spans="1:21">
+      <c r="V91" s="17"/>
+    </row>
+    <row r="92" spans="1:22">
       <c r="A92" t="s">
         <v>186</v>
       </c>
-      <c r="U92" s="17"/>
-    </row>
-    <row r="93" spans="1:21">
+      <c r="V92" s="17"/>
+    </row>
+    <row r="93" spans="1:22">
       <c r="A93" t="s">
         <v>187</v>
       </c>
-      <c r="U93" s="17"/>
-    </row>
-    <row r="94" spans="1:21">
+      <c r="V93" s="17"/>
+    </row>
+    <row r="94" spans="1:22">
       <c r="A94" t="s">
         <v>188</v>
       </c>
-      <c r="U94" s="17"/>
-    </row>
-    <row r="95" spans="1:21">
+      <c r="V94" s="17"/>
+    </row>
+    <row r="95" spans="1:22">
       <c r="A95" t="s">
         <v>189</v>
       </c>
-      <c r="U95" s="17"/>
-    </row>
-    <row r="96" spans="1:21">
+      <c r="V95" s="17"/>
+    </row>
+    <row r="96" spans="1:22">
       <c r="A96" t="s">
         <v>190</v>
       </c>
-      <c r="U96" s="17"/>
-    </row>
-    <row r="97" spans="1:21">
+      <c r="V96" s="17"/>
+    </row>
+    <row r="97" spans="1:22">
       <c r="A97" t="s">
         <v>191</v>
       </c>
-      <c r="U97" s="17"/>
-    </row>
-    <row r="98" spans="1:21">
+      <c r="V97" s="17"/>
+    </row>
+    <row r="98" spans="1:22">
       <c r="A98" t="s">
         <v>192</v>
       </c>
-      <c r="U98" s="17"/>
-    </row>
-    <row r="99" spans="1:21">
+      <c r="V98" s="17"/>
+    </row>
+    <row r="99" spans="1:22">
       <c r="A99" t="s">
         <v>193</v>
       </c>
-      <c r="U99" s="17"/>
-    </row>
-    <row r="100" spans="1:21">
+      <c r="V99" s="17"/>
+    </row>
+    <row r="100" spans="1:22">
       <c r="A100" t="s">
         <v>194</v>
       </c>
-      <c r="U100" s="17"/>
-    </row>
-    <row r="101" spans="1:21">
+      <c r="V100" s="17"/>
+    </row>
+    <row r="101" spans="1:22">
       <c r="A101" t="s">
         <v>195</v>
       </c>
-      <c r="U101" s="17"/>
-    </row>
-    <row r="102" spans="1:21">
+      <c r="V101" s="17"/>
+    </row>
+    <row r="102" spans="1:22">
       <c r="A102" t="s">
         <v>196</v>
       </c>
-      <c r="U102" s="17"/>
-    </row>
-    <row r="103" spans="1:21">
+      <c r="V102" s="17"/>
+    </row>
+    <row r="103" spans="1:22">
       <c r="A103" t="s">
         <v>197</v>
       </c>
-      <c r="U103" s="17"/>
-    </row>
-    <row r="104" spans="1:21">
+      <c r="V103" s="17"/>
+    </row>
+    <row r="104" spans="1:22">
       <c r="A104" t="s">
         <v>198</v>
       </c>
-      <c r="U104" s="17"/>
-    </row>
-    <row r="105" spans="1:21">
+      <c r="V104" s="17"/>
+    </row>
+    <row r="105" spans="1:22">
       <c r="A105" t="s">
         <v>199</v>
       </c>
-      <c r="U105" s="17"/>
-    </row>
-    <row r="106" spans="1:21">
+      <c r="V105" s="17"/>
+    </row>
+    <row r="106" spans="1:22">
       <c r="A106" t="s">
         <v>200</v>
       </c>
-      <c r="U106" s="17"/>
-    </row>
-    <row r="107" spans="1:21">
+      <c r="V106" s="17"/>
+    </row>
+    <row r="107" spans="1:22">
       <c r="A107" t="s">
         <v>201</v>
       </c>
-      <c r="U107" s="17"/>
-    </row>
-    <row r="108" spans="1:21">
+      <c r="V107" s="17"/>
+    </row>
+    <row r="108" spans="1:22">
       <c r="A108" t="s">
         <v>202</v>
       </c>
-      <c r="U108" s="17"/>
-    </row>
-    <row r="109" spans="1:21">
+      <c r="V108" s="17"/>
+    </row>
+    <row r="109" spans="1:22">
       <c r="A109" t="s">
         <v>203</v>
       </c>
-      <c r="U109" s="17"/>
-    </row>
-    <row r="110" spans="1:21">
+      <c r="V109" s="17"/>
+    </row>
+    <row r="110" spans="1:22">
       <c r="A110" t="s">
         <v>204</v>
       </c>
-      <c r="U110" s="17"/>
-    </row>
-    <row r="111" spans="1:21">
+      <c r="V110" s="17"/>
+    </row>
+    <row r="111" spans="1:22">
       <c r="A111" t="s">
         <v>205</v>
       </c>
-      <c r="U111" s="17"/>
-    </row>
-    <row r="112" spans="1:21">
+      <c r="V111" s="17"/>
+    </row>
+    <row r="112" spans="1:22">
       <c r="A112" t="s">
         <v>206</v>
       </c>
-      <c r="U112" s="17"/>
-    </row>
-    <row r="113" spans="1:21">
+      <c r="V112" s="17"/>
+    </row>
+    <row r="113" spans="1:22">
       <c r="A113" t="s">
         <v>207</v>
       </c>
-      <c r="U113" s="17"/>
-    </row>
-    <row r="114" spans="1:21">
+      <c r="V113" s="17"/>
+    </row>
+    <row r="114" spans="1:22">
       <c r="A114" t="s">
         <v>208</v>
       </c>
-      <c r="U114" s="17"/>
-    </row>
-    <row r="115" spans="1:21">
-      <c r="U115" s="17"/>
-    </row>
-    <row r="116" spans="1:21">
-      <c r="U116" s="17"/>
-    </row>
-    <row r="117" spans="1:21">
-      <c r="U117" s="17"/>
-    </row>
-    <row r="118" spans="1:21">
-      <c r="U118" s="17"/>
-    </row>
-    <row r="119" spans="1:21">
-      <c r="U119" s="17"/>
-    </row>
-    <row r="120" spans="1:21">
-      <c r="U120" s="17"/>
-    </row>
-    <row r="121" spans="1:21">
+      <c r="V114" s="17"/>
+    </row>
+    <row r="115" spans="1:22">
+      <c r="V115" s="17"/>
+    </row>
+    <row r="116" spans="1:22">
+      <c r="V116" s="17"/>
+    </row>
+    <row r="117" spans="1:22">
+      <c r="V117" s="17"/>
+    </row>
+    <row r="118" spans="1:22">
+      <c r="V118" s="17"/>
+    </row>
+    <row r="119" spans="1:22">
+      <c r="V119" s="17"/>
+    </row>
+    <row r="120" spans="1:22">
+      <c r="V120" s="17"/>
+    </row>
+    <row r="121" spans="1:22">
       <c r="A121" t="s">
         <v>133</v>
       </c>
-      <c r="U121" s="17"/>
-    </row>
-    <row r="122" spans="1:21">
+      <c r="V121" s="17"/>
+    </row>
+    <row r="122" spans="1:22">
       <c r="A122" t="s">
         <v>134</v>
       </c>
-      <c r="U122" s="17"/>
-    </row>
-    <row r="123" spans="1:21">
+      <c r="V122" s="17"/>
+    </row>
+    <row r="123" spans="1:22">
       <c r="A123" t="s">
         <v>135</v>
       </c>
-      <c r="U123" s="17"/>
-    </row>
-    <row r="124" spans="1:21">
+      <c r="V123" s="17"/>
+    </row>
+    <row r="124" spans="1:22">
       <c r="A124" t="s">
         <v>136</v>
       </c>
-      <c r="U124" s="17"/>
-    </row>
-    <row r="125" spans="1:21">
+      <c r="V124" s="17"/>
+    </row>
+    <row r="125" spans="1:22">
       <c r="A125" t="s">
         <v>137</v>
       </c>
-      <c r="U125" s="17"/>
-    </row>
-    <row r="126" spans="1:21">
+      <c r="V125" s="17"/>
+    </row>
+    <row r="126" spans="1:22">
       <c r="A126" t="s">
         <v>138</v>
       </c>
-      <c r="U126" s="17"/>
-    </row>
-    <row r="127" spans="1:21">
+      <c r="V126" s="17"/>
+    </row>
+    <row r="127" spans="1:22">
       <c r="A127" t="s">
         <v>139</v>
       </c>
-      <c r="U127" s="17"/>
-    </row>
-    <row r="128" spans="1:21">
+      <c r="V127" s="17"/>
+    </row>
+    <row r="128" spans="1:22">
       <c r="A128" t="s">
         <v>140</v>
       </c>
-      <c r="U128" s="17"/>
-    </row>
-    <row r="129" spans="1:21">
+      <c r="V128" s="17"/>
+    </row>
+    <row r="129" spans="1:22">
       <c r="A129" t="s">
         <v>141</v>
       </c>
-      <c r="U129" s="17"/>
-    </row>
-    <row r="130" spans="1:21">
+      <c r="V129" s="17"/>
+    </row>
+    <row r="130" spans="1:22">
       <c r="A130" t="s">
         <v>142</v>
       </c>
-      <c r="U130" s="17"/>
-    </row>
-    <row r="131" spans="1:21">
+      <c r="V130" s="17"/>
+    </row>
+    <row r="131" spans="1:22">
       <c r="A131" t="s">
         <v>143</v>
       </c>
-      <c r="U131" s="17"/>
-    </row>
-    <row r="132" spans="1:21">
+      <c r="V131" s="17"/>
+    </row>
+    <row r="132" spans="1:22">
       <c r="A132" t="s">
         <v>144</v>
       </c>
-      <c r="U132" s="17"/>
-    </row>
-    <row r="133" spans="1:21">
+      <c r="V132" s="17"/>
+    </row>
+    <row r="133" spans="1:22">
       <c r="A133" t="s">
         <v>145</v>
       </c>
-      <c r="U133" s="17"/>
-    </row>
-    <row r="134" spans="1:21">
+      <c r="V133" s="17"/>
+    </row>
+    <row r="134" spans="1:22">
       <c r="A134" t="s">
         <v>146</v>
       </c>
-      <c r="U134" s="17"/>
-    </row>
-    <row r="135" spans="1:21">
+      <c r="V134" s="17"/>
+    </row>
+    <row r="135" spans="1:22">
       <c r="A135" t="s">
         <v>147</v>
       </c>
-      <c r="U135" s="17"/>
-    </row>
-    <row r="136" spans="1:21">
+      <c r="V135" s="17"/>
+    </row>
+    <row r="136" spans="1:22">
       <c r="A136" t="s">
         <v>148</v>
       </c>
-      <c r="U136" s="17"/>
-    </row>
-    <row r="137" spans="1:21">
+      <c r="V136" s="17"/>
+    </row>
+    <row r="137" spans="1:22">
       <c r="A137" t="s">
         <v>149</v>
       </c>
-      <c r="U137" s="17"/>
-    </row>
-    <row r="138" spans="1:21">
+      <c r="V137" s="17"/>
+    </row>
+    <row r="138" spans="1:22">
       <c r="A138" t="s">
         <v>150</v>
       </c>
-      <c r="U138" s="17"/>
-    </row>
-    <row r="139" spans="1:21">
+      <c r="V138" s="17"/>
+    </row>
+    <row r="139" spans="1:22">
       <c r="A139" t="s">
         <v>151</v>
       </c>
-      <c r="U139" s="17"/>
-    </row>
-    <row r="140" spans="1:21">
+      <c r="V139" s="17"/>
+    </row>
+    <row r="140" spans="1:22">
       <c r="A140" t="s">
         <v>152</v>
       </c>
-      <c r="U140" s="17"/>
-    </row>
-    <row r="141" spans="1:21">
+      <c r="V140" s="17"/>
+    </row>
+    <row r="141" spans="1:22">
       <c r="A141" t="s">
         <v>153</v>
       </c>
-      <c r="U141" s="17"/>
-    </row>
-    <row r="142" spans="1:21">
+      <c r="V141" s="17"/>
+    </row>
+    <row r="142" spans="1:22">
       <c r="A142" t="s">
         <v>154</v>
       </c>
-      <c r="U142" s="17"/>
-    </row>
-    <row r="143" spans="1:21">
+      <c r="V142" s="17"/>
+    </row>
+    <row r="143" spans="1:22">
       <c r="A143" t="s">
         <v>155</v>
       </c>
-      <c r="U143" s="17"/>
-    </row>
-    <row r="144" spans="1:21">
+      <c r="V143" s="17"/>
+    </row>
+    <row r="144" spans="1:22">
       <c r="A144" t="s">
         <v>156</v>
       </c>
-      <c r="U144" s="17"/>
-    </row>
-    <row r="145" spans="1:21">
+      <c r="V144" s="17"/>
+    </row>
+    <row r="145" spans="1:22">
       <c r="A145" t="s">
         <v>157</v>
       </c>
-      <c r="U145" s="17"/>
-    </row>
-    <row r="146" spans="1:21">
+      <c r="V145" s="17"/>
+    </row>
+    <row r="146" spans="1:22">
       <c r="A146" t="s">
         <v>158</v>
       </c>
-      <c r="U146" s="17"/>
-    </row>
-    <row r="147" spans="1:21">
+      <c r="V146" s="17"/>
+    </row>
+    <row r="147" spans="1:22">
       <c r="A147" t="s">
         <v>159</v>
       </c>
-      <c r="U147" s="17"/>
-    </row>
-    <row r="148" spans="1:21">
+      <c r="V147" s="17"/>
+    </row>
+    <row r="148" spans="1:22">
       <c r="A148" t="s">
         <v>160</v>
       </c>
-      <c r="U148" s="17"/>
-    </row>
-    <row r="149" spans="1:21">
+      <c r="V148" s="17"/>
+    </row>
+    <row r="149" spans="1:22">
       <c r="A149" t="s">
         <v>161</v>
       </c>
-      <c r="U149" s="17"/>
-    </row>
-    <row r="150" spans="1:21">
+      <c r="V149" s="17"/>
+    </row>
+    <row r="150" spans="1:22">
       <c r="A150" t="s">
         <v>162</v>
       </c>
-      <c r="U150" s="17"/>
-    </row>
-    <row r="151" spans="1:21">
+      <c r="V150" s="17"/>
+    </row>
+    <row r="151" spans="1:22">
       <c r="A151" t="s">
         <v>163</v>
       </c>
-      <c r="U151" s="17"/>
-    </row>
-    <row r="152" spans="1:21">
+      <c r="V151" s="17"/>
+    </row>
+    <row r="152" spans="1:22">
       <c r="A152" t="s">
         <v>164</v>
       </c>
-      <c r="U152" s="17"/>
-    </row>
-    <row r="153" spans="1:21">
+      <c r="V152" s="17"/>
+    </row>
+    <row r="153" spans="1:22">
       <c r="A153" t="s">
         <v>165</v>
       </c>
-      <c r="U153" s="17"/>
-    </row>
-    <row r="154" spans="1:21">
+      <c r="V153" s="17"/>
+    </row>
+    <row r="154" spans="1:22">
       <c r="A154" t="s">
         <v>166</v>
       </c>
-      <c r="U154" s="17"/>
-    </row>
-    <row r="155" spans="1:21">
+      <c r="V154" s="17"/>
+    </row>
+    <row r="155" spans="1:22">
       <c r="A155" t="s">
         <v>167</v>
       </c>
-      <c r="U155" s="17"/>
-    </row>
-    <row r="156" spans="1:21">
+      <c r="V155" s="17"/>
+    </row>
+    <row r="156" spans="1:22">
       <c r="A156" t="s">
         <v>168</v>
       </c>
-      <c r="U156" s="17"/>
-    </row>
-    <row r="157" spans="1:21">
+      <c r="V156" s="17"/>
+    </row>
+    <row r="157" spans="1:22">
       <c r="A157" t="s">
         <v>169</v>
       </c>
-      <c r="U157" s="17"/>
-    </row>
-    <row r="158" spans="1:21">
+      <c r="V157" s="17"/>
+    </row>
+    <row r="158" spans="1:22">
       <c r="A158" t="s">
         <v>170</v>
       </c>
-      <c r="U158" s="17"/>
-    </row>
-    <row r="159" spans="1:21">
-      <c r="U159" s="17"/>
-    </row>
-    <row r="160" spans="1:21">
-      <c r="U160" s="17"/>
-    </row>
-    <row r="161" spans="1:21">
-      <c r="U161" s="17"/>
-    </row>
-    <row r="162" spans="1:21">
-      <c r="U162" s="17"/>
-    </row>
-    <row r="163" spans="1:21">
-      <c r="U163" s="17"/>
-    </row>
-    <row r="164" spans="1:21">
-      <c r="U164" s="17"/>
-    </row>
-    <row r="165" spans="1:21">
+      <c r="V158" s="17"/>
+    </row>
+    <row r="159" spans="1:22">
+      <c r="V159" s="17"/>
+    </row>
+    <row r="160" spans="1:22">
+      <c r="V160" s="17"/>
+    </row>
+    <row r="161" spans="1:22">
+      <c r="V161" s="17"/>
+    </row>
+    <row r="162" spans="1:22">
+      <c r="V162" s="17"/>
+    </row>
+    <row r="163" spans="1:22">
+      <c r="V163" s="17"/>
+    </row>
+    <row r="164" spans="1:22">
+      <c r="V164" s="17"/>
+    </row>
+    <row r="165" spans="1:22">
       <c r="A165" t="s">
         <v>95</v>
       </c>
-      <c r="U165" s="17"/>
-    </row>
-    <row r="166" spans="1:21">
+      <c r="V165" s="17"/>
+    </row>
+    <row r="166" spans="1:22">
       <c r="A166" t="s">
         <v>96</v>
       </c>
-      <c r="U166" s="17"/>
-    </row>
-    <row r="167" spans="1:21">
+      <c r="V166" s="17"/>
+    </row>
+    <row r="167" spans="1:22">
       <c r="A167" t="s">
         <v>97</v>
       </c>
-      <c r="U167" s="17"/>
-    </row>
-    <row r="168" spans="1:21">
+      <c r="V167" s="17"/>
+    </row>
+    <row r="168" spans="1:22">
       <c r="A168" t="s">
         <v>98</v>
       </c>
-      <c r="U168" s="17"/>
-    </row>
-    <row r="169" spans="1:21">
+      <c r="V168" s="17"/>
+    </row>
+    <row r="169" spans="1:22">
       <c r="A169" t="s">
         <v>99</v>
       </c>
-      <c r="U169" s="17"/>
-    </row>
-    <row r="170" spans="1:21">
+      <c r="V169" s="17"/>
+    </row>
+    <row r="170" spans="1:22">
       <c r="A170" t="s">
         <v>100</v>
       </c>
-      <c r="U170" s="17"/>
-    </row>
-    <row r="171" spans="1:21">
+      <c r="V170" s="17"/>
+    </row>
+    <row r="171" spans="1:22">
       <c r="A171" t="s">
         <v>101</v>
       </c>
-      <c r="U171" s="17"/>
-    </row>
-    <row r="172" spans="1:21">
+      <c r="V171" s="17"/>
+    </row>
+    <row r="172" spans="1:22">
       <c r="A172" t="s">
         <v>102</v>
       </c>
-      <c r="U172" s="17"/>
-    </row>
-    <row r="173" spans="1:21">
+      <c r="V172" s="17"/>
+    </row>
+    <row r="173" spans="1:22">
       <c r="A173" t="s">
         <v>103</v>
       </c>
-      <c r="U173" s="17"/>
-    </row>
-    <row r="174" spans="1:21">
+      <c r="V173" s="17"/>
+    </row>
+    <row r="174" spans="1:22">
       <c r="A174" t="s">
         <v>104</v>
       </c>
-      <c r="U174" s="17"/>
-    </row>
-    <row r="175" spans="1:21">
+      <c r="V174" s="17"/>
+    </row>
+    <row r="175" spans="1:22">
       <c r="A175" t="s">
         <v>105</v>
       </c>
-      <c r="U175" s="17"/>
-    </row>
-    <row r="176" spans="1:21">
+      <c r="V175" s="17"/>
+    </row>
+    <row r="176" spans="1:22">
       <c r="A176" t="s">
         <v>106</v>
       </c>
-      <c r="U176" s="17"/>
-    </row>
-    <row r="177" spans="1:21">
+      <c r="V176" s="17"/>
+    </row>
+    <row r="177" spans="1:22">
       <c r="A177" t="s">
         <v>107</v>
       </c>
-      <c r="U177" s="17"/>
-    </row>
-    <row r="178" spans="1:21">
+      <c r="V177" s="17"/>
+    </row>
+    <row r="178" spans="1:22">
       <c r="A178" t="s">
         <v>108</v>
       </c>
-      <c r="U178" s="17"/>
-    </row>
-    <row r="179" spans="1:21">
+      <c r="V178" s="17"/>
+    </row>
+    <row r="179" spans="1:22">
       <c r="A179" t="s">
         <v>109</v>
       </c>
-      <c r="U179" s="17"/>
-    </row>
-    <row r="180" spans="1:21">
+      <c r="V179" s="17"/>
+    </row>
+    <row r="180" spans="1:22">
       <c r="A180" t="s">
         <v>110</v>
       </c>
-      <c r="U180" s="17"/>
-    </row>
-    <row r="181" spans="1:21">
+      <c r="V180" s="17"/>
+    </row>
+    <row r="181" spans="1:22">
       <c r="A181" t="s">
         <v>111</v>
       </c>
-      <c r="U181" s="17"/>
-    </row>
-    <row r="182" spans="1:21">
+      <c r="V181" s="17"/>
+    </row>
+    <row r="182" spans="1:22">
       <c r="A182" t="s">
         <v>112</v>
       </c>
-      <c r="U182" s="17"/>
-    </row>
-    <row r="183" spans="1:21">
+      <c r="V182" s="17"/>
+    </row>
+    <row r="183" spans="1:22">
       <c r="A183" t="s">
         <v>113</v>
       </c>
-      <c r="U183" s="17"/>
-    </row>
-    <row r="184" spans="1:21">
+      <c r="V183" s="17"/>
+    </row>
+    <row r="184" spans="1:22">
       <c r="A184" t="s">
         <v>114</v>
       </c>
-      <c r="U184" s="17"/>
-    </row>
-    <row r="185" spans="1:21">
+      <c r="V184" s="17"/>
+    </row>
+    <row r="185" spans="1:22">
       <c r="A185" t="s">
         <v>115</v>
       </c>
-      <c r="U185" s="17"/>
-    </row>
-    <row r="186" spans="1:21">
+      <c r="V185" s="17"/>
+    </row>
+    <row r="186" spans="1:22">
       <c r="A186" t="s">
         <v>116</v>
       </c>
-      <c r="O186" s="22"/>
       <c r="P186" s="22"/>
       <c r="Q186" s="22"/>
       <c r="R186" s="22"/>
       <c r="S186" s="22"/>
       <c r="T186" s="22"/>
-      <c r="U186" s="17"/>
-    </row>
-    <row r="187" spans="1:21">
+      <c r="U186" s="22"/>
+      <c r="V186" s="17"/>
+    </row>
+    <row r="187" spans="1:22">
       <c r="A187" t="s">
         <v>117</v>
       </c>
-      <c r="O187" s="22"/>
       <c r="P187" s="22"/>
       <c r="Q187" s="22"/>
       <c r="R187" s="22"/>
       <c r="S187" s="22"/>
       <c r="T187" s="22"/>
-      <c r="U187" s="17"/>
-    </row>
-    <row r="188" spans="1:21">
+      <c r="U187" s="22"/>
+      <c r="V187" s="17"/>
+    </row>
+    <row r="188" spans="1:22">
       <c r="A188" t="s">
         <v>118</v>
       </c>
-      <c r="O188" s="22"/>
       <c r="P188" s="22"/>
       <c r="Q188" s="22"/>
       <c r="R188" s="22"/>
       <c r="S188" s="22"/>
       <c r="T188" s="22"/>
-      <c r="U188" s="17"/>
-    </row>
-    <row r="189" spans="1:21">
+      <c r="U188" s="22"/>
+      <c r="V188" s="17"/>
+    </row>
+    <row r="189" spans="1:22">
       <c r="A189" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="190" spans="1:21">
+    <row r="190" spans="1:22">
       <c r="A190" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="191" spans="1:21">
+    <row r="191" spans="1:22">
       <c r="A191" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="192" spans="1:21">
+    <row r="192" spans="1:22">
       <c r="A192" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="193" spans="1:14">
+    <row r="193" spans="1:15">
       <c r="A193" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="194" spans="1:14">
+    <row r="194" spans="1:15">
       <c r="A194" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="195" spans="1:14">
+    <row r="195" spans="1:15">
       <c r="A195" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="196" spans="1:14">
+    <row r="196" spans="1:15">
       <c r="A196" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="197" spans="1:14">
+    <row r="197" spans="1:15">
       <c r="A197" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="198" spans="1:14">
+    <row r="198" spans="1:15">
       <c r="A198" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="199" spans="1:14">
+    <row r="199" spans="1:15">
       <c r="A199" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="200" spans="1:14">
+    <row r="200" spans="1:15">
       <c r="A200" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="201" spans="1:14">
+    <row r="201" spans="1:15">
       <c r="A201" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="202" spans="1:14">
+    <row r="202" spans="1:15">
       <c r="A202" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="203" spans="1:14">
+    <row r="203" spans="1:15">
       <c r="A203" s="17"/>
       <c r="B203" s="17"/>
       <c r="C203" s="17"/>
@@ -7789,8 +7852,9 @@
       <c r="L203" s="17"/>
       <c r="M203" s="17"/>
       <c r="N203" s="17"/>
-    </row>
-    <row r="204" spans="1:14">
+      <c r="O203" s="17"/>
+    </row>
+    <row r="204" spans="1:15">
       <c r="A204" s="17"/>
       <c r="B204" s="17"/>
       <c r="C204" s="17"/>
@@ -7805,8 +7869,9 @@
       <c r="L204" s="17"/>
       <c r="M204" s="17"/>
       <c r="N204" s="17"/>
-    </row>
-    <row r="205" spans="1:14">
+      <c r="O204" s="17"/>
+    </row>
+    <row r="205" spans="1:15">
       <c r="A205" s="17"/>
       <c r="B205" s="17"/>
       <c r="C205" s="17"/>
@@ -7821,8 +7886,9 @@
       <c r="L205" s="17"/>
       <c r="M205" s="17"/>
       <c r="N205" s="17"/>
-    </row>
-    <row r="206" spans="1:14">
+      <c r="O205" s="17"/>
+    </row>
+    <row r="206" spans="1:15">
       <c r="A206" s="17"/>
       <c r="B206" s="17"/>
       <c r="C206" s="17"/>
@@ -7837,8 +7903,9 @@
       <c r="L206" s="17"/>
       <c r="M206" s="17"/>
       <c r="N206" s="17"/>
-    </row>
-    <row r="207" spans="1:14">
+      <c r="O206" s="17"/>
+    </row>
+    <row r="207" spans="1:15">
       <c r="A207" s="17"/>
       <c r="B207" s="17"/>
       <c r="C207" s="17"/>
@@ -7853,8 +7920,9 @@
       <c r="L207" s="17"/>
       <c r="M207" s="17"/>
       <c r="N207" s="17"/>
-    </row>
-    <row r="208" spans="1:14">
+      <c r="O207" s="17"/>
+    </row>
+    <row r="208" spans="1:15">
       <c r="A208" s="17"/>
       <c r="B208" s="17"/>
       <c r="C208" s="17"/>
@@ -7869,6 +7937,7 @@
       <c r="L208" s="17"/>
       <c r="M208" s="17"/>
       <c r="N208" s="17"/>
+      <c r="O208" s="17"/>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
@@ -8025,27 +8094,27 @@
         <v>273</v>
       </c>
     </row>
-    <row r="241" spans="1:14">
+    <row r="241" spans="1:15">
       <c r="A241" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="242" spans="1:14">
+    <row r="242" spans="1:15">
       <c r="A242" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="243" spans="1:14">
+    <row r="243" spans="1:15">
       <c r="A243" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="244" spans="1:14">
+    <row r="244" spans="1:15">
       <c r="A244" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="253" spans="1:14">
+    <row r="253" spans="1:15">
       <c r="A253" s="15" t="s">
         <v>283</v>
       </c>
@@ -8062,18 +8131,19 @@
       <c r="L253" s="15"/>
       <c r="M253" s="15"/>
       <c r="N253" s="15"/>
-    </row>
-    <row r="254" spans="1:14">
+      <c r="O253" s="15"/>
+    </row>
+    <row r="254" spans="1:15">
       <c r="A254" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="255" spans="1:14">
+    <row r="255" spans="1:15">
       <c r="A255" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="256" spans="1:14">
+    <row r="256" spans="1:15">
       <c r="A256" t="s">
         <v>59</v>
       </c>
@@ -11918,181 +11988,181 @@
         <v>904</v>
       </c>
     </row>
-    <row r="1025" spans="1:21">
+    <row r="1025" spans="1:22">
       <c r="A1025" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="1026" spans="1:21">
+    <row r="1026" spans="1:22">
       <c r="A1026" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="1027" spans="1:21">
+    <row r="1027" spans="1:22">
       <c r="A1027" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="1028" spans="1:21">
+    <row r="1028" spans="1:22">
       <c r="A1028" t="s">
         <v>908</v>
       </c>
-      <c r="U1028" s="17"/>
-    </row>
-    <row r="1029" spans="1:21">
+      <c r="V1028" s="17"/>
+    </row>
+    <row r="1029" spans="1:22">
       <c r="A1029" t="s">
         <v>909</v>
       </c>
-      <c r="U1029" s="17"/>
-    </row>
-    <row r="1030" spans="1:21">
+      <c r="V1029" s="17"/>
+    </row>
+    <row r="1030" spans="1:22">
       <c r="A1030" t="s">
         <v>910</v>
       </c>
-      <c r="U1030" s="17"/>
-    </row>
-    <row r="1031" spans="1:21">
+      <c r="V1030" s="17"/>
+    </row>
+    <row r="1031" spans="1:22">
       <c r="A1031" t="s">
         <v>911</v>
       </c>
-      <c r="U1031" s="17"/>
-    </row>
-    <row r="1032" spans="1:21">
+      <c r="V1031" s="17"/>
+    </row>
+    <row r="1032" spans="1:22">
       <c r="A1032" t="s">
         <v>912</v>
       </c>
-      <c r="U1032" s="17"/>
-    </row>
-    <row r="1033" spans="1:21">
+      <c r="V1032" s="17"/>
+    </row>
+    <row r="1033" spans="1:22">
       <c r="A1033" t="s">
         <v>913</v>
       </c>
-      <c r="U1033" s="17"/>
-    </row>
-    <row r="1034" spans="1:21">
+      <c r="V1033" s="17"/>
+    </row>
+    <row r="1034" spans="1:22">
       <c r="A1034" t="s">
         <v>914</v>
       </c>
-      <c r="U1034" s="17"/>
-    </row>
-    <row r="1035" spans="1:21">
+      <c r="V1034" s="17"/>
+    </row>
+    <row r="1035" spans="1:22">
       <c r="A1035" t="s">
         <v>915</v>
       </c>
-      <c r="U1035" s="17"/>
-    </row>
-    <row r="1036" spans="1:21">
+      <c r="V1035" s="17"/>
+    </row>
+    <row r="1036" spans="1:22">
       <c r="A1036" t="s">
         <v>916</v>
       </c>
-      <c r="U1036" s="17"/>
-    </row>
-    <row r="1037" spans="1:21">
+      <c r="V1036" s="17"/>
+    </row>
+    <row r="1037" spans="1:22">
       <c r="A1037" t="s">
         <v>917</v>
       </c>
-      <c r="U1037" s="17"/>
-    </row>
-    <row r="1038" spans="1:21">
+      <c r="V1037" s="17"/>
+    </row>
+    <row r="1038" spans="1:22">
       <c r="A1038" t="s">
         <v>918</v>
       </c>
-      <c r="U1038" s="17"/>
-    </row>
-    <row r="1039" spans="1:21">
+      <c r="V1038" s="17"/>
+    </row>
+    <row r="1039" spans="1:22">
       <c r="A1039" t="s">
         <v>919</v>
       </c>
-      <c r="U1039" s="17"/>
-    </row>
-    <row r="1040" spans="1:21">
+      <c r="V1039" s="17"/>
+    </row>
+    <row r="1040" spans="1:22">
       <c r="A1040" t="s">
         <v>920</v>
       </c>
-      <c r="U1040" s="17"/>
-    </row>
-    <row r="1041" spans="1:21">
+      <c r="V1040" s="17"/>
+    </row>
+    <row r="1041" spans="1:22">
       <c r="A1041" t="s">
         <v>921</v>
       </c>
-      <c r="U1041" s="17"/>
-    </row>
-    <row r="1042" spans="1:21">
+      <c r="V1041" s="17"/>
+    </row>
+    <row r="1042" spans="1:22">
       <c r="A1042" t="s">
         <v>922</v>
       </c>
-      <c r="U1042" s="17"/>
-    </row>
-    <row r="1043" spans="1:21">
+      <c r="V1042" s="17"/>
+    </row>
+    <row r="1043" spans="1:22">
       <c r="A1043" t="s">
         <v>923</v>
       </c>
-      <c r="U1043" s="17"/>
-    </row>
-    <row r="1044" spans="1:21">
+      <c r="V1043" s="17"/>
+    </row>
+    <row r="1044" spans="1:22">
       <c r="A1044" t="s">
         <v>924</v>
       </c>
-      <c r="U1044" s="17"/>
-    </row>
-    <row r="1045" spans="1:21">
+      <c r="V1044" s="17"/>
+    </row>
+    <row r="1045" spans="1:22">
       <c r="A1045" t="s">
         <v>925</v>
       </c>
-      <c r="U1045" s="17"/>
-    </row>
-    <row r="1046" spans="1:21">
+      <c r="V1045" s="17"/>
+    </row>
+    <row r="1046" spans="1:22">
       <c r="A1046" t="s">
         <v>926</v>
       </c>
-      <c r="U1046" s="17"/>
-    </row>
-    <row r="1047" spans="1:21">
+      <c r="V1046" s="17"/>
+    </row>
+    <row r="1047" spans="1:22">
       <c r="A1047" t="s">
         <v>927</v>
       </c>
-      <c r="U1047" s="17"/>
-    </row>
-    <row r="1048" spans="1:21">
+      <c r="V1047" s="17"/>
+    </row>
+    <row r="1048" spans="1:22">
       <c r="A1048" t="s">
         <v>928</v>
       </c>
-      <c r="U1048" s="17"/>
-    </row>
-    <row r="1049" spans="1:21">
+      <c r="V1048" s="17"/>
+    </row>
+    <row r="1049" spans="1:22">
       <c r="A1049" t="s">
         <v>929</v>
       </c>
-      <c r="U1049" s="17"/>
-    </row>
-    <row r="1050" spans="1:21">
+      <c r="V1049" s="17"/>
+    </row>
+    <row r="1050" spans="1:22">
       <c r="A1050" t="s">
         <v>930</v>
       </c>
-      <c r="U1050" s="17"/>
-    </row>
-    <row r="1051" spans="1:21">
+      <c r="V1050" s="17"/>
+    </row>
+    <row r="1051" spans="1:22">
       <c r="A1051" t="s">
         <v>931</v>
       </c>
-      <c r="U1051" s="17"/>
-    </row>
-    <row r="1052" spans="1:21">
+      <c r="V1051" s="17"/>
+    </row>
+    <row r="1052" spans="1:22">
       <c r="A1052" t="s">
         <v>932</v>
       </c>
-      <c r="U1052" s="17"/>
-    </row>
-    <row r="1053" spans="1:21">
+      <c r="V1052" s="17"/>
+    </row>
+    <row r="1053" spans="1:22">
       <c r="A1053" t="s">
         <v>933</v>
       </c>
-      <c r="U1053" s="17"/>
-    </row>
-    <row r="1054" spans="1:21">
-      <c r="U1054" s="17"/>
-    </row>
-    <row r="1055" spans="1:21">
+      <c r="V1053" s="17"/>
+    </row>
+    <row r="1054" spans="1:22">
+      <c r="V1054" s="17"/>
+    </row>
+    <row r="1055" spans="1:22">
       <c r="A1055" s="17" t="s">
         <v>243</v>
       </c>
@@ -12109,9 +12179,10 @@
       <c r="L1055" s="17"/>
       <c r="M1055" s="17"/>
       <c r="N1055" s="17"/>
-      <c r="U1055" s="17"/>
-    </row>
-    <row r="1056" spans="1:21">
+      <c r="O1055" s="17"/>
+      <c r="V1055" s="17"/>
+    </row>
+    <row r="1056" spans="1:22">
       <c r="A1056" s="17" t="s">
         <v>244</v>
       </c>
@@ -12128,9 +12199,10 @@
       <c r="L1056" s="17"/>
       <c r="M1056" s="17"/>
       <c r="N1056" s="17"/>
-      <c r="U1056" s="17"/>
-    </row>
-    <row r="1057" spans="1:21">
+      <c r="O1056" s="17"/>
+      <c r="V1056" s="17"/>
+    </row>
+    <row r="1057" spans="1:22">
       <c r="A1057" s="17" t="s">
         <v>245</v>
       </c>
@@ -12147,9 +12219,10 @@
       <c r="L1057" s="17"/>
       <c r="M1057" s="17"/>
       <c r="N1057" s="17"/>
-      <c r="U1057" s="17"/>
-    </row>
-    <row r="1058" spans="1:21">
+      <c r="O1057" s="17"/>
+      <c r="V1057" s="17"/>
+    </row>
+    <row r="1058" spans="1:22">
       <c r="A1058" s="17" t="s">
         <v>246</v>
       </c>
@@ -12166,9 +12239,10 @@
       <c r="L1058" s="17"/>
       <c r="M1058" s="17"/>
       <c r="N1058" s="17"/>
-      <c r="U1058" s="17"/>
-    </row>
-    <row r="1059" spans="1:21">
+      <c r="O1058" s="17"/>
+      <c r="V1058" s="17"/>
+    </row>
+    <row r="1059" spans="1:22">
       <c r="A1059" s="17" t="s">
         <v>247</v>
       </c>
@@ -12185,9 +12259,10 @@
       <c r="L1059" s="17"/>
       <c r="M1059" s="17"/>
       <c r="N1059" s="17"/>
-      <c r="U1059" s="17"/>
-    </row>
-    <row r="1060" spans="1:21">
+      <c r="O1059" s="17"/>
+      <c r="V1059" s="17"/>
+    </row>
+    <row r="1060" spans="1:22">
       <c r="A1060" s="17" t="s">
         <v>248</v>
       </c>
@@ -12204,9 +12279,10 @@
       <c r="L1060" s="17"/>
       <c r="M1060" s="17"/>
       <c r="N1060" s="17"/>
-      <c r="U1060" s="17"/>
-    </row>
-    <row r="1061" spans="1:21">
+      <c r="O1060" s="17"/>
+      <c r="V1060" s="17"/>
+    </row>
+    <row r="1061" spans="1:22">
       <c r="A1061" s="17" t="s">
         <v>249</v>
       </c>
@@ -12223,9 +12299,10 @@
       <c r="L1061" s="17"/>
       <c r="M1061" s="17"/>
       <c r="N1061" s="17"/>
-      <c r="U1061" s="17"/>
-    </row>
-    <row r="1062" spans="1:21">
+      <c r="O1061" s="17"/>
+      <c r="V1061" s="17"/>
+    </row>
+    <row r="1062" spans="1:22">
       <c r="A1062" s="17" t="s">
         <v>250</v>
       </c>
@@ -12242,9 +12319,10 @@
       <c r="L1062" s="17"/>
       <c r="M1062" s="17"/>
       <c r="N1062" s="17"/>
-      <c r="U1062" s="17"/>
-    </row>
-    <row r="1063" spans="1:21">
+      <c r="O1062" s="17"/>
+      <c r="V1062" s="17"/>
+    </row>
+    <row r="1063" spans="1:22">
       <c r="A1063" s="17" t="s">
         <v>251</v>
       </c>
@@ -12261,9 +12339,10 @@
       <c r="L1063" s="17"/>
       <c r="M1063" s="17"/>
       <c r="N1063" s="17"/>
-      <c r="U1063" s="17"/>
-    </row>
-    <row r="1064" spans="1:21">
+      <c r="O1063" s="17"/>
+      <c r="V1063" s="17"/>
+    </row>
+    <row r="1064" spans="1:22">
       <c r="A1064" s="17" t="s">
         <v>252</v>
       </c>
@@ -12280,9 +12359,10 @@
       <c r="L1064" s="17"/>
       <c r="M1064" s="17"/>
       <c r="N1064" s="17"/>
-      <c r="U1064" s="17"/>
-    </row>
-    <row r="1065" spans="1:21">
+      <c r="O1064" s="17"/>
+      <c r="V1064" s="17"/>
+    </row>
+    <row r="1065" spans="1:22">
       <c r="A1065" s="17" t="s">
         <v>253</v>
       </c>
@@ -12299,9 +12379,10 @@
       <c r="L1065" s="17"/>
       <c r="M1065" s="17"/>
       <c r="N1065" s="17"/>
-      <c r="U1065" s="17"/>
-    </row>
-    <row r="1066" spans="1:21">
+      <c r="O1065" s="17"/>
+      <c r="V1065" s="17"/>
+    </row>
+    <row r="1066" spans="1:22">
       <c r="A1066" s="17" t="s">
         <v>254</v>
       </c>
@@ -12318,9 +12399,10 @@
       <c r="L1066" s="17"/>
       <c r="M1066" s="17"/>
       <c r="N1066" s="17"/>
-      <c r="U1066" s="17"/>
-    </row>
-    <row r="1067" spans="1:21">
+      <c r="O1066" s="17"/>
+      <c r="V1066" s="17"/>
+    </row>
+    <row r="1067" spans="1:22">
       <c r="A1067" s="17" t="s">
         <v>255</v>
       </c>
@@ -12337,9 +12419,10 @@
       <c r="L1067" s="17"/>
       <c r="M1067" s="17"/>
       <c r="N1067" s="17"/>
-      <c r="U1067" s="17"/>
-    </row>
-    <row r="1068" spans="1:21">
+      <c r="O1067" s="17"/>
+      <c r="V1067" s="17"/>
+    </row>
+    <row r="1068" spans="1:22">
       <c r="A1068" s="17" t="s">
         <v>256</v>
       </c>
@@ -12356,14 +12439,15 @@
       <c r="L1068" s="17"/>
       <c r="M1068" s="17"/>
       <c r="N1068" s="17"/>
-      <c r="O1068"/>
+      <c r="O1068" s="17"/>
       <c r="P1068"/>
       <c r="Q1068"/>
       <c r="R1068"/>
       <c r="S1068"/>
       <c r="T1068"/>
-    </row>
-    <row r="1069" spans="1:21">
+      <c r="U1068"/>
+    </row>
+    <row r="1069" spans="1:22">
       <c r="A1069" s="17" t="s">
         <v>257</v>
       </c>
@@ -12380,14 +12464,15 @@
       <c r="L1069" s="17"/>
       <c r="M1069" s="17"/>
       <c r="N1069" s="17"/>
-      <c r="O1069"/>
+      <c r="O1069" s="17"/>
       <c r="P1069"/>
       <c r="Q1069"/>
       <c r="R1069"/>
       <c r="S1069"/>
       <c r="T1069"/>
-    </row>
-    <row r="1070" spans="1:21">
+      <c r="U1069"/>
+    </row>
+    <row r="1070" spans="1:22">
       <c r="A1070" s="17" t="s">
         <v>258</v>
       </c>
@@ -12404,14 +12489,15 @@
       <c r="L1070" s="17"/>
       <c r="M1070" s="17"/>
       <c r="N1070" s="17"/>
-      <c r="O1070"/>
+      <c r="O1070" s="17"/>
       <c r="P1070"/>
       <c r="Q1070"/>
       <c r="R1070"/>
       <c r="S1070"/>
       <c r="T1070"/>
-    </row>
-    <row r="1071" spans="1:21">
+      <c r="U1070"/>
+    </row>
+    <row r="1071" spans="1:22">
       <c r="A1071" s="17" t="s">
         <v>259</v>
       </c>
@@ -12428,14 +12514,15 @@
       <c r="L1071" s="17"/>
       <c r="M1071" s="17"/>
       <c r="N1071" s="17"/>
-      <c r="O1071"/>
+      <c r="O1071" s="17"/>
       <c r="P1071"/>
       <c r="Q1071"/>
       <c r="R1071"/>
       <c r="S1071"/>
       <c r="T1071"/>
-    </row>
-    <row r="1072" spans="1:21">
+      <c r="U1071"/>
+    </row>
+    <row r="1072" spans="1:22">
       <c r="A1072" s="17" t="s">
         <v>260</v>
       </c>
@@ -12452,14 +12539,15 @@
       <c r="L1072" s="17"/>
       <c r="M1072" s="17"/>
       <c r="N1072" s="17"/>
-      <c r="O1072"/>
+      <c r="O1072" s="17"/>
       <c r="P1072"/>
       <c r="Q1072"/>
       <c r="R1072"/>
       <c r="S1072"/>
       <c r="T1072"/>
-    </row>
-    <row r="1073" spans="1:20">
+      <c r="U1072"/>
+    </row>
+    <row r="1073" spans="1:21">
       <c r="A1073" s="17" t="s">
         <v>261</v>
       </c>
@@ -12476,14 +12564,15 @@
       <c r="L1073" s="17"/>
       <c r="M1073" s="17"/>
       <c r="N1073" s="17"/>
-      <c r="O1073"/>
+      <c r="O1073" s="17"/>
       <c r="P1073"/>
       <c r="Q1073"/>
       <c r="R1073"/>
       <c r="S1073"/>
       <c r="T1073"/>
-    </row>
-    <row r="1074" spans="1:20">
+      <c r="U1073"/>
+    </row>
+    <row r="1074" spans="1:21">
       <c r="A1074" s="17" t="s">
         <v>262</v>
       </c>
@@ -12500,14 +12589,15 @@
       <c r="L1074" s="17"/>
       <c r="M1074" s="17"/>
       <c r="N1074" s="17"/>
-      <c r="O1074"/>
+      <c r="O1074" s="17"/>
       <c r="P1074"/>
       <c r="Q1074"/>
       <c r="R1074"/>
       <c r="S1074"/>
       <c r="T1074"/>
-    </row>
-    <row r="1075" spans="1:20">
+      <c r="U1074"/>
+    </row>
+    <row r="1075" spans="1:21">
       <c r="A1075" s="17" t="s">
         <v>263</v>
       </c>
@@ -12524,14 +12614,15 @@
       <c r="L1075" s="17"/>
       <c r="M1075" s="17"/>
       <c r="N1075" s="17"/>
-      <c r="O1075"/>
+      <c r="O1075" s="17"/>
       <c r="P1075"/>
       <c r="Q1075"/>
       <c r="R1075"/>
       <c r="S1075"/>
       <c r="T1075"/>
-    </row>
-    <row r="1076" spans="1:20">
+      <c r="U1075"/>
+    </row>
+    <row r="1076" spans="1:21">
       <c r="A1076" s="17" t="s">
         <v>264</v>
       </c>
@@ -12548,14 +12639,15 @@
       <c r="L1076" s="17"/>
       <c r="M1076" s="17"/>
       <c r="N1076" s="17"/>
-      <c r="O1076"/>
+      <c r="O1076" s="17"/>
       <c r="P1076"/>
       <c r="Q1076"/>
       <c r="R1076"/>
       <c r="S1076"/>
       <c r="T1076"/>
-    </row>
-    <row r="1077" spans="1:20">
+      <c r="U1076"/>
+    </row>
+    <row r="1077" spans="1:21">
       <c r="A1077" s="17" t="s">
         <v>265</v>
       </c>
@@ -12572,14 +12664,15 @@
       <c r="L1077" s="17"/>
       <c r="M1077" s="17"/>
       <c r="N1077" s="17"/>
-      <c r="O1077"/>
+      <c r="O1077" s="17"/>
       <c r="P1077"/>
       <c r="Q1077"/>
       <c r="R1077"/>
       <c r="S1077"/>
       <c r="T1077"/>
-    </row>
-    <row r="1078" spans="1:20">
+      <c r="U1077"/>
+    </row>
+    <row r="1078" spans="1:21">
       <c r="A1078" s="17" t="s">
         <v>266</v>
       </c>
@@ -12596,14 +12689,15 @@
       <c r="L1078" s="17"/>
       <c r="M1078" s="17"/>
       <c r="N1078" s="17"/>
-      <c r="O1078"/>
+      <c r="O1078" s="17"/>
       <c r="P1078"/>
       <c r="Q1078"/>
       <c r="R1078"/>
       <c r="S1078"/>
       <c r="T1078"/>
-    </row>
-    <row r="1079" spans="1:20">
+      <c r="U1078"/>
+    </row>
+    <row r="1079" spans="1:21">
       <c r="A1079" s="17" t="s">
         <v>267</v>
       </c>
@@ -12620,14 +12714,15 @@
       <c r="L1079" s="17"/>
       <c r="M1079" s="17"/>
       <c r="N1079" s="17"/>
-      <c r="O1079"/>
+      <c r="O1079" s="17"/>
       <c r="P1079"/>
       <c r="Q1079"/>
       <c r="R1079"/>
       <c r="S1079"/>
       <c r="T1079"/>
-    </row>
-    <row r="1080" spans="1:20">
+      <c r="U1079"/>
+    </row>
+    <row r="1080" spans="1:21">
       <c r="A1080" s="17" t="s">
         <v>268</v>
       </c>
@@ -12644,14 +12739,15 @@
       <c r="L1080" s="17"/>
       <c r="M1080" s="17"/>
       <c r="N1080" s="17"/>
-      <c r="O1080"/>
+      <c r="O1080" s="17"/>
       <c r="P1080"/>
       <c r="Q1080"/>
       <c r="R1080"/>
       <c r="S1080"/>
       <c r="T1080"/>
-    </row>
-    <row r="1081" spans="1:20">
+      <c r="U1080"/>
+    </row>
+    <row r="1081" spans="1:21">
       <c r="A1081" s="17" t="s">
         <v>269</v>
       </c>
@@ -12668,14 +12764,15 @@
       <c r="L1081" s="17"/>
       <c r="M1081" s="17"/>
       <c r="N1081" s="17"/>
-      <c r="O1081"/>
+      <c r="O1081" s="17"/>
       <c r="P1081"/>
       <c r="Q1081"/>
       <c r="R1081"/>
       <c r="S1081"/>
       <c r="T1081"/>
-    </row>
-    <row r="1082" spans="1:20">
+      <c r="U1081"/>
+    </row>
+    <row r="1082" spans="1:21">
       <c r="A1082" s="17" t="s">
         <v>270</v>
       </c>
@@ -12692,14 +12789,15 @@
       <c r="L1082" s="17"/>
       <c r="M1082" s="17"/>
       <c r="N1082" s="17"/>
-      <c r="O1082"/>
+      <c r="O1082" s="17"/>
       <c r="P1082"/>
       <c r="Q1082"/>
       <c r="R1082"/>
       <c r="S1082"/>
       <c r="T1082"/>
-    </row>
-    <row r="1083" spans="1:20">
+      <c r="U1082"/>
+    </row>
+    <row r="1083" spans="1:21">
       <c r="A1083" s="17" t="s">
         <v>271</v>
       </c>
@@ -12716,14 +12814,15 @@
       <c r="L1083" s="17"/>
       <c r="M1083" s="17"/>
       <c r="N1083" s="17"/>
-      <c r="O1083"/>
+      <c r="O1083" s="17"/>
       <c r="P1083"/>
       <c r="Q1083"/>
       <c r="R1083"/>
       <c r="S1083"/>
       <c r="T1083"/>
-    </row>
-    <row r="1084" spans="1:20">
+      <c r="U1083"/>
+    </row>
+    <row r="1084" spans="1:21">
       <c r="A1084" s="17" t="s">
         <v>272</v>
       </c>
@@ -12740,14 +12839,15 @@
       <c r="L1084" s="17"/>
       <c r="M1084" s="17"/>
       <c r="N1084" s="17"/>
-      <c r="O1084"/>
+      <c r="O1084" s="17"/>
       <c r="P1084"/>
       <c r="Q1084"/>
       <c r="R1084"/>
       <c r="S1084"/>
       <c r="T1084"/>
-    </row>
-    <row r="1085" spans="1:20">
+      <c r="U1084"/>
+    </row>
+    <row r="1085" spans="1:21">
       <c r="A1085" s="17" t="s">
         <v>273</v>
       </c>
@@ -12764,14 +12864,15 @@
       <c r="L1085" s="17"/>
       <c r="M1085" s="17"/>
       <c r="N1085" s="17"/>
-      <c r="O1085"/>
+      <c r="O1085" s="17"/>
       <c r="P1085"/>
       <c r="Q1085"/>
       <c r="R1085"/>
       <c r="S1085"/>
       <c r="T1085"/>
-    </row>
-    <row r="1086" spans="1:20">
+      <c r="U1085"/>
+    </row>
+    <row r="1086" spans="1:21">
       <c r="A1086" s="17" t="s">
         <v>274</v>
       </c>
@@ -12788,14 +12889,15 @@
       <c r="L1086" s="17"/>
       <c r="M1086" s="17"/>
       <c r="N1086" s="17"/>
-      <c r="O1086"/>
+      <c r="O1086" s="17"/>
       <c r="P1086"/>
       <c r="Q1086"/>
       <c r="R1086"/>
       <c r="S1086"/>
       <c r="T1086"/>
-    </row>
-    <row r="1087" spans="1:20">
+      <c r="U1086"/>
+    </row>
+    <row r="1087" spans="1:21">
       <c r="A1087" s="17" t="s">
         <v>275</v>
       </c>
@@ -12812,14 +12914,15 @@
       <c r="L1087" s="17"/>
       <c r="M1087" s="17"/>
       <c r="N1087" s="17"/>
-      <c r="O1087"/>
+      <c r="O1087" s="17"/>
       <c r="P1087"/>
       <c r="Q1087"/>
       <c r="R1087"/>
       <c r="S1087"/>
       <c r="T1087"/>
-    </row>
-    <row r="1088" spans="1:20">
+      <c r="U1087"/>
+    </row>
+    <row r="1088" spans="1:21">
       <c r="A1088" s="17" t="s">
         <v>276</v>
       </c>
@@ -12836,14 +12939,15 @@
       <c r="L1088" s="17"/>
       <c r="M1088" s="17"/>
       <c r="N1088" s="17"/>
-      <c r="O1088"/>
+      <c r="O1088" s="17"/>
       <c r="P1088"/>
       <c r="Q1088"/>
       <c r="R1088"/>
       <c r="S1088"/>
       <c r="T1088"/>
-    </row>
-    <row r="1089" spans="1:20">
+      <c r="U1088"/>
+    </row>
+    <row r="1089" spans="1:21">
       <c r="A1089" s="17" t="s">
         <v>277</v>
       </c>
@@ -12860,14 +12964,15 @@
       <c r="L1089" s="17"/>
       <c r="M1089" s="17"/>
       <c r="N1089" s="17"/>
-      <c r="O1089"/>
+      <c r="O1089" s="17"/>
       <c r="P1089"/>
       <c r="Q1089"/>
       <c r="R1089"/>
       <c r="S1089"/>
       <c r="T1089"/>
-    </row>
-    <row r="1090" spans="1:20">
+      <c r="U1089"/>
+    </row>
+    <row r="1090" spans="1:21">
       <c r="A1090" s="17" t="s">
         <v>934</v>
       </c>
@@ -12884,14 +12989,15 @@
       <c r="L1090" s="17"/>
       <c r="M1090" s="17"/>
       <c r="N1090" s="17"/>
-      <c r="O1090"/>
+      <c r="O1090" s="17"/>
       <c r="P1090"/>
       <c r="Q1090"/>
       <c r="R1090"/>
       <c r="S1090"/>
       <c r="T1090"/>
-    </row>
-    <row r="1091" spans="1:20">
+      <c r="U1090"/>
+    </row>
+    <row r="1091" spans="1:21">
       <c r="A1091" s="17" t="s">
         <v>935</v>
       </c>
@@ -12908,14 +13014,15 @@
       <c r="L1091" s="17"/>
       <c r="M1091" s="17"/>
       <c r="N1091" s="17"/>
-      <c r="O1091"/>
+      <c r="O1091" s="17"/>
       <c r="P1091"/>
       <c r="Q1091"/>
       <c r="R1091"/>
       <c r="S1091"/>
       <c r="T1091"/>
-    </row>
-    <row r="1092" spans="1:20">
+      <c r="U1091"/>
+    </row>
+    <row r="1092" spans="1:21">
       <c r="A1092" s="17" t="s">
         <v>936</v>
       </c>
@@ -12932,14 +13039,15 @@
       <c r="L1092" s="17"/>
       <c r="M1092" s="17"/>
       <c r="N1092" s="17"/>
-      <c r="O1092"/>
+      <c r="O1092" s="17"/>
       <c r="P1092"/>
       <c r="Q1092"/>
       <c r="R1092"/>
       <c r="S1092"/>
       <c r="T1092"/>
-    </row>
-    <row r="1093" spans="1:20">
+      <c r="U1092"/>
+    </row>
+    <row r="1093" spans="1:21">
       <c r="A1093" s="17" t="s">
         <v>937</v>
       </c>
@@ -12956,14 +13064,15 @@
       <c r="L1093" s="17"/>
       <c r="M1093" s="17"/>
       <c r="N1093" s="17"/>
-      <c r="O1093"/>
+      <c r="O1093" s="17"/>
       <c r="P1093"/>
       <c r="Q1093"/>
       <c r="R1093"/>
       <c r="S1093"/>
       <c r="T1093"/>
-    </row>
-    <row r="1094" spans="1:20">
+      <c r="U1093"/>
+    </row>
+    <row r="1094" spans="1:21">
       <c r="A1094" s="17" t="s">
         <v>938</v>
       </c>
@@ -12980,572 +13089,573 @@
       <c r="L1094" s="17"/>
       <c r="M1094" s="17"/>
       <c r="N1094" s="17"/>
-      <c r="O1094"/>
+      <c r="O1094" s="17"/>
       <c r="P1094"/>
       <c r="Q1094"/>
       <c r="R1094"/>
       <c r="S1094"/>
       <c r="T1094"/>
-    </row>
-    <row r="1095" spans="1:20">
-      <c r="O1095"/>
+      <c r="U1094"/>
+    </row>
+    <row r="1095" spans="1:21">
       <c r="P1095"/>
       <c r="Q1095"/>
       <c r="R1095"/>
       <c r="S1095"/>
       <c r="T1095"/>
-    </row>
-    <row r="1096" spans="1:20">
-      <c r="O1096"/>
+      <c r="U1095"/>
+    </row>
+    <row r="1096" spans="1:21">
       <c r="P1096"/>
       <c r="Q1096"/>
       <c r="R1096"/>
       <c r="S1096"/>
       <c r="T1096"/>
-    </row>
-    <row r="1097" spans="1:20">
-      <c r="O1097"/>
+      <c r="U1096"/>
+    </row>
+    <row r="1097" spans="1:21">
       <c r="P1097"/>
       <c r="Q1097"/>
       <c r="R1097"/>
       <c r="S1097"/>
       <c r="T1097"/>
-    </row>
-    <row r="1098" spans="1:20">
-      <c r="O1098"/>
+      <c r="U1097"/>
+    </row>
+    <row r="1098" spans="1:21">
       <c r="P1098"/>
       <c r="Q1098"/>
       <c r="R1098"/>
       <c r="S1098"/>
       <c r="T1098"/>
-    </row>
-    <row r="1099" spans="1:20">
-      <c r="O1099"/>
+      <c r="U1098"/>
+    </row>
+    <row r="1099" spans="1:21">
       <c r="P1099"/>
       <c r="Q1099"/>
       <c r="R1099"/>
       <c r="S1099"/>
       <c r="T1099"/>
-    </row>
-    <row r="1100" spans="1:20">
-      <c r="O1100"/>
+      <c r="U1099"/>
+    </row>
+    <row r="1100" spans="1:21">
       <c r="P1100"/>
       <c r="Q1100"/>
       <c r="R1100"/>
       <c r="S1100"/>
       <c r="T1100"/>
-    </row>
-    <row r="1101" spans="1:20">
-      <c r="O1101"/>
+      <c r="U1100"/>
+    </row>
+    <row r="1101" spans="1:21">
       <c r="P1101"/>
       <c r="Q1101"/>
       <c r="R1101"/>
       <c r="S1101"/>
       <c r="T1101"/>
-    </row>
-    <row r="1102" spans="1:20">
-      <c r="O1102"/>
+      <c r="U1101"/>
+    </row>
+    <row r="1102" spans="1:21">
       <c r="P1102"/>
       <c r="Q1102"/>
       <c r="R1102"/>
       <c r="S1102"/>
       <c r="T1102"/>
-    </row>
-    <row r="1103" spans="1:20">
-      <c r="O1103"/>
+      <c r="U1102"/>
+    </row>
+    <row r="1103" spans="1:21">
       <c r="P1103"/>
       <c r="Q1103"/>
       <c r="R1103"/>
       <c r="S1103"/>
       <c r="T1103"/>
-    </row>
-    <row r="1104" spans="1:20">
-      <c r="O1104"/>
+      <c r="U1103"/>
+    </row>
+    <row r="1104" spans="1:21">
       <c r="P1104"/>
       <c r="Q1104"/>
       <c r="R1104"/>
       <c r="S1104"/>
       <c r="T1104"/>
-    </row>
-    <row r="1105" spans="15:20">
-      <c r="O1105"/>
+      <c r="U1104"/>
+    </row>
+    <row r="1105" spans="16:21">
       <c r="P1105"/>
       <c r="Q1105"/>
       <c r="R1105"/>
       <c r="S1105"/>
       <c r="T1105"/>
-    </row>
-    <row r="1106" spans="15:20">
-      <c r="O1106"/>
+      <c r="U1105"/>
+    </row>
+    <row r="1106" spans="16:21">
       <c r="P1106"/>
       <c r="Q1106"/>
       <c r="R1106"/>
       <c r="S1106"/>
       <c r="T1106"/>
-    </row>
-    <row r="1107" spans="15:20">
-      <c r="O1107"/>
+      <c r="U1106"/>
+    </row>
+    <row r="1107" spans="16:21">
       <c r="P1107"/>
       <c r="Q1107"/>
       <c r="R1107"/>
       <c r="S1107"/>
       <c r="T1107"/>
-    </row>
-    <row r="1108" spans="15:20">
-      <c r="O1108"/>
+      <c r="U1107"/>
+    </row>
+    <row r="1108" spans="16:21">
       <c r="P1108"/>
       <c r="Q1108"/>
       <c r="R1108"/>
       <c r="S1108"/>
       <c r="T1108"/>
-    </row>
-    <row r="1109" spans="15:20">
-      <c r="O1109"/>
+      <c r="U1108"/>
+    </row>
+    <row r="1109" spans="16:21">
       <c r="P1109"/>
       <c r="Q1109"/>
       <c r="R1109"/>
       <c r="S1109"/>
       <c r="T1109"/>
-    </row>
-    <row r="1110" spans="15:20">
-      <c r="O1110"/>
+      <c r="U1109"/>
+    </row>
+    <row r="1110" spans="16:21">
       <c r="P1110"/>
       <c r="Q1110"/>
       <c r="R1110"/>
       <c r="S1110"/>
       <c r="T1110"/>
-    </row>
-    <row r="1111" spans="15:20">
-      <c r="O1111"/>
+      <c r="U1110"/>
+    </row>
+    <row r="1111" spans="16:21">
       <c r="P1111"/>
       <c r="Q1111"/>
       <c r="R1111"/>
       <c r="S1111"/>
       <c r="T1111"/>
-    </row>
-    <row r="1112" spans="15:20">
-      <c r="O1112"/>
+      <c r="U1111"/>
+    </row>
+    <row r="1112" spans="16:21">
       <c r="P1112"/>
       <c r="Q1112"/>
       <c r="R1112"/>
       <c r="S1112"/>
       <c r="T1112"/>
-    </row>
-    <row r="1113" spans="15:20">
-      <c r="O1113"/>
+      <c r="U1112"/>
+    </row>
+    <row r="1113" spans="16:21">
       <c r="P1113"/>
       <c r="Q1113"/>
       <c r="R1113"/>
       <c r="S1113"/>
       <c r="T1113"/>
-    </row>
-    <row r="1114" spans="15:20">
-      <c r="O1114"/>
+      <c r="U1113"/>
+    </row>
+    <row r="1114" spans="16:21">
       <c r="P1114"/>
       <c r="Q1114"/>
       <c r="R1114"/>
       <c r="S1114"/>
       <c r="T1114"/>
-    </row>
-    <row r="1115" spans="15:20">
-      <c r="O1115"/>
+      <c r="U1114"/>
+    </row>
+    <row r="1115" spans="16:21">
       <c r="P1115"/>
       <c r="Q1115"/>
       <c r="R1115"/>
       <c r="S1115"/>
       <c r="T1115"/>
-    </row>
-    <row r="1116" spans="15:20">
-      <c r="O1116"/>
+      <c r="U1115"/>
+    </row>
+    <row r="1116" spans="16:21">
       <c r="P1116"/>
       <c r="Q1116"/>
       <c r="R1116"/>
       <c r="S1116"/>
       <c r="T1116"/>
-    </row>
-    <row r="1117" spans="15:20">
-      <c r="O1117"/>
+      <c r="U1116"/>
+    </row>
+    <row r="1117" spans="16:21">
       <c r="P1117"/>
       <c r="Q1117"/>
       <c r="R1117"/>
       <c r="S1117"/>
       <c r="T1117"/>
-    </row>
-    <row r="1118" spans="15:20">
-      <c r="O1118"/>
+      <c r="U1117"/>
+    </row>
+    <row r="1118" spans="16:21">
       <c r="P1118"/>
       <c r="Q1118"/>
       <c r="R1118"/>
       <c r="S1118"/>
       <c r="T1118"/>
-    </row>
-    <row r="1119" spans="15:20">
-      <c r="O1119"/>
+      <c r="U1118"/>
+    </row>
+    <row r="1119" spans="16:21">
       <c r="P1119"/>
       <c r="Q1119"/>
       <c r="R1119"/>
       <c r="S1119"/>
       <c r="T1119"/>
-    </row>
-    <row r="1120" spans="15:20">
-      <c r="O1120"/>
+      <c r="U1119"/>
+    </row>
+    <row r="1120" spans="16:21">
       <c r="P1120"/>
       <c r="Q1120"/>
       <c r="R1120"/>
       <c r="S1120"/>
       <c r="T1120"/>
-    </row>
-    <row r="1121" spans="15:20">
-      <c r="O1121"/>
+      <c r="U1120"/>
+    </row>
+    <row r="1121" spans="16:21">
       <c r="P1121"/>
       <c r="Q1121"/>
       <c r="R1121"/>
       <c r="S1121"/>
       <c r="T1121"/>
-    </row>
-    <row r="1122" spans="15:20">
-      <c r="O1122"/>
+      <c r="U1121"/>
+    </row>
+    <row r="1122" spans="16:21">
       <c r="P1122"/>
       <c r="Q1122"/>
       <c r="R1122"/>
       <c r="S1122"/>
       <c r="T1122"/>
-    </row>
-    <row r="1123" spans="15:20">
-      <c r="O1123"/>
+      <c r="U1122"/>
+    </row>
+    <row r="1123" spans="16:21">
       <c r="P1123"/>
       <c r="Q1123"/>
       <c r="R1123"/>
       <c r="S1123"/>
       <c r="T1123"/>
-    </row>
-    <row r="1124" spans="15:20">
-      <c r="O1124"/>
+      <c r="U1123"/>
+    </row>
+    <row r="1124" spans="16:21">
       <c r="P1124"/>
       <c r="Q1124"/>
       <c r="R1124"/>
       <c r="S1124"/>
       <c r="T1124"/>
-    </row>
-    <row r="1125" spans="15:20">
-      <c r="O1125"/>
+      <c r="U1124"/>
+    </row>
+    <row r="1125" spans="16:21">
       <c r="P1125"/>
       <c r="Q1125"/>
       <c r="R1125"/>
       <c r="S1125"/>
       <c r="T1125"/>
-    </row>
-    <row r="1126" spans="15:20">
-      <c r="O1126"/>
+      <c r="U1125"/>
+    </row>
+    <row r="1126" spans="16:21">
       <c r="P1126"/>
       <c r="Q1126"/>
       <c r="R1126"/>
       <c r="S1126"/>
       <c r="T1126"/>
-    </row>
-    <row r="1127" spans="15:20">
-      <c r="O1127"/>
+      <c r="U1126"/>
+    </row>
+    <row r="1127" spans="16:21">
       <c r="P1127"/>
       <c r="Q1127"/>
       <c r="R1127"/>
       <c r="S1127"/>
       <c r="T1127"/>
-    </row>
-    <row r="1128" spans="15:20">
-      <c r="O1128"/>
+      <c r="U1127"/>
+    </row>
+    <row r="1128" spans="16:21">
       <c r="P1128"/>
       <c r="Q1128"/>
       <c r="R1128"/>
       <c r="S1128"/>
       <c r="T1128"/>
-    </row>
-    <row r="1129" spans="15:20">
-      <c r="O1129"/>
+      <c r="U1128"/>
+    </row>
+    <row r="1129" spans="16:21">
       <c r="P1129"/>
       <c r="Q1129"/>
       <c r="R1129"/>
       <c r="S1129"/>
       <c r="T1129"/>
-    </row>
-    <row r="1130" spans="15:20">
-      <c r="O1130"/>
+      <c r="U1129"/>
+    </row>
+    <row r="1130" spans="16:21">
       <c r="P1130"/>
       <c r="Q1130"/>
       <c r="R1130"/>
       <c r="S1130"/>
       <c r="T1130"/>
-    </row>
-    <row r="1131" spans="15:20">
-      <c r="O1131"/>
+      <c r="U1130"/>
+    </row>
+    <row r="1131" spans="16:21">
       <c r="P1131"/>
       <c r="Q1131"/>
       <c r="R1131"/>
       <c r="S1131"/>
       <c r="T1131"/>
-    </row>
-    <row r="1132" spans="15:20">
-      <c r="O1132"/>
+      <c r="U1131"/>
+    </row>
+    <row r="1132" spans="16:21">
       <c r="P1132"/>
       <c r="Q1132"/>
       <c r="R1132"/>
       <c r="S1132"/>
       <c r="T1132"/>
-    </row>
-    <row r="1133" spans="15:20">
-      <c r="O1133"/>
+      <c r="U1132"/>
+    </row>
+    <row r="1133" spans="16:21">
       <c r="P1133"/>
       <c r="Q1133"/>
       <c r="R1133"/>
       <c r="S1133"/>
       <c r="T1133"/>
-    </row>
-    <row r="1134" spans="15:20">
-      <c r="O1134"/>
+      <c r="U1133"/>
+    </row>
+    <row r="1134" spans="16:21">
       <c r="P1134"/>
       <c r="Q1134"/>
       <c r="R1134"/>
       <c r="S1134"/>
       <c r="T1134"/>
-    </row>
-    <row r="1135" spans="15:20">
-      <c r="O1135"/>
+      <c r="U1134"/>
+    </row>
+    <row r="1135" spans="16:21">
       <c r="P1135"/>
       <c r="Q1135"/>
       <c r="R1135"/>
       <c r="S1135"/>
       <c r="T1135"/>
-    </row>
-    <row r="1136" spans="15:20">
-      <c r="O1136"/>
+      <c r="U1135"/>
+    </row>
+    <row r="1136" spans="16:21">
       <c r="P1136"/>
       <c r="Q1136"/>
       <c r="R1136"/>
       <c r="S1136"/>
       <c r="T1136"/>
-    </row>
-    <row r="1137" spans="15:20">
-      <c r="O1137"/>
+      <c r="U1136"/>
+    </row>
+    <row r="1137" spans="16:21">
       <c r="P1137"/>
       <c r="Q1137"/>
       <c r="R1137"/>
       <c r="S1137"/>
       <c r="T1137"/>
-    </row>
-    <row r="1138" spans="15:20">
-      <c r="O1138"/>
+      <c r="U1137"/>
+    </row>
+    <row r="1138" spans="16:21">
       <c r="P1138"/>
       <c r="Q1138"/>
       <c r="R1138"/>
       <c r="S1138"/>
       <c r="T1138"/>
-    </row>
-    <row r="1139" spans="15:20">
-      <c r="O1139"/>
+      <c r="U1138"/>
+    </row>
+    <row r="1139" spans="16:21">
       <c r="P1139"/>
       <c r="Q1139"/>
       <c r="R1139"/>
       <c r="S1139"/>
       <c r="T1139"/>
-    </row>
-    <row r="1140" spans="15:20">
-      <c r="O1140"/>
+      <c r="U1139"/>
+    </row>
+    <row r="1140" spans="16:21">
       <c r="P1140"/>
       <c r="Q1140"/>
       <c r="R1140"/>
       <c r="S1140"/>
       <c r="T1140"/>
-    </row>
-    <row r="1141" spans="15:20">
-      <c r="O1141"/>
+      <c r="U1140"/>
+    </row>
+    <row r="1141" spans="16:21">
       <c r="P1141"/>
       <c r="Q1141"/>
       <c r="R1141"/>
       <c r="S1141"/>
       <c r="T1141"/>
-    </row>
-    <row r="1142" spans="15:20">
-      <c r="O1142"/>
+      <c r="U1141"/>
+    </row>
+    <row r="1142" spans="16:21">
       <c r="P1142"/>
       <c r="Q1142"/>
       <c r="R1142"/>
       <c r="S1142"/>
       <c r="T1142"/>
-    </row>
-    <row r="1143" spans="15:20">
-      <c r="O1143"/>
+      <c r="U1142"/>
+    </row>
+    <row r="1143" spans="16:21">
       <c r="P1143"/>
       <c r="Q1143"/>
       <c r="R1143"/>
       <c r="S1143"/>
       <c r="T1143"/>
-    </row>
-    <row r="1144" spans="15:20">
-      <c r="O1144"/>
+      <c r="U1143"/>
+    </row>
+    <row r="1144" spans="16:21">
       <c r="P1144"/>
       <c r="Q1144"/>
       <c r="R1144"/>
       <c r="S1144"/>
       <c r="T1144"/>
-    </row>
-    <row r="1145" spans="15:20">
-      <c r="O1145"/>
+      <c r="U1144"/>
+    </row>
+    <row r="1145" spans="16:21">
       <c r="P1145"/>
       <c r="Q1145"/>
       <c r="R1145"/>
       <c r="S1145"/>
       <c r="T1145"/>
-    </row>
-    <row r="1146" spans="15:20">
-      <c r="O1146"/>
+      <c r="U1145"/>
+    </row>
+    <row r="1146" spans="16:21">
       <c r="P1146"/>
       <c r="Q1146"/>
       <c r="R1146"/>
       <c r="S1146"/>
       <c r="T1146"/>
-    </row>
-    <row r="1147" spans="15:20">
-      <c r="O1147"/>
+      <c r="U1146"/>
+    </row>
+    <row r="1147" spans="16:21">
       <c r="P1147"/>
       <c r="Q1147"/>
       <c r="R1147"/>
       <c r="S1147"/>
       <c r="T1147"/>
-    </row>
-    <row r="1148" spans="15:20">
-      <c r="O1148"/>
+      <c r="U1147"/>
+    </row>
+    <row r="1148" spans="16:21">
       <c r="P1148"/>
       <c r="Q1148"/>
       <c r="R1148"/>
       <c r="S1148"/>
       <c r="T1148"/>
-    </row>
-    <row r="1149" spans="15:20">
-      <c r="O1149"/>
+      <c r="U1148"/>
+    </row>
+    <row r="1149" spans="16:21">
       <c r="P1149"/>
       <c r="Q1149"/>
       <c r="R1149"/>
       <c r="S1149"/>
       <c r="T1149"/>
-    </row>
-    <row r="1150" spans="15:20">
-      <c r="O1150"/>
+      <c r="U1149"/>
+    </row>
+    <row r="1150" spans="16:21">
       <c r="P1150"/>
       <c r="Q1150"/>
       <c r="R1150"/>
       <c r="S1150"/>
       <c r="T1150"/>
-    </row>
-    <row r="1151" spans="15:20">
-      <c r="O1151"/>
+      <c r="U1150"/>
+    </row>
+    <row r="1151" spans="16:21">
       <c r="P1151"/>
       <c r="Q1151"/>
       <c r="R1151"/>
       <c r="S1151"/>
       <c r="T1151"/>
-    </row>
-    <row r="1152" spans="15:20">
-      <c r="O1152"/>
+      <c r="U1151"/>
+    </row>
+    <row r="1152" spans="16:21">
       <c r="P1152"/>
       <c r="Q1152"/>
       <c r="R1152"/>
       <c r="S1152"/>
       <c r="T1152"/>
-    </row>
-    <row r="1153" spans="15:20">
-      <c r="O1153"/>
+      <c r="U1152"/>
+    </row>
+    <row r="1153" spans="16:21">
       <c r="P1153"/>
       <c r="Q1153"/>
       <c r="R1153"/>
       <c r="S1153"/>
       <c r="T1153"/>
-    </row>
-    <row r="1154" spans="15:20">
-      <c r="O1154"/>
+      <c r="U1153"/>
+    </row>
+    <row r="1154" spans="16:21">
       <c r="P1154"/>
       <c r="Q1154"/>
       <c r="R1154"/>
       <c r="S1154"/>
       <c r="T1154"/>
-    </row>
-    <row r="1155" spans="15:20">
-      <c r="O1155"/>
+      <c r="U1154"/>
+    </row>
+    <row r="1155" spans="16:21">
       <c r="P1155"/>
       <c r="Q1155"/>
       <c r="R1155"/>
       <c r="S1155"/>
       <c r="T1155"/>
-    </row>
-    <row r="1156" spans="15:20">
-      <c r="O1156"/>
+      <c r="U1155"/>
+    </row>
+    <row r="1156" spans="16:21">
       <c r="P1156"/>
       <c r="Q1156"/>
       <c r="R1156"/>
       <c r="S1156"/>
       <c r="T1156"/>
-    </row>
-    <row r="1157" spans="15:20">
-      <c r="O1157"/>
+      <c r="U1156"/>
+    </row>
+    <row r="1157" spans="16:21">
       <c r="P1157"/>
       <c r="Q1157"/>
       <c r="R1157"/>
       <c r="S1157"/>
       <c r="T1157"/>
-    </row>
-    <row r="1158" spans="15:20">
-      <c r="O1158"/>
+      <c r="U1157"/>
+    </row>
+    <row r="1158" spans="16:21">
       <c r="P1158"/>
       <c r="Q1158"/>
       <c r="R1158"/>
       <c r="S1158"/>
       <c r="T1158"/>
-    </row>
-    <row r="1159" spans="15:20">
-      <c r="O1159"/>
+      <c r="U1158"/>
+    </row>
+    <row r="1159" spans="16:21">
       <c r="P1159"/>
       <c r="Q1159"/>
       <c r="R1159"/>
       <c r="S1159"/>
       <c r="T1159"/>
-    </row>
-    <row r="1160" spans="15:20">
-      <c r="O1160"/>
+      <c r="U1159"/>
+    </row>
+    <row r="1160" spans="16:21">
       <c r="P1160"/>
       <c r="Q1160"/>
       <c r="R1160"/>
       <c r="S1160"/>
       <c r="T1160"/>
-    </row>
-    <row r="1161" spans="15:20">
-      <c r="O1161"/>
+      <c r="U1160"/>
+    </row>
+    <row r="1161" spans="16:21">
       <c r="P1161"/>
       <c r="Q1161"/>
       <c r="R1161"/>
       <c r="S1161"/>
       <c r="T1161"/>
-    </row>
-    <row r="1162" spans="15:20">
-      <c r="O1162"/>
+      <c r="U1161"/>
+    </row>
+    <row r="1162" spans="16:21">
       <c r="P1162"/>
       <c r="Q1162"/>
       <c r="R1162"/>
       <c r="S1162"/>
       <c r="T1162"/>
-    </row>
-    <row r="1163" spans="15:20">
-      <c r="O1163"/>
+      <c r="U1162"/>
+    </row>
+    <row r="1163" spans="16:21">
       <c r="P1163"/>
       <c r="Q1163"/>
       <c r="R1163"/>
       <c r="S1163"/>
       <c r="T1163"/>
-    </row>
-    <row r="1164" spans="15:20">
-      <c r="O1164"/>
+      <c r="U1163"/>
+    </row>
+    <row r="1164" spans="16:21">
       <c r="P1164"/>
       <c r="Q1164"/>
       <c r="R1164"/>
       <c r="S1164"/>
       <c r="T1164"/>
+      <c r="U1164"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
new weinberger model outputs
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="460" windowWidth="25600" windowHeight="16000" tabRatio="902" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21260" yWindow="5480" windowWidth="25600" windowHeight="16000" tabRatio="902" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4121" uniqueCount="1073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4123" uniqueCount="1075">
   <si>
     <t>param</t>
   </si>
@@ -3327,6 +3327,12 @@
   </si>
   <si>
     <t>Run with Utah chilling</t>
+  </si>
+  <si>
+    <t>see weinberger_modelsummaries.xls for updated info</t>
+  </si>
+  <si>
+    <t>STOP: before you care about any of this…</t>
   </si>
 </sst>
 </file>
@@ -3365,6 +3371,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3387,10 +3394,11 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3424,6 +3432,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3914,7 +3928,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3986,6 +4000,8 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="395">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -5060,10 +5076,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5563,6 +5579,34 @@
       <c r="J20" s="43">
         <v>-2.5314768999999999</v>
       </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C23" s="45" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D23" s="45"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C24" s="45" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D24" s="45"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C26" s="46"/>
+      <c r="D26" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
adding to model comparison
</commit_message>
<xml_diff>
--- a/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
+++ b/analyses/bb_analysis/modelnotes/models_bb_compare.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10312"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielbuonaiuto/Documents/git/ospree/analyses/bb_analysis/modelnotes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ailene.ettinger/Documents/GitHub/ospree/analyses/bb_analysis/modelnotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC47DD23-B3CC-844E-9CEA-D206D1F0D784}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21260" yWindow="5480" windowWidth="25600" windowHeight="16000" tabRatio="902" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21260" yWindow="5480" windowWidth="25600" windowHeight="16000" tabRatio="902" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="3" r:id="rId1"/>
     <sheet name="weinberger" sheetId="13" r:id="rId2"/>
     <sheet name="chillportmods" sheetId="14" r:id="rId3"/>
-    <sheet name="OSPREE_after6Dec2018" sheetId="6" r:id="rId4"/>
-    <sheet name="OSPREE_compare_ALL (4 Dec 2018)" sheetId="12" r:id="rId5"/>
-    <sheet name="OSPREE_compare" sheetId="4" r:id="rId6"/>
-    <sheet name="Flynn_exp" sheetId="2" r:id="rId7"/>
-    <sheet name="2018NovEarly_Lizzie" sheetId="5" r:id="rId8"/>
-    <sheet name="2018Jun-Aug_LizzieAilene" sheetId="1" r:id="rId9"/>
+    <sheet name="OSPREE_Mar2019" sheetId="15" r:id="rId4"/>
+    <sheet name="OSPREE_after6Dec2018" sheetId="6" r:id="rId5"/>
+    <sheet name="OSPREE_compare_ALL (4 Dec 2018)" sheetId="12" r:id="rId6"/>
+    <sheet name="OSPREE_compare" sheetId="4" r:id="rId7"/>
+    <sheet name="Flynn_exp" sheetId="2" r:id="rId8"/>
+    <sheet name="2018NovEarly_Lizzie" sheetId="5" r:id="rId9"/>
+    <sheet name="2018Jun-Aug_LizzieAilene" sheetId="1" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4123" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4176" uniqueCount="1077">
   <si>
     <t>param</t>
   </si>
@@ -3333,6 +3335,12 @@
   </si>
   <si>
     <t>STOP: before you care about any of this…</t>
+  </si>
+  <si>
+    <t>chill.units</t>
+  </si>
+  <si>
+    <t>use.expramptypes.fp =TRUE</t>
   </si>
 </sst>
 </file>
@@ -5074,11 +5082,2219 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:R177"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="7.5" customWidth="1"/>
+    <col min="8" max="8" width="7.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" customWidth="1"/>
+    <col min="10" max="11" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="3"/>
+    <col min="16" max="16" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>71.099999999999994</v>
+      </c>
+      <c r="C3">
+        <v>94.8</v>
+      </c>
+      <c r="D3">
+        <v>32</v>
+      </c>
+      <c r="E3" s="3">
+        <v>28.6</v>
+      </c>
+      <c r="F3">
+        <v>28.8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3">
+        <v>69</v>
+      </c>
+      <c r="I3">
+        <v>97.1</v>
+      </c>
+      <c r="J3">
+        <v>71</v>
+      </c>
+      <c r="K3">
+        <v>102.3</v>
+      </c>
+      <c r="L3" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="3">
+        <v>28.41</v>
+      </c>
+      <c r="N3">
+        <v>28.9</v>
+      </c>
+      <c r="O3">
+        <v>30.33</v>
+      </c>
+      <c r="P3" s="3">
+        <v>71.34</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>94.77</v>
+      </c>
+      <c r="R3">
+        <v>128.21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>41</v>
+      </c>
+      <c r="Q4" s="5"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C5">
+        <v>-1.9</v>
+      </c>
+      <c r="D5">
+        <v>-1.3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>-4.9000000000000004</v>
+      </c>
+      <c r="F5">
+        <v>-5</v>
+      </c>
+      <c r="H5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="I5">
+        <v>-1.9</v>
+      </c>
+      <c r="J5">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="K5">
+        <v>-1.9</v>
+      </c>
+      <c r="L5">
+        <v>-1.4</v>
+      </c>
+      <c r="M5" s="3">
+        <v>-4.55</v>
+      </c>
+      <c r="N5">
+        <v>-4.63</v>
+      </c>
+      <c r="O5">
+        <v>-4.7300000000000004</v>
+      </c>
+      <c r="P5" s="3">
+        <v>-1.24</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>-1.85</v>
+      </c>
+      <c r="R5">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>-0.6</v>
+      </c>
+      <c r="C6">
+        <v>-1.3</v>
+      </c>
+      <c r="D6">
+        <v>-0.3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-3.7</v>
+      </c>
+      <c r="F6">
+        <v>-4.3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>-0.7</v>
+      </c>
+      <c r="I6">
+        <v>-1.5</v>
+      </c>
+      <c r="J6">
+        <v>-0.4</v>
+      </c>
+      <c r="K6">
+        <v>-2</v>
+      </c>
+      <c r="L6">
+        <v>-0.3</v>
+      </c>
+      <c r="M6" s="3">
+        <v>-3.83</v>
+      </c>
+      <c r="N6">
+        <v>-4.43</v>
+      </c>
+      <c r="O6">
+        <v>-2</v>
+      </c>
+      <c r="P6" s="3">
+        <v>-0.38</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>-1.41</v>
+      </c>
+      <c r="R6">
+        <v>-8.57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>-2.9</v>
+      </c>
+      <c r="C7">
+        <v>-6.9</v>
+      </c>
+      <c r="D7">
+        <v>-3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-9.5</v>
+      </c>
+      <c r="F7">
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-2.7</v>
+      </c>
+      <c r="I7">
+        <v>-7.1</v>
+      </c>
+      <c r="J7">
+        <v>-2.8</v>
+      </c>
+      <c r="K7">
+        <v>-7.4</v>
+      </c>
+      <c r="L7">
+        <v>-1.9</v>
+      </c>
+      <c r="M7" s="3">
+        <v>-8.81</v>
+      </c>
+      <c r="N7">
+        <v>-9.64</v>
+      </c>
+      <c r="O7">
+        <v>-9.35</v>
+      </c>
+      <c r="P7" s="3">
+        <v>-2.5</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>-6.94</v>
+      </c>
+      <c r="R7">
+        <v>-0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0.12</v>
+      </c>
+      <c r="F8">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I8">
+        <v>0.1</v>
+      </c>
+      <c r="K8">
+        <v>0.1</v>
+      </c>
+      <c r="N8">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>0.1</v>
+      </c>
+      <c r="F9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I9">
+        <v>0.1</v>
+      </c>
+      <c r="K9">
+        <v>0.2</v>
+      </c>
+      <c r="N9">
+        <v>2.16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F10">
+        <v>0.4</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="17">
+        <v>94.814463700000005</v>
+      </c>
+      <c r="F14">
+        <v>28.872777539617999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="17">
+        <v>-1.860117198</v>
+      </c>
+      <c r="F15">
+        <v>-4.9562006055646002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="17">
+        <v>-1.3263480139999999</v>
+      </c>
+      <c r="F16">
+        <v>-4.2589914505628004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="17">
+        <v>-6.8969933729999999</v>
+      </c>
+      <c r="F17">
+        <v>-10.240670101168901</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="17">
+        <v>25.112935619999998</v>
+      </c>
+      <c r="F18">
+        <v>9.8248067343748602</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="17">
+        <v>1.029588543</v>
+      </c>
+      <c r="F19">
+        <v>5.9249822487714203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="17">
+        <v>0.85328422800000003</v>
+      </c>
+      <c r="F20">
+        <v>5.5081353669091202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="17">
+        <v>1.9058692450000001</v>
+      </c>
+      <c r="F21">
+        <v>6.8662963935424903</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="17">
+        <v>14.64285143</v>
+      </c>
+      <c r="F22">
+        <v>14.576457996142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="17">
+        <v>110.5143128</v>
+      </c>
+      <c r="F23">
+        <v>36.0742584453942</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="17">
+        <v>79.248405340000005</v>
+      </c>
+      <c r="F24">
+        <v>29.777249149686501</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="17">
+        <v>117.639062</v>
+      </c>
+      <c r="F25">
+        <v>37.084387520987001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="17">
+        <v>93.611210380000003</v>
+      </c>
+      <c r="F26">
+        <v>31.6588994701502</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="17">
+        <v>77.547297169999993</v>
+      </c>
+      <c r="F27">
+        <v>31.9968569977116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="17">
+        <v>106.098086</v>
+      </c>
+      <c r="F28">
+        <v>32.2374466525226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C29" s="17">
+        <v>100.1006405</v>
+      </c>
+      <c r="F29">
+        <v>31.6828410408663</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="17">
+        <v>99.937920500000004</v>
+      </c>
+      <c r="F30">
+        <v>28.511381598813699</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="17">
+        <v>54.929282360000002</v>
+      </c>
+      <c r="F31">
+        <v>18.9990208169569</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="17">
+        <v>52.213019520000003</v>
+      </c>
+      <c r="F32">
+        <v>18.5438871879768</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="17">
+        <v>96.846787230000004</v>
+      </c>
+      <c r="F33">
+        <v>29.4793194429358</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="17">
+        <v>95.262957450000002</v>
+      </c>
+      <c r="F34">
+        <v>27.025363791550301</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="17">
+        <v>87.891082220000001</v>
+      </c>
+      <c r="F35">
+        <v>22.741965056386402</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="17">
+        <v>85.843369199999998</v>
+      </c>
+      <c r="F36">
+        <v>19.607586871152499</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="17">
+        <v>152.1433112</v>
+      </c>
+      <c r="F37">
+        <v>46.869632122144502</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="17">
+        <v>143.9225194</v>
+      </c>
+      <c r="F38">
+        <v>53.760615123866799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="17">
+        <v>95.667895459999997</v>
+      </c>
+      <c r="F39">
+        <v>35.259097752470602</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="17">
+        <v>73.744354599999994</v>
+      </c>
+      <c r="F40">
+        <v>20.147456494830301</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="17">
+        <v>106.9252761</v>
+      </c>
+      <c r="F41">
+        <v>31.851274133252101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="17">
+        <v>105.9088204</v>
+      </c>
+      <c r="F42">
+        <v>43.790248393613098</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="17">
+        <v>90.158385490000001</v>
+      </c>
+      <c r="F43">
+        <v>22.369492630013699</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="17">
+        <v>96.865078490000002</v>
+      </c>
+      <c r="F44">
+        <v>32.090613090099701</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="17">
+        <v>75.11756733</v>
+      </c>
+      <c r="F45">
+        <v>23.825673139029799</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="17">
+        <v>79.427001750000002</v>
+      </c>
+      <c r="F46">
+        <v>24.472450110836299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="17">
+        <v>94.170321270000002</v>
+      </c>
+      <c r="F47">
+        <v>22.622747976625899</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="17">
+        <v>147.87725549999999</v>
+      </c>
+      <c r="F48">
+        <v>37.767461164483002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" s="17">
+        <v>142.45959959999999</v>
+      </c>
+      <c r="F49">
+        <v>42.987997380496097</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C50" s="17">
+        <v>102.8968931</v>
+      </c>
+      <c r="F50">
+        <v>37.623748144585598</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" s="17">
+        <v>94.960570599999997</v>
+      </c>
+      <c r="F51">
+        <v>29.771227537573701</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="17">
+        <v>58.289234149999999</v>
+      </c>
+      <c r="F52">
+        <v>22.198221481673201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="C53" s="17">
+        <v>84.971670439999997</v>
+      </c>
+      <c r="F53">
+        <v>27.575649772829902</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" s="17">
+        <v>76.931306950000007</v>
+      </c>
+      <c r="F54">
+        <v>19.0758077887103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="17">
+        <v>79.814054229999996</v>
+      </c>
+      <c r="F55">
+        <v>15.9349819449343</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" s="17">
+        <v>88.67181961</v>
+      </c>
+      <c r="F56">
+        <v>24.005080989770502</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C57" s="17">
+        <v>75.010805500000004</v>
+      </c>
+      <c r="F57">
+        <v>20.755401162536501</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" s="17">
+        <v>96.224918869999996</v>
+      </c>
+      <c r="F58">
+        <v>20.368347391399901</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C59" s="17">
+        <v>104.2732484</v>
+      </c>
+      <c r="F59">
+        <v>19.766051348883099</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="17">
+        <v>101.4558696</v>
+      </c>
+      <c r="F60">
+        <v>27.9274234955287</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" s="17">
+        <v>-2.211713848</v>
+      </c>
+      <c r="F61">
+        <v>-7.6044208361044703</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C62" s="17">
+        <v>-1.11959371</v>
+      </c>
+      <c r="F62">
+        <v>-0.79935892096311001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="17">
+        <v>-2.2994903029999998</v>
+      </c>
+      <c r="F63">
+        <v>-7.4304054034129097</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C64" s="17">
+        <v>-1.6205861939999999</v>
+      </c>
+      <c r="F64">
+        <v>-2.0627900491187399</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" s="17">
+        <v>-0.82331376899999997</v>
+      </c>
+      <c r="F65">
+        <v>0.88222690937126702</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" s="17">
+        <v>-2.4049952889999999</v>
+      </c>
+      <c r="F66">
+        <v>-9.4037386928712099</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C67" s="17">
+        <v>-2.4274128730000002</v>
+      </c>
+      <c r="F67">
+        <v>-8.7973570037979503</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C68" s="17">
+        <v>-2.0218172870000002</v>
+      </c>
+      <c r="F68">
+        <v>-6.3460202592396699</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="C69" s="17">
+        <v>-0.98675659400000004</v>
+      </c>
+      <c r="F69">
+        <v>-0.255387708596715</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="17" t="s">
+        <v>104</v>
+      </c>
+      <c r="C70" s="17">
+        <v>-1.0824256539999999</v>
+      </c>
+      <c r="F70">
+        <v>-0.59797458502107603</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71" s="17">
+        <v>-1.538400907</v>
+      </c>
+      <c r="F71">
+        <v>-3.4219332781429701</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" s="17">
+        <v>-2.1347896369999999</v>
+      </c>
+      <c r="F72">
+        <v>-6.8620097334040802</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" s="17">
+        <v>-2.0072762819999999</v>
+      </c>
+      <c r="F73">
+        <v>-5.2631478529636802</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C74" s="17">
+        <v>-2.2132342569999999</v>
+      </c>
+      <c r="F74">
+        <v>-6.4685831937033296</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C75" s="17">
+        <v>-1.0861069409999999</v>
+      </c>
+      <c r="F75">
+        <v>-1.64852628233444</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C76" s="17">
+        <v>-3.6722116219999998</v>
+      </c>
+      <c r="F76">
+        <v>-15.6888579113165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C77" s="17">
+        <v>-1.503086105</v>
+      </c>
+      <c r="F77">
+        <v>-3.3517179050517698</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C78" s="17">
+        <v>-1.330016563</v>
+      </c>
+      <c r="F78">
+        <v>-1.699141433359</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="C79" s="17">
+        <v>-1.7371725730000001</v>
+      </c>
+      <c r="F79">
+        <v>-5.4429735076255596</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C80" s="17">
+        <v>-3.5863414050000002</v>
+      </c>
+      <c r="F80">
+        <v>-14.0978090444989</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="C81" s="17">
+        <v>-1.4353871460000001</v>
+      </c>
+      <c r="F81">
+        <v>-2.1874988960713999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C82" s="17">
+        <v>-2.0120124509999999</v>
+      </c>
+      <c r="F82">
+        <v>-6.1232093943700603</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C83" s="17">
+        <v>-1.0002978360000001</v>
+      </c>
+      <c r="F83">
+        <v>0.64368775634179298</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C84" s="17">
+        <v>-1.399484602</v>
+      </c>
+      <c r="F84">
+        <v>-0.35726724661598003</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C85" s="17">
+        <v>-2.2618060400000002</v>
+      </c>
+      <c r="F85">
+        <v>-7.2826415060251097</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C86" s="17">
+        <v>-3.525203876</v>
+      </c>
+      <c r="F86">
+        <v>-15.2741953597024</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C87" s="17">
+        <v>-3.2320859099999999</v>
+      </c>
+      <c r="F87">
+        <v>-12.5357089588242</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C88" s="17">
+        <v>-2.1571557619999999</v>
+      </c>
+      <c r="F88">
+        <v>-6.4894932240029402</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C89" s="17">
+        <v>-1.822812305</v>
+      </c>
+      <c r="F89">
+        <v>-4.33369475559034</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C90" s="17">
+        <v>0.547821259</v>
+      </c>
+      <c r="F90">
+        <v>7.5382172491077997</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C91" s="17">
+        <v>-1.5082813180000001</v>
+      </c>
+      <c r="F91">
+        <v>-1.81606289253831</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C92" s="17">
+        <v>-1.6162300940000001</v>
+      </c>
+      <c r="F92">
+        <v>-2.87593378127346</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C93" s="17">
+        <v>-2.106364605</v>
+      </c>
+      <c r="F93">
+        <v>-4.4559349265356802</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C94" s="17">
+        <v>-1.6255794729999999</v>
+      </c>
+      <c r="F94">
+        <v>-3.47352961711064</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="C95" s="17">
+        <v>-1.469568502</v>
+      </c>
+      <c r="F95">
+        <v>-2.4734316101729998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C96" s="17">
+        <v>-2.1437939309999998</v>
+      </c>
+      <c r="F96">
+        <v>-6.5560231842482999</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="C97" s="17">
+        <v>-2.5343310290000001</v>
+      </c>
+      <c r="F97">
+        <v>-8.7558381888342698</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="C98" s="17">
+        <v>-1.6384720500000001</v>
+      </c>
+      <c r="F98">
+        <v>-5.1458331569432003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C99" s="17">
+        <v>-1.292939751</v>
+      </c>
+      <c r="F99">
+        <v>-5.7545240231605304</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="C100" s="17">
+        <v>-1.0607837339999999</v>
+      </c>
+      <c r="F100">
+        <v>-2.2116331485436</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C101" s="17">
+        <v>-1.6967920000000001</v>
+      </c>
+      <c r="F101">
+        <v>-8.0863605263077396</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C102" s="17">
+        <v>-1.3187428299999999</v>
+      </c>
+      <c r="F102">
+        <v>-4.3160484095908096</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="C103" s="17">
+        <v>-1.2755335160000001</v>
+      </c>
+      <c r="F103">
+        <v>-3.4546581835470498</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C104" s="17">
+        <v>-0.98444991000000004</v>
+      </c>
+      <c r="F104">
+        <v>-2.1818301142508698</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C105" s="17">
+        <v>-1.0058950250000001</v>
+      </c>
+      <c r="F105">
+        <v>-2.0520507170885698</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C106" s="17">
+        <v>-2.1869500450000001</v>
+      </c>
+      <c r="F106">
+        <v>-9.3491398805293198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="C107" s="17">
+        <v>-1.000557524</v>
+      </c>
+      <c r="F107">
+        <v>-1.7989081023675799</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C108" s="17">
+        <v>-0.85144982499999999</v>
+      </c>
+      <c r="F108">
+        <v>-0.88203705218684703</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C109" s="17">
+        <v>-1.2034885479999999</v>
+      </c>
+      <c r="F109">
+        <v>-3.5229240185414601</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="C110" s="17">
+        <v>-1.3264061700000001</v>
+      </c>
+      <c r="F110">
+        <v>-3.8979243771010901</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C111" s="17">
+        <v>-1.2605519510000001</v>
+      </c>
+      <c r="F111">
+        <v>-2.8514176399676598</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A112" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="C112" s="17">
+        <v>-1.0713101410000001</v>
+      </c>
+      <c r="F112">
+        <v>-2.13344840547648</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="C113" s="17">
+        <v>-3.4554528709999999</v>
+      </c>
+      <c r="F113">
+        <v>-17.723878642431099</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C114" s="17">
+        <v>-0.73228888199999997</v>
+      </c>
+      <c r="F114">
+        <v>-2.8115836833671199</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A115" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C115" s="17">
+        <v>-1.2694831440000001</v>
+      </c>
+      <c r="F115">
+        <v>-4.8778867493016902</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A116" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C116" s="17">
+        <v>-1.277481262</v>
+      </c>
+      <c r="F116">
+        <v>-2.2300566411645102</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A117" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C117" s="17">
+        <v>-1.8540429970000001</v>
+      </c>
+      <c r="F117">
+        <v>-7.9201708601130996</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A118" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C118" s="17">
+        <v>0.47940949799999999</v>
+      </c>
+      <c r="F118">
+        <v>7.1145900034110499</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A119" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="C119" s="17">
+        <v>-1.1936774699999999</v>
+      </c>
+      <c r="F119">
+        <v>-2.92396248645142</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A120" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C120" s="17">
+        <v>-0.92901788399999996</v>
+      </c>
+      <c r="F120">
+        <v>-1.5818151757586201</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A121" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C121" s="17">
+        <v>-1.3161578249999999</v>
+      </c>
+      <c r="F121">
+        <v>-2.3392034180091801</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A122" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="C122" s="17">
+        <v>-1.134418047</v>
+      </c>
+      <c r="F122">
+        <v>-1.9141370813698899</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A123" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C123" s="17">
+        <v>-0.99250506999999999</v>
+      </c>
+      <c r="F123">
+        <v>-2.0471495556789301</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A124" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C124" s="17">
+        <v>-1.0473612050000001</v>
+      </c>
+      <c r="F124">
+        <v>-7.0492602941017299</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A125" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="C125" s="17">
+        <v>-1.1508566309999999</v>
+      </c>
+      <c r="F125">
+        <v>-4.8474910488270799</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A126" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C126" s="17">
+        <v>-1.1209454940000001</v>
+      </c>
+      <c r="F126">
+        <v>-3.9040360299961598</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A127" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C127" s="17">
+        <v>-1.664803402</v>
+      </c>
+      <c r="F127">
+        <v>-6.4809363851313604</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A128" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="C128" s="17">
+        <v>-2.335638957</v>
+      </c>
+      <c r="F128">
+        <v>-10.324207438637099</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C129" s="17">
+        <v>-1.094796404</v>
+      </c>
+      <c r="F129">
+        <v>-2.2602169770151002</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C130" s="17">
+        <v>-1.7747992429999999</v>
+      </c>
+      <c r="F130">
+        <v>-5.5378084506324203</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="C131" s="17">
+        <v>-0.97719068200000003</v>
+      </c>
+      <c r="F131">
+        <v>-0.78779205675369102</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C132" s="17">
+        <v>-1.308950882</v>
+      </c>
+      <c r="F132">
+        <v>-3.26822786862023</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C133" s="17">
+        <v>-1.2509183610000001</v>
+      </c>
+      <c r="F133">
+        <v>-2.2152855838393402</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="C134" s="17">
+        <v>-2.300630575</v>
+      </c>
+      <c r="F134">
+        <v>-10.108073257002401</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C135" s="17">
+        <v>-1.341631349</v>
+      </c>
+      <c r="F135">
+        <v>-4.2767398602837803</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C136" s="17">
+        <v>-1.8308629780000001</v>
+      </c>
+      <c r="F136">
+        <v>-8.6070487815047496</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="C137" s="17">
+        <v>-6.897118539</v>
+      </c>
+      <c r="F137">
+        <v>-11.536988066518299</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C138" s="17">
+        <v>-6.7552686480000004</v>
+      </c>
+      <c r="F138">
+        <v>-10.2488752061957</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C139" s="17">
+        <v>-6.8046791879999997</v>
+      </c>
+      <c r="F139">
+        <v>-11.1573953090369</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C140" s="17">
+        <v>-6.1646410429999996</v>
+      </c>
+      <c r="F140">
+        <v>-8.2061103698879894</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C141" s="17">
+        <v>-6.2656440150000003</v>
+      </c>
+      <c r="F141">
+        <v>-6.7929176799041997</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="C142" s="17">
+        <v>-7.2948766149999997</v>
+      </c>
+      <c r="F142">
+        <v>-12.447441878663099</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C143" s="17">
+        <v>-6.0828205300000002</v>
+      </c>
+      <c r="F143">
+        <v>-7.4790176849791603</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C144" s="17">
+        <v>-4.8291021670000003</v>
+      </c>
+      <c r="F144">
+        <v>-3.70463860250939</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A145" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="C145" s="17">
+        <v>-4.958667653</v>
+      </c>
+      <c r="F145">
+        <v>-3.9136786401124302</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A146" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="C146" s="17">
+        <v>-4.577585193</v>
+      </c>
+      <c r="F146">
+        <v>-2.8563714470575898</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A147" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C147" s="17">
+        <v>-8.4265167569999999</v>
+      </c>
+      <c r="F147">
+        <v>-16.0898029702625</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A148" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="C148" s="17">
+        <v>-6.3206566400000002</v>
+      </c>
+      <c r="F148">
+        <v>-8.4383380086097795</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A149" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="C149" s="17">
+        <v>-6.5234073840000004</v>
+      </c>
+      <c r="F149">
+        <v>-8.80634264258115</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A150" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C150" s="17">
+        <v>-6.5338266909999998</v>
+      </c>
+      <c r="F150">
+        <v>-9.2068654020608598</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A151" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="C151" s="17">
+        <v>-10.665304020000001</v>
+      </c>
+      <c r="F151">
+        <v>-23.790441957207801</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A152" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="C152" s="17">
+        <v>-6.887223724</v>
+      </c>
+      <c r="F152">
+        <v>-10.5906045462725</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A153" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C153" s="17">
+        <v>-6.7165885860000003</v>
+      </c>
+      <c r="F153">
+        <v>-9.6175177507994896</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A154" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="C154" s="17">
+        <v>-6.6846708530000001</v>
+      </c>
+      <c r="F154">
+        <v>-8.6090538816656696</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A155" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="C155" s="17">
+        <v>-7.7230365299999999</v>
+      </c>
+      <c r="F155">
+        <v>-13.877554918440801</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A156" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C156" s="17">
+        <v>-5.3369577369999996</v>
+      </c>
+      <c r="F156">
+        <v>-5.3041465413262099</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A157" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="C157" s="17">
+        <v>-9.098733824</v>
+      </c>
+      <c r="F157">
+        <v>-17.126830884541999</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A158" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="C158" s="17">
+        <v>-7.1151102570000004</v>
+      </c>
+      <c r="F158">
+        <v>-11.2340640120901</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A159" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C159" s="17">
+        <v>-7.2546955930000001</v>
+      </c>
+      <c r="F159">
+        <v>-9.8983598549914102</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A160" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C160" s="17">
+        <v>-6.8537062649999996</v>
+      </c>
+      <c r="F160">
+        <v>-8.4847366465141594</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="C161" s="17">
+        <v>-7.6229570889999998</v>
+      </c>
+      <c r="F161">
+        <v>-13.4419296536323</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C162" s="17">
+        <v>-10.40300238</v>
+      </c>
+      <c r="F162">
+        <v>-24.536435340682299</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="C163" s="17">
+        <v>-8.8452509450000001</v>
+      </c>
+      <c r="F163">
+        <v>-18.941298822543299</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C164" s="17">
+        <v>-5.8638908220000001</v>
+      </c>
+      <c r="F164">
+        <v>-6.5501243787505201</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C165" s="17">
+        <v>-5.5828554160000001</v>
+      </c>
+      <c r="F165">
+        <v>-5.7087471246316897</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C166" s="17">
+        <v>-6.1100515660000001</v>
+      </c>
+      <c r="F166">
+        <v>-8.0214845535710602</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="C167" s="17">
+        <v>-6.7188374749999999</v>
+      </c>
+      <c r="F167">
+        <v>-8.79301280547846</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C168" s="17">
+        <v>-4.9407132650000003</v>
+      </c>
+      <c r="F168">
+        <v>-2.9714934190400801</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="C169" s="17">
+        <v>-7.599781267</v>
+      </c>
+      <c r="F169">
+        <v>-7.5180384367053001</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A170" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C170" s="17">
+        <v>-7.4875352900000003</v>
+      </c>
+      <c r="F170">
+        <v>-12.3244639894406</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C171" s="17">
+        <v>-6.2956824239999998</v>
+      </c>
+      <c r="F171">
+        <v>-7.4308129320985401</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="C172" s="17">
+        <v>-5.1578048179999998</v>
+      </c>
+      <c r="F172">
+        <v>-4.2959740161039104</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C173" s="17">
+        <v>-8.0718366469999996</v>
+      </c>
+      <c r="F173">
+        <v>-14.704543884051899</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C174" s="17">
+        <v>-8.4299853099999993</v>
+      </c>
+      <c r="F174">
+        <v>-14.357072917312401</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C175" s="17">
+        <v>0.125935295</v>
+      </c>
+      <c r="F175">
+        <v>2.2046594901758398</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C176" s="17">
+        <v>0.104218877</v>
+      </c>
+      <c r="F176">
+        <v>2.1628863085605099</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C177" s="17">
+        <v>7.256635E-3</v>
+      </c>
+      <c r="F177">
+        <v>0.42242222246427802</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -5825,11 +8041,347 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DC7BEF-3AEF-3A4E-BEE2-FDE625199ACD}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="2" max="5" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>212</v>
+      </c>
+      <c r="B1" t="s">
+        <v>992</v>
+      </c>
+      <c r="C1" t="s">
+        <v>992</v>
+      </c>
+      <c r="D1" t="s">
+        <v>992</v>
+      </c>
+      <c r="E1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="18"/>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="40" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>1032</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>221</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>1031</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>1031</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1076</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1076</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1075</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>1056</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>1062</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>214</v>
+      </c>
+      <c r="B11">
+        <v>1729</v>
+      </c>
+      <c r="C11">
+        <v>1729</v>
+      </c>
+      <c r="D11">
+        <v>1729</v>
+      </c>
+      <c r="E11">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>211</v>
+      </c>
+      <c r="B12">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>37</v>
+      </c>
+      <c r="D12">
+        <v>37</v>
+      </c>
+      <c r="E12">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>215</v>
+      </c>
+      <c r="B14" t="s">
+        <v>214</v>
+      </c>
+      <c r="C14" t="s">
+        <v>216</v>
+      </c>
+      <c r="D14" t="s">
+        <v>214</v>
+      </c>
+      <c r="E14" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="21">
+        <v>67.040000000000006</v>
+      </c>
+      <c r="C16" s="21">
+        <v>30.73</v>
+      </c>
+      <c r="D16">
+        <v>62.78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="21">
+        <v>-0.85</v>
+      </c>
+      <c r="C18" s="21">
+        <v>-4.18</v>
+      </c>
+      <c r="D18">
+        <v>-0.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="21">
+        <v>-0.53</v>
+      </c>
+      <c r="C19" s="21">
+        <v>-3.17</v>
+      </c>
+      <c r="D19">
+        <v>-0.54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="21">
+        <v>-0.25</v>
+      </c>
+      <c r="C20" s="21">
+        <v>-8.16</v>
+      </c>
+      <c r="D20">
+        <v>-2.84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="21">
+        <v>22.06</v>
+      </c>
+      <c r="C23" s="21">
+        <v>10.16</v>
+      </c>
+      <c r="D23">
+        <v>19.2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="21">
+        <v>1</v>
+      </c>
+      <c r="C24" s="21">
+        <v>6.02</v>
+      </c>
+      <c r="D24">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="21">
+        <v>0.71</v>
+      </c>
+      <c r="C25" s="21">
+        <v>4.49</v>
+      </c>
+      <c r="D25">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="21">
+        <v>0.21</v>
+      </c>
+      <c r="C26" s="21">
+        <v>7.85</v>
+      </c>
+      <c r="D26">
+        <v>2.06</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="21">
+        <v>15.52</v>
+      </c>
+      <c r="C27" s="21">
+        <v>15.47</v>
+      </c>
+      <c r="D27">
+        <v>15.82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AF1164"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A21" sqref="A21:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13767,12 +16319,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:BA1207"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:F27"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -65102,7 +67654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M1187"/>
   <sheetViews>
@@ -80059,7 +82611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -80251,7 +82803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A3:N39"/>
   <sheetViews>
@@ -81163,2212 +83715,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:R177"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="7.5" customWidth="1"/>
-    <col min="8" max="8" width="7.83203125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="9.83203125" customWidth="1"/>
-    <col min="10" max="11" width="8.6640625" customWidth="1"/>
-    <col min="12" max="12" width="8" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="3"/>
-    <col min="16" max="16" width="10.83203125" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>71.099999999999994</v>
-      </c>
-      <c r="C3">
-        <v>94.8</v>
-      </c>
-      <c r="D3">
-        <v>32</v>
-      </c>
-      <c r="E3" s="3">
-        <v>28.6</v>
-      </c>
-      <c r="F3">
-        <v>28.8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="3">
-        <v>69</v>
-      </c>
-      <c r="I3">
-        <v>97.1</v>
-      </c>
-      <c r="J3">
-        <v>71</v>
-      </c>
-      <c r="K3">
-        <v>102.3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" s="3">
-        <v>28.41</v>
-      </c>
-      <c r="N3">
-        <v>28.9</v>
-      </c>
-      <c r="O3">
-        <v>30.33</v>
-      </c>
-      <c r="P3" s="3">
-        <v>71.34</v>
-      </c>
-      <c r="Q3" s="5">
-        <v>94.77</v>
-      </c>
-      <c r="R3">
-        <v>128.21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4">
-        <v>41</v>
-      </c>
-      <c r="Q4" s="5"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="C5">
-        <v>-1.9</v>
-      </c>
-      <c r="D5">
-        <v>-1.3</v>
-      </c>
-      <c r="E5" s="3">
-        <v>-4.9000000000000004</v>
-      </c>
-      <c r="F5">
-        <v>-5</v>
-      </c>
-      <c r="H5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="I5">
-        <v>-1.9</v>
-      </c>
-      <c r="J5">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="K5">
-        <v>-1.9</v>
-      </c>
-      <c r="L5">
-        <v>-1.4</v>
-      </c>
-      <c r="M5" s="3">
-        <v>-4.55</v>
-      </c>
-      <c r="N5">
-        <v>-4.63</v>
-      </c>
-      <c r="O5">
-        <v>-4.7300000000000004</v>
-      </c>
-      <c r="P5" s="3">
-        <v>-1.24</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>-1.85</v>
-      </c>
-      <c r="R5">
-        <v>5.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>-0.6</v>
-      </c>
-      <c r="C6">
-        <v>-1.3</v>
-      </c>
-      <c r="D6">
-        <v>-0.3</v>
-      </c>
-      <c r="E6" s="3">
-        <v>-3.7</v>
-      </c>
-      <c r="F6">
-        <v>-4.3</v>
-      </c>
-      <c r="H6" s="3">
-        <v>-0.7</v>
-      </c>
-      <c r="I6">
-        <v>-1.5</v>
-      </c>
-      <c r="J6">
-        <v>-0.4</v>
-      </c>
-      <c r="K6">
-        <v>-2</v>
-      </c>
-      <c r="L6">
-        <v>-0.3</v>
-      </c>
-      <c r="M6" s="3">
-        <v>-3.83</v>
-      </c>
-      <c r="N6">
-        <v>-4.43</v>
-      </c>
-      <c r="O6">
-        <v>-2</v>
-      </c>
-      <c r="P6" s="3">
-        <v>-0.38</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>-1.41</v>
-      </c>
-      <c r="R6">
-        <v>-8.57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>-2.9</v>
-      </c>
-      <c r="C7">
-        <v>-6.9</v>
-      </c>
-      <c r="D7">
-        <v>-3</v>
-      </c>
-      <c r="E7" s="3">
-        <v>-9.5</v>
-      </c>
-      <c r="F7">
-        <v>-10.199999999999999</v>
-      </c>
-      <c r="H7" s="3">
-        <v>-2.7</v>
-      </c>
-      <c r="I7">
-        <v>-7.1</v>
-      </c>
-      <c r="J7">
-        <v>-2.8</v>
-      </c>
-      <c r="K7">
-        <v>-7.4</v>
-      </c>
-      <c r="L7">
-        <v>-1.9</v>
-      </c>
-      <c r="M7" s="3">
-        <v>-8.81</v>
-      </c>
-      <c r="N7">
-        <v>-9.64</v>
-      </c>
-      <c r="O7">
-        <v>-9.35</v>
-      </c>
-      <c r="P7" s="3">
-        <v>-2.5</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>-6.94</v>
-      </c>
-      <c r="R7">
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>0.12</v>
-      </c>
-      <c r="F8">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I8">
-        <v>0.1</v>
-      </c>
-      <c r="K8">
-        <v>0.1</v>
-      </c>
-      <c r="N8">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>0.1</v>
-      </c>
-      <c r="F9">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="I9">
-        <v>0.1</v>
-      </c>
-      <c r="K9">
-        <v>0.2</v>
-      </c>
-      <c r="N9">
-        <v>2.16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="F10">
-        <v>0.4</v>
-      </c>
-      <c r="I10">
-        <v>0</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="N10">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="17">
-        <v>94.814463700000005</v>
-      </c>
-      <c r="F14">
-        <v>28.872777539617999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="17">
-        <v>-1.860117198</v>
-      </c>
-      <c r="F15">
-        <v>-4.9562006055646002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="17">
-        <v>-1.3263480139999999</v>
-      </c>
-      <c r="F16">
-        <v>-4.2589914505628004</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="17">
-        <v>-6.8969933729999999</v>
-      </c>
-      <c r="F17">
-        <v>-10.240670101168901</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C18" s="17">
-        <v>25.112935619999998</v>
-      </c>
-      <c r="F18">
-        <v>9.8248067343748602</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="17">
-        <v>1.029588543</v>
-      </c>
-      <c r="F19">
-        <v>5.9249822487714203</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="17">
-        <v>0.85328422800000003</v>
-      </c>
-      <c r="F20">
-        <v>5.5081353669091202</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="17">
-        <v>1.9058692450000001</v>
-      </c>
-      <c r="F21">
-        <v>6.8662963935424903</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="17">
-        <v>14.64285143</v>
-      </c>
-      <c r="F22">
-        <v>14.576457996142</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="17">
-        <v>110.5143128</v>
-      </c>
-      <c r="F23">
-        <v>36.0742584453942</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="17">
-        <v>79.248405340000005</v>
-      </c>
-      <c r="F24">
-        <v>29.777249149686501</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="17">
-        <v>117.639062</v>
-      </c>
-      <c r="F25">
-        <v>37.084387520987001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C26" s="17">
-        <v>93.611210380000003</v>
-      </c>
-      <c r="F26">
-        <v>31.6588994701502</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="17">
-        <v>77.547297169999993</v>
-      </c>
-      <c r="F27">
-        <v>31.9968569977116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="17">
-        <v>106.098086</v>
-      </c>
-      <c r="F28">
-        <v>32.2374466525226</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="17">
-        <v>100.1006405</v>
-      </c>
-      <c r="F29">
-        <v>31.6828410408663</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="17">
-        <v>99.937920500000004</v>
-      </c>
-      <c r="F30">
-        <v>28.511381598813699</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="17">
-        <v>54.929282360000002</v>
-      </c>
-      <c r="F31">
-        <v>18.9990208169569</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="17">
-        <v>52.213019520000003</v>
-      </c>
-      <c r="F32">
-        <v>18.5438871879768</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" s="17">
-        <v>96.846787230000004</v>
-      </c>
-      <c r="F33">
-        <v>29.4793194429358</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="17">
-        <v>95.262957450000002</v>
-      </c>
-      <c r="F34">
-        <v>27.025363791550301</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="17">
-        <v>87.891082220000001</v>
-      </c>
-      <c r="F35">
-        <v>22.741965056386402</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="17">
-        <v>85.843369199999998</v>
-      </c>
-      <c r="F36">
-        <v>19.607586871152499</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="C37" s="17">
-        <v>152.1433112</v>
-      </c>
-      <c r="F37">
-        <v>46.869632122144502</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="17">
-        <v>143.9225194</v>
-      </c>
-      <c r="F38">
-        <v>53.760615123866799</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="C39" s="17">
-        <v>95.667895459999997</v>
-      </c>
-      <c r="F39">
-        <v>35.259097752470602</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C40" s="17">
-        <v>73.744354599999994</v>
-      </c>
-      <c r="F40">
-        <v>20.147456494830301</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="17">
-        <v>106.9252761</v>
-      </c>
-      <c r="F41">
-        <v>31.851274133252101</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="17">
-        <v>105.9088204</v>
-      </c>
-      <c r="F42">
-        <v>43.790248393613098</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="17">
-        <v>90.158385490000001</v>
-      </c>
-      <c r="F43">
-        <v>22.369492630013699</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="C44" s="17">
-        <v>96.865078490000002</v>
-      </c>
-      <c r="F44">
-        <v>32.090613090099701</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C45" s="17">
-        <v>75.11756733</v>
-      </c>
-      <c r="F45">
-        <v>23.825673139029799</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="C46" s="17">
-        <v>79.427001750000002</v>
-      </c>
-      <c r="F46">
-        <v>24.472450110836299</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="17">
-        <v>94.170321270000002</v>
-      </c>
-      <c r="F47">
-        <v>22.622747976625899</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="C48" s="17">
-        <v>147.87725549999999</v>
-      </c>
-      <c r="F48">
-        <v>37.767461164483002</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="C49" s="17">
-        <v>142.45959959999999</v>
-      </c>
-      <c r="F49">
-        <v>42.987997380496097</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="17">
-        <v>102.8968931</v>
-      </c>
-      <c r="F50">
-        <v>37.623748144585598</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" s="17">
-        <v>94.960570599999997</v>
-      </c>
-      <c r="F51">
-        <v>29.771227537573701</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="17" t="s">
-        <v>86</v>
-      </c>
-      <c r="C52" s="17">
-        <v>58.289234149999999</v>
-      </c>
-      <c r="F52">
-        <v>22.198221481673201</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="C53" s="17">
-        <v>84.971670439999997</v>
-      </c>
-      <c r="F53">
-        <v>27.575649772829902</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="C54" s="17">
-        <v>76.931306950000007</v>
-      </c>
-      <c r="F54">
-        <v>19.0758077887103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C55" s="17">
-        <v>79.814054229999996</v>
-      </c>
-      <c r="F55">
-        <v>15.9349819449343</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="C56" s="17">
-        <v>88.67181961</v>
-      </c>
-      <c r="F56">
-        <v>24.005080989770502</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C57" s="17">
-        <v>75.010805500000004</v>
-      </c>
-      <c r="F57">
-        <v>20.755401162536501</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="C58" s="17">
-        <v>96.224918869999996</v>
-      </c>
-      <c r="F58">
-        <v>20.368347391399901</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="17" t="s">
-        <v>93</v>
-      </c>
-      <c r="C59" s="17">
-        <v>104.2732484</v>
-      </c>
-      <c r="F59">
-        <v>19.766051348883099</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="C60" s="17">
-        <v>101.4558696</v>
-      </c>
-      <c r="F60">
-        <v>27.9274234955287</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="C61" s="17">
-        <v>-2.211713848</v>
-      </c>
-      <c r="F61">
-        <v>-7.6044208361044703</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="C62" s="17">
-        <v>-1.11959371</v>
-      </c>
-      <c r="F62">
-        <v>-0.79935892096311001</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C63" s="17">
-        <v>-2.2994903029999998</v>
-      </c>
-      <c r="F63">
-        <v>-7.4304054034129097</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C64" s="17">
-        <v>-1.6205861939999999</v>
-      </c>
-      <c r="F64">
-        <v>-2.0627900491187399</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C65" s="17">
-        <v>-0.82331376899999997</v>
-      </c>
-      <c r="F65">
-        <v>0.88222690937126702</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C66" s="17">
-        <v>-2.4049952889999999</v>
-      </c>
-      <c r="F66">
-        <v>-9.4037386928712099</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="C67" s="17">
-        <v>-2.4274128730000002</v>
-      </c>
-      <c r="F67">
-        <v>-8.7973570037979503</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C68" s="17">
-        <v>-2.0218172870000002</v>
-      </c>
-      <c r="F68">
-        <v>-6.3460202592396699</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C69" s="17">
-        <v>-0.98675659400000004</v>
-      </c>
-      <c r="F69">
-        <v>-0.255387708596715</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C70" s="17">
-        <v>-1.0824256539999999</v>
-      </c>
-      <c r="F70">
-        <v>-0.59797458502107603</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="C71" s="17">
-        <v>-1.538400907</v>
-      </c>
-      <c r="F71">
-        <v>-3.4219332781429701</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="C72" s="17">
-        <v>-2.1347896369999999</v>
-      </c>
-      <c r="F72">
-        <v>-6.8620097334040802</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="C73" s="17">
-        <v>-2.0072762819999999</v>
-      </c>
-      <c r="F73">
-        <v>-5.2631478529636802</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="C74" s="17">
-        <v>-2.2132342569999999</v>
-      </c>
-      <c r="F74">
-        <v>-6.4685831937033296</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="C75" s="17">
-        <v>-1.0861069409999999</v>
-      </c>
-      <c r="F75">
-        <v>-1.64852628233444</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="C76" s="17">
-        <v>-3.6722116219999998</v>
-      </c>
-      <c r="F76">
-        <v>-15.6888579113165</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="17" t="s">
-        <v>111</v>
-      </c>
-      <c r="C77" s="17">
-        <v>-1.503086105</v>
-      </c>
-      <c r="F77">
-        <v>-3.3517179050517698</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="C78" s="17">
-        <v>-1.330016563</v>
-      </c>
-      <c r="F78">
-        <v>-1.699141433359</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C79" s="17">
-        <v>-1.7371725730000001</v>
-      </c>
-      <c r="F79">
-        <v>-5.4429735076255596</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="C80" s="17">
-        <v>-3.5863414050000002</v>
-      </c>
-      <c r="F80">
-        <v>-14.0978090444989</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C81" s="17">
-        <v>-1.4353871460000001</v>
-      </c>
-      <c r="F81">
-        <v>-2.1874988960713999</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="C82" s="17">
-        <v>-2.0120124509999999</v>
-      </c>
-      <c r="F82">
-        <v>-6.1232093943700603</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C83" s="17">
-        <v>-1.0002978360000001</v>
-      </c>
-      <c r="F83">
-        <v>0.64368775634179298</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C84" s="17">
-        <v>-1.399484602</v>
-      </c>
-      <c r="F84">
-        <v>-0.35726724661598003</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C85" s="17">
-        <v>-2.2618060400000002</v>
-      </c>
-      <c r="F85">
-        <v>-7.2826415060251097</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="C86" s="17">
-        <v>-3.525203876</v>
-      </c>
-      <c r="F86">
-        <v>-15.2741953597024</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="C87" s="17">
-        <v>-3.2320859099999999</v>
-      </c>
-      <c r="F87">
-        <v>-12.5357089588242</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="C88" s="17">
-        <v>-2.1571557619999999</v>
-      </c>
-      <c r="F88">
-        <v>-6.4894932240029402</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C89" s="17">
-        <v>-1.822812305</v>
-      </c>
-      <c r="F89">
-        <v>-4.33369475559034</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="C90" s="17">
-        <v>0.547821259</v>
-      </c>
-      <c r="F90">
-        <v>7.5382172491077997</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="C91" s="17">
-        <v>-1.5082813180000001</v>
-      </c>
-      <c r="F91">
-        <v>-1.81606289253831</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="C92" s="17">
-        <v>-1.6162300940000001</v>
-      </c>
-      <c r="F92">
-        <v>-2.87593378127346</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="C93" s="17">
-        <v>-2.106364605</v>
-      </c>
-      <c r="F93">
-        <v>-4.4559349265356802</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="C94" s="17">
-        <v>-1.6255794729999999</v>
-      </c>
-      <c r="F94">
-        <v>-3.47352961711064</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="C95" s="17">
-        <v>-1.469568502</v>
-      </c>
-      <c r="F95">
-        <v>-2.4734316101729998</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="C96" s="17">
-        <v>-2.1437939309999998</v>
-      </c>
-      <c r="F96">
-        <v>-6.5560231842482999</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="C97" s="17">
-        <v>-2.5343310290000001</v>
-      </c>
-      <c r="F97">
-        <v>-8.7558381888342698</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="C98" s="17">
-        <v>-1.6384720500000001</v>
-      </c>
-      <c r="F98">
-        <v>-5.1458331569432003</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A99" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="C99" s="17">
-        <v>-1.292939751</v>
-      </c>
-      <c r="F99">
-        <v>-5.7545240231605304</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A100" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="C100" s="17">
-        <v>-1.0607837339999999</v>
-      </c>
-      <c r="F100">
-        <v>-2.2116331485436</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A101" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C101" s="17">
-        <v>-1.6967920000000001</v>
-      </c>
-      <c r="F101">
-        <v>-8.0863605263077396</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="C102" s="17">
-        <v>-1.3187428299999999</v>
-      </c>
-      <c r="F102">
-        <v>-4.3160484095908096</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="C103" s="17">
-        <v>-1.2755335160000001</v>
-      </c>
-      <c r="F103">
-        <v>-3.4546581835470498</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="C104" s="17">
-        <v>-0.98444991000000004</v>
-      </c>
-      <c r="F104">
-        <v>-2.1818301142508698</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="17" t="s">
-        <v>139</v>
-      </c>
-      <c r="C105" s="17">
-        <v>-1.0058950250000001</v>
-      </c>
-      <c r="F105">
-        <v>-2.0520507170885698</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="C106" s="17">
-        <v>-2.1869500450000001</v>
-      </c>
-      <c r="F106">
-        <v>-9.3491398805293198</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="C107" s="17">
-        <v>-1.000557524</v>
-      </c>
-      <c r="F107">
-        <v>-1.7989081023675799</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="C108" s="17">
-        <v>-0.85144982499999999</v>
-      </c>
-      <c r="F108">
-        <v>-0.88203705218684703</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C109" s="17">
-        <v>-1.2034885479999999</v>
-      </c>
-      <c r="F109">
-        <v>-3.5229240185414601</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A110" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="C110" s="17">
-        <v>-1.3264061700000001</v>
-      </c>
-      <c r="F110">
-        <v>-3.8979243771010901</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="C111" s="17">
-        <v>-1.2605519510000001</v>
-      </c>
-      <c r="F111">
-        <v>-2.8514176399676598</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="C112" s="17">
-        <v>-1.0713101410000001</v>
-      </c>
-      <c r="F112">
-        <v>-2.13344840547648</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="C113" s="17">
-        <v>-3.4554528709999999</v>
-      </c>
-      <c r="F113">
-        <v>-17.723878642431099</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A114" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="C114" s="17">
-        <v>-0.73228888199999997</v>
-      </c>
-      <c r="F114">
-        <v>-2.8115836833671199</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A115" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C115" s="17">
-        <v>-1.2694831440000001</v>
-      </c>
-      <c r="F115">
-        <v>-4.8778867493016902</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A116" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="C116" s="17">
-        <v>-1.277481262</v>
-      </c>
-      <c r="F116">
-        <v>-2.2300566411645102</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A117" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="C117" s="17">
-        <v>-1.8540429970000001</v>
-      </c>
-      <c r="F117">
-        <v>-7.9201708601130996</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="C118" s="17">
-        <v>0.47940949799999999</v>
-      </c>
-      <c r="F118">
-        <v>7.1145900034110499</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A119" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="C119" s="17">
-        <v>-1.1936774699999999</v>
-      </c>
-      <c r="F119">
-        <v>-2.92396248645142</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A120" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C120" s="17">
-        <v>-0.92901788399999996</v>
-      </c>
-      <c r="F120">
-        <v>-1.5818151757586201</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A121" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="C121" s="17">
-        <v>-1.3161578249999999</v>
-      </c>
-      <c r="F121">
-        <v>-2.3392034180091801</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A122" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="C122" s="17">
-        <v>-1.134418047</v>
-      </c>
-      <c r="F122">
-        <v>-1.9141370813698899</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A123" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="C123" s="17">
-        <v>-0.99250506999999999</v>
-      </c>
-      <c r="F123">
-        <v>-2.0471495556789301</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A124" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C124" s="17">
-        <v>-1.0473612050000001</v>
-      </c>
-      <c r="F124">
-        <v>-7.0492602941017299</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A125" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="C125" s="17">
-        <v>-1.1508566309999999</v>
-      </c>
-      <c r="F125">
-        <v>-4.8474910488270799</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A126" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="C126" s="17">
-        <v>-1.1209454940000001</v>
-      </c>
-      <c r="F126">
-        <v>-3.9040360299961598</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A127" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="C127" s="17">
-        <v>-1.664803402</v>
-      </c>
-      <c r="F127">
-        <v>-6.4809363851313604</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A128" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="C128" s="17">
-        <v>-2.335638957</v>
-      </c>
-      <c r="F128">
-        <v>-10.324207438637099</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A129" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="C129" s="17">
-        <v>-1.094796404</v>
-      </c>
-      <c r="F129">
-        <v>-2.2602169770151002</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A130" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="C130" s="17">
-        <v>-1.7747992429999999</v>
-      </c>
-      <c r="F130">
-        <v>-5.5378084506324203</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A131" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="C131" s="17">
-        <v>-0.97719068200000003</v>
-      </c>
-      <c r="F131">
-        <v>-0.78779205675369102</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C132" s="17">
-        <v>-1.308950882</v>
-      </c>
-      <c r="F132">
-        <v>-3.26822786862023</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A133" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="C133" s="17">
-        <v>-1.2509183610000001</v>
-      </c>
-      <c r="F133">
-        <v>-2.2152855838393402</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A134" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="C134" s="17">
-        <v>-2.300630575</v>
-      </c>
-      <c r="F134">
-        <v>-10.108073257002401</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A135" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="C135" s="17">
-        <v>-1.341631349</v>
-      </c>
-      <c r="F135">
-        <v>-4.2767398602837803</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A136" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="C136" s="17">
-        <v>-1.8308629780000001</v>
-      </c>
-      <c r="F136">
-        <v>-8.6070487815047496</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A137" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="C137" s="17">
-        <v>-6.897118539</v>
-      </c>
-      <c r="F137">
-        <v>-11.536988066518299</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A138" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="C138" s="17">
-        <v>-6.7552686480000004</v>
-      </c>
-      <c r="F138">
-        <v>-10.2488752061957</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A139" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="C139" s="17">
-        <v>-6.8046791879999997</v>
-      </c>
-      <c r="F139">
-        <v>-11.1573953090369</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A140" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C140" s="17">
-        <v>-6.1646410429999996</v>
-      </c>
-      <c r="F140">
-        <v>-8.2061103698879894</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A141" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C141" s="17">
-        <v>-6.2656440150000003</v>
-      </c>
-      <c r="F141">
-        <v>-6.7929176799041997</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A142" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="C142" s="17">
-        <v>-7.2948766149999997</v>
-      </c>
-      <c r="F142">
-        <v>-12.447441878663099</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A143" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C143" s="17">
-        <v>-6.0828205300000002</v>
-      </c>
-      <c r="F143">
-        <v>-7.4790176849791603</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A144" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C144" s="17">
-        <v>-4.8291021670000003</v>
-      </c>
-      <c r="F144">
-        <v>-3.70463860250939</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="C145" s="17">
-        <v>-4.958667653</v>
-      </c>
-      <c r="F145">
-        <v>-3.9136786401124302</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="C146" s="17">
-        <v>-4.577585193</v>
-      </c>
-      <c r="F146">
-        <v>-2.8563714470575898</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" s="17" t="s">
-        <v>181</v>
-      </c>
-      <c r="C147" s="17">
-        <v>-8.4265167569999999</v>
-      </c>
-      <c r="F147">
-        <v>-16.0898029702625</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A148" s="17" t="s">
-        <v>182</v>
-      </c>
-      <c r="C148" s="17">
-        <v>-6.3206566400000002</v>
-      </c>
-      <c r="F148">
-        <v>-8.4383380086097795</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A149" s="17" t="s">
-        <v>183</v>
-      </c>
-      <c r="C149" s="17">
-        <v>-6.5234073840000004</v>
-      </c>
-      <c r="F149">
-        <v>-8.80634264258115</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A150" s="17" t="s">
-        <v>184</v>
-      </c>
-      <c r="C150" s="17">
-        <v>-6.5338266909999998</v>
-      </c>
-      <c r="F150">
-        <v>-9.2068654020608598</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="C151" s="17">
-        <v>-10.665304020000001</v>
-      </c>
-      <c r="F151">
-        <v>-23.790441957207801</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A152" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="C152" s="17">
-        <v>-6.887223724</v>
-      </c>
-      <c r="F152">
-        <v>-10.5906045462725</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="C153" s="17">
-        <v>-6.7165885860000003</v>
-      </c>
-      <c r="F153">
-        <v>-9.6175177507994896</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="C154" s="17">
-        <v>-6.6846708530000001</v>
-      </c>
-      <c r="F154">
-        <v>-8.6090538816656696</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A155" s="17" t="s">
-        <v>189</v>
-      </c>
-      <c r="C155" s="17">
-        <v>-7.7230365299999999</v>
-      </c>
-      <c r="F155">
-        <v>-13.877554918440801</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A156" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="C156" s="17">
-        <v>-5.3369577369999996</v>
-      </c>
-      <c r="F156">
-        <v>-5.3041465413262099</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A157" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="C157" s="17">
-        <v>-9.098733824</v>
-      </c>
-      <c r="F157">
-        <v>-17.126830884541999</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A158" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="C158" s="17">
-        <v>-7.1151102570000004</v>
-      </c>
-      <c r="F158">
-        <v>-11.2340640120901</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A159" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="C159" s="17">
-        <v>-7.2546955930000001</v>
-      </c>
-      <c r="F159">
-        <v>-9.8983598549914102</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A160" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="C160" s="17">
-        <v>-6.8537062649999996</v>
-      </c>
-      <c r="F160">
-        <v>-8.4847366465141594</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A161" s="17" t="s">
-        <v>195</v>
-      </c>
-      <c r="C161" s="17">
-        <v>-7.6229570889999998</v>
-      </c>
-      <c r="F161">
-        <v>-13.4419296536323</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A162" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C162" s="17">
-        <v>-10.40300238</v>
-      </c>
-      <c r="F162">
-        <v>-24.536435340682299</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A163" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="C163" s="17">
-        <v>-8.8452509450000001</v>
-      </c>
-      <c r="F163">
-        <v>-18.941298822543299</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A164" s="17" t="s">
-        <v>198</v>
-      </c>
-      <c r="C164" s="17">
-        <v>-5.8638908220000001</v>
-      </c>
-      <c r="F164">
-        <v>-6.5501243787505201</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A165" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="C165" s="17">
-        <v>-5.5828554160000001</v>
-      </c>
-      <c r="F165">
-        <v>-5.7087471246316897</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A166" s="17" t="s">
-        <v>200</v>
-      </c>
-      <c r="C166" s="17">
-        <v>-6.1100515660000001</v>
-      </c>
-      <c r="F166">
-        <v>-8.0214845535710602</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A167" s="17" t="s">
-        <v>201</v>
-      </c>
-      <c r="C167" s="17">
-        <v>-6.7188374749999999</v>
-      </c>
-      <c r="F167">
-        <v>-8.79301280547846</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A168" s="17" t="s">
-        <v>202</v>
-      </c>
-      <c r="C168" s="17">
-        <v>-4.9407132650000003</v>
-      </c>
-      <c r="F168">
-        <v>-2.9714934190400801</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A169" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="C169" s="17">
-        <v>-7.599781267</v>
-      </c>
-      <c r="F169">
-        <v>-7.5180384367053001</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A170" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="C170" s="17">
-        <v>-7.4875352900000003</v>
-      </c>
-      <c r="F170">
-        <v>-12.3244639894406</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A171" s="17" t="s">
-        <v>205</v>
-      </c>
-      <c r="C171" s="17">
-        <v>-6.2956824239999998</v>
-      </c>
-      <c r="F171">
-        <v>-7.4308129320985401</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A172" s="17" t="s">
-        <v>206</v>
-      </c>
-      <c r="C172" s="17">
-        <v>-5.1578048179999998</v>
-      </c>
-      <c r="F172">
-        <v>-4.2959740161039104</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A173" s="17" t="s">
-        <v>207</v>
-      </c>
-      <c r="C173" s="17">
-        <v>-8.0718366469999996</v>
-      </c>
-      <c r="F173">
-        <v>-14.704543884051899</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A174" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="C174" s="17">
-        <v>-8.4299853099999993</v>
-      </c>
-      <c r="F174">
-        <v>-14.357072917312401</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A175" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C175" s="17">
-        <v>0.125935295</v>
-      </c>
-      <c r="F175">
-        <v>2.2046594901758398</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A176" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="C176" s="17">
-        <v>0.104218877</v>
-      </c>
-      <c r="F176">
-        <v>2.1628863085605099</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A177" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="C177" s="17">
-        <v>7.256635E-3</v>
-      </c>
-      <c r="F177">
-        <v>0.42242222246427802</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>